<commit_message>
update 2x2 scalar test
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\BoxSync\CGE\MPSGE-JL\CGE_GAMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1898F46C-900A-4CFC-8136-1B7489C66DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5C5D3-53EF-4678-8FAE-81DFC928B160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="680" windowWidth="14400" windowHeight="7460" firstSheet="1" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1600" yWindow="1520" windowWidth="6410" windowHeight="3320" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -539,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261E1F9A-63EC-417B-A1CC-BD7ADDD403FF}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -714,170 +714,206 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>52.433302256670352</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>52.440442408507586</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>52.440442408500388</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>1.0095490890260126</v>
+        <v>21.173597011026523</v>
       </c>
       <c r="D12">
-        <v>1.009576582776887</v>
+        <v>21.17705705843569</v>
       </c>
       <c r="E12">
-        <v>1.0095765827768624</v>
+        <v>21.177057058432069</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>1.0031729514067342</v>
+        <v>47.679621391858859</v>
       </c>
       <c r="D13">
-        <v>1.0031820580257143</v>
+        <v>47.673129462279633</v>
       </c>
       <c r="E13">
-        <v>1.0031820580257051</v>
+        <v>47.673129462283626</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C14">
-        <v>0.95359242784919818</v>
+        <v>28.880951004956579</v>
       </c>
       <c r="D14">
-        <v>0.95346258924559202</v>
+        <v>28.877805079685029</v>
       </c>
       <c r="E14">
-        <v>0.95346258924580818</v>
+        <v>28.877805079687114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C15">
-        <v>1.0486660451591012</v>
+        <v>100.3172951406718</v>
       </c>
       <c r="D15">
-        <v>1.0488088481701519</v>
+        <v>100.31820580257144</v>
       </c>
       <c r="E15">
-        <v>1.0488088481700457</v>
+        <v>100.31820580257069</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>49.684208638846584</v>
+      </c>
+      <c r="D16">
+        <v>49.683306602972891</v>
+      </c>
+      <c r="E16">
+        <v>49.683306602973595</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1.0095490890260126</v>
+      </c>
+      <c r="D18">
+        <v>1.009576582776887</v>
+      </c>
+      <c r="E18">
+        <v>1.0095765827768624</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1.0031729514067342</v>
+      </c>
+      <c r="D19">
+        <v>1.0031820580257143</v>
+      </c>
+      <c r="E19">
+        <v>1.0031820580257051</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0.95359242784919818</v>
+      </c>
+      <c r="D20">
+        <v>0.95346258924559202</v>
+      </c>
+      <c r="E20">
+        <v>0.95346258924580818</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1.0486660451591012</v>
+      </c>
+      <c r="D21">
+        <v>1.0488088481701519</v>
+      </c>
+      <c r="E21">
+        <v>1.0488088481700457</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16">
+      <c r="B22">
         <v>150</v>
       </c>
-      <c r="C16">
+      <c r="C22">
         <v>157</v>
       </c>
-      <c r="D16">
+      <c r="D22">
         <v>157.32132722552274</v>
       </c>
-      <c r="E16">
+      <c r="E22">
         <v>157.32132722553087</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <v>52.433302256670352</v>
-      </c>
-      <c r="D17">
-        <v>52.440442408507586</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18">
-        <v>21.173597011026523</v>
-      </c>
-      <c r="D18">
-        <v>21.17705705843569</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <v>47.679621391858859</v>
-      </c>
-      <c r="D19">
-        <v>47.673129462279633</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <v>28.880951004956579</v>
-      </c>
-      <c r="D20">
-        <v>28.877805079685029</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21">
-        <v>100.3172951406718</v>
-      </c>
-      <c r="D21">
-        <v>100.31820580257144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>49.684208638846584</v>
-      </c>
-      <c r="D22">
-        <v>49.683306602972891</v>
       </c>
     </row>
   </sheetData>
@@ -2342,7 +2378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A14746-3E00-4CD5-9B40-B03C7F420D4C}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>

<commit_message>
clean up jpmge test (impl vars)
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B946A61-DE4A-4E68-AD5F-32CB5900BC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9159EA5F-4CAC-4F5D-B764-2B9506C72D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="1860" windowWidth="6410" windowHeight="3320" firstSheet="3" activeTab="3" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7460" firstSheet="3" activeTab="3" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="59">
   <si>
     <t>X.L</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>D Y=6.4</t>
+  </si>
+  <si>
+    <t>CWI</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1712,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9A728-5CCB-48DE-B29A-AA0B43EB195B}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
@@ -1799,58 +1802,58 @@
         <v>4</v>
       </c>
       <c r="E2" s="2">
-        <v>6.0086272827607878</v>
+        <v>6.0271570694089363</v>
       </c>
       <c r="F2" s="2">
-        <v>3.969734742721247</v>
+        <v>3.9819768629877865</v>
       </c>
       <c r="G2" s="2">
-        <v>6.0086273837631206</v>
+        <v>6.0271570813322075</v>
       </c>
       <c r="H2" s="2">
-        <v>3.9697347814888042</v>
+        <v>3.9819768428170277</v>
       </c>
       <c r="I2" s="2">
-        <v>6.0086272827461693</v>
+        <v>6.0271570694027758</v>
       </c>
       <c r="J2" s="2">
-        <v>3.9697347427227063</v>
+        <v>3.9819768629948684</v>
       </c>
       <c r="K2" s="2">
-        <v>6.070435101918509</v>
+        <v>6.0285029175131495</v>
       </c>
       <c r="L2" s="2">
-        <v>4.0087789692547222</v>
+        <v>3.9810878966780647</v>
       </c>
       <c r="M2">
-        <v>6.0704352490597788</v>
+        <v>6.0285029321430184</v>
       </c>
       <c r="N2">
-        <v>4.0087790323026393</v>
+        <v>3.9810878724541241</v>
       </c>
       <c r="O2">
-        <v>6.0704351019154714</v>
+        <v>6.0285029175126947</v>
       </c>
       <c r="P2">
-        <v>4.0087789692526794</v>
+        <v>3.9810878966777277</v>
       </c>
       <c r="Q2">
-        <v>5.9527613306717484</v>
+        <v>6.0259370963253147</v>
       </c>
       <c r="R2">
-        <v>3.9344182362759095</v>
+        <v>3.9827830288230945</v>
       </c>
       <c r="S2">
-        <v>5.9527613780232977</v>
+        <v>6.025937105223008</v>
       </c>
       <c r="T2">
-        <v>3.9344182460282098</v>
+        <v>3.9827830128948642</v>
       </c>
       <c r="U2">
-        <v>5.9527613306711453</v>
+        <v>6.0259370963252268</v>
       </c>
       <c r="V2">
-        <v>3.9344182362754143</v>
+        <v>3.9827830288229387</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
@@ -1867,58 +1870,58 @@
         <v>2</v>
       </c>
       <c r="E3" s="2">
-        <v>2.2332352321214946</v>
+        <v>2.0306618580514879</v>
       </c>
       <c r="F3" s="2">
-        <v>2.1663031890054865</v>
+        <v>1.9698011188502622</v>
       </c>
       <c r="G3" s="2">
-        <v>2.2332352424687842</v>
+        <v>2.0306618717316747</v>
       </c>
       <c r="H3" s="2">
-        <v>2.1663031645018793</v>
+        <v>1.9698011007128038</v>
       </c>
       <c r="I3" s="2">
-        <v>2.2332352320993802</v>
+        <v>2.0306618580444193</v>
       </c>
       <c r="J3" s="2">
-        <v>2.1663031890009434</v>
+        <v>1.9698011188587803</v>
       </c>
       <c r="K3" s="2">
-        <v>2.2245672645540826</v>
+        <v>2.0322072644723499</v>
       </c>
       <c r="L3" s="2">
-        <v>2.1546142829123349</v>
+        <v>1.968303169627029</v>
       </c>
       <c r="M3">
-        <v>2.2245672727916879</v>
+        <v>2.0322072812850394</v>
       </c>
       <c r="N3">
-        <v>2.1546142489574196</v>
+        <v>1.9683031476035679</v>
       </c>
       <c r="O3">
-        <v>2.2245672645490631</v>
+        <v>2.0322072644718245</v>
       </c>
       <c r="P3">
-        <v>2.1546142829083506</v>
+        <v>1.9683031696273214</v>
       </c>
       <c r="Q3">
-        <v>2.2410583217899034</v>
+        <v>2.0292631412455764</v>
       </c>
       <c r="R3">
-        <v>2.1768896575049337</v>
+        <v>1.9711588500763715</v>
       </c>
       <c r="S3">
-        <v>2.2410583348961191</v>
+        <v>2.0292631514394697</v>
       </c>
       <c r="T3">
-        <v>2.1768896440189911</v>
+        <v>1.9711588362391685</v>
       </c>
       <c r="U3">
-        <v>2.2410583217882571</v>
+        <v>2.0292631412454765</v>
       </c>
       <c r="V3">
-        <v>2.1768896575034709</v>
+        <v>1.9711588500763977</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -1935,58 +1938,58 @@
         <v>2</v>
       </c>
       <c r="E4" s="2">
-        <v>1.966529187661999</v>
+        <v>1.9725936953390322</v>
       </c>
       <c r="F4" s="2">
-        <v>2.0215528819412558</v>
+        <v>2.0277870751833285</v>
       </c>
       <c r="G4" s="2">
-        <v>1.9665292047218597</v>
+        <v>1.9725936831953861</v>
       </c>
       <c r="H4" s="2">
-        <v>2.0215529181274978</v>
+        <v>2.0277870814064576</v>
       </c>
       <c r="I4" s="2">
-        <v>1.9665291876654798</v>
+        <v>1.9725936953453067</v>
       </c>
       <c r="J4" s="2">
-        <v>2.021552881933502</v>
+        <v>2.0277870751784119</v>
       </c>
       <c r="K4" s="2">
-        <v>1.9849334846109026</v>
+        <v>1.9712223427385891</v>
       </c>
       <c r="L4" s="2">
-        <v>2.0433121780876582</v>
+        <v>2.0291977791012972</v>
       </c>
       <c r="M4">
-        <v>1.9849335128890031</v>
+        <v>1.9712223278246288</v>
       </c>
       <c r="N4">
-        <v>2.0433122306418272</v>
+        <v>2.0291977870311428</v>
       </c>
       <c r="O4">
-        <v>1.9849334846105282</v>
+        <v>1.9712223427390549</v>
       </c>
       <c r="P4">
-        <v>2.0433121780859791</v>
+        <v>2.029197779100492</v>
       </c>
       <c r="Q4">
-        <v>1.9498664921172697</v>
+        <v>1.9738356999448601</v>
       </c>
       <c r="R4">
-        <v>2.0019022524769183</v>
+        <v>2.026511122537574</v>
       </c>
       <c r="S4">
-        <v>1.9498664958038201</v>
+        <v>1.9738356908902481</v>
       </c>
       <c r="T4">
-        <v>2.0019022695783657</v>
+        <v>2.0265111267215343</v>
       </c>
       <c r="U4">
-        <v>1.949866492117188</v>
+        <v>1.9738356999449487</v>
       </c>
       <c r="V4">
-        <v>2.0019022524765471</v>
+        <v>2.0265111225373742</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
@@ -2003,58 +2006,58 @@
         <v>6</v>
       </c>
       <c r="E5" s="2">
-        <v>10.963541405244653</v>
+        <v>9.9690552256106191</v>
       </c>
       <c r="F5" s="2">
-        <v>6.6190263159355167</v>
+        <v>6.018624497716182</v>
       </c>
       <c r="G5" s="2">
-        <v>10.96354136685996</v>
+        <v>9.9690552116775866</v>
       </c>
       <c r="H5" s="2">
-        <v>6.6190262949080987</v>
+        <v>6.0186244912562668</v>
       </c>
       <c r="I5" s="2">
-        <v>10.963541405182166</v>
+        <v>9.9690552256178169</v>
       </c>
       <c r="J5" s="2">
-        <v>6.6190263158938167</v>
+        <v>6.018624497716913</v>
       </c>
       <c r="K5" s="2">
-        <v>10.910959374527764</v>
+        <v>9.9674805327690024</v>
       </c>
       <c r="L5" s="2">
-        <v>6.5893624524400236</v>
+        <v>6.019575338295823</v>
       </c>
       <c r="M5">
-        <v>10.910959305902068</v>
+        <v>9.9674805156298323</v>
       </c>
       <c r="N5">
-        <v>6.5893624144422303</v>
+        <v>6.0195753310938045</v>
       </c>
       <c r="O5">
-        <v>10.910959374506552</v>
+        <v>9.9674805327695388</v>
       </c>
       <c r="P5">
-        <v>6.5893624524257799</v>
+        <v>6.0195753382948372</v>
       </c>
       <c r="Q5">
-        <v>11.011102963317315</v>
+        <v>9.9704792020198632</v>
       </c>
       <c r="R5">
-        <v>6.645841972628391</v>
+        <v>6.0177649222561822</v>
       </c>
       <c r="S5">
-        <v>11.011102960942685</v>
+        <v>9.9704791916461968</v>
       </c>
       <c r="T5">
-        <v>6.6458419717566732</v>
+        <v>6.0177649165035128</v>
       </c>
       <c r="U5">
-        <v>11.011102963309883</v>
+        <v>9.9704792020199662</v>
       </c>
       <c r="V5">
-        <v>6.6458419726235292</v>
+        <v>6.0177649222559033</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
@@ -2069,35 +2072,35 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>1.0294255138385817</v>
+        <v>1.0326001216556313</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <v>1.0294255431580739</v>
+        <v>1.0326001357507444</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2">
-        <v>1.0294255138282276</v>
+        <v>1.032600121646702</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2">
-        <v>1.0414586403838779</v>
+        <v>1.0342646526340822</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6">
-        <v>1.0414586805191435</v>
+        <v>1.0342646699325051</v>
       </c>
       <c r="O6">
-        <v>1.0414586403827182</v>
+        <v>1.0342646526333701</v>
       </c>
       <c r="Q6">
-        <v>1.0185742873068173</v>
+        <v>1.0310953593284131</v>
       </c>
       <c r="S6">
-        <v>1.0185743040856408</v>
+        <v>1.031095369634073</v>
       </c>
       <c r="U6">
-        <v>1.0185742873065731</v>
+        <v>1.0310953593282555</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -2112,35 +2115,35 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
-        <v>3.3705744862087736</v>
+        <v>3.0648347968089404</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <v>3.3705745111657768</v>
+        <v>3.0648348259489921</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2">
-        <v>3.3705744861665643</v>
+        <v>3.0648347967902407</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2">
-        <v>3.3585413596161509</v>
+        <v>3.068125768905853</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7">
-        <v>3.3585413832969815</v>
+        <v>3.0681258045606343</v>
       </c>
       <c r="O7">
-        <v>3.3585413596079117</v>
+        <v>3.0681257689044559</v>
       </c>
       <c r="Q7">
-        <v>3.3814257126931051</v>
+        <v>3.0618580948610665</v>
       </c>
       <c r="S7">
-        <v>3.3814257390651354</v>
+        <v>3.0618581162154008</v>
       </c>
       <c r="U7">
-        <v>3.3814257126904477</v>
+        <v>3.0618580948607583</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -2155,35 +2158,35 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
-        <v>0.95629285402282127</v>
+        <v>0.95924193069612929</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <v>0.95629286865924534</v>
+        <v>0.95924193115089085</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2">
-        <v>0.95629285402757258</v>
+        <v>0.95924193070224861</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2">
-        <v>0.9638796195720013</v>
+        <v>0.9572215172656795</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8">
-        <v>0.96387964040158569</v>
+        <v>0.957221517072259</v>
       </c>
       <c r="O8">
-        <v>0.96387961957334634</v>
+        <v>0.957221517267422</v>
       </c>
       <c r="Q8">
-        <v>0.94940262027556399</v>
+        <v>0.96107338276594034</v>
       </c>
       <c r="S8">
-        <v>0.94940262820400689</v>
+        <v>0.96107338456602553</v>
       </c>
       <c r="U8">
-        <v>0.94940262027596189</v>
+        <v>0.96107338276642651</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -2198,35 +2201,35 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
-        <v>1.0437071459705156</v>
+        <v>0.9490340568757426</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <v>1.0437071399465965</v>
+        <v>0.94903405339453106</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
-        <v>1.0437071459731286</v>
+        <v>0.94903405688421294</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2">
-        <v>1.0361203804279788</v>
+        <v>0.94652627390687871</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9">
-        <v>1.0361203701947646</v>
+        <v>0.94652626888426039</v>
       </c>
       <c r="O9">
-        <v>1.0361203804280366</v>
+        <v>0.94652627390882238</v>
       </c>
       <c r="Q9">
-        <v>1.0505973797245405</v>
+        <v>0.95130881612284057</v>
       </c>
       <c r="S9">
-        <v>1.0505973793854231</v>
+        <v>0.95130881503115117</v>
       </c>
       <c r="U9">
-        <v>1.050597379724407</v>
+        <v>0.95130881612337159</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
@@ -2542,7 +2545,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2">
-        <v>2.1058245831109526</v>
+        <v>2.1058245831317985</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
@@ -2585,7 +2588,7 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2">
-        <v>4.2894913950169853</v>
+        <v>4.2894913950594482</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
@@ -2614,6 +2617,17 @@
       </c>
       <c r="U18">
         <v>4.3132252303282845</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for CET
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9159EA5F-4CAC-4F5D-B764-2B9506C72D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2C741E-0ABA-4B88-9D47-BC3694400CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7460" firstSheet="3" activeTab="3" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7460" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
     <sheet name="TwoxTwoJPMGE" sheetId="4" r:id="rId2"/>
     <sheet name="TwoxTwoCESProd" sheetId="5" r:id="rId3"/>
     <sheet name="JPMGE" sheetId="6" r:id="rId4"/>
+    <sheet name="TwoxTwoCET-Scalar" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="89">
   <si>
     <t>X.L</t>
   </si>
@@ -213,6 +214,96 @@
   </si>
   <si>
     <t>CWI</t>
+  </si>
+  <si>
+    <t>A.L</t>
+  </si>
+  <si>
+    <t>B.L</t>
+  </si>
+  <si>
+    <t>W.L</t>
+  </si>
+  <si>
+    <t>PW.L</t>
+  </si>
+  <si>
+    <t>CONS.L</t>
+  </si>
+  <si>
+    <t>SAX.L</t>
+  </si>
+  <si>
+    <t>SAY.L</t>
+  </si>
+  <si>
+    <t>SBX.L</t>
+  </si>
+  <si>
+    <t>SBY.L</t>
+  </si>
+  <si>
+    <t>DAL.L</t>
+  </si>
+  <si>
+    <t>DAK.L</t>
+  </si>
+  <si>
+    <t>DBL.L</t>
+  </si>
+  <si>
+    <t>DBK.L</t>
+  </si>
+  <si>
+    <t>SW.L</t>
+  </si>
+  <si>
+    <t>DWX.L</t>
+  </si>
+  <si>
+    <t>DWY.L</t>
+  </si>
+  <si>
+    <t>DW.L</t>
+  </si>
+  <si>
+    <t>CWI.L</t>
+  </si>
+  <si>
+    <t>PX.L/PW.L</t>
+  </si>
+  <si>
+    <t>PY.L/PW.L</t>
+  </si>
+  <si>
+    <t>PW.L/PW.L</t>
+  </si>
+  <si>
+    <t>PL.L/PW.L</t>
+  </si>
+  <si>
+    <t>PK.L/PW.L</t>
+  </si>
+  <si>
+    <t>CONS.L/PW.L</t>
+  </si>
+  <si>
+    <t>diff=10</t>
+  </si>
+  <si>
+    <t>PW.FX=1</t>
+  </si>
+  <si>
+    <t>TrA=2, TrB=1.5</t>
+  </si>
+  <si>
+    <t>TA=0.1</t>
+  </si>
+  <si>
+    <t>TA=100%</t>
+  </si>
+  <si>
+    <t>Undf</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9A728-5CCB-48DE-B29A-AA0B43EB195B}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2633,4 +2724,678 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E4E009-E95D-4525-8C72-CDF28BC03388}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.84841617526015112</v>
+      </c>
+      <c r="D2">
+        <v>0.8484161751970315</v>
+      </c>
+      <c r="E2">
+        <v>0.70716515735515006</v>
+      </c>
+      <c r="F2">
+        <v>0.38751484805497743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.1506325096039884</v>
+      </c>
+      <c r="D3">
+        <v>1.1506325095207364</v>
+      </c>
+      <c r="E3">
+        <v>1.2893059702343606</v>
+      </c>
+      <c r="F3">
+        <v>1.5972629436210768</v>
+      </c>
+      <c r="G3">
+        <v>1.9601317042077897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0035850931326258</v>
+      </c>
+      <c r="D4">
+        <v>1.0035850930478027</v>
+      </c>
+      <c r="E4">
+        <v>1.0068914996667162</v>
+      </c>
+      <c r="F4">
+        <v>0.99916851890038427</v>
+      </c>
+      <c r="G4">
+        <v>0.97073779227082346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0231427182799986</v>
+      </c>
+      <c r="D5">
+        <v>1.026810780303149</v>
+      </c>
+      <c r="E5">
+        <v>1.0161855054344244</v>
+      </c>
+      <c r="F5">
+        <v>1.0862618717772732</v>
+      </c>
+      <c r="G5">
+        <v>1.1690468695684746</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.87359232216492444</v>
+      </c>
+      <c r="D6">
+        <v>0.87672423219236795</v>
+      </c>
+      <c r="E6">
+        <v>0.88681325620491058</v>
+      </c>
+      <c r="F6">
+        <v>0.8240896931384919</v>
+      </c>
+      <c r="G6">
+        <v>0.76012909543532714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.99642771370717265</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.0314650721357199</v>
+      </c>
+      <c r="D8">
+        <v>1.0351629708854646</v>
+      </c>
+      <c r="E8">
+        <v>1.0678356276899741</v>
+      </c>
+      <c r="F8">
+        <v>1.1033933594907179</v>
+      </c>
+      <c r="G8">
+        <v>1.1648853507249877</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.96853492724769141</v>
+      </c>
+      <c r="D9">
+        <v>0.97200721521014155</v>
+      </c>
+      <c r="E9">
+        <v>0.94594737164343623</v>
+      </c>
+      <c r="F9">
+        <v>0.85817103861968913</v>
+      </c>
+      <c r="G9">
+        <v>0.77659023381665881</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>200.71701860956063</v>
+      </c>
+      <c r="E10">
+        <v>201.37829993334105</v>
+      </c>
+      <c r="F10">
+        <v>199.83370377972741</v>
+      </c>
+      <c r="G10">
+        <v>194.14755845416465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>80.000000000000014</v>
+      </c>
+      <c r="D11">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>83.789979418307453</v>
+      </c>
+      <c r="F11">
+        <v>86.636474448757937</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>20.000000000000004</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>15.953297102016906</v>
+      </c>
+      <c r="F12">
+        <v>12.465814866890884</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>30.000000000000004</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>34.553784903611799</v>
+      </c>
+      <c r="F13">
+        <v>39.310669882974452</v>
+      </c>
+      <c r="G13">
+        <v>44.380086793200221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>80</v>
+      </c>
+      <c r="E14">
+        <v>75.119576065481453</v>
+      </c>
+      <c r="F14">
+        <v>69.26902850423329</v>
+      </c>
+      <c r="G14">
+        <v>62.049748999369605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>38.517354230045243</v>
+      </c>
+      <c r="D15">
+        <v>38.517354222141414</v>
+      </c>
+      <c r="E15">
+        <v>37.194397849630214</v>
+      </c>
+      <c r="F15">
+        <v>34.40060528627518</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>61.530004404080294</v>
+      </c>
+      <c r="D16">
+        <v>61.53000441249764</v>
+      </c>
+      <c r="E16">
+        <v>62.98051725431754</v>
+      </c>
+      <c r="F16">
+        <v>66.345864158482783</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>58.508040668387657</v>
+      </c>
+      <c r="D17">
+        <v>58.508040660383685</v>
+      </c>
+      <c r="E17">
+        <v>57.160534034089842</v>
+      </c>
+      <c r="F17">
+        <v>54.261106485862463</v>
+      </c>
+      <c r="G17">
+        <v>51.016980025031643</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>41.539717147859804</v>
+      </c>
+      <c r="D18">
+        <v>41.539717156383809</v>
+      </c>
+      <c r="E18">
+        <v>43.017230886987115</v>
+      </c>
+      <c r="F18">
+        <v>46.51080952457405</v>
+      </c>
+      <c r="G18">
+        <v>51.016980025031621</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>200.71701862652515</v>
+      </c>
+      <c r="D19">
+        <v>200.71701860956054</v>
+      </c>
+      <c r="E19">
+        <v>201.37829993334324</v>
+      </c>
+      <c r="F19">
+        <v>199.83370378007686</v>
+      </c>
+      <c r="G19">
+        <v>194.14755845416468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>102.3922693035888</v>
+      </c>
+      <c r="D20">
+        <v>102.39226930136157</v>
+      </c>
+      <c r="E20">
+        <v>103.80375515055297</v>
+      </c>
+      <c r="F20">
+        <v>96.362396524949176</v>
+      </c>
+      <c r="G20">
+        <v>86.990815158845137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>109.01892428236799</v>
+      </c>
+      <c r="D21">
+        <v>109.0189242656265</v>
+      </c>
+      <c r="E21">
+        <v>108.13373375818081</v>
+      </c>
+      <c r="F21">
+        <v>115.47154072457153</v>
+      </c>
+      <c r="G21">
+        <v>121.62568025179993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>200.71701859259665</v>
+      </c>
+      <c r="D22">
+        <v>200.71701860956063</v>
+      </c>
+      <c r="E22">
+        <v>201.37829993334105</v>
+      </c>
+      <c r="F22">
+        <v>199.83370377972741</v>
+      </c>
+      <c r="G22">
+        <v>194.14755845416465</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1.0035850929629833</v>
+      </c>
+      <c r="D23">
+        <v>1.0035850930478032</v>
+      </c>
+      <c r="E23">
+        <v>1.0068914996667053</v>
+      </c>
+      <c r="F23">
+        <v>0.99916851889863711</v>
+      </c>
+      <c r="G23">
+        <v>0.97073779227082324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1.0268107803559916</v>
+      </c>
+      <c r="D24">
+        <v>1.026810780303149</v>
+      </c>
+      <c r="E24">
+        <v>1.0161855054344244</v>
+      </c>
+      <c r="F24">
+        <v>1.0862618717772732</v>
+      </c>
+      <c r="G24">
+        <v>1.1690468695684746</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.87672423212192319</v>
+      </c>
+      <c r="D25">
+        <v>0.87672423219236795</v>
+      </c>
+      <c r="E25">
+        <v>0.88681325620491058</v>
+      </c>
+      <c r="F25">
+        <v>0.8240896931384919</v>
+      </c>
+      <c r="G25">
+        <v>0.76012909543532714</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1.0351629706265315</v>
+      </c>
+      <c r="D27">
+        <v>1.0351629708854646</v>
+      </c>
+      <c r="E27">
+        <v>1.0678356276899741</v>
+      </c>
+      <c r="F27">
+        <v>1.1033933594907179</v>
+      </c>
+      <c r="G27">
+        <v>1.1648853507249877</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.9720072152994349</v>
+      </c>
+      <c r="D28">
+        <v>0.97200721521014155</v>
+      </c>
+      <c r="E28">
+        <v>0.94594737164343623</v>
+      </c>
+      <c r="F28">
+        <v>0.85817103861968913</v>
+      </c>
+      <c r="G28">
+        <v>0.77659023381665881</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29">
+        <v>200</v>
+      </c>
+      <c r="C29">
+        <v>200.71701865447656</v>
+      </c>
+      <c r="D29">
+        <v>200.71701860956063</v>
+      </c>
+      <c r="E29">
+        <v>201.37829993334105</v>
+      </c>
+      <c r="F29">
+        <v>199.83370377972741</v>
+      </c>
+      <c r="G29">
+        <v>194.14755845416465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add Test for outtax indexed
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9159EA5F-4CAC-4F5D-B764-2B9506C72D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86643BD2-E8CC-4F3A-BB7E-5C441037A306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7460" firstSheet="3" activeTab="3" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="270" yWindow="-13350" windowWidth="14400" windowHeight="7455" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
     <sheet name="TwoxTwoJPMGE" sheetId="4" r:id="rId2"/>
     <sheet name="TwoxTwoCESProd" sheetId="5" r:id="rId3"/>
     <sheet name="JPMGE" sheetId="6" r:id="rId4"/>
+    <sheet name="TwoxTwowTax" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>X.L</t>
   </si>
@@ -213,6 +214,39 @@
   </si>
   <si>
     <t>CWI</t>
+  </si>
+  <si>
+    <t>SX.L</t>
+  </si>
+  <si>
+    <t>SY.L</t>
+  </si>
+  <si>
+    <t>DXL.L</t>
+  </si>
+  <si>
+    <t>DXK.L</t>
+  </si>
+  <si>
+    <t>DYL.L</t>
+  </si>
+  <si>
+    <t>DYK.L</t>
+  </si>
+  <si>
+    <t>SU.L</t>
+  </si>
+  <si>
+    <t>DUX.L</t>
+  </si>
+  <si>
+    <t>DUY.L</t>
+  </si>
+  <si>
+    <t>DU.L</t>
+  </si>
+  <si>
+    <t>CWI.L</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E9A728-5CCB-48DE-B29A-AA0B43EB195B}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2633,4 +2667,371 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999B2CB6-D228-42B8-B68B-E63D641C5E20}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0488088482495366</v>
+      </c>
+      <c r="D2">
+        <v>1.048808848291152</v>
+      </c>
+      <c r="E2">
+        <v>1.0488088481593842</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0388601183172488</v>
+      </c>
+      <c r="D3">
+        <v>1.0388601180790369</v>
+      </c>
+      <c r="E3">
+        <v>1.0388601182505068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0454820636535147</v>
+      </c>
+      <c r="D4">
+        <v>1.0454820633736372</v>
+      </c>
+      <c r="E4">
+        <v>1.0454820635708237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.98905852579244424</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.048808848138622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.99853032667237385</v>
+      </c>
+      <c r="D6">
+        <v>1.0095765827722971</v>
+      </c>
+      <c r="E6">
+        <v>1.058852852879361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.9922057674249718</v>
+      </c>
+      <c r="D7">
+        <v>1.0031820580243815</v>
+      </c>
+      <c r="E7">
+        <v>1.0521462187479544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.94303030266405441</v>
+      </c>
+      <c r="D8">
+        <v>0.95346258924320726</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0373333333393082</v>
+      </c>
+      <c r="D9">
+        <v>1.048808848128669</v>
+      </c>
+      <c r="E9">
+        <v>1.0999999998972825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>187.5</v>
+      </c>
+      <c r="C10">
+        <v>194.5</v>
+      </c>
+      <c r="D10">
+        <v>196.65165902915749</v>
+      </c>
+      <c r="E10">
+        <v>206.24999999007531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>125</v>
+      </c>
+      <c r="C11">
+        <v>125</v>
+      </c>
+      <c r="D11">
+        <v>124.99999999999999</v>
+      </c>
+      <c r="E11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>62.5</v>
+      </c>
+      <c r="C12">
+        <v>62.500000000000007</v>
+      </c>
+      <c r="D12">
+        <v>62.500000000000007</v>
+      </c>
+      <c r="E12">
+        <v>62.499999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52.440442418841862</v>
+      </c>
+      <c r="D13">
+        <v>52.440442407536104</v>
+      </c>
+      <c r="E13">
+        <v>52.440442406059141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>47.673129452884808</v>
+      </c>
+      <c r="D14">
+        <v>47.673129463162773</v>
+      </c>
+      <c r="E14">
+        <v>47.673129464505458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>21.177057063443652</v>
+      </c>
+      <c r="D15">
+        <v>21.177057057964916</v>
+      </c>
+      <c r="E15">
+        <v>21.17705705724919</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.877805075132347</v>
+      </c>
+      <c r="D16">
+        <v>28.877805080113006</v>
+      </c>
+      <c r="E16">
+        <v>28.877805080763672</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>187.5</v>
+      </c>
+      <c r="C17">
+        <v>196.02788693503402</v>
+      </c>
+      <c r="D17">
+        <v>196.02788688255697</v>
+      </c>
+      <c r="E17">
+        <v>196.02788691952946</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
+        <v>125</v>
+      </c>
+      <c r="C18">
+        <v>131.10110603221005</v>
+      </c>
+      <c r="D18">
+        <v>131.10110599531828</v>
+      </c>
+      <c r="E18">
+        <v>131.10110601980654</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>62.5</v>
+      </c>
+      <c r="C19">
+        <v>64.928757393926062</v>
+      </c>
+      <c r="D19">
+        <v>64.928757378323226</v>
+      </c>
+      <c r="E19">
+        <v>64.928757390805515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20">
+        <v>187.5</v>
+      </c>
+      <c r="C20">
+        <v>187.49999997857734</v>
+      </c>
+      <c r="D20">
+        <v>187.50000003446129</v>
+      </c>
+      <c r="E20">
+        <v>187.49999999867345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21">
+        <v>187.5</v>
+      </c>
+      <c r="C21">
+        <v>196.027886912637</v>
+      </c>
+      <c r="D21">
+        <v>196.02788691858564</v>
+      </c>
+      <c r="E21">
+        <v>196.02788691814257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All tests pass incl Tr elas
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE404EE-4DBF-4459-A75E-F604EBE60C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152DDCCF-6882-4CBE-9AF6-D933155FD53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="792" windowWidth="17280" windowHeight="9024" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="12384" yWindow="348" windowWidth="10656" windowHeight="10008" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -2765,13 +2765,13 @@
         <v>0.84841617526015112</v>
       </c>
       <c r="D2">
-        <v>0.8484161751970315</v>
+        <v>0.84841617519703094</v>
       </c>
       <c r="E2">
-        <v>0.70716515735515006</v>
+        <v>0.70716515735515251</v>
       </c>
       <c r="F2">
-        <v>0.38751484805497743</v>
+        <v>0.38751484805497977</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2785,16 +2785,16 @@
         <v>1.1506325096039884</v>
       </c>
       <c r="D3">
-        <v>1.1506325095207364</v>
+        <v>1.150632509520737</v>
       </c>
       <c r="E3">
-        <v>1.2893059702343606</v>
+        <v>1.2893059702343586</v>
       </c>
       <c r="F3">
-        <v>1.5972629436210768</v>
+        <v>1.597262943621075</v>
       </c>
       <c r="G3">
-        <v>1.9601317042077897</v>
+        <v>1.9601317042077893</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2811,13 +2811,13 @@
         <v>1.0035850930478027</v>
       </c>
       <c r="E4">
-        <v>1.0068914996667162</v>
+        <v>1.0068914996667164</v>
       </c>
       <c r="F4">
-        <v>0.99916851890038427</v>
+        <v>0.99916851890038483</v>
       </c>
       <c r="G4">
-        <v>0.97073779227082346</v>
+        <v>0.97073779227082335</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2831,16 +2831,16 @@
         <v>1.0231427182799986</v>
       </c>
       <c r="D5">
-        <v>1.026810780303149</v>
+        <v>1.0268107803031492</v>
       </c>
       <c r="E5">
-        <v>1.0161855054344244</v>
+        <v>1.016185505434424</v>
       </c>
       <c r="F5">
-        <v>1.0862618717772732</v>
+        <v>1.0862618717772727</v>
       </c>
       <c r="G5">
-        <v>1.1690468695684746</v>
+        <v>1.1690468695684744</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2854,16 +2854,16 @@
         <v>0.87359232216492444</v>
       </c>
       <c r="D6">
-        <v>0.87672423219236795</v>
+        <v>0.87672423219236773</v>
       </c>
       <c r="E6">
-        <v>0.88681325620491058</v>
+        <v>0.88681325620491103</v>
       </c>
       <c r="F6">
-        <v>0.8240896931384919</v>
+        <v>0.82408969313849223</v>
       </c>
       <c r="G6">
-        <v>0.76012909543532714</v>
+        <v>0.76012909543532692</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2900,16 +2900,16 @@
         <v>1.0314650721357199</v>
       </c>
       <c r="D8">
-        <v>1.0351629708854646</v>
+        <v>1.0351629708854644</v>
       </c>
       <c r="E8">
-        <v>1.0678356276899741</v>
+        <v>1.0678356276899736</v>
       </c>
       <c r="F8">
-        <v>1.1033933594907179</v>
+        <v>1.1033933594907175</v>
       </c>
       <c r="G8">
-        <v>1.1648853507249877</v>
+        <v>1.1648853507249886</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2923,16 +2923,16 @@
         <v>0.96853492724769141</v>
       </c>
       <c r="D9">
-        <v>0.97200721521014155</v>
+        <v>0.97200721521014122</v>
       </c>
       <c r="E9">
-        <v>0.94594737164343623</v>
+        <v>0.94594737164343634</v>
       </c>
       <c r="F9">
-        <v>0.85817103861968913</v>
+        <v>0.85817103861968957</v>
       </c>
       <c r="G9">
-        <v>0.77659023381665881</v>
+        <v>0.7765902338166587</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2946,16 +2946,16 @@
         <v>200</v>
       </c>
       <c r="D10">
-        <v>200.71701860956063</v>
+        <v>200</v>
       </c>
       <c r="E10">
-        <v>201.37829993334105</v>
+        <v>200</v>
       </c>
       <c r="F10">
-        <v>199.83370377972741</v>
+        <v>200</v>
       </c>
       <c r="G10">
-        <v>194.14755845416465</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2969,10 +2969,10 @@
         <v>80.000000000000014</v>
       </c>
       <c r="D11">
-        <v>80</v>
+        <v>79.999999999999986</v>
       </c>
       <c r="E11">
-        <v>83.789979418307453</v>
+        <v>83.789979418307439</v>
       </c>
       <c r="F11">
         <v>86.636474448757937</v>
@@ -2992,13 +2992,13 @@
         <v>20.000000000000004</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>19.999999999999996</v>
       </c>
       <c r="E12">
-        <v>15.953297102016906</v>
+        <v>15.953297102016929</v>
       </c>
       <c r="F12">
-        <v>12.465814866890884</v>
+        <v>12.465814866890906</v>
       </c>
       <c r="G12" t="s">
         <v>88</v>
@@ -3018,13 +3018,13 @@
         <v>30</v>
       </c>
       <c r="E13">
-        <v>34.553784903611799</v>
+        <v>34.553784903611771</v>
       </c>
       <c r="F13">
-        <v>39.310669882974452</v>
+        <v>39.310669882974416</v>
       </c>
       <c r="G13">
-        <v>44.380086793200221</v>
+        <v>44.380086793200228</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3041,10 +3041,10 @@
         <v>80</v>
       </c>
       <c r="E14">
-        <v>75.119576065481453</v>
+        <v>75.119576065481496</v>
       </c>
       <c r="F14">
-        <v>69.26902850423329</v>
+        <v>69.269028504233304</v>
       </c>
       <c r="G14">
         <v>62.049748999369605</v>
@@ -3061,13 +3061,13 @@
         <v>38.517354230045243</v>
       </c>
       <c r="D15">
-        <v>38.517354222141414</v>
+        <v>38.517354222141421</v>
       </c>
       <c r="E15">
-        <v>37.194397849630214</v>
+        <v>37.194397849630228</v>
       </c>
       <c r="F15">
-        <v>34.40060528627518</v>
+        <v>34.400605286275194</v>
       </c>
       <c r="G15" t="s">
         <v>88</v>
@@ -3084,13 +3084,13 @@
         <v>61.530004404080294</v>
       </c>
       <c r="D16">
-        <v>61.53000441249764</v>
+        <v>61.530004412497654</v>
       </c>
       <c r="E16">
-        <v>62.98051725431754</v>
+        <v>62.980517254317519</v>
       </c>
       <c r="F16">
-        <v>66.345864158482783</v>
+        <v>66.345864158482755</v>
       </c>
       <c r="G16" t="s">
         <v>88</v>
@@ -3107,16 +3107,16 @@
         <v>58.508040668387657</v>
       </c>
       <c r="D17">
-        <v>58.508040660383685</v>
+        <v>58.508040660383678</v>
       </c>
       <c r="E17">
-        <v>57.160534034089842</v>
+        <v>57.160534034089849</v>
       </c>
       <c r="F17">
-        <v>54.261106485862463</v>
+        <v>54.261106485862491</v>
       </c>
       <c r="G17">
-        <v>51.016980025031643</v>
+        <v>51.016980025031629</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3130,16 +3130,16 @@
         <v>41.539717147859804</v>
       </c>
       <c r="D18">
-        <v>41.539717156383809</v>
+        <v>41.539717156383801</v>
       </c>
       <c r="E18">
-        <v>43.017230886987115</v>
+        <v>43.017230886987093</v>
       </c>
       <c r="F18">
-        <v>46.51080952457405</v>
+        <v>46.510809524574043</v>
       </c>
       <c r="G18">
-        <v>51.016980025031621</v>
+        <v>51.016980025031643</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3150,19 +3150,19 @@
         <v>200</v>
       </c>
       <c r="C19">
-        <v>200.71701862652515</v>
+        <v>200</v>
       </c>
       <c r="D19">
-        <v>200.71701860956054</v>
+        <v>200</v>
       </c>
       <c r="E19">
-        <v>201.37829993334324</v>
+        <v>200</v>
       </c>
       <c r="F19">
-        <v>199.83370378007686</v>
+        <v>200</v>
       </c>
       <c r="G19">
-        <v>194.14755845416468</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3173,19 +3173,19 @@
         <v>100</v>
       </c>
       <c r="C20">
-        <v>102.3922693035888</v>
+        <v>102.02649481767209</v>
       </c>
       <c r="D20">
-        <v>102.39226930136157</v>
+        <v>102.02649482407605</v>
       </c>
       <c r="E20">
-        <v>103.80375515055297</v>
+        <v>103.09328779209312</v>
       </c>
       <c r="F20">
-        <v>96.362396524949176</v>
+        <v>96.442586712999145</v>
       </c>
       <c r="G20">
-        <v>86.990815158845137</v>
+        <v>89.613092074379438</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3196,19 +3196,19 @@
         <v>100</v>
       </c>
       <c r="C21">
-        <v>109.01892428236799</v>
+        <v>108.6294774886228</v>
       </c>
       <c r="D21">
-        <v>109.0189242656265</v>
+        <v>108.62947748112251</v>
       </c>
       <c r="E21">
-        <v>108.13373375818081</v>
+        <v>107.3936305887708</v>
       </c>
       <c r="F21">
-        <v>115.47154072457153</v>
+        <v>115.56763302716089</v>
       </c>
       <c r="G21">
-        <v>121.62568025179993</v>
+        <v>125.29200080619496</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3219,19 +3219,19 @@
         <v>200</v>
       </c>
       <c r="C22">
-        <v>200.71701859259665</v>
+        <v>200.71701865447653</v>
       </c>
       <c r="D22">
-        <v>200.71701860956063</v>
+        <v>200</v>
       </c>
       <c r="E22">
-        <v>201.37829993334105</v>
+        <v>200</v>
       </c>
       <c r="F22">
-        <v>199.83370377972741</v>
+        <v>200</v>
       </c>
       <c r="G22">
-        <v>194.14755845416465</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3242,19 +3242,19 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1.0035850929629833</v>
+        <v>1.0035850932723827</v>
       </c>
       <c r="D23">
-        <v>1.0035850930478032</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1.0068914996667053</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0.99916851889863711</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0.97073779227082324</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3268,16 +3268,16 @@
         <v>1.0268107803559916</v>
       </c>
       <c r="D24">
-        <v>1.026810780303149</v>
+        <v>1.0268107803031492</v>
       </c>
       <c r="E24">
-        <v>1.0161855054344244</v>
+        <v>1.016185505434424</v>
       </c>
       <c r="F24">
-        <v>1.0862618717772732</v>
+        <v>1.0862618717772727</v>
       </c>
       <c r="G24">
-        <v>1.1690468695684746</v>
+        <v>1.1690468695684744</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3291,16 +3291,16 @@
         <v>0.87672423212192319</v>
       </c>
       <c r="D25">
-        <v>0.87672423219236795</v>
+        <v>0.87672423219236773</v>
       </c>
       <c r="E25">
-        <v>0.88681325620491058</v>
+        <v>0.88681325620491103</v>
       </c>
       <c r="F25">
-        <v>0.8240896931384919</v>
+        <v>0.82408969313849223</v>
       </c>
       <c r="G25">
-        <v>0.76012909543532714</v>
+        <v>0.76012909543532692</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3337,16 +3337,16 @@
         <v>1.0351629706265315</v>
       </c>
       <c r="D27">
-        <v>1.0351629708854646</v>
+        <v>1.0351629708854644</v>
       </c>
       <c r="E27">
-        <v>1.0678356276899741</v>
+        <v>1.0678356276899736</v>
       </c>
       <c r="F27">
-        <v>1.1033933594907179</v>
+        <v>1.1033933594907175</v>
       </c>
       <c r="G27">
-        <v>1.1648853507249877</v>
+        <v>1.1648853507249886</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -3360,16 +3360,16 @@
         <v>0.9720072152994349</v>
       </c>
       <c r="D28">
-        <v>0.97200721521014155</v>
+        <v>0.97200721521014122</v>
       </c>
       <c r="E28">
-        <v>0.94594737164343623</v>
+        <v>0.94594737164343634</v>
       </c>
       <c r="F28">
-        <v>0.85817103861968913</v>
+        <v>0.85817103861968957</v>
       </c>
       <c r="G28">
-        <v>0.77659023381665881</v>
+        <v>0.7765902338166587</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3383,16 +3383,16 @@
         <v>200.71701865447656</v>
       </c>
       <c r="D29">
-        <v>200.71701860956063</v>
+        <v>200</v>
       </c>
       <c r="E29">
-        <v>201.37829993334105</v>
+        <v>200</v>
       </c>
       <c r="F29">
-        <v>199.83370377972741</v>
+        <v>200</v>
       </c>
       <c r="G29">
-        <v>194.14755845416465</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diff & CET working except diff in inputs for s!=1
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152DDCCF-6882-4CBE-9AF6-D933155FD53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24C9A5E-0D3F-4BC2-8487-958957C13EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12384" yWindow="348" windowWidth="10656" windowHeight="10008" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="12384" yWindow="696" windowWidth="10656" windowHeight="10008" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
   <si>
     <t>X.L</t>
   </si>
@@ -270,40 +270,55 @@
     <t>CWI.L</t>
   </si>
   <si>
+    <t>diff=10</t>
+  </si>
+  <si>
+    <t>PW.FX=1</t>
+  </si>
+  <si>
+    <t>TA=0.1</t>
+  </si>
+  <si>
+    <t>TA=100%</t>
+  </si>
+  <si>
+    <t>Undf</t>
+  </si>
+  <si>
+    <t>TA=2B=1.5</t>
+  </si>
+  <si>
+    <t>TrA=3B=1</t>
+  </si>
+  <si>
+    <t>TrA/B=1</t>
+  </si>
+  <si>
+    <t>Sub=0Tr=0</t>
+  </si>
+  <si>
+    <t>S0Tr2,1.5</t>
+  </si>
+  <si>
+    <t>S0Tr=3,1</t>
+  </si>
+  <si>
+    <t>Sub=0Tr=1</t>
+  </si>
+  <si>
+    <t>1.52,.5T0</t>
+  </si>
+  <si>
+    <t>S..T2,1.5</t>
+  </si>
+  <si>
+    <t>S...T3,1</t>
+  </si>
+  <si>
+    <t>S...T1,1</t>
+  </si>
+  <si>
     <t>PX.L/PW.L</t>
-  </si>
-  <si>
-    <t>PY.L/PW.L</t>
-  </si>
-  <si>
-    <t>PW.L/PW.L</t>
-  </si>
-  <si>
-    <t>PL.L/PW.L</t>
-  </si>
-  <si>
-    <t>PK.L/PW.L</t>
-  </si>
-  <si>
-    <t>CONS.L/PW.L</t>
-  </si>
-  <si>
-    <t>diff=10</t>
-  </si>
-  <si>
-    <t>PW.FX=1</t>
-  </si>
-  <si>
-    <t>TrA=2, TrB=1.5</t>
-  </si>
-  <si>
-    <t>TA=0.1</t>
-  </si>
-  <si>
-    <t>TA=100%</t>
-  </si>
-  <si>
-    <t>Undf</t>
   </si>
 </sst>
 </file>
@@ -2728,33 +2743,65 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E4E009-E95D-4525-8C72-CDF28BC03388}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -2762,19 +2809,49 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.84841617526015112</v>
+        <v>0.99999999969167375</v>
       </c>
       <c r="D2">
-        <v>0.84841617519703094</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="E2">
-        <v>0.70716515735515251</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="F2">
-        <v>0.38751484805497977</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="G2">
+        <v>0.84841617519705081</v>
+      </c>
+      <c r="H2">
+        <v>0.84841617519703227</v>
+      </c>
+      <c r="I2">
+        <v>0.70716515735515162</v>
+      </c>
+      <c r="J2">
+        <v>0.72509467112342096</v>
+      </c>
+      <c r="K2">
+        <v>0.75612889144439288</v>
+      </c>
+      <c r="L2">
+        <v>0.91659821359054672</v>
+      </c>
+      <c r="M2">
+        <v>0.73369015208861166</v>
+      </c>
+      <c r="N2">
+        <v>0.75685954678370782</v>
+      </c>
+      <c r="O2">
+        <v>0.80071809649126724</v>
+      </c>
+      <c r="P2">
+        <v>0.57048205371293126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -2782,22 +2859,52 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.1506325096039884</v>
+        <v>0.99999999965367625</v>
       </c>
       <c r="D3">
-        <v>1.150632509520737</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="E3">
-        <v>1.2893059702343586</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="F3">
-        <v>1.597262943621075</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G3">
-        <v>1.9601317042077893</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.150632509520773</v>
+      </c>
+      <c r="H3">
+        <v>1.1506325095207364</v>
+      </c>
+      <c r="I3">
+        <v>1.2893059702343592</v>
+      </c>
+      <c r="J3">
+        <v>1.2717929473142071</v>
+      </c>
+      <c r="K3">
+        <v>1.2414185056039873</v>
+      </c>
+      <c r="L3">
+        <v>1.0832385402482214</v>
+      </c>
+      <c r="M3">
+        <v>1.2646965132512462</v>
+      </c>
+      <c r="N3">
+        <v>1.241790354991813</v>
+      </c>
+      <c r="O3">
+        <v>1.1983681743653367</v>
+      </c>
+      <c r="P3">
+        <v>1.4254342349963718</v>
+      </c>
+      <c r="Q3">
+        <v>1.9797958971135601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
@@ -2805,22 +2912,52 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1.0035850931326258</v>
+        <v>0.99999999937602346</v>
       </c>
       <c r="D4">
-        <v>1.0035850930478027</v>
+        <v>1.0000000000000835</v>
       </c>
       <c r="E4">
-        <v>1.0068914996667164</v>
+        <v>1.0000000000000835</v>
       </c>
       <c r="F4">
-        <v>0.99916851890038483</v>
+        <v>1.0000000000000835</v>
       </c>
       <c r="G4">
-        <v>0.97073779227082335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.0035850930478354</v>
+      </c>
+      <c r="H4">
+        <v>1.0035850930478032</v>
+      </c>
+      <c r="I4">
+        <v>1.0068914996667158</v>
+      </c>
+      <c r="J4">
+        <v>1.0066737049684853</v>
+      </c>
+      <c r="K4">
+        <v>1.0057135773586174</v>
+      </c>
+      <c r="L4">
+        <v>1.0019757361058046</v>
+      </c>
+      <c r="M4">
+        <v>1.0062537377172633</v>
+      </c>
+      <c r="N4">
+        <v>1.0059749908396223</v>
+      </c>
+      <c r="O4">
+        <v>1.0046559044043992</v>
+      </c>
+      <c r="P4">
+        <v>0.9989805146510895</v>
+      </c>
+      <c r="Q4">
+        <v>0.94407743479945161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2828,22 +2965,52 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1.0231427182799986</v>
+        <v>1.0246978500088042</v>
       </c>
       <c r="D5">
-        <v>1.0268107803031492</v>
+        <v>0.9523809523809269</v>
       </c>
       <c r="E5">
+        <v>0.9523809523809269</v>
+      </c>
+      <c r="F5">
+        <v>0.9523809523809269</v>
+      </c>
+      <c r="G5">
+        <v>1.0231427184558559</v>
+      </c>
+      <c r="H5">
+        <v>1.0268107803029183</v>
+      </c>
+      <c r="I5">
         <v>1.016185505434424</v>
       </c>
-      <c r="F5">
-        <v>1.0862618717772727</v>
-      </c>
-      <c r="G5">
-        <v>1.1690468695684744</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>1.0155313673319299</v>
+      </c>
+      <c r="K5">
+        <v>1.0202925382350085</v>
+      </c>
+      <c r="L5">
+        <v>1.0330796752807549</v>
+      </c>
+      <c r="M5">
+        <v>1.0263074053285333</v>
+      </c>
+      <c r="N5">
+        <v>1.0245496568517749</v>
+      </c>
+      <c r="O5">
+        <v>1.0292660659587862</v>
+      </c>
+      <c r="P5">
+        <v>1.1136635243164417</v>
+      </c>
+      <c r="Q5">
+        <v>1.2983516200037846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2851,22 +3018,52 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.87359232216492444</v>
+        <v>0.87283237043207507</v>
       </c>
       <c r="D6">
-        <v>0.87672423219236773</v>
+        <v>0.95238095238098064</v>
       </c>
       <c r="E6">
-        <v>0.88681325620491103</v>
+        <v>0.95238095238098064</v>
       </c>
       <c r="F6">
-        <v>0.82408969313849223</v>
+        <v>0.95238095238098064</v>
       </c>
       <c r="G6">
-        <v>0.76012909543532692</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.87359232243054408</v>
+      </c>
+      <c r="H6">
+        <v>0.87672423219258488</v>
+      </c>
+      <c r="I6">
+        <v>0.88681325620491125</v>
+      </c>
+      <c r="J6">
+        <v>0.88744162549260985</v>
+      </c>
+      <c r="K6">
+        <v>0.88288734202338981</v>
+      </c>
+      <c r="L6">
+        <v>0.86740230739395141</v>
+      </c>
+      <c r="M6">
+        <v>0.87425306835177607</v>
+      </c>
+      <c r="N6">
+        <v>0.87603929679048465</v>
+      </c>
+      <c r="O6">
+        <v>0.87125402922695383</v>
+      </c>
+      <c r="P6">
+        <v>0.78953411260391282</v>
+      </c>
+      <c r="Q6">
+        <v>0.63360419775310972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
@@ -2874,7 +3071,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.99642771370717265</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2886,10 +3083,40 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.99642771392989316</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2897,22 +3124,52 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.0314650721357199</v>
+        <v>1.0283762514304395</v>
       </c>
       <c r="D8">
-        <v>1.0351629708854644</v>
+        <v>1.2380952380952241</v>
       </c>
       <c r="E8">
-        <v>1.0678356276899736</v>
+        <v>1.2380952380952241</v>
       </c>
       <c r="F8">
-        <v>1.1033933594907175</v>
+        <v>1.2380952380952241</v>
       </c>
       <c r="G8">
-        <v>1.1648853507249886</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.0314650726247152</v>
+      </c>
+      <c r="H8">
+        <v>1.0351629708860788</v>
+      </c>
+      <c r="I8">
+        <v>1.0678356276899739</v>
+      </c>
+      <c r="J8">
+        <v>1.0639075291153643</v>
+      </c>
+      <c r="K8">
+        <v>1.0564877098287575</v>
+      </c>
+      <c r="L8">
+        <v>1.0117879320523542</v>
+      </c>
+      <c r="M8">
+        <v>1.0367784125216681</v>
+      </c>
+      <c r="N8">
+        <v>1.0339436215788291</v>
+      </c>
+      <c r="O8">
+        <v>1.0277166820777672</v>
+      </c>
+      <c r="P8">
+        <v>1.0178419107760996</v>
+      </c>
+      <c r="Q8">
+        <v>1.0394486229277171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2920,22 +3177,52 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.96853492724769141</v>
+        <v>0.97162375401182643</v>
       </c>
       <c r="D9">
-        <v>0.97200721521014122</v>
+        <v>0.76190476190460876</v>
       </c>
       <c r="E9">
-        <v>0.94594737164343634</v>
+        <v>0.76190476190460876</v>
       </c>
       <c r="F9">
-        <v>0.85817103861968957</v>
+        <v>0.76190476190460876</v>
       </c>
       <c r="G9">
-        <v>0.7765902338166587</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.96853492737470426</v>
+      </c>
+      <c r="H9">
+        <v>0.97200721520952771</v>
+      </c>
+      <c r="I9">
+        <v>0.94594737164343645</v>
+      </c>
+      <c r="J9">
+        <v>0.94943988081630226</v>
+      </c>
+      <c r="K9">
+        <v>0.95493944473687198</v>
+      </c>
+      <c r="L9">
+        <v>0.9921635401381601</v>
+      </c>
+      <c r="M9">
+        <v>0.97572906291222694</v>
+      </c>
+      <c r="N9">
+        <v>0.97800635973064054</v>
+      </c>
+      <c r="O9">
+        <v>0.98159512233037882</v>
+      </c>
+      <c r="P9">
+        <v>0.92531027852785397</v>
+      </c>
+      <c r="Q9">
+        <v>0.84870624666994454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -2957,8 +3244,38 @@
       <c r="G10">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>200</v>
+      </c>
+      <c r="I10">
+        <v>200</v>
+      </c>
+      <c r="J10">
+        <v>200</v>
+      </c>
+      <c r="K10">
+        <v>200</v>
+      </c>
+      <c r="L10">
+        <v>200</v>
+      </c>
+      <c r="M10">
+        <v>200</v>
+      </c>
+      <c r="N10">
+        <v>200</v>
+      </c>
+      <c r="O10">
+        <v>200</v>
+      </c>
+      <c r="P10">
+        <v>200</v>
+      </c>
+      <c r="Q10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -2969,19 +3286,49 @@
         <v>80.000000000000014</v>
       </c>
       <c r="D11">
-        <v>79.999999999999986</v>
+        <v>79.999999999998181</v>
       </c>
       <c r="E11">
+        <v>79.999999999997286</v>
+      </c>
+      <c r="F11">
+        <v>79.999999999999119</v>
+      </c>
+      <c r="G11">
+        <v>80</v>
+      </c>
+      <c r="H11">
+        <v>80</v>
+      </c>
+      <c r="I11">
         <v>83.789979418307439</v>
       </c>
-      <c r="F11">
-        <v>86.636474448757937</v>
-      </c>
-      <c r="G11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>85.397254560161699</v>
+      </c>
+      <c r="K11">
+        <v>82.088707595463845</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+      <c r="M11">
+        <v>84.351462627766139</v>
+      </c>
+      <c r="N11">
+        <v>86.083347199002077</v>
+      </c>
+      <c r="O11">
+        <v>82.36898138312101</v>
+      </c>
+      <c r="P11">
+        <v>84.302930903518373</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -2992,19 +3339,49 @@
         <v>20.000000000000004</v>
       </c>
       <c r="D12">
-        <v>19.999999999999996</v>
+        <v>20.000000000001805</v>
       </c>
       <c r="E12">
-        <v>15.953297102016929</v>
+        <v>20.000000000002704</v>
       </c>
       <c r="F12">
-        <v>12.465814866890906</v>
-      </c>
-      <c r="G12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20.000000000000906</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>15.953297102016936</v>
+      </c>
+      <c r="J12">
+        <v>14.246995168670852</v>
+      </c>
+      <c r="K12">
+        <v>17.758407060505427</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>15.302135083504712</v>
+      </c>
+      <c r="N12">
+        <v>13.453363640181522</v>
+      </c>
+      <c r="O12">
+        <v>17.430941640564519</v>
+      </c>
+      <c r="P12">
+        <v>14.941685322250365</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
@@ -3012,22 +3389,52 @@
         <v>20</v>
       </c>
       <c r="C13">
-        <v>30.000000000000004</v>
+        <v>30</v>
       </c>
       <c r="D13">
+        <v>29.999999999998153</v>
+      </c>
+      <c r="E13">
+        <v>29.999999999998767</v>
+      </c>
+      <c r="F13">
+        <v>29.999999999998767</v>
+      </c>
+      <c r="G13">
         <v>30</v>
       </c>
-      <c r="E13">
-        <v>34.553784903611771</v>
-      </c>
-      <c r="F13">
-        <v>39.310669882974416</v>
-      </c>
-      <c r="G13">
-        <v>44.380086793200228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <v>34.553784903611756</v>
+      </c>
+      <c r="J13">
+        <v>32.966888913499105</v>
+      </c>
+      <c r="K13">
+        <v>33.184069765209088</v>
+      </c>
+      <c r="L13">
+        <v>30</v>
+      </c>
+      <c r="M13">
+        <v>35.375340199360892</v>
+      </c>
+      <c r="N13">
+        <v>33.448293412545176</v>
+      </c>
+      <c r="O13">
+        <v>33.670905403089371</v>
+      </c>
+      <c r="P13">
+        <v>37.550960863227068</v>
+      </c>
+      <c r="Q13">
+        <v>44.925101910602201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
@@ -3038,19 +3445,49 @@
         <v>80</v>
       </c>
       <c r="D14">
+        <v>80.000000000001847</v>
+      </c>
+      <c r="E14">
+        <v>80.000000000001251</v>
+      </c>
+      <c r="F14">
+        <v>80.000000000001251</v>
+      </c>
+      <c r="G14">
         <v>80</v>
       </c>
-      <c r="E14">
+      <c r="H14">
+        <v>80</v>
+      </c>
+      <c r="I14">
         <v>75.119576065481496</v>
       </c>
-      <c r="F14">
-        <v>69.269028504233304</v>
-      </c>
-      <c r="G14">
-        <v>62.049748999369605</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>76.823333874806721</v>
+      </c>
+      <c r="K14">
+        <v>76.57358141148049</v>
+      </c>
+      <c r="L14">
+        <v>80</v>
+      </c>
+      <c r="M14">
+        <v>74.166692410395541</v>
+      </c>
+      <c r="N14">
+        <v>76.266404448062389</v>
+      </c>
+      <c r="O14">
+        <v>76.004738963413018</v>
+      </c>
+      <c r="P14">
+        <v>70.991555145634763</v>
+      </c>
+      <c r="Q14">
+        <v>58.463326814268953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
@@ -3058,22 +3495,52 @@
         <v>40</v>
       </c>
       <c r="C15">
-        <v>38.517354230045243</v>
+        <v>40.000000000000007</v>
       </c>
       <c r="D15">
-        <v>38.517354222141421</v>
+        <v>40</v>
       </c>
       <c r="E15">
+        <v>40</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15">
+        <v>38.517354222119764</v>
+      </c>
+      <c r="H15">
+        <v>38.517354222113113</v>
+      </c>
+      <c r="I15">
         <v>37.194397849630228</v>
       </c>
-      <c r="F15">
-        <v>34.400605286275194</v>
-      </c>
-      <c r="G15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>37.359249566828282</v>
+      </c>
+      <c r="K15">
+        <v>37.646692039851665</v>
+      </c>
+      <c r="L15">
+        <v>39.299714763812808</v>
+      </c>
+      <c r="M15">
+        <v>37.861280098811257</v>
+      </c>
+      <c r="N15">
+        <v>38.036420747024273</v>
+      </c>
+      <c r="O15">
+        <v>38.373445987225587</v>
+      </c>
+      <c r="P15">
+        <v>36.681951520633213</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
@@ -3081,22 +3548,52 @@
         <v>60</v>
       </c>
       <c r="C16">
-        <v>61.530004404080294</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>61.530004412497654</v>
+        <v>60</v>
       </c>
       <c r="E16">
-        <v>62.980517254317519</v>
+        <v>60</v>
       </c>
       <c r="F16">
-        <v>66.345864158482755</v>
-      </c>
-      <c r="G16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>61.530004412520697</v>
+      </c>
+      <c r="H16">
+        <v>61.530004412527788</v>
+      </c>
+      <c r="I16">
+        <v>62.980517254317533</v>
+      </c>
+      <c r="J16">
+        <v>62.795108515046778</v>
+      </c>
+      <c r="K16">
+        <v>62.475062175440918</v>
+      </c>
+      <c r="L16">
+        <v>60.70717235830665</v>
+      </c>
+      <c r="M16">
+        <v>62.204472249917288</v>
+      </c>
+      <c r="N16">
+        <v>62.018844587381608</v>
+      </c>
+      <c r="O16">
+        <v>61.664268208122358</v>
+      </c>
+      <c r="P16">
+        <v>63.479442824149956</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -3104,22 +3601,52 @@
         <v>60</v>
       </c>
       <c r="C17">
-        <v>58.508040668387657</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>58.508040660383678</v>
+        <v>60</v>
       </c>
       <c r="E17">
-        <v>57.160534034089849</v>
+        <v>60</v>
       </c>
       <c r="F17">
-        <v>54.261106485862491</v>
+        <v>60</v>
       </c>
       <c r="G17">
-        <v>51.016980025031629</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58.508040660361765</v>
+      </c>
+      <c r="H17">
+        <v>58.508040660355036</v>
+      </c>
+      <c r="I17">
+        <v>57.160534034089856</v>
+      </c>
+      <c r="J17">
+        <v>57.329306137553353</v>
+      </c>
+      <c r="K17">
+        <v>57.622991872990376</v>
+      </c>
+      <c r="L17">
+        <v>59.061738735805712</v>
+      </c>
+      <c r="M17">
+        <v>57.105835976687644</v>
+      </c>
+      <c r="N17">
+        <v>57.346050021717431</v>
+      </c>
+      <c r="O17">
+        <v>57.806681291667282</v>
+      </c>
+      <c r="P17">
+        <v>55.473344908633187</v>
+      </c>
+      <c r="Q17">
+        <v>50.510257216791416</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -3127,22 +3654,52 @@
         <v>40</v>
       </c>
       <c r="C18">
-        <v>41.539717147859804</v>
+        <v>40</v>
       </c>
       <c r="D18">
-        <v>41.539717156383801</v>
+        <v>40</v>
       </c>
       <c r="E18">
-        <v>43.017230886987093</v>
+        <v>40</v>
       </c>
       <c r="F18">
-        <v>46.510809524574043</v>
+        <v>40</v>
       </c>
       <c r="G18">
-        <v>51.016980025031643</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>41.53971715640715</v>
+      </c>
+      <c r="H18">
+        <v>41.539717156414333</v>
+      </c>
+      <c r="I18">
+        <v>43.017230886987107</v>
+      </c>
+      <c r="J18">
+        <v>42.827412717108196</v>
+      </c>
+      <c r="K18">
+        <v>42.500414068420355</v>
+      </c>
+      <c r="L18">
+        <v>40.947503820589965</v>
+      </c>
+      <c r="M18">
+        <v>42.983585962975859</v>
+      </c>
+      <c r="N18">
+        <v>42.728988202870738</v>
+      </c>
+      <c r="O18">
+        <v>42.244367000459199</v>
+      </c>
+      <c r="P18">
+        <v>44.748551369743367</v>
+      </c>
+      <c r="Q18">
+        <v>50.510257216859216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -3164,8 +3721,38 @@
       <c r="G19">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <v>200</v>
+      </c>
+      <c r="I19">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>200</v>
+      </c>
+      <c r="K19">
+        <v>200</v>
+      </c>
+      <c r="L19">
+        <v>200</v>
+      </c>
+      <c r="M19">
+        <v>200</v>
+      </c>
+      <c r="N19">
+        <v>200</v>
+      </c>
+      <c r="O19">
+        <v>200</v>
+      </c>
+      <c r="P19">
+        <v>200</v>
+      </c>
+      <c r="Q19">
+        <v>200.00000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -3173,22 +3760,52 @@
         <v>100</v>
       </c>
       <c r="C20">
-        <v>102.02649481767209</v>
+        <v>110</v>
       </c>
       <c r="D20">
-        <v>102.02649482407605</v>
+        <v>110</v>
       </c>
       <c r="E20">
-        <v>103.09328779209312</v>
+        <v>110</v>
       </c>
       <c r="F20">
-        <v>96.442586712999145</v>
+        <v>110</v>
       </c>
       <c r="G20">
-        <v>89.613092074379438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102.02649482409367</v>
+      </c>
+      <c r="H20">
+        <v>102.02649482409902</v>
+      </c>
+      <c r="I20">
+        <v>103.09328779209314</v>
+      </c>
+      <c r="J20">
+        <v>103.15969366572165</v>
+      </c>
+      <c r="K20">
+        <v>102.67830140301544</v>
+      </c>
+      <c r="L20">
+        <v>105.61634327199572</v>
+      </c>
+      <c r="M20">
+        <v>105.96423432063044</v>
+      </c>
+      <c r="N20">
+        <v>106.05509309478073</v>
+      </c>
+      <c r="O20">
+        <v>105.81182579537368</v>
+      </c>
+      <c r="P20">
+        <v>101.72343988424672</v>
+      </c>
+      <c r="Q20">
+        <v>94.211056383210959</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -3196,22 +3813,52 @@
         <v>100</v>
       </c>
       <c r="C21">
-        <v>108.6294774886228</v>
+        <v>100</v>
       </c>
       <c r="D21">
-        <v>108.62947748112251</v>
+        <v>100</v>
       </c>
       <c r="E21">
-        <v>107.3936305887708</v>
+        <v>100</v>
       </c>
       <c r="F21">
-        <v>115.56763302716089</v>
+        <v>100</v>
       </c>
       <c r="G21">
-        <v>125.29200080619496</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108.62947748110187</v>
+      </c>
+      <c r="H21">
+        <v>108.62947748109562</v>
+      </c>
+      <c r="I21">
+        <v>107.39363058877078</v>
+      </c>
+      <c r="J21">
+        <v>107.31758856276224</v>
+      </c>
+      <c r="K21">
+        <v>107.8711752942648</v>
+      </c>
+      <c r="L21">
+        <v>104.78402191624163</v>
+      </c>
+      <c r="M21">
+        <v>104.37266384297195</v>
+      </c>
+      <c r="N21">
+        <v>104.26620255060061</v>
+      </c>
+      <c r="O21">
+        <v>104.55214581680687</v>
+      </c>
+      <c r="P21">
+        <v>109.82972622532756</v>
+      </c>
+      <c r="Q21">
+        <v>122.60165352131571</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
@@ -3219,7 +3866,7 @@
         <v>200</v>
       </c>
       <c r="C22">
-        <v>200.71701865447653</v>
+        <v>200</v>
       </c>
       <c r="D22">
         <v>200</v>
@@ -3231,10 +3878,40 @@
         <v>200</v>
       </c>
       <c r="G22">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200.7170186096125</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+      <c r="I22">
+        <v>200</v>
+      </c>
+      <c r="J22">
+        <v>200</v>
+      </c>
+      <c r="K22">
+        <v>200</v>
+      </c>
+      <c r="L22">
+        <v>200</v>
+      </c>
+      <c r="M22">
+        <v>200</v>
+      </c>
+      <c r="N22">
+        <v>200</v>
+      </c>
+      <c r="O22">
+        <v>200</v>
+      </c>
+      <c r="P22">
+        <v>200</v>
+      </c>
+      <c r="Q22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -3242,7 +3919,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1.0035850932723827</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3254,145 +3931,45 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.0035850930480625</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>1.0268107803559916</v>
-      </c>
-      <c r="D24">
-        <v>1.0268107803031492</v>
-      </c>
-      <c r="E24">
+        <v>93</v>
+      </c>
+      <c r="I24">
         <v>1.016185505434424</v>
-      </c>
-      <c r="F24">
-        <v>1.0862618717772727</v>
-      </c>
-      <c r="G24">
-        <v>1.1690468695684744</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>0.87672423212192319</v>
-      </c>
-      <c r="D25">
-        <v>0.87672423219236773</v>
-      </c>
-      <c r="E25">
-        <v>0.88681325620491103</v>
-      </c>
-      <c r="F25">
-        <v>0.82408969313849223</v>
-      </c>
-      <c r="G25">
-        <v>0.76012909543532692</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1.0351629706265315</v>
-      </c>
-      <c r="D27">
-        <v>1.0351629708854644</v>
-      </c>
-      <c r="E27">
-        <v>1.0678356276899736</v>
-      </c>
-      <c r="F27">
-        <v>1.1033933594907175</v>
-      </c>
-      <c r="G27">
-        <v>1.1648853507249886</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0.9720072152994349</v>
-      </c>
-      <c r="D28">
-        <v>0.97200721521014122</v>
-      </c>
-      <c r="E28">
-        <v>0.94594737164343634</v>
-      </c>
-      <c r="F28">
-        <v>0.85817103861968957</v>
-      </c>
-      <c r="G28">
-        <v>0.7765902338166587</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29">
-        <v>200</v>
-      </c>
-      <c r="C29">
-        <v>200.71701865447656</v>
-      </c>
-      <c r="D29">
-        <v>200</v>
-      </c>
-      <c r="E29">
-        <v>200</v>
-      </c>
-      <c r="F29">
-        <v>200</v>
-      </c>
-      <c r="G29">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update CET test re sub elasts
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24C9A5E-0D3F-4BC2-8487-958957C13EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C4FA66-8F24-47B7-B8D6-A17650EDB7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12384" yWindow="696" windowWidth="10656" windowHeight="10008" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -24,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
   <si>
     <t>X.L</t>
   </si>
@@ -316,9 +308,6 @@
   </si>
   <si>
     <t>S...T1,1</t>
-  </si>
-  <si>
-    <t>PX.L/PW.L</t>
   </si>
 </sst>
 </file>
@@ -2759,28 +2748,28 @@
         <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>89</v>
@@ -2809,46 +2798,46 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.99999999969167375</v>
+        <v>0.99999999999737876</v>
       </c>
       <c r="D2">
+        <v>0.84841617521004631</v>
+      </c>
+      <c r="E2">
+        <v>0.84841617519703261</v>
+      </c>
+      <c r="F2">
+        <v>0.70716515735515217</v>
+      </c>
+      <c r="G2">
+        <v>0.72509467112342285</v>
+      </c>
+      <c r="H2">
+        <v>0.75612889144439233</v>
+      </c>
+      <c r="I2">
         <v>0.99999999999999989</v>
       </c>
-      <c r="E2">
+      <c r="J2">
         <v>0.99999999999999989</v>
       </c>
-      <c r="F2">
+      <c r="K2">
         <v>0.99999999999999989</v>
       </c>
-      <c r="G2">
-        <v>0.84841617519705081</v>
-      </c>
-      <c r="H2">
-        <v>0.84841617519703227</v>
-      </c>
-      <c r="I2">
-        <v>0.70716515735515162</v>
-      </c>
-      <c r="J2">
-        <v>0.72509467112342096</v>
-      </c>
-      <c r="K2">
-        <v>0.75612889144439288</v>
-      </c>
       <c r="L2">
-        <v>0.91659821359054672</v>
+        <v>0.91659821358300797</v>
       </c>
       <c r="M2">
-        <v>0.73369015208861166</v>
+        <v>0.73369015208861088</v>
       </c>
       <c r="N2">
-        <v>0.75685954678370782</v>
+        <v>0.75685954678370604</v>
       </c>
       <c r="O2">
-        <v>0.80071809649126724</v>
+        <v>0.80071809649126657</v>
       </c>
       <c r="P2">
-        <v>0.57048205371293126</v>
+        <v>0.57048205371293015</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -2859,49 +2848,49 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.99999999965367625</v>
+        <v>1.0000000000023659</v>
       </c>
       <c r="D3">
+        <v>1.1506325095176519</v>
+      </c>
+      <c r="E3">
+        <v>1.1506325095207361</v>
+      </c>
+      <c r="F3">
+        <v>1.2893059702343586</v>
+      </c>
+      <c r="G3">
+        <v>1.2717929473142049</v>
+      </c>
+      <c r="H3">
+        <v>1.2414185056039879</v>
+      </c>
+      <c r="I3">
         <v>1.0000000000000002</v>
       </c>
-      <c r="E3">
+      <c r="J3">
         <v>1.0000000000000002</v>
       </c>
-      <c r="F3">
+      <c r="K3">
         <v>1.0000000000000002</v>
       </c>
-      <c r="G3">
-        <v>1.150632509520773</v>
-      </c>
-      <c r="H3">
-        <v>1.1506325095207364</v>
-      </c>
-      <c r="I3">
-        <v>1.2893059702343592</v>
-      </c>
-      <c r="J3">
-        <v>1.2717929473142071</v>
-      </c>
-      <c r="K3">
-        <v>1.2414185056039873</v>
-      </c>
       <c r="L3">
-        <v>1.0832385402482214</v>
+        <v>1.0832385402476867</v>
       </c>
       <c r="M3">
         <v>1.2646965132512462</v>
       </c>
       <c r="N3">
-        <v>1.241790354991813</v>
+        <v>1.241790354991815</v>
       </c>
       <c r="O3">
-        <v>1.1983681743653367</v>
+        <v>1.1983681743653383</v>
       </c>
       <c r="P3">
-        <v>1.4254342349963718</v>
+        <v>1.4254342349963727</v>
       </c>
       <c r="Q3">
-        <v>1.9797958971135601</v>
+        <v>1.9797958971135603</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -2912,49 +2901,49 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.99999999937602346</v>
+        <v>0.99999999999981315</v>
       </c>
       <c r="D4">
-        <v>1.0000000000000835</v>
+        <v>1.0035850930534891</v>
       </c>
       <c r="E4">
-        <v>1.0000000000000835</v>
+        <v>1.0035850930478032</v>
       </c>
       <c r="F4">
-        <v>1.0000000000000835</v>
+        <v>1.0068914996667162</v>
       </c>
       <c r="G4">
-        <v>1.0035850930478354</v>
+        <v>1.006673704968486</v>
       </c>
       <c r="H4">
-        <v>1.0035850930478032</v>
+        <v>1.0057135773586172</v>
       </c>
       <c r="I4">
-        <v>1.0068914996667158</v>
+        <v>1.0000000000002727</v>
       </c>
       <c r="J4">
-        <v>1.0066737049684853</v>
+        <v>1.0000000000002727</v>
       </c>
       <c r="K4">
-        <v>1.0057135773586174</v>
+        <v>1.0000000000002727</v>
       </c>
       <c r="L4">
-        <v>1.0019757361058046</v>
+        <v>1.0019757361014827</v>
       </c>
       <c r="M4">
-        <v>1.0062537377172633</v>
+        <v>1.0062537377172638</v>
       </c>
       <c r="N4">
         <v>1.0059749908396223</v>
       </c>
       <c r="O4">
-        <v>1.0046559044043992</v>
+        <v>1.0046559044043997</v>
       </c>
       <c r="P4">
-        <v>0.9989805146510895</v>
+        <v>0.99898051465108928</v>
       </c>
       <c r="Q4">
-        <v>0.94407743479945161</v>
+        <v>0.94407743479945183</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -2965,49 +2954,49 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1.0246978500088042</v>
+        <v>1.0246978470350661</v>
       </c>
       <c r="D5">
-        <v>0.9523809523809269</v>
+        <v>1.0231427180776311</v>
       </c>
       <c r="E5">
-        <v>0.9523809523809269</v>
+        <v>1.0268107803027984</v>
       </c>
       <c r="F5">
-        <v>0.9523809523809269</v>
+        <v>1.016185505434424</v>
       </c>
       <c r="G5">
-        <v>1.0231427184558559</v>
+        <v>1.0155313673319302</v>
       </c>
       <c r="H5">
-        <v>1.0268107803029183</v>
+        <v>1.0202925382350085</v>
       </c>
       <c r="I5">
-        <v>1.016185505434424</v>
+        <v>0.95238095238086795</v>
       </c>
       <c r="J5">
-        <v>1.0155313673319299</v>
+        <v>0.95238095238086795</v>
       </c>
       <c r="K5">
-        <v>1.0202925382350085</v>
+        <v>0.95238095238086795</v>
       </c>
       <c r="L5">
-        <v>1.0330796752807549</v>
+        <v>1.0330796752850495</v>
       </c>
       <c r="M5">
-        <v>1.0263074053285333</v>
+        <v>1.0263074053285339</v>
       </c>
       <c r="N5">
-        <v>1.0245496568517749</v>
+        <v>1.0245496568517756</v>
       </c>
       <c r="O5">
-        <v>1.0292660659587862</v>
+        <v>1.0292660659587864</v>
       </c>
       <c r="P5">
-        <v>1.1136635243164417</v>
+        <v>1.1136635243164419</v>
       </c>
       <c r="Q5">
-        <v>1.2983516200037846</v>
+        <v>1.2983516200037848</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -3018,46 +3007,46 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.87283237043207507</v>
+        <v>0.87283236793118379</v>
       </c>
       <c r="D6">
-        <v>0.95238095238098064</v>
+        <v>0.87359232216741645</v>
       </c>
       <c r="E6">
-        <v>0.95238095238098064</v>
+        <v>0.87672423219269724</v>
       </c>
       <c r="F6">
-        <v>0.95238095238098064</v>
+        <v>0.88681325620491125</v>
       </c>
       <c r="G6">
-        <v>0.87359232243054408</v>
+        <v>0.88744162549260963</v>
       </c>
       <c r="H6">
-        <v>0.87672423219258488</v>
+        <v>0.88288734202338981</v>
       </c>
       <c r="I6">
-        <v>0.88681325620491125</v>
+        <v>0.95238095238104503</v>
       </c>
       <c r="J6">
-        <v>0.88744162549260985</v>
+        <v>0.95238095238104503</v>
       </c>
       <c r="K6">
-        <v>0.88288734202338981</v>
+        <v>0.95238095238104503</v>
       </c>
       <c r="L6">
-        <v>0.86740230739395141</v>
+        <v>0.86740230739016488</v>
       </c>
       <c r="M6">
-        <v>0.87425306835177607</v>
+        <v>0.87425306835177496</v>
       </c>
       <c r="N6">
-        <v>0.87603929679048465</v>
+        <v>0.87603929679048409</v>
       </c>
       <c r="O6">
-        <v>0.87125402922695383</v>
+        <v>0.87125402922695339</v>
       </c>
       <c r="P6">
-        <v>0.78953411260391282</v>
+        <v>0.78953411260391237</v>
       </c>
       <c r="Q6">
         <v>0.63360419775310972</v>
@@ -3074,7 +3063,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.99642771359477822</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3083,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.99642771392989316</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -3124,46 +3113,46 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.0283762514304395</v>
+        <v>1.0283762485106709</v>
       </c>
       <c r="D8">
-        <v>1.2380952380952241</v>
+        <v>1.0314650723607428</v>
       </c>
       <c r="E8">
-        <v>1.2380952380952241</v>
+        <v>1.035162970886397</v>
       </c>
       <c r="F8">
-        <v>1.2380952380952241</v>
+        <v>1.0678356276899734</v>
       </c>
       <c r="G8">
-        <v>1.0314650726247152</v>
+        <v>1.0639075291153639</v>
       </c>
       <c r="H8">
-        <v>1.0351629708860788</v>
+        <v>1.0564877098287577</v>
       </c>
       <c r="I8">
-        <v>1.0678356276899739</v>
+        <v>1.2380952380951948</v>
       </c>
       <c r="J8">
-        <v>1.0639075291153643</v>
+        <v>1.2380952380951948</v>
       </c>
       <c r="K8">
-        <v>1.0564877098287575</v>
+        <v>1.2380952380951948</v>
       </c>
       <c r="L8">
-        <v>1.0117879320523542</v>
+        <v>1.0117879320484757</v>
       </c>
       <c r="M8">
-        <v>1.0367784125216681</v>
+        <v>1.0367784125216684</v>
       </c>
       <c r="N8">
-        <v>1.0339436215788291</v>
+        <v>1.0339436215788289</v>
       </c>
       <c r="O8">
-        <v>1.0277166820777672</v>
+        <v>1.027716682077767</v>
       </c>
       <c r="P8">
-        <v>1.0178419107760996</v>
+        <v>1.0178419107760999</v>
       </c>
       <c r="Q8">
         <v>1.0394486229277171</v>
@@ -3177,46 +3166,46 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.97162375401182643</v>
+        <v>0.97162375115908584</v>
       </c>
       <c r="D9">
-        <v>0.76190476190460876</v>
+        <v>0.96853492695477694</v>
       </c>
       <c r="E9">
-        <v>0.76190476190460876</v>
+        <v>0.97200721520920963</v>
       </c>
       <c r="F9">
-        <v>0.76190476190460876</v>
+        <v>0.94594737164343656</v>
       </c>
       <c r="G9">
-        <v>0.96853492737470426</v>
+        <v>0.94943988081630282</v>
       </c>
       <c r="H9">
-        <v>0.97200721520952771</v>
+        <v>0.95493944473687153</v>
       </c>
       <c r="I9">
-        <v>0.94594737164343645</v>
+        <v>0.76190476190425982</v>
       </c>
       <c r="J9">
-        <v>0.94943988081630226</v>
+        <v>0.76190476190425982</v>
       </c>
       <c r="K9">
-        <v>0.95493944473687198</v>
+        <v>0.76190476190425982</v>
       </c>
       <c r="L9">
-        <v>0.9921635401381601</v>
+        <v>0.99216354015068353</v>
       </c>
       <c r="M9">
-        <v>0.97572906291222694</v>
+        <v>0.97572906291222683</v>
       </c>
       <c r="N9">
-        <v>0.97800635973064054</v>
+        <v>0.97800635973064065</v>
       </c>
       <c r="O9">
-        <v>0.98159512233037882</v>
+        <v>0.98159512233037849</v>
       </c>
       <c r="P9">
-        <v>0.92531027852785397</v>
+        <v>0.92531027852785408</v>
       </c>
       <c r="Q9">
         <v>0.84870624666994454</v>
@@ -3283,43 +3272,43 @@
         <v>80</v>
       </c>
       <c r="C11">
-        <v>80.000000000000014</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>79.999999999998181</v>
+        <v>79.999999999999986</v>
       </c>
       <c r="E11">
-        <v>79.999999999997286</v>
+        <v>80</v>
       </c>
       <c r="F11">
-        <v>79.999999999999119</v>
+        <v>83.789979418307439</v>
       </c>
       <c r="G11">
-        <v>80</v>
+        <v>85.397254560161727</v>
       </c>
       <c r="H11">
-        <v>80</v>
+        <v>82.088707595463845</v>
       </c>
       <c r="I11">
-        <v>83.789979418307439</v>
+        <v>79.99999999999406</v>
       </c>
       <c r="J11">
-        <v>85.397254560161699</v>
+        <v>79.999999999991104</v>
       </c>
       <c r="K11">
-        <v>82.088707595463845</v>
+        <v>79.999999999997016</v>
       </c>
       <c r="L11">
         <v>80</v>
       </c>
       <c r="M11">
-        <v>84.351462627766139</v>
+        <v>84.351462627766182</v>
       </c>
       <c r="N11">
-        <v>86.083347199002077</v>
+        <v>86.083347199002148</v>
       </c>
       <c r="O11">
-        <v>82.36898138312101</v>
+        <v>82.368981383121024</v>
       </c>
       <c r="P11">
         <v>84.302930903518373</v>
@@ -3336,46 +3325,46 @@
         <v>20</v>
       </c>
       <c r="C12">
-        <v>20.000000000000004</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>20.000000000001805</v>
+        <v>19.999999999999996</v>
       </c>
       <c r="E12">
-        <v>20.000000000002704</v>
+        <v>20</v>
       </c>
       <c r="F12">
-        <v>20.000000000000906</v>
+        <v>15.953297102016936</v>
       </c>
       <c r="G12">
-        <v>20</v>
+        <v>14.246995168670836</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>17.758407060505427</v>
       </c>
       <c r="I12">
-        <v>15.953297102016936</v>
+        <v>20.000000000005951</v>
       </c>
       <c r="J12">
-        <v>14.246995168670852</v>
+        <v>20.000000000008924</v>
       </c>
       <c r="K12">
-        <v>17.758407060505427</v>
+        <v>20.000000000002977</v>
       </c>
       <c r="L12">
         <v>20</v>
       </c>
       <c r="M12">
-        <v>15.302135083504712</v>
+        <v>15.302135083504657</v>
       </c>
       <c r="N12">
-        <v>13.453363640181522</v>
+        <v>13.453363640181482</v>
       </c>
       <c r="O12">
-        <v>17.430941640564519</v>
+        <v>17.430941640564509</v>
       </c>
       <c r="P12">
-        <v>14.941685322250365</v>
+        <v>14.941685322250358</v>
       </c>
       <c r="Q12" t="s">
         <v>81</v>
@@ -3392,43 +3381,43 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <v>29.999999999998153</v>
+        <v>30</v>
       </c>
       <c r="E13">
-        <v>29.999999999998767</v>
+        <v>30</v>
       </c>
       <c r="F13">
-        <v>29.999999999998767</v>
+        <v>34.553784903611756</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <v>32.966888913499105</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>33.184069765209088</v>
       </c>
       <c r="I13">
-        <v>34.553784903611756</v>
+        <v>29.999999999993904</v>
       </c>
       <c r="J13">
-        <v>32.966888913499105</v>
+        <v>29.999999999995943</v>
       </c>
       <c r="K13">
-        <v>33.184069765209088</v>
+        <v>29.999999999995943</v>
       </c>
       <c r="L13">
-        <v>30</v>
+        <v>29.999999999999996</v>
       </c>
       <c r="M13">
-        <v>35.375340199360892</v>
+        <v>35.375340199360956</v>
       </c>
       <c r="N13">
-        <v>33.448293412545176</v>
+        <v>33.448293412545205</v>
       </c>
       <c r="O13">
-        <v>33.670905403089371</v>
+        <v>33.670905403089385</v>
       </c>
       <c r="P13">
-        <v>37.550960863227068</v>
+        <v>37.550960863227083</v>
       </c>
       <c r="Q13">
         <v>44.925101910602201</v>
@@ -3445,40 +3434,40 @@
         <v>80</v>
       </c>
       <c r="D14">
-        <v>80.000000000001847</v>
+        <v>80</v>
       </c>
       <c r="E14">
-        <v>80.000000000001251</v>
+        <v>80</v>
       </c>
       <c r="F14">
-        <v>80.000000000001251</v>
+        <v>75.119576065481496</v>
       </c>
       <c r="G14">
-        <v>80</v>
+        <v>76.823333874806707</v>
       </c>
       <c r="H14">
-        <v>80</v>
+        <v>76.57358141148049</v>
       </c>
       <c r="I14">
-        <v>75.119576065481496</v>
+        <v>80.000000000006082</v>
       </c>
       <c r="J14">
-        <v>76.823333874806721</v>
+        <v>80.000000000004064</v>
       </c>
       <c r="K14">
-        <v>76.57358141148049</v>
+        <v>80.000000000004064</v>
       </c>
       <c r="L14">
         <v>80</v>
       </c>
       <c r="M14">
-        <v>74.166692410395541</v>
+        <v>74.166692410395456</v>
       </c>
       <c r="N14">
-        <v>76.266404448062389</v>
+        <v>76.26640444806236</v>
       </c>
       <c r="O14">
-        <v>76.004738963413018</v>
+        <v>76.004738963413004</v>
       </c>
       <c r="P14">
         <v>70.991555145634763</v>
@@ -3495,46 +3484,46 @@
         <v>40</v>
       </c>
       <c r="C15">
-        <v>40.000000000000007</v>
+        <v>40</v>
       </c>
       <c r="D15">
+        <v>38.517354218014205</v>
+      </c>
+      <c r="E15">
+        <v>38.51735422209844</v>
+      </c>
+      <c r="F15">
+        <v>37.194397849630235</v>
+      </c>
+      <c r="G15">
+        <v>37.359249566828296</v>
+      </c>
+      <c r="H15">
+        <v>37.646692039851651</v>
+      </c>
+      <c r="I15">
         <v>40</v>
       </c>
-      <c r="E15">
+      <c r="J15">
         <v>40</v>
       </c>
-      <c r="F15">
+      <c r="K15">
         <v>40</v>
       </c>
-      <c r="G15">
-        <v>38.517354222119764</v>
-      </c>
-      <c r="H15">
-        <v>38.517354222113113</v>
-      </c>
-      <c r="I15">
-        <v>37.194397849630228</v>
-      </c>
-      <c r="J15">
-        <v>37.359249566828282</v>
-      </c>
-      <c r="K15">
-        <v>37.646692039851665</v>
-      </c>
       <c r="L15">
-        <v>39.299714763812808</v>
+        <v>39.299714764397095</v>
       </c>
       <c r="M15">
-        <v>37.861280098811257</v>
+        <v>37.861280098811243</v>
       </c>
       <c r="N15">
-        <v>38.036420747024273</v>
+        <v>38.036420747024287</v>
       </c>
       <c r="O15">
-        <v>38.373445987225587</v>
+        <v>38.373445987225573</v>
       </c>
       <c r="P15">
-        <v>36.681951520633213</v>
+        <v>36.681951520633206</v>
       </c>
       <c r="Q15" t="s">
         <v>81</v>
@@ -3551,40 +3540,40 @@
         <v>60</v>
       </c>
       <c r="D16">
+        <v>61.530004416893014</v>
+      </c>
+      <c r="E16">
+        <v>61.530004412543398</v>
+      </c>
+      <c r="F16">
+        <v>62.980517254317519</v>
+      </c>
+      <c r="G16">
+        <v>62.795108515046742</v>
+      </c>
+      <c r="H16">
+        <v>62.475062175440947</v>
+      </c>
+      <c r="I16">
         <v>60</v>
       </c>
-      <c r="E16">
+      <c r="J16">
         <v>60</v>
       </c>
-      <c r="F16">
+      <c r="K16">
         <v>60</v>
       </c>
-      <c r="G16">
-        <v>61.530004412520697</v>
-      </c>
-      <c r="H16">
-        <v>61.530004412527788</v>
-      </c>
-      <c r="I16">
-        <v>62.980517254317533</v>
-      </c>
-      <c r="J16">
-        <v>62.795108515046778</v>
-      </c>
-      <c r="K16">
-        <v>62.475062175440918</v>
-      </c>
       <c r="L16">
-        <v>60.70717235830665</v>
+        <v>60.707172357710768</v>
       </c>
       <c r="M16">
-        <v>62.204472249917288</v>
+        <v>62.204472249917309</v>
       </c>
       <c r="N16">
-        <v>62.018844587381608</v>
+        <v>62.018844587381579</v>
       </c>
       <c r="O16">
-        <v>61.664268208122358</v>
+        <v>61.664268208122351</v>
       </c>
       <c r="P16">
         <v>63.479442824149956</v>
@@ -3604,46 +3593,46 @@
         <v>60</v>
       </c>
       <c r="D17">
+        <v>58.508040656204173</v>
+      </c>
+      <c r="E17">
+        <v>58.508040660340178</v>
+      </c>
+      <c r="F17">
+        <v>57.160534034089871</v>
+      </c>
+      <c r="G17">
+        <v>57.329306137553374</v>
+      </c>
+      <c r="H17">
+        <v>57.62299187299034</v>
+      </c>
+      <c r="I17">
         <v>60</v>
       </c>
-      <c r="E17">
+      <c r="J17">
         <v>60</v>
       </c>
-      <c r="F17">
+      <c r="K17">
         <v>60</v>
       </c>
-      <c r="G17">
-        <v>58.508040660361765</v>
-      </c>
-      <c r="H17">
-        <v>58.508040660355036</v>
-      </c>
-      <c r="I17">
-        <v>57.160534034089856</v>
-      </c>
-      <c r="J17">
-        <v>57.329306137553353</v>
-      </c>
-      <c r="K17">
-        <v>57.622991872990376</v>
-      </c>
       <c r="L17">
-        <v>59.061738735805712</v>
+        <v>59.061738736592389</v>
       </c>
       <c r="M17">
-        <v>57.105835976687644</v>
+        <v>57.105835976687651</v>
       </c>
       <c r="N17">
         <v>57.346050021717431</v>
       </c>
       <c r="O17">
-        <v>57.806681291667282</v>
+        <v>57.806681291667296</v>
       </c>
       <c r="P17">
         <v>55.473344908633187</v>
       </c>
       <c r="Q17">
-        <v>50.510257216791416</v>
+        <v>50.510257216791409</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -3657,40 +3646,40 @@
         <v>40</v>
       </c>
       <c r="D18">
+        <v>41.539717160834861</v>
+      </c>
+      <c r="E18">
+        <v>41.539717156430143</v>
+      </c>
+      <c r="F18">
+        <v>43.017230886987086</v>
+      </c>
+      <c r="G18">
+        <v>42.82741271710816</v>
+      </c>
+      <c r="H18">
+        <v>42.500414068420362</v>
+      </c>
+      <c r="I18">
         <v>40</v>
       </c>
-      <c r="E18">
+      <c r="J18">
         <v>40</v>
       </c>
-      <c r="F18">
+      <c r="K18">
         <v>40</v>
       </c>
-      <c r="G18">
-        <v>41.53971715640715</v>
-      </c>
-      <c r="H18">
-        <v>41.539717156414333</v>
-      </c>
-      <c r="I18">
-        <v>43.017230886987107</v>
-      </c>
-      <c r="J18">
-        <v>42.827412717108196</v>
-      </c>
-      <c r="K18">
-        <v>42.500414068420355</v>
-      </c>
       <c r="L18">
-        <v>40.947503820589965</v>
+        <v>40.947503819787705</v>
       </c>
       <c r="M18">
-        <v>42.983585962975859</v>
+        <v>42.983585962975887</v>
       </c>
       <c r="N18">
-        <v>42.728988202870738</v>
+        <v>42.728988202870696</v>
       </c>
       <c r="O18">
-        <v>42.244367000459199</v>
+        <v>42.244367000459214</v>
       </c>
       <c r="P18">
         <v>44.748551369743367</v>
@@ -3746,10 +3735,10 @@
         <v>200</v>
       </c>
       <c r="P19">
-        <v>200</v>
+        <v>199.99999999999997</v>
       </c>
       <c r="Q19">
-        <v>200.00000000000003</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -3763,40 +3752,40 @@
         <v>110</v>
       </c>
       <c r="D20">
+        <v>102.02649482742012</v>
+      </c>
+      <c r="E20">
+        <v>102.02649482411091</v>
+      </c>
+      <c r="F20">
+        <v>103.09328779209314</v>
+      </c>
+      <c r="G20">
+        <v>103.1596936657216</v>
+      </c>
+      <c r="H20">
+        <v>102.67830140301544</v>
+      </c>
+      <c r="I20">
         <v>110</v>
       </c>
-      <c r="E20">
+      <c r="J20">
         <v>110</v>
       </c>
-      <c r="F20">
+      <c r="K20">
         <v>110</v>
       </c>
-      <c r="G20">
-        <v>102.02649482409367</v>
-      </c>
-      <c r="H20">
-        <v>102.02649482409902</v>
-      </c>
-      <c r="I20">
-        <v>103.09328779209314</v>
-      </c>
-      <c r="J20">
-        <v>103.15969366572165</v>
-      </c>
-      <c r="K20">
-        <v>102.67830140301544</v>
-      </c>
       <c r="L20">
-        <v>105.61634327199572</v>
+        <v>105.61634327179119</v>
       </c>
       <c r="M20">
-        <v>105.96423432063044</v>
+        <v>105.9642343206304</v>
       </c>
       <c r="N20">
-        <v>106.05509309478073</v>
+        <v>106.05509309478072</v>
       </c>
       <c r="O20">
-        <v>105.81182579537368</v>
+        <v>105.81182579537366</v>
       </c>
       <c r="P20">
         <v>101.72343988424672</v>
@@ -3816,43 +3805,43 @@
         <v>100</v>
       </c>
       <c r="D21">
+        <v>108.629477477206</v>
+      </c>
+      <c r="E21">
+        <v>108.62947748108166</v>
+      </c>
+      <c r="F21">
+        <v>107.39363058877078</v>
+      </c>
+      <c r="G21">
+        <v>107.31758856276225</v>
+      </c>
+      <c r="H21">
+        <v>107.8711752942648</v>
+      </c>
+      <c r="I21">
         <v>100</v>
       </c>
-      <c r="E21">
+      <c r="J21">
         <v>100</v>
       </c>
-      <c r="F21">
+      <c r="K21">
         <v>100</v>
       </c>
-      <c r="G21">
-        <v>108.62947748110187</v>
-      </c>
-      <c r="H21">
-        <v>108.62947748109562</v>
-      </c>
-      <c r="I21">
-        <v>107.39363058877078</v>
-      </c>
-      <c r="J21">
-        <v>107.31758856276224</v>
-      </c>
-      <c r="K21">
-        <v>107.8711752942648</v>
-      </c>
       <c r="L21">
-        <v>104.78402191624163</v>
+        <v>104.78402191648524</v>
       </c>
       <c r="M21">
-        <v>104.37266384297195</v>
+        <v>104.37266384297199</v>
       </c>
       <c r="N21">
-        <v>104.26620255060061</v>
+        <v>104.26620255060067</v>
       </c>
       <c r="O21">
-        <v>104.55214581680687</v>
+        <v>104.5521458168069</v>
       </c>
       <c r="P21">
-        <v>109.82972622532756</v>
+        <v>109.82972622532759</v>
       </c>
       <c r="Q21">
         <v>122.60165352131571</v>
@@ -3869,7 +3858,7 @@
         <v>200</v>
       </c>
       <c r="D22">
-        <v>200</v>
+        <v>200.7170186771169</v>
       </c>
       <c r="E22">
         <v>200</v>
@@ -3878,7 +3867,7 @@
         <v>200</v>
       </c>
       <c r="G22">
-        <v>200.7170186096125</v>
+        <v>200</v>
       </c>
       <c r="H22">
         <v>200</v>
@@ -3922,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>1.0035850933855845</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -3931,7 +3920,7 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>1.0035850930480625</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -3965,12 +3954,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24">
-        <v>1.016185505434424</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add out.commod to tax rev, and test
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86643BD2-E8CC-4F3A-BB7E-5C441037A306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B07E8E5-8819-4B64-BA9C-263D6EE7BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="-13350" windowWidth="14400" windowHeight="7455" firstSheet="3" activeTab="4" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" firstSheet="3" activeTab="6" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -18,26 +18,20 @@
     <sheet name="TwoxTwoCESProd" sheetId="5" r:id="rId3"/>
     <sheet name="JPMGE" sheetId="6" r:id="rId4"/>
     <sheet name="TwoxTwowTax" sheetId="7" r:id="rId5"/>
+    <sheet name="TwoxTwowOTax" sheetId="8" r:id="rId6"/>
+    <sheet name="TwoxTwoCET-Scalar" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="107">
   <si>
     <t>X.L</t>
   </si>
@@ -247,6 +241,117 @@
   </si>
   <si>
     <t>CWI.L</t>
+  </si>
+  <si>
+    <t>Otax=.1</t>
+  </si>
+  <si>
+    <t>Otax=.2</t>
+  </si>
+  <si>
+    <t>Otax=.5</t>
+  </si>
+  <si>
+    <t>Otax=.9</t>
+  </si>
+  <si>
+    <t>A.L</t>
+  </si>
+  <si>
+    <t>B.L</t>
+  </si>
+  <si>
+    <t>W.L</t>
+  </si>
+  <si>
+    <t>PW.L</t>
+  </si>
+  <si>
+    <t>CONS.L</t>
+  </si>
+  <si>
+    <t>SAX.L</t>
+  </si>
+  <si>
+    <t>SAY.L</t>
+  </si>
+  <si>
+    <t>SBX.L</t>
+  </si>
+  <si>
+    <t>SBY.L</t>
+  </si>
+  <si>
+    <t>DAL.L</t>
+  </si>
+  <si>
+    <t>DAK.L</t>
+  </si>
+  <si>
+    <t>DBL.L</t>
+  </si>
+  <si>
+    <t>DBK.L</t>
+  </si>
+  <si>
+    <t>SW.L</t>
+  </si>
+  <si>
+    <t>DWX.L</t>
+  </si>
+  <si>
+    <t>DWY.L</t>
+  </si>
+  <si>
+    <t>DW.L</t>
+  </si>
+  <si>
+    <t>Sub=0Tr=0</t>
+  </si>
+  <si>
+    <t>diff=10</t>
+  </si>
+  <si>
+    <t>PW.FX=1</t>
+  </si>
+  <si>
+    <t>TA=2B=1.5</t>
+  </si>
+  <si>
+    <t>TrA=3B=1</t>
+  </si>
+  <si>
+    <t>TrA/B=1</t>
+  </si>
+  <si>
+    <t>S0Tr2,1.5</t>
+  </si>
+  <si>
+    <t>S0Tr=3,1</t>
+  </si>
+  <si>
+    <t>Sub=0Tr=1</t>
+  </si>
+  <si>
+    <t>1.52,.5T0</t>
+  </si>
+  <si>
+    <t>S..T2,1.5</t>
+  </si>
+  <si>
+    <t>S...T3,1</t>
+  </si>
+  <si>
+    <t>S...T1,1</t>
+  </si>
+  <si>
+    <t>TA=0.1</t>
+  </si>
+  <si>
+    <t>TA=100%</t>
+  </si>
+  <si>
+    <t>Undf</t>
   </si>
 </sst>
 </file>
@@ -609,9 +714,9 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -625,7 +730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,7 +747,7 @@
         <v>1.0488088481700486</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -659,7 +764,7 @@
         <v>1.0388601182540098</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -676,7 +781,7 @@
         <v>1.0454820635789062</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -693,7 +798,7 @@
         <v>1.048808848169914</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -710,7 +815,7 @@
         <v>1.0588528529215189</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -727,7 +832,7 @@
         <v>1.0521462187826638</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -744,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -761,7 +866,7 @@
         <v>1.0999999999996399</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -778,7 +883,7 @@
         <v>164.99999999997118</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -795,7 +900,7 @@
         <v>52.440442408500388</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -812,7 +917,7 @@
         <v>21.177057058432069</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -829,7 +934,7 @@
         <v>47.673129462283626</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -846,7 +951,7 @@
         <v>28.877805079687114</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -863,7 +968,7 @@
         <v>100.31820580257069</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -880,7 +985,7 @@
         <v>49.683306602973595</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -897,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -914,7 +1019,7 @@
         <v>1.0095765827768624</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -931,7 +1036,7 @@
         <v>1.0031820580257051</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -948,7 +1053,7 @@
         <v>0.95346258924580818</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -965,7 +1070,7 @@
         <v>1.0488088481700457</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -995,9 +1100,9 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1011,7 +1116,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1031,7 +1136,7 @@
         <v>2.0451802919810183</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1048,7 +1153,7 @@
         <v>6.086084552975235E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1065,7 +1170,7 @@
         <v>-5.5193504067180932E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1085,7 +1190,7 @@
         <v>3.9504305501987567</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1105,7 +1210,7 @@
         <v>1.0326000343166328</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1125,7 +1230,7 @@
         <v>3.0648345557341203</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1145,7 +1250,7 @@
         <v>0.95924189654998493</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1165,7 +1270,7 @@
         <v>0.94903401664811615</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1185,7 +1290,7 @@
         <v>0.99692550469586405</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1205,7 +1310,7 @@
         <v>1.0997574149564511</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1225,7 +1330,7 @@
         <v>2.1058244871455893</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1245,7 +1350,7 @@
         <v>4.2894913534466479</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1265,7 +1370,7 @@
         <v>1.0372737425956957</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1285,7 +1390,7 @@
         <v>1.018450090273892</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1305,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1325,7 +1430,7 @@
         <v>1.0764751417262008</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1358,9 +1463,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1374,7 +1479,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1496,7 @@
         <v>1.0505065382287513</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1408,7 +1513,7 @@
         <v>1.0324804191325847</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1425,7 +1530,7 @@
         <v>1.0444631317219772</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1442,7 +1547,7 @@
         <v>1.0950935908893114</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1459,7 +1564,7 @@
         <v>1.1142128759827274</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1581,7 @@
         <v>1.1014299521552819</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1493,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1615,7 @@
         <v>1.1945055822716992</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1527,7 +1632,7 @@
         <v>172.56044658173593</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1544,7 +1649,7 @@
         <v>52.32335976642014</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1561,7 +1666,7 @@
         <v>21.340810008438144</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1683,7 @@
         <v>47.874200147361819</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1595,7 +1700,7 @@
         <v>28.773271804644232</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1612,7 +1717,7 @@
         <v>100.57861367465195</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1629,7 +1734,7 @@
         <v>49.426369767125827</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1646,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1663,7 +1768,7 @@
         <v>1.0174590420877996</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1680,7 +1785,7 @@
         <v>1.0057861367454675</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1697,7 +1802,7 @@
         <v>0.91316395997525013</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1819,7 @@
         <v>1.0907794477197668</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1731,7 +1836,7 @@
         <v>157.57598073567559</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1755,12 +1860,12 @@
       <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="12" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1822,7 +1927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1890,7 +1995,7 @@
         <v>3.9827830288229387</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1958,7 +2063,7 @@
         <v>1.9711588500763977</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -2026,7 +2131,7 @@
         <v>2.0265111225373742</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -2094,7 +2199,7 @@
         <v>6.0177649222559033</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2137,7 +2242,7 @@
         <v>1.0310953593282555</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2180,7 +2285,7 @@
         <v>3.0618580948607583</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -2223,7 +2328,7 @@
         <v>0.96107338276642651</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2266,7 +2371,7 @@
         <v>0.95130881612337159</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2309,7 +2414,7 @@
         <v>0.98785653343465762</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2352,7 +2457,7 @@
         <v>1.1043704861326116</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -2395,7 +2500,7 @@
         <v>1.0355526292708772</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -2438,7 +2543,7 @@
         <v>1.0176064151448934</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -2481,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -2524,7 +2629,7 @@
         <v>1.0728580957681633</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -2567,7 +2672,7 @@
         <v>6.5457161915363269</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -2610,7 +2715,7 @@
         <v>2.0825117586808339</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -2653,7 +2758,7 @@
         <v>4.3132252303282845</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -2673,76 +2778,1203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999B2CB6-D228-42B8-B68B-E63D641C5E20}">
   <dimension ref="A1:E21"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0488088482495366</v>
+      </c>
+      <c r="D2">
+        <v>1.048808848291152</v>
+      </c>
+      <c r="E2">
+        <v>1.0488088481593842</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0388601183172488</v>
+      </c>
+      <c r="D3">
+        <v>1.0388601180790369</v>
+      </c>
+      <c r="E3">
+        <v>1.0388601182505068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0454820636535147</v>
+      </c>
+      <c r="D4">
+        <v>1.0454820633736372</v>
+      </c>
+      <c r="E4">
+        <v>1.0454820635708237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.98905852579244424</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.048808848138622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.99853032667237385</v>
+      </c>
+      <c r="D6">
+        <v>1.0095765827722971</v>
+      </c>
+      <c r="E6">
+        <v>1.058852852879361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.9922057674249718</v>
+      </c>
+      <c r="D7">
+        <v>1.0031820580243815</v>
+      </c>
+      <c r="E7">
+        <v>1.0521462187479544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.94303030266405441</v>
+      </c>
+      <c r="D8">
+        <v>0.95346258924320726</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0373333333393082</v>
+      </c>
+      <c r="D9">
+        <v>1.048808848128669</v>
+      </c>
+      <c r="E9">
+        <v>1.0999999998972825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>187.5</v>
+      </c>
+      <c r="C10">
+        <v>194.5</v>
+      </c>
+      <c r="D10">
+        <v>196.65165902915749</v>
+      </c>
+      <c r="E10">
+        <v>206.24999999007531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>125</v>
+      </c>
+      <c r="C11">
+        <v>125</v>
+      </c>
+      <c r="D11">
+        <v>124.99999999999999</v>
+      </c>
+      <c r="E11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>62.5</v>
+      </c>
+      <c r="C12">
+        <v>62.500000000000007</v>
+      </c>
+      <c r="D12">
+        <v>62.500000000000007</v>
+      </c>
+      <c r="E12">
+        <v>62.499999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52.440442418841862</v>
+      </c>
+      <c r="D13">
+        <v>52.440442407536104</v>
+      </c>
+      <c r="E13">
+        <v>52.440442406059141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>47.673129452884808</v>
+      </c>
+      <c r="D14">
+        <v>47.673129463162773</v>
+      </c>
+      <c r="E14">
+        <v>47.673129464505458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>21.177057063443652</v>
+      </c>
+      <c r="D15">
+        <v>21.177057057964916</v>
+      </c>
+      <c r="E15">
+        <v>21.17705705724919</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.877805075132347</v>
+      </c>
+      <c r="D16">
+        <v>28.877805080113006</v>
+      </c>
+      <c r="E16">
+        <v>28.877805080763672</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>187.5</v>
+      </c>
+      <c r="C17">
+        <v>196.02788693503402</v>
+      </c>
+      <c r="D17">
+        <v>196.02788688255697</v>
+      </c>
+      <c r="E17">
+        <v>196.02788691952946</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
+        <v>125</v>
+      </c>
+      <c r="C18">
+        <v>131.10110603221005</v>
+      </c>
+      <c r="D18">
+        <v>131.10110599531828</v>
+      </c>
+      <c r="E18">
+        <v>131.10110601980654</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>62.5</v>
+      </c>
+      <c r="C19">
+        <v>64.928757393926062</v>
+      </c>
+      <c r="D19">
+        <v>64.928757378323226</v>
+      </c>
+      <c r="E19">
+        <v>64.928757390805515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20">
+        <v>187.5</v>
+      </c>
+      <c r="C20">
+        <v>187.49999997857734</v>
+      </c>
+      <c r="D20">
+        <v>187.50000003446129</v>
+      </c>
+      <c r="E20">
+        <v>187.49999999867345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21">
+        <v>187.5</v>
+      </c>
+      <c r="C21">
+        <v>196.027886912637</v>
+      </c>
+      <c r="D21">
+        <v>196.02788691858564</v>
+      </c>
+      <c r="E21">
+        <v>196.02788691814257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEAD0FC-6E99-420C-BC7A-3D842CD4A7CD}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0488088482223459</v>
+      </c>
+      <c r="D2">
+        <v>1.0488088481702906</v>
+      </c>
+      <c r="E2">
+        <v>1.0488088481593985</v>
+      </c>
+      <c r="F2">
+        <v>1.0116855688658395</v>
+      </c>
+      <c r="G2">
+        <v>0.96884811102168134</v>
+      </c>
+      <c r="H2">
+        <v>0.78881063774659022</v>
+      </c>
+      <c r="I2">
+        <v>0.26532998322513834</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0388601182966062</v>
+      </c>
+      <c r="D3">
+        <v>1.038860118253863</v>
+      </c>
+      <c r="E3">
+        <v>1.0388601182505193</v>
+      </c>
+      <c r="F3">
+        <v>1.1123672179049628</v>
+      </c>
+      <c r="G3">
+        <v>1.197101452804781</v>
+      </c>
+      <c r="H3">
+        <v>1.5521999426621624</v>
+      </c>
+      <c r="I3">
+        <v>2.5753333516762882</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0454820636283344</v>
+      </c>
+      <c r="D4">
+        <v>1.0454820635787618</v>
+      </c>
+      <c r="E4">
+        <v>1.0454820635708377</v>
+      </c>
+      <c r="F4">
+        <v>1.0441905629409307</v>
+      </c>
+      <c r="G4">
+        <v>1.039634741431309</v>
+      </c>
+      <c r="H4">
+        <v>0.98847204957489676</v>
+      </c>
+      <c r="I4">
+        <v>0.56598124103192959</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.99795751000197275</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.0488088481386348</v>
+      </c>
+      <c r="F5">
+        <v>1.1709323695052041</v>
+      </c>
+      <c r="G5">
+        <v>1.3245970219534051</v>
+      </c>
+      <c r="H5">
+        <v>2.1692292538029863</v>
+      </c>
+      <c r="I5">
+        <v>11.608186765877146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.0075145327263733</v>
+      </c>
+      <c r="D6">
+        <v>1.0095765827768821</v>
+      </c>
+      <c r="E6">
+        <v>1.0588528528793759</v>
+      </c>
+      <c r="F6">
+        <v>1.0649499204188559</v>
+      </c>
+      <c r="G6">
+        <v>1.0720338858305598</v>
+      </c>
+      <c r="H6">
+        <v>1.102378027521483</v>
+      </c>
+      <c r="I6">
+        <v>1.195961679231847</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.0011330687136686</v>
+      </c>
+      <c r="D7">
+        <v>1.0031820580257127</v>
+      </c>
+      <c r="E7">
+        <v>1.0521462187479675</v>
+      </c>
+      <c r="F7">
+        <v>1.1344819828665367</v>
+      </c>
+      <c r="G7">
+        <v>1.2344078852090752</v>
+      </c>
+      <c r="H7">
+        <v>1.731066762936565</v>
+      </c>
+      <c r="I7">
+        <v>5.4418764732304421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.95151515128525777</v>
+      </c>
+      <c r="D8">
+        <v>0.95346258924559502</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0466666666627262</v>
+      </c>
+      <c r="D9">
+        <v>1.0488088481701119</v>
+      </c>
+      <c r="E9">
+        <v>1.0999999998973022</v>
+      </c>
+      <c r="F9">
+        <v>1.1105769136174084</v>
+      </c>
+      <c r="G9">
+        <v>1.1229166445216221</v>
+      </c>
+      <c r="H9">
+        <v>1.1763888888885616</v>
+      </c>
+      <c r="I9">
+        <v>1.347499999874207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>150</v>
+      </c>
+      <c r="C10">
+        <v>157</v>
+      </c>
+      <c r="D10">
+        <v>157.32132722551978</v>
+      </c>
+      <c r="E10">
+        <v>164.99999999178419</v>
+      </c>
+      <c r="F10">
+        <v>177.69230689285564</v>
+      </c>
+      <c r="G10">
+        <v>192.49999801341977</v>
+      </c>
+      <c r="H10">
+        <v>256.66666666662962</v>
+      </c>
+      <c r="I10">
+        <v>461.99999997773762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>101.16855688658394</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52.440442414743885</v>
+      </c>
+      <c r="D13">
+        <v>52.440442408506513</v>
+      </c>
+      <c r="E13">
+        <v>52.440442406059617</v>
+      </c>
+      <c r="F13">
+        <v>52.691956540287258</v>
+      </c>
+      <c r="G13">
+        <v>52.983880674258423</v>
+      </c>
+      <c r="H13">
+        <v>54.230731345072272</v>
+      </c>
+      <c r="I13">
+        <v>58.040933828510354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>47.673129456610248</v>
+      </c>
+      <c r="D14">
+        <v>47.673129462280592</v>
+      </c>
+      <c r="E14">
+        <v>47.673129464505038</v>
+      </c>
+      <c r="F14">
+        <v>47.445571661180352</v>
+      </c>
+      <c r="G14">
+        <v>47.184161827817846</v>
+      </c>
+      <c r="H14">
+        <v>46.099322985198228</v>
+      </c>
+      <c r="I14">
+        <v>43.073049227405299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>21.177057061457788</v>
+      </c>
+      <c r="D15">
+        <v>21.177057058435174</v>
+      </c>
+      <c r="E15">
+        <v>21.177057057249414</v>
+      </c>
+      <c r="F15">
+        <v>21.298998374443727</v>
+      </c>
+      <c r="G15">
+        <v>21.440677637410172</v>
+      </c>
+      <c r="H15">
+        <v>22.047560550428731</v>
+      </c>
+      <c r="I15">
+        <v>23.919233584290627</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.87780507693768</v>
+      </c>
+      <c r="D16">
+        <v>28.877805079685501</v>
+      </c>
+      <c r="E16">
+        <v>28.877805080763462</v>
+      </c>
+      <c r="F16">
+        <v>28.767478568955543</v>
+      </c>
+      <c r="G16">
+        <v>28.640608911640356</v>
+      </c>
+      <c r="H16">
+        <v>28.112591965135366</v>
+      </c>
+      <c r="I16">
+        <v>26.626234048078171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>150</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+      <c r="E17">
+        <v>150</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+      <c r="G17">
+        <v>150</v>
+      </c>
+      <c r="H17">
+        <v>150</v>
+      </c>
+      <c r="I17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>100.31820580330329</v>
+      </c>
+      <c r="D18">
+        <v>100.31820580257127</v>
+      </c>
+      <c r="E18">
+        <v>100.31820580223697</v>
+      </c>
+      <c r="F18">
+        <v>96.887063026974317</v>
+      </c>
+      <c r="G18">
+        <v>93.191201905025864</v>
+      </c>
+      <c r="H18">
+        <v>79.801005813550731</v>
+      </c>
+      <c r="I18">
+        <v>46.879642643468536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>49.683306602247974</v>
+      </c>
+      <c r="D19">
+        <v>49.683306602973047</v>
+      </c>
+      <c r="E19">
+        <v>49.683306603304153</v>
+      </c>
+      <c r="F19">
+        <v>53.264569586499768</v>
+      </c>
+      <c r="G19">
+        <v>57.573174760245493</v>
+      </c>
+      <c r="H19">
+        <v>78.515115492123201</v>
+      </c>
+      <c r="I19">
+        <v>227.51048665392318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20">
+        <v>150</v>
+      </c>
+      <c r="C20">
+        <v>149.99999998584357</v>
+      </c>
+      <c r="D20">
+        <v>150.00000000003155</v>
+      </c>
+      <c r="E20">
+        <v>149.99999999868393</v>
+      </c>
+      <c r="F20">
+        <v>149.99999986703938</v>
+      </c>
+      <c r="G20">
+        <v>149.99999971122381</v>
+      </c>
+      <c r="H20">
+        <v>149.99999999999787</v>
+      </c>
+      <c r="I20">
+        <v>149.9999999995207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21">
+        <v>150</v>
+      </c>
+      <c r="C21">
+        <v>156.82230952944988</v>
+      </c>
+      <c r="D21">
+        <v>156.82230953684726</v>
+      </c>
+      <c r="E21">
+        <v>156.82230953424974</v>
+      </c>
+      <c r="F21">
+        <v>156.62858430230338</v>
+      </c>
+      <c r="G21">
+        <v>155.94521091447459</v>
+      </c>
+      <c r="H21">
+        <v>148.27080743623242</v>
+      </c>
+      <c r="I21">
+        <v>84.897186154518167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABAD22F-3EC2-4900-9FF5-8F65369CA290}">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.0488088482495366</v>
+        <v>0.99999999999737876</v>
       </c>
       <c r="D2">
-        <v>1.048808848291152</v>
+        <v>0.84841617521004631</v>
       </c>
       <c r="E2">
-        <v>1.0488088481593842</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.84841617519703261</v>
+      </c>
+      <c r="F2">
+        <v>0.70716515735515217</v>
+      </c>
+      <c r="G2">
+        <v>0.72509467112342285</v>
+      </c>
+      <c r="H2">
+        <v>0.75612889144439233</v>
+      </c>
+      <c r="I2">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="J2">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="K2">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="L2">
+        <v>0.91659821358300797</v>
+      </c>
+      <c r="M2">
+        <v>0.73369015208861088</v>
+      </c>
+      <c r="N2">
+        <v>0.75685954678370604</v>
+      </c>
+      <c r="O2">
+        <v>0.80071809649126657</v>
+      </c>
+      <c r="P2">
+        <v>0.57048205371293015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.0388601183172488</v>
+        <v>1.0000000000023659</v>
       </c>
       <c r="D3">
-        <v>1.0388601180790369</v>
+        <v>1.1506325095176519</v>
       </c>
       <c r="E3">
-        <v>1.0388601182505068</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.1506325095207361</v>
+      </c>
+      <c r="F3">
+        <v>1.2893059702343586</v>
+      </c>
+      <c r="G3">
+        <v>1.2717929473142049</v>
+      </c>
+      <c r="H3">
+        <v>1.2414185056039879</v>
+      </c>
+      <c r="I3">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="J3">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="K3">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="L3">
+        <v>1.0832385402476867</v>
+      </c>
+      <c r="M3">
+        <v>1.2646965132512462</v>
+      </c>
+      <c r="N3">
+        <v>1.241790354991815</v>
+      </c>
+      <c r="O3">
+        <v>1.1983681743653383</v>
+      </c>
+      <c r="P3">
+        <v>1.4254342349963727</v>
+      </c>
+      <c r="Q3">
+        <v>1.9797958971135603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1.0454820636535147</v>
+        <v>0.99999999999981315</v>
       </c>
       <c r="D4">
-        <v>1.0454820633736372</v>
+        <v>1.0035850930534891</v>
       </c>
       <c r="E4">
-        <v>1.0454820635708237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.0035850930478032</v>
+      </c>
+      <c r="F4">
+        <v>1.0068914996667162</v>
+      </c>
+      <c r="G4">
+        <v>1.006673704968486</v>
+      </c>
+      <c r="H4">
+        <v>1.0057135773586172</v>
+      </c>
+      <c r="I4">
+        <v>1.0000000000002727</v>
+      </c>
+      <c r="J4">
+        <v>1.0000000000002727</v>
+      </c>
+      <c r="K4">
+        <v>1.0000000000002727</v>
+      </c>
+      <c r="L4">
+        <v>1.0019757361014827</v>
+      </c>
+      <c r="M4">
+        <v>1.0062537377172638</v>
+      </c>
+      <c r="N4">
+        <v>1.0059749908396223</v>
+      </c>
+      <c r="O4">
+        <v>1.0046559044043997</v>
+      </c>
+      <c r="P4">
+        <v>0.99898051465108928</v>
+      </c>
+      <c r="Q4">
+        <v>0.94407743479945183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2750,16 +3982,52 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.98905852579244424</v>
+        <v>1.0246978470350661</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>1.0231427180776311</v>
       </c>
       <c r="E5">
-        <v>1.048808848138622</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.0268107803027984</v>
+      </c>
+      <c r="F5">
+        <v>1.016185505434424</v>
+      </c>
+      <c r="G5">
+        <v>1.0155313673319302</v>
+      </c>
+      <c r="H5">
+        <v>1.0202925382350085</v>
+      </c>
+      <c r="I5">
+        <v>0.95238095238086795</v>
+      </c>
+      <c r="J5">
+        <v>0.95238095238086795</v>
+      </c>
+      <c r="K5">
+        <v>0.95238095238086795</v>
+      </c>
+      <c r="L5">
+        <v>1.0330796752850495</v>
+      </c>
+      <c r="M5">
+        <v>1.0263074053285339</v>
+      </c>
+      <c r="N5">
+        <v>1.0245496568517756</v>
+      </c>
+      <c r="O5">
+        <v>1.0292660659587864</v>
+      </c>
+      <c r="P5">
+        <v>1.1136635243164419</v>
+      </c>
+      <c r="Q5">
+        <v>1.2983516200037848</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2767,33 +4035,105 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.99853032667237385</v>
+        <v>0.87283236793118379</v>
       </c>
       <c r="D6">
-        <v>1.0095765827722971</v>
+        <v>0.87359232216741645</v>
       </c>
       <c r="E6">
-        <v>1.058852852879361</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.87672423219269724</v>
+      </c>
+      <c r="F6">
+        <v>0.88681325620491125</v>
+      </c>
+      <c r="G6">
+        <v>0.88744162549260963</v>
+      </c>
+      <c r="H6">
+        <v>0.88288734202338981</v>
+      </c>
+      <c r="I6">
+        <v>0.95238095238104503</v>
+      </c>
+      <c r="J6">
+        <v>0.95238095238104503</v>
+      </c>
+      <c r="K6">
+        <v>0.95238095238104503</v>
+      </c>
+      <c r="L6">
+        <v>0.86740230739016488</v>
+      </c>
+      <c r="M6">
+        <v>0.87425306835177496</v>
+      </c>
+      <c r="N6">
+        <v>0.87603929679048409</v>
+      </c>
+      <c r="O6">
+        <v>0.87125402922695339</v>
+      </c>
+      <c r="P6">
+        <v>0.78953411260391237</v>
+      </c>
+      <c r="Q6">
+        <v>0.63360419775310972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.9922057674249718</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1.0031820580243815</v>
+        <v>0.99642771359477822</v>
       </c>
       <c r="E7">
-        <v>1.0521462187479544</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2801,16 +4141,52 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.94303030266405441</v>
+        <v>1.0283762485106709</v>
       </c>
       <c r="D8">
-        <v>0.95346258924320726</v>
+        <v>1.0314650723607428</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.035162970886397</v>
+      </c>
+      <c r="F8">
+        <v>1.0678356276899734</v>
+      </c>
+      <c r="G8">
+        <v>1.0639075291153639</v>
+      </c>
+      <c r="H8">
+        <v>1.0564877098287577</v>
+      </c>
+      <c r="I8">
+        <v>1.2380952380951948</v>
+      </c>
+      <c r="J8">
+        <v>1.2380952380951948</v>
+      </c>
+      <c r="K8">
+        <v>1.2380952380951948</v>
+      </c>
+      <c r="L8">
+        <v>1.0117879320484757</v>
+      </c>
+      <c r="M8">
+        <v>1.0367784125216684</v>
+      </c>
+      <c r="N8">
+        <v>1.0339436215788289</v>
+      </c>
+      <c r="O8">
+        <v>1.027716682077767</v>
+      </c>
+      <c r="P8">
+        <v>1.0178419107760999</v>
+      </c>
+      <c r="Q8">
+        <v>1.0394486229277171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2818,217 +4194,791 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1.0373333333393082</v>
+        <v>0.97162375115908584</v>
       </c>
       <c r="D9">
-        <v>1.048808848128669</v>
+        <v>0.96853492695477694</v>
       </c>
       <c r="E9">
-        <v>1.0999999998972825</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.97200721520920963</v>
+      </c>
+      <c r="F9">
+        <v>0.94594737164343656</v>
+      </c>
+      <c r="G9">
+        <v>0.94943988081630282</v>
+      </c>
+      <c r="H9">
+        <v>0.95493944473687153</v>
+      </c>
+      <c r="I9">
+        <v>0.76190476190425982</v>
+      </c>
+      <c r="J9">
+        <v>0.76190476190425982</v>
+      </c>
+      <c r="K9">
+        <v>0.76190476190425982</v>
+      </c>
+      <c r="L9">
+        <v>0.99216354015068353</v>
+      </c>
+      <c r="M9">
+        <v>0.97572906291222683</v>
+      </c>
+      <c r="N9">
+        <v>0.97800635973064065</v>
+      </c>
+      <c r="O9">
+        <v>0.98159512233037849</v>
+      </c>
+      <c r="P9">
+        <v>0.92531027852785408</v>
+      </c>
+      <c r="Q9">
+        <v>0.84870624666994454</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B10">
-        <v>187.5</v>
+        <v>200</v>
       </c>
       <c r="C10">
-        <v>194.5</v>
+        <v>200</v>
       </c>
       <c r="D10">
-        <v>196.65165902915749</v>
+        <v>200</v>
       </c>
       <c r="E10">
-        <v>206.24999999007531</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
+      <c r="G10">
+        <v>200</v>
+      </c>
+      <c r="H10">
+        <v>200</v>
+      </c>
+      <c r="I10">
+        <v>200</v>
+      </c>
+      <c r="J10">
+        <v>200</v>
+      </c>
+      <c r="K10">
+        <v>200</v>
+      </c>
+      <c r="L10">
+        <v>200</v>
+      </c>
+      <c r="M10">
+        <v>200</v>
+      </c>
+      <c r="N10">
+        <v>200</v>
+      </c>
+      <c r="O10">
+        <v>200</v>
+      </c>
+      <c r="P10">
+        <v>200</v>
+      </c>
+      <c r="Q10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B11">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="C11">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>124.99999999999999</v>
+        <v>79.999999999999986</v>
       </c>
       <c r="E11">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+      <c r="F11">
+        <v>83.789979418307439</v>
+      </c>
+      <c r="G11">
+        <v>85.397254560161727</v>
+      </c>
+      <c r="H11">
+        <v>82.088707595463845</v>
+      </c>
+      <c r="I11">
+        <v>79.99999999999406</v>
+      </c>
+      <c r="J11">
+        <v>79.999999999991104</v>
+      </c>
+      <c r="K11">
+        <v>79.999999999997016</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+      <c r="M11">
+        <v>84.351462627766182</v>
+      </c>
+      <c r="N11">
+        <v>86.083347199002148</v>
+      </c>
+      <c r="O11">
+        <v>82.368981383121024</v>
+      </c>
+      <c r="P11">
+        <v>84.302930903518373</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>19.999999999999996</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>15.953297102016936</v>
+      </c>
+      <c r="G12">
+        <v>14.246995168670836</v>
+      </c>
+      <c r="H12">
+        <v>17.758407060505427</v>
+      </c>
+      <c r="I12">
+        <v>20.000000000005951</v>
+      </c>
+      <c r="J12">
+        <v>20.000000000008924</v>
+      </c>
+      <c r="K12">
+        <v>20.000000000002977</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>15.302135083504657</v>
+      </c>
+      <c r="N12">
+        <v>13.453363640181482</v>
+      </c>
+      <c r="O12">
+        <v>17.430941640564509</v>
+      </c>
+      <c r="P12">
+        <v>14.941685322250358</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>34.553784903611756</v>
+      </c>
+      <c r="G13">
+        <v>32.966888913499105</v>
+      </c>
+      <c r="H13">
+        <v>33.184069765209088</v>
+      </c>
+      <c r="I13">
+        <v>29.999999999993904</v>
+      </c>
+      <c r="J13">
+        <v>29.999999999995943</v>
+      </c>
+      <c r="K13">
+        <v>29.999999999995943</v>
+      </c>
+      <c r="L13">
+        <v>29.999999999999996</v>
+      </c>
+      <c r="M13">
+        <v>35.375340199360956</v>
+      </c>
+      <c r="N13">
+        <v>33.448293412545205</v>
+      </c>
+      <c r="O13">
+        <v>33.670905403089385</v>
+      </c>
+      <c r="P13">
+        <v>37.550960863227083</v>
+      </c>
+      <c r="Q13">
+        <v>44.925101910602201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>80</v>
+      </c>
+      <c r="E14">
+        <v>80</v>
+      </c>
+      <c r="F14">
+        <v>75.119576065481496</v>
+      </c>
+      <c r="G14">
+        <v>76.823333874806707</v>
+      </c>
+      <c r="H14">
+        <v>76.57358141148049</v>
+      </c>
+      <c r="I14">
+        <v>80.000000000006082</v>
+      </c>
+      <c r="J14">
+        <v>80.000000000004064</v>
+      </c>
+      <c r="K14">
+        <v>80.000000000004064</v>
+      </c>
+      <c r="L14">
+        <v>80</v>
+      </c>
+      <c r="M14">
+        <v>74.166692410395456</v>
+      </c>
+      <c r="N14">
+        <v>76.26640444806236</v>
+      </c>
+      <c r="O14">
+        <v>76.004738963413004</v>
+      </c>
+      <c r="P14">
+        <v>70.991555145634763</v>
+      </c>
+      <c r="Q14">
+        <v>58.463326814268953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>38.517354218014205</v>
+      </c>
+      <c r="E15">
+        <v>38.51735422209844</v>
+      </c>
+      <c r="F15">
+        <v>37.194397849630235</v>
+      </c>
+      <c r="G15">
+        <v>37.359249566828296</v>
+      </c>
+      <c r="H15">
+        <v>37.646692039851651</v>
+      </c>
+      <c r="I15">
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <v>40</v>
+      </c>
+      <c r="K15">
+        <v>40</v>
+      </c>
+      <c r="L15">
+        <v>39.299714764397095</v>
+      </c>
+      <c r="M15">
+        <v>37.861280098811243</v>
+      </c>
+      <c r="N15">
+        <v>38.036420747024287</v>
+      </c>
+      <c r="O15">
+        <v>38.373445987225573</v>
+      </c>
+      <c r="P15">
+        <v>36.681951520633206</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16">
         <v>60</v>
       </c>
-      <c r="B12">
-        <v>62.5</v>
-      </c>
-      <c r="C12">
-        <v>62.500000000000007</v>
-      </c>
-      <c r="D12">
-        <v>62.500000000000007</v>
-      </c>
-      <c r="E12">
-        <v>62.499999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>52.440442418841862</v>
-      </c>
-      <c r="D13">
-        <v>52.440442407536104</v>
-      </c>
-      <c r="E13">
-        <v>52.440442406059141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14">
-        <v>50</v>
-      </c>
-      <c r="C14">
-        <v>47.673129452884808</v>
-      </c>
-      <c r="D14">
-        <v>47.673129463162773</v>
-      </c>
-      <c r="E14">
-        <v>47.673129464505458</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>21.177057063443652</v>
-      </c>
-      <c r="D15">
-        <v>21.177057057964916</v>
-      </c>
-      <c r="E15">
-        <v>21.17705705724919</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16">
-        <v>30</v>
-      </c>
       <c r="C16">
-        <v>28.877805075132347</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>28.877805080113006</v>
+        <v>61.530004416893014</v>
       </c>
       <c r="E16">
-        <v>28.877805080763672</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>61.530004412543398</v>
+      </c>
+      <c r="F16">
+        <v>62.980517254317519</v>
+      </c>
+      <c r="G16">
+        <v>62.795108515046742</v>
+      </c>
+      <c r="H16">
+        <v>62.475062175440947</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="J16">
+        <v>60</v>
+      </c>
+      <c r="K16">
+        <v>60</v>
+      </c>
+      <c r="L16">
+        <v>60.707172357710768</v>
+      </c>
+      <c r="M16">
+        <v>62.204472249917309</v>
+      </c>
+      <c r="N16">
+        <v>62.018844587381579</v>
+      </c>
+      <c r="O16">
+        <v>61.664268208122351</v>
+      </c>
+      <c r="P16">
+        <v>63.479442824149956</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B17">
-        <v>187.5</v>
+        <v>60</v>
       </c>
       <c r="C17">
-        <v>196.02788693503402</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>196.02788688255697</v>
+        <v>58.508040656204173</v>
       </c>
       <c r="E17">
-        <v>196.02788691952946</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>58.508040660340178</v>
+      </c>
+      <c r="F17">
+        <v>57.160534034089871</v>
+      </c>
+      <c r="G17">
+        <v>57.329306137553374</v>
+      </c>
+      <c r="H17">
+        <v>57.62299187299034</v>
+      </c>
+      <c r="I17">
+        <v>60</v>
+      </c>
+      <c r="J17">
+        <v>60</v>
+      </c>
+      <c r="K17">
+        <v>60</v>
+      </c>
+      <c r="L17">
+        <v>59.061738736592389</v>
+      </c>
+      <c r="M17">
+        <v>57.105835976687651</v>
+      </c>
+      <c r="N17">
+        <v>57.346050021717431</v>
+      </c>
+      <c r="O17">
+        <v>57.806681291667296</v>
+      </c>
+      <c r="P17">
+        <v>55.473344908633187</v>
+      </c>
+      <c r="Q17">
+        <v>50.510257216791409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B18">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>131.10110603221005</v>
+        <v>40</v>
       </c>
       <c r="D18">
-        <v>131.10110599531828</v>
+        <v>41.539717160834861</v>
       </c>
       <c r="E18">
-        <v>131.10110601980654</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>41.539717156430143</v>
+      </c>
+      <c r="F18">
+        <v>43.017230886987086</v>
+      </c>
+      <c r="G18">
+        <v>42.82741271710816</v>
+      </c>
+      <c r="H18">
+        <v>42.500414068420362</v>
+      </c>
+      <c r="I18">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>40</v>
+      </c>
+      <c r="K18">
+        <v>40</v>
+      </c>
+      <c r="L18">
+        <v>40.947503819787705</v>
+      </c>
+      <c r="M18">
+        <v>42.983585962975887</v>
+      </c>
+      <c r="N18">
+        <v>42.728988202870696</v>
+      </c>
+      <c r="O18">
+        <v>42.244367000459214</v>
+      </c>
+      <c r="P18">
+        <v>44.748551369743367</v>
+      </c>
+      <c r="Q18">
+        <v>50.510257216859216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B19">
-        <v>62.5</v>
+        <v>200</v>
       </c>
       <c r="C19">
-        <v>64.928757393926062</v>
+        <v>200</v>
       </c>
       <c r="D19">
-        <v>64.928757378323226</v>
+        <v>200</v>
       </c>
       <c r="E19">
-        <v>64.928757390805515</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="F19">
+        <v>200</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+      <c r="H19">
+        <v>200</v>
+      </c>
+      <c r="I19">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>200</v>
+      </c>
+      <c r="K19">
+        <v>200</v>
+      </c>
+      <c r="L19">
+        <v>200</v>
+      </c>
+      <c r="M19">
+        <v>200</v>
+      </c>
+      <c r="N19">
+        <v>200</v>
+      </c>
+      <c r="O19">
+        <v>200</v>
+      </c>
+      <c r="P19">
+        <v>199.99999999999997</v>
+      </c>
+      <c r="Q19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B20">
-        <v>187.5</v>
+        <v>100</v>
       </c>
       <c r="C20">
-        <v>187.49999997857734</v>
+        <v>110</v>
       </c>
       <c r="D20">
-        <v>187.50000003446129</v>
+        <v>102.02649482742012</v>
       </c>
       <c r="E20">
-        <v>187.49999999867345</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>102.02649482411091</v>
+      </c>
+      <c r="F20">
+        <v>103.09328779209314</v>
+      </c>
+      <c r="G20">
+        <v>103.1596936657216</v>
+      </c>
+      <c r="H20">
+        <v>102.67830140301544</v>
+      </c>
+      <c r="I20">
+        <v>110</v>
+      </c>
+      <c r="J20">
+        <v>110</v>
+      </c>
+      <c r="K20">
+        <v>110</v>
+      </c>
+      <c r="L20">
+        <v>105.61634327179119</v>
+      </c>
+      <c r="M20">
+        <v>105.9642343206304</v>
+      </c>
+      <c r="N20">
+        <v>106.05509309478072</v>
+      </c>
+      <c r="O20">
+        <v>105.81182579537366</v>
+      </c>
+      <c r="P20">
+        <v>101.72343988424672</v>
+      </c>
+      <c r="Q20">
+        <v>94.211056383210959</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>108.629477477206</v>
+      </c>
+      <c r="E21">
+        <v>108.62947748108166</v>
+      </c>
+      <c r="F21">
+        <v>107.39363058877078</v>
+      </c>
+      <c r="G21">
+        <v>107.31758856276225</v>
+      </c>
+      <c r="H21">
+        <v>107.8711752942648</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>104.78402191648524</v>
+      </c>
+      <c r="M21">
+        <v>104.37266384297199</v>
+      </c>
+      <c r="N21">
+        <v>104.26620255060067</v>
+      </c>
+      <c r="O21">
+        <v>104.5521458168069</v>
+      </c>
+      <c r="P21">
+        <v>109.82972622532759</v>
+      </c>
+      <c r="Q21">
+        <v>122.60165352131571</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+      <c r="D22">
+        <v>200.7170186771169</v>
+      </c>
+      <c r="E22">
+        <v>200</v>
+      </c>
+      <c r="F22">
+        <v>200</v>
+      </c>
+      <c r="G22">
+        <v>200</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+      <c r="I22">
+        <v>200</v>
+      </c>
+      <c r="J22">
+        <v>200</v>
+      </c>
+      <c r="K22">
+        <v>200</v>
+      </c>
+      <c r="L22">
+        <v>200</v>
+      </c>
+      <c r="M22">
+        <v>200</v>
+      </c>
+      <c r="N22">
+        <v>200</v>
+      </c>
+      <c r="O22">
+        <v>200</v>
+      </c>
+      <c r="P22">
+        <v>200</v>
+      </c>
+      <c r="Q22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B21">
-        <v>187.5</v>
-      </c>
-      <c r="C21">
-        <v>196.027886912637</v>
-      </c>
-      <c r="D21">
-        <v>196.02788691858564</v>
-      </c>
-      <c r="E21">
-        <v>196.02788691814257</v>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1.0035850933855845</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SectorRef to Val, test passing
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B07E8E5-8819-4B64-BA9C-263D6EE7BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE2E16D-3A5C-43DA-95BD-FEB39BD5ABA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" firstSheet="3" activeTab="6" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" firstSheet="3" activeTab="5" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -3145,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEAD0FC-6E99-420C-BC7A-3D842CD4A7CD}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3453,7 +3453,7 @@
         <v>100</v>
       </c>
       <c r="F11">
-        <v>101.16855688658394</v>
+        <v>100</v>
       </c>
       <c r="G11">
         <v>100</v>
@@ -3764,7 +3764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABAD22F-3EC2-4900-9FF5-8F65369CA290}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Fix Otax for indexed consumer, & add tests
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE2E16D-3A5C-43DA-95BD-FEB39BD5ABA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021B2191-4E62-4B3D-9789-BE5856971FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" firstSheet="3" activeTab="5" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="5" activeTab="7" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="TwoxTwowTax" sheetId="7" r:id="rId5"/>
     <sheet name="TwoxTwowOTax" sheetId="8" r:id="rId6"/>
     <sheet name="TwoxTwoCET-Scalar" sheetId="9" r:id="rId7"/>
+    <sheet name="TwoxTwowOTax_IndCon" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="115">
   <si>
     <t>X.L</t>
   </si>
@@ -352,6 +353,30 @@
   </si>
   <si>
     <t>Undf</t>
+  </si>
+  <si>
+    <t>RAA.L</t>
+  </si>
+  <si>
+    <t>RAB.L</t>
+  </si>
+  <si>
+    <t>DURAA.L</t>
+  </si>
+  <si>
+    <t>DURAB.L</t>
+  </si>
+  <si>
+    <t>Otaxa=.1</t>
+  </si>
+  <si>
+    <t>Otaxa=.2</t>
+  </si>
+  <si>
+    <t>Otaxa=.5</t>
+  </si>
+  <si>
+    <t>Otaxa=.9</t>
   </si>
 </sst>
 </file>
@@ -3145,7 +3170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEAD0FC-6E99-420C-BC7A-3D842CD4A7CD}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4984,4 +5009,916 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7451895E-4CE7-43DD-A1ED-1D95ED3FA1C3}">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0488088483186848</v>
+      </c>
+      <c r="D2">
+        <v>1.0488088481702902</v>
+      </c>
+      <c r="E2">
+        <v>1.0488088481593985</v>
+      </c>
+      <c r="F2">
+        <v>1.0116855688658399</v>
+      </c>
+      <c r="G2">
+        <v>0.96884811102168134</v>
+      </c>
+      <c r="H2">
+        <v>0.78881063774659033</v>
+      </c>
+      <c r="I2">
+        <v>0.26532998322513918</v>
+      </c>
+      <c r="J2">
+        <v>1.0488088477828985</v>
+      </c>
+      <c r="K2">
+        <v>1.0488088481701499</v>
+      </c>
+      <c r="L2">
+        <v>1.0488088481508704</v>
+      </c>
+      <c r="M2">
+        <v>1.0488088481700473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0388601183809216</v>
+      </c>
+      <c r="D3">
+        <v>1.0388601182538633</v>
+      </c>
+      <c r="E3">
+        <v>1.0388601182505182</v>
+      </c>
+      <c r="F3">
+        <v>1.1123672179049622</v>
+      </c>
+      <c r="G3">
+        <v>1.1971014528047808</v>
+      </c>
+      <c r="H3">
+        <v>1.5521999426621618</v>
+      </c>
+      <c r="I3">
+        <v>2.5753333516762922</v>
+      </c>
+      <c r="J3">
+        <v>1.03886011809678</v>
+      </c>
+      <c r="K3">
+        <v>1.038860118254084</v>
+      </c>
+      <c r="L3">
+        <v>1.0388601182463502</v>
+      </c>
+      <c r="M3">
+        <v>1.0388601182540023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0454820637214235</v>
+      </c>
+      <c r="D4">
+        <v>1.0454820635787621</v>
+      </c>
+      <c r="E4">
+        <v>1.0454820635708375</v>
+      </c>
+      <c r="F4">
+        <v>1.0441905629409312</v>
+      </c>
+      <c r="G4">
+        <v>1.0396347414313092</v>
+      </c>
+      <c r="H4">
+        <v>0.98847204957489676</v>
+      </c>
+      <c r="I4">
+        <v>0.56598124103193115</v>
+      </c>
+      <c r="J4">
+        <v>1.0454820632747557</v>
+      </c>
+      <c r="K4">
+        <v>1.0454820635789983</v>
+      </c>
+      <c r="L4">
+        <v>1.0454820635638864</v>
+      </c>
+      <c r="M4">
+        <v>1.0454820635789031</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.9979575093627594</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.048808848138634</v>
+      </c>
+      <c r="F5">
+        <v>1.1709323695052041</v>
+      </c>
+      <c r="G5">
+        <v>1.3245970219534056</v>
+      </c>
+      <c r="H5">
+        <v>2.1692292538029858</v>
+      </c>
+      <c r="I5">
+        <v>11.608186765877173</v>
+      </c>
+      <c r="J5">
+        <v>1.1653431632449567</v>
+      </c>
+      <c r="K5">
+        <v>1.3110110602126839</v>
+      </c>
+      <c r="L5">
+        <v>2.0976176962134967</v>
+      </c>
+      <c r="M5">
+        <v>10.488088481700085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.0075145321457899</v>
+      </c>
+      <c r="D6">
+        <v>1.0095765827768821</v>
+      </c>
+      <c r="E6">
+        <v>1.0588528528793753</v>
+      </c>
+      <c r="F6">
+        <v>1.0649499204188564</v>
+      </c>
+      <c r="G6">
+        <v>1.07203388583056</v>
+      </c>
+      <c r="H6">
+        <v>1.102378027521483</v>
+      </c>
+      <c r="I6">
+        <v>1.1959616792318508</v>
+      </c>
+      <c r="J6">
+        <v>1.1765031680734017</v>
+      </c>
+      <c r="K6">
+        <v>1.3235660661522233</v>
+      </c>
+      <c r="L6">
+        <v>2.1177057056757684</v>
+      </c>
+      <c r="M6">
+        <v>10.588528529216054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.0011330680946173</v>
+      </c>
+      <c r="D7">
+        <v>1.0031820580257129</v>
+      </c>
+      <c r="E7">
+        <v>1.0521462187479667</v>
+      </c>
+      <c r="F7">
+        <v>1.1344819828665369</v>
+      </c>
+      <c r="G7">
+        <v>1.2344078852090754</v>
+      </c>
+      <c r="H7">
+        <v>1.731066762936565</v>
+      </c>
+      <c r="I7">
+        <v>5.4418764732304545</v>
+      </c>
+      <c r="J7">
+        <v>1.1690513526718143</v>
+      </c>
+      <c r="K7">
+        <v>1.3151827734786337</v>
+      </c>
+      <c r="L7">
+        <v>2.1042924374260297</v>
+      </c>
+      <c r="M7">
+        <v>10.521462187827565</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.95151515026786349</v>
+      </c>
+      <c r="D8">
+        <v>0.95346258924559524</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0466666662537283</v>
+      </c>
+      <c r="D9">
+        <v>1.0488088481701119</v>
+      </c>
+      <c r="E9">
+        <v>1.0999999998973014</v>
+      </c>
+      <c r="F9">
+        <v>1.1105769136174086</v>
+      </c>
+      <c r="G9">
+        <v>1.1229166445216223</v>
+      </c>
+      <c r="H9">
+        <v>1.1763888888885614</v>
+      </c>
+      <c r="I9">
+        <v>1.3474999998742136</v>
+      </c>
+      <c r="J9">
+        <v>1.0999999961516416</v>
+      </c>
+      <c r="K9">
+        <v>1.0999999999999863</v>
+      </c>
+      <c r="L9">
+        <v>1.0999999998056436</v>
+      </c>
+      <c r="M9">
+        <v>1.0999999999996521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>50.000000000000007</v>
+      </c>
+      <c r="I11">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+      <c r="D12">
+        <v>150</v>
+      </c>
+      <c r="E12">
+        <v>150</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="G12">
+        <v>150</v>
+      </c>
+      <c r="H12">
+        <v>150</v>
+      </c>
+      <c r="I12">
+        <v>150</v>
+      </c>
+      <c r="J12">
+        <v>150</v>
+      </c>
+      <c r="K12">
+        <v>150</v>
+      </c>
+      <c r="L12">
+        <v>150</v>
+      </c>
+      <c r="M12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52.440442432533608</v>
+      </c>
+      <c r="D13">
+        <v>52.440442408506506</v>
+      </c>
+      <c r="E13">
+        <v>52.440442406059596</v>
+      </c>
+      <c r="F13">
+        <v>52.691956540287265</v>
+      </c>
+      <c r="G13">
+        <v>52.983880674258423</v>
+      </c>
+      <c r="H13">
+        <v>54.230731345072272</v>
+      </c>
+      <c r="I13">
+        <v>58.040933828510497</v>
+      </c>
+      <c r="J13">
+        <v>52.440442316775936</v>
+      </c>
+      <c r="K13">
+        <v>52.440442408507252</v>
+      </c>
+      <c r="L13">
+        <v>52.440442403874791</v>
+      </c>
+      <c r="M13">
+        <v>52.440442408499287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>47.673129440437769</v>
+      </c>
+      <c r="D14">
+        <v>47.673129462280592</v>
+      </c>
+      <c r="E14">
+        <v>47.673129464505053</v>
+      </c>
+      <c r="F14">
+        <v>47.445571661180352</v>
+      </c>
+      <c r="G14">
+        <v>47.184161827817846</v>
+      </c>
+      <c r="H14">
+        <v>46.099322985198235</v>
+      </c>
+      <c r="I14">
+        <v>43.0730492274052</v>
+      </c>
+      <c r="J14">
+        <v>47.673129545672026</v>
+      </c>
+      <c r="K14">
+        <v>47.67312946227991</v>
+      </c>
+      <c r="L14">
+        <v>47.67312946649124</v>
+      </c>
+      <c r="M14">
+        <v>47.673129462287157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>21.177057070078629</v>
+      </c>
+      <c r="D15">
+        <v>21.177057058435174</v>
+      </c>
+      <c r="E15">
+        <v>21.177057057249407</v>
+      </c>
+      <c r="F15">
+        <v>21.29899837444373</v>
+      </c>
+      <c r="G15">
+        <v>21.440677637410175</v>
+      </c>
+      <c r="H15">
+        <v>22.047560550428727</v>
+      </c>
+      <c r="I15">
+        <v>23.919233584290698</v>
+      </c>
+      <c r="J15">
+        <v>21.177057013982832</v>
+      </c>
+      <c r="K15">
+        <v>21.177057058435533</v>
+      </c>
+      <c r="L15">
+        <v>21.177057056190659</v>
+      </c>
+      <c r="M15">
+        <v>21.177057058431675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.877805069100546</v>
+      </c>
+      <c r="D16">
+        <v>28.877805079685508</v>
+      </c>
+      <c r="E16">
+        <v>28.877805080763476</v>
+      </c>
+      <c r="F16">
+        <v>28.767478568955539</v>
+      </c>
+      <c r="G16">
+        <v>28.640608911640356</v>
+      </c>
+      <c r="H16">
+        <v>28.112591965135362</v>
+      </c>
+      <c r="I16">
+        <v>26.626234048078118</v>
+      </c>
+      <c r="J16">
+        <v>28.877805120096724</v>
+      </c>
+      <c r="K16">
+        <v>28.877805079685178</v>
+      </c>
+      <c r="L16">
+        <v>28.877805081725974</v>
+      </c>
+      <c r="M16">
+        <v>28.877805079688688</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>100.31820580545239</v>
+      </c>
+      <c r="D17">
+        <v>100.31820580257127</v>
+      </c>
+      <c r="E17">
+        <v>100.318205802237</v>
+      </c>
+      <c r="F17">
+        <v>96.887063026974317</v>
+      </c>
+      <c r="G17">
+        <v>93.191201905025878</v>
+      </c>
+      <c r="H17">
+        <v>79.801005813550731</v>
+      </c>
+      <c r="I17">
+        <v>46.879642643468557</v>
+      </c>
+      <c r="J17">
+        <v>100.31820579012654</v>
+      </c>
+      <c r="K17">
+        <v>100.31820580257138</v>
+      </c>
+      <c r="L17">
+        <v>100.31820580194328</v>
+      </c>
+      <c r="M17">
+        <v>100.31820580257032</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>49.683306600119259</v>
+      </c>
+      <c r="D18">
+        <v>49.683306602973047</v>
+      </c>
+      <c r="E18">
+        <v>49.683306603304153</v>
+      </c>
+      <c r="F18">
+        <v>53.264569586499746</v>
+      </c>
+      <c r="G18">
+        <v>57.573174760245507</v>
+      </c>
+      <c r="H18">
+        <v>78.515115492123186</v>
+      </c>
+      <c r="I18">
+        <v>227.51048665392312</v>
+      </c>
+      <c r="J18">
+        <v>49.683306615299706</v>
+      </c>
+      <c r="K18">
+        <v>49.683306602972934</v>
+      </c>
+      <c r="L18">
+        <v>49.683306603595071</v>
+      </c>
+      <c r="M18">
+        <v>49.683306602973971</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <v>78.5</v>
+      </c>
+      <c r="D19">
+        <v>78.66066361275989</v>
+      </c>
+      <c r="E19">
+        <v>82.499999995892054</v>
+      </c>
+      <c r="F19">
+        <v>94.769230348159326</v>
+      </c>
+      <c r="G19">
+        <v>109.08333223255492</v>
+      </c>
+      <c r="H19">
+        <v>171.11111111108713</v>
+      </c>
+      <c r="I19">
+        <v>369.59999998277107</v>
+      </c>
+      <c r="J19">
+        <v>94.722222049211879</v>
+      </c>
+      <c r="K19">
+        <v>109.99999999999929</v>
+      </c>
+      <c r="L19">
+        <v>192.49999998355372</v>
+      </c>
+      <c r="M19">
+        <v>1072.4999999997528</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20">
+        <v>75</v>
+      </c>
+      <c r="C20">
+        <v>78.499999935461872</v>
+      </c>
+      <c r="D20">
+        <v>78.66066361275989</v>
+      </c>
+      <c r="E20">
+        <v>82.499999995892054</v>
+      </c>
+      <c r="F20">
+        <v>82.923076544696343</v>
+      </c>
+      <c r="G20">
+        <v>83.416665780864889</v>
+      </c>
+      <c r="H20">
+        <v>85.555555555542455</v>
+      </c>
+      <c r="I20">
+        <v>92.399999994968539</v>
+      </c>
+      <c r="J20">
+        <v>88.611110946695504</v>
+      </c>
+      <c r="K20">
+        <v>96.249999999999375</v>
+      </c>
+      <c r="L20">
+        <v>137.49999998745824</v>
+      </c>
+      <c r="M20">
+        <v>577.49999999986312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21">
+        <v>75</v>
+      </c>
+      <c r="C21">
+        <v>78.411154757743773</v>
+      </c>
+      <c r="D21">
+        <v>78.411154768423614</v>
+      </c>
+      <c r="E21">
+        <v>78.411154767124899</v>
+      </c>
+      <c r="F21">
+        <v>83.53524496590282</v>
+      </c>
+      <c r="G21">
+        <v>88.368952871748021</v>
+      </c>
+      <c r="H21">
+        <v>98.847204957488685</v>
+      </c>
+      <c r="I21">
+        <v>67.917748923721135</v>
+      </c>
+      <c r="J21">
+        <v>81.024859885520428</v>
+      </c>
+      <c r="K21">
+        <v>83.638565086319787</v>
+      </c>
+      <c r="L21">
+        <v>91.479680561424104</v>
+      </c>
+      <c r="M21">
+        <v>101.93450119894401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22">
+        <v>75</v>
+      </c>
+      <c r="C22">
+        <v>78.411154757743773</v>
+      </c>
+      <c r="D22">
+        <v>78.411154768423614</v>
+      </c>
+      <c r="E22">
+        <v>78.411154767124899</v>
+      </c>
+      <c r="F22">
+        <v>73.093339336400547</v>
+      </c>
+      <c r="G22">
+        <v>67.576258042726579</v>
+      </c>
+      <c r="H22">
+        <v>49.423602478743703</v>
+      </c>
+      <c r="I22">
+        <v>16.979437230797199</v>
+      </c>
+      <c r="J22">
+        <v>75.797449568129579</v>
+      </c>
+      <c r="K22">
+        <v>73.183744450529815</v>
+      </c>
+      <c r="L22">
+        <v>65.342628972068269</v>
+      </c>
+      <c r="M22">
+        <v>54.887808337892558</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add test, scratch for outTax non-0 tr_elas
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021B2191-4E62-4B3D-9789-BE5856971FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EC14CB-8026-4392-8FDC-CB6AF227E69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="5" activeTab="7" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="3864" yWindow="3072" windowWidth="13824" windowHeight="7260" firstSheet="7" activeTab="8" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="TwoxTwowOTax" sheetId="8" r:id="rId6"/>
     <sheet name="TwoxTwoCET-Scalar" sheetId="9" r:id="rId7"/>
     <sheet name="TwoxTwowOTax_IndCon" sheetId="10" r:id="rId8"/>
+    <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="119">
   <si>
     <t>X.L</t>
   </si>
@@ -377,6 +378,18 @@
   </si>
   <si>
     <t>Otaxa=.9</t>
+  </si>
+  <si>
+    <t>OUTTAX=0.1</t>
+  </si>
+  <si>
+    <t>SUBes=1</t>
+  </si>
+  <si>
+    <t>OUTTAX=0.2</t>
+  </si>
+  <si>
+    <t>S1Tr=3,1</t>
   </si>
 </sst>
 </file>
@@ -5015,7 +5028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7451895E-4CE7-43DD-A1ED-1D95ED3FA1C3}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5921,4 +5934,1230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F07C38F-0BBA-4014-8D0C-146F422C055E}">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.89337249339501046</v>
+      </c>
+      <c r="E2">
+        <v>0.89337249339497415</v>
+      </c>
+      <c r="F2">
+        <v>0.77047179008375588</v>
+      </c>
+      <c r="G2">
+        <v>0.64533631428135496</v>
+      </c>
+      <c r="H2">
+        <v>0.65743472294980465</v>
+      </c>
+      <c r="I2">
+        <v>0.59043552853534853</v>
+      </c>
+      <c r="J2">
+        <v>0.64533631351198184</v>
+      </c>
+      <c r="K2">
+        <v>0.65743472294980621</v>
+      </c>
+      <c r="L2">
+        <v>0.87514262265812059</v>
+      </c>
+      <c r="M2">
+        <v>0.65301554051929644</v>
+      </c>
+      <c r="N2">
+        <v>0.71778700395030315</v>
+      </c>
+      <c r="O2">
+        <v>0.74236189253677176</v>
+      </c>
+      <c r="P2">
+        <v>0.54435839325680246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D3">
+        <v>1.1061558951437069</v>
+      </c>
+      <c r="E3">
+        <v>1.1061558951436663</v>
+      </c>
+      <c r="F3">
+        <v>1.2273542775350592</v>
+      </c>
+      <c r="G3">
+        <v>1.3495011899745444</v>
+      </c>
+      <c r="H3">
+        <v>1.3377464494522329</v>
+      </c>
+      <c r="I3">
+        <v>1.4026964717016865</v>
+      </c>
+      <c r="J3">
+        <v>1.3495011908864791</v>
+      </c>
+      <c r="K3">
+        <v>1.3377464494522311</v>
+      </c>
+      <c r="L3">
+        <v>1.1244941079798842</v>
+      </c>
+      <c r="M3">
+        <v>1.3442824845818007</v>
+      </c>
+      <c r="N3">
+        <v>1.2804060756948956</v>
+      </c>
+      <c r="O3">
+        <v>1.2561259176857724</v>
+      </c>
+      <c r="P3">
+        <v>1.4510658620714896</v>
+      </c>
+      <c r="Q3">
+        <v>1.9797958971136496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D4">
+        <v>0.99772417746473985</v>
+      </c>
+      <c r="E4">
+        <v>0.99772417746469655</v>
+      </c>
+      <c r="F4">
+        <v>0.98946475655091437</v>
+      </c>
+      <c r="G4">
+        <v>0.98384389955615403</v>
+      </c>
+      <c r="H4">
+        <v>0.98388691369682391</v>
+      </c>
+      <c r="I4">
+        <v>0.98045633684843492</v>
+      </c>
+      <c r="J4">
+        <v>0.98384389959535268</v>
+      </c>
+      <c r="K4">
+        <v>0.98388691369682346</v>
+      </c>
+      <c r="L4">
+        <v>0.99422149404419036</v>
+      </c>
+      <c r="M4">
+        <v>0.98334630994723393</v>
+      </c>
+      <c r="N4">
+        <v>0.98762504070267321</v>
+      </c>
+      <c r="O4">
+        <v>0.98786684869299235</v>
+      </c>
+      <c r="P4">
+        <v>0.96551294640069996</v>
+      </c>
+      <c r="Q4">
+        <v>0.85094165473951278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0638297871620572</v>
+      </c>
+      <c r="D5">
+        <v>1.0684569174936085</v>
+      </c>
+      <c r="E5">
+        <v>1.0660252991930357</v>
+      </c>
+      <c r="F5">
+        <v>1.1480730086871633</v>
+      </c>
+      <c r="G5">
+        <v>1.143932026014441</v>
+      </c>
+      <c r="H5">
+        <v>1.145388031746748</v>
+      </c>
+      <c r="I5">
+        <v>1.1430546388918983</v>
+      </c>
+      <c r="J5">
+        <v>1.1439320266250896</v>
+      </c>
+      <c r="K5">
+        <v>1.1453880317467473</v>
+      </c>
+      <c r="L5">
+        <v>1.1552359586956371</v>
+      </c>
+      <c r="M5">
+        <v>1.1581490156249072</v>
+      </c>
+      <c r="N5">
+        <v>1.155598046894343</v>
+      </c>
+      <c r="O5">
+        <v>1.1575889833220461</v>
+      </c>
+      <c r="P5">
+        <v>1.2537168559460676</v>
+      </c>
+      <c r="Q5">
+        <v>1.5055868680147453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.93617021283726842</v>
+      </c>
+      <c r="D6">
+        <v>0.94020377794879728</v>
+      </c>
+      <c r="E6">
+        <v>0.93806404102884222</v>
+      </c>
+      <c r="F6">
+        <v>0.87102474531723251</v>
+      </c>
+      <c r="G6">
+        <v>0.87417781586558641</v>
+      </c>
+      <c r="H6">
+        <v>0.87306656982859454</v>
+      </c>
+      <c r="I6">
+        <v>0.87484881821820093</v>
+      </c>
+      <c r="J6">
+        <v>0.87417781537648442</v>
+      </c>
+      <c r="K6">
+        <v>0.8730665698285951</v>
+      </c>
+      <c r="L6">
+        <v>0.85595981739436022</v>
+      </c>
+      <c r="M6">
+        <v>0.85345573386848617</v>
+      </c>
+      <c r="N6">
+        <v>0.85564819249958657</v>
+      </c>
+      <c r="O6">
+        <v>0.85393661198955706</v>
+      </c>
+      <c r="P6">
+        <v>0.7749369221744975</v>
+      </c>
+      <c r="Q6">
+        <v>0.59749254452861233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.0022810136897868</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.9787234044661598</v>
+      </c>
+      <c r="D8">
+        <v>0.98313214830210061</v>
+      </c>
+      <c r="E8">
+        <v>0.98089471402976547</v>
+      </c>
+      <c r="F8">
+        <v>0.96237274603924516</v>
+      </c>
+      <c r="G8">
+        <v>0.99079613084182516</v>
+      </c>
+      <c r="H8">
+        <v>0.98833168062153587</v>
+      </c>
+      <c r="I8">
+        <v>1.0035788978164959</v>
+      </c>
+      <c r="J8">
+        <v>0.99079612939730155</v>
+      </c>
+      <c r="K8">
+        <v>0.98833168062153542</v>
+      </c>
+      <c r="L8">
+        <v>0.92664016312691877</v>
+      </c>
+      <c r="M8">
+        <v>0.95693303095438265</v>
+      </c>
+      <c r="N8">
+        <v>0.94793633761497709</v>
+      </c>
+      <c r="O8">
+        <v>0.94504731852562995</v>
+      </c>
+      <c r="P8">
+        <v>0.92927845149325294</v>
+      </c>
+      <c r="Q8">
+        <v>0.93690421845409078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.93617021255885335</v>
+      </c>
+      <c r="D9">
+        <v>0.94050545000475572</v>
+      </c>
+      <c r="E9">
+        <v>0.93836502653465148</v>
+      </c>
+      <c r="F9">
+        <v>0.87502750843624399</v>
+      </c>
+      <c r="G9">
+        <v>0.85572088168510851</v>
+      </c>
+      <c r="H9">
+        <v>0.8578333330738287</v>
+      </c>
+      <c r="I9">
+        <v>0.84752137041884756</v>
+      </c>
+      <c r="J9">
+        <v>0.8557208828592785</v>
+      </c>
+      <c r="K9">
+        <v>0.85783333307382881</v>
+      </c>
+      <c r="L9">
+        <v>0.90004342852983255</v>
+      </c>
+      <c r="M9">
+        <v>0.88509599493431801</v>
+      </c>
+      <c r="N9">
+        <v>0.88903972814453491</v>
+      </c>
+      <c r="O9">
+        <v>0.89108439606482159</v>
+      </c>
+      <c r="P9">
+        <v>0.84027401686099978</v>
+      </c>
+      <c r="Q9">
+        <v>0.76497909102369444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>199.99999999979775</v>
+      </c>
+      <c r="D10">
+        <v>199.99999999979775</v>
+      </c>
+      <c r="E10">
+        <v>199.54483549293934</v>
+      </c>
+      <c r="F10">
+        <v>197.89295130594959</v>
+      </c>
+      <c r="G10">
+        <v>196.76877991123038</v>
+      </c>
+      <c r="H10">
+        <v>196.77738273926926</v>
+      </c>
+      <c r="I10">
+        <v>196.09126736158467</v>
+      </c>
+      <c r="J10">
+        <v>196.76877988306461</v>
+      </c>
+      <c r="K10">
+        <v>196.77738273926923</v>
+      </c>
+      <c r="L10">
+        <v>198.84429879258502</v>
+      </c>
+      <c r="M10">
+        <v>196.66926198933004</v>
+      </c>
+      <c r="N10">
+        <v>197.52500814053451</v>
+      </c>
+      <c r="O10">
+        <v>197.57336970586019</v>
+      </c>
+      <c r="P10">
+        <v>193.10258927643696</v>
+      </c>
+      <c r="Q10">
+        <v>170.18833094777852</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>80</v>
+      </c>
+      <c r="F11">
+        <v>80</v>
+      </c>
+      <c r="G11">
+        <v>82.069466121608045</v>
+      </c>
+      <c r="H11">
+        <v>80.747628722199408</v>
+      </c>
+      <c r="I11">
+        <v>81.354566612697411</v>
+      </c>
+      <c r="J11">
+        <v>82.069466167985382</v>
+      </c>
+      <c r="K11">
+        <v>80.747628722199366</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+      <c r="M11">
+        <v>82.417927311586453</v>
+      </c>
+      <c r="N11">
+        <v>83.35049623579954</v>
+      </c>
+      <c r="O11">
+        <v>81.225339410207141</v>
+      </c>
+      <c r="P11">
+        <v>83.433232535582817</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>17.883410386329814</v>
+      </c>
+      <c r="H12">
+        <v>19.234217268593486</v>
+      </c>
+      <c r="I12">
+        <v>18.615470122805476</v>
+      </c>
+      <c r="J12">
+        <v>17.883410337779104</v>
+      </c>
+      <c r="K12">
+        <v>19.2342172685935</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>17.482954987675999</v>
+      </c>
+      <c r="N12">
+        <v>16.521274681467307</v>
+      </c>
+      <c r="O12">
+        <v>18.72461106202643</v>
+      </c>
+      <c r="P12">
+        <v>16.115952567746049</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>24.485376219145216</v>
+      </c>
+      <c r="H13">
+        <v>24.528999781244689</v>
+      </c>
+      <c r="I13">
+        <v>26.905664219245825</v>
+      </c>
+      <c r="J13">
+        <v>24.485376237890613</v>
+      </c>
+      <c r="K13">
+        <v>24.528999781244671</v>
+      </c>
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <v>27.936209019788301</v>
+      </c>
+      <c r="N13">
+        <v>25.027423604599701</v>
+      </c>
+      <c r="O13">
+        <v>25.091438252400668</v>
+      </c>
+      <c r="P13">
+        <v>28.125819289701205</v>
+      </c>
+      <c r="Q13">
+        <v>35.02889636959808</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>80</v>
+      </c>
+      <c r="E14">
+        <v>80</v>
+      </c>
+      <c r="F14">
+        <v>80</v>
+      </c>
+      <c r="G14">
+        <v>74.845610463324249</v>
+      </c>
+      <c r="H14">
+        <v>74.788452844852941</v>
+      </c>
+      <c r="I14">
+        <v>72.061407044880269</v>
+      </c>
+      <c r="J14">
+        <v>74.845610438794367</v>
+      </c>
+      <c r="K14">
+        <v>74.788452844852955</v>
+      </c>
+      <c r="L14">
+        <v>80</v>
+      </c>
+      <c r="M14">
+        <v>70.68907519906378</v>
+      </c>
+      <c r="N14">
+        <v>74.124977375131124</v>
+      </c>
+      <c r="O14">
+        <v>74.038361041448354</v>
+      </c>
+      <c r="P14">
+        <v>69.5395797882924</v>
+      </c>
+      <c r="Q14">
+        <v>55.604906946346318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>38.950195569881757</v>
+      </c>
+      <c r="E15">
+        <v>38.950195569950637</v>
+      </c>
+      <c r="F15">
+        <v>37.780441241921935</v>
+      </c>
+      <c r="G15">
+        <v>36.6326796525479</v>
+      </c>
+      <c r="H15">
+        <v>36.74177319144264</v>
+      </c>
+      <c r="I15">
+        <v>36.142606841209023</v>
+      </c>
+      <c r="J15">
+        <v>36.63267971475203</v>
+      </c>
+      <c r="K15">
+        <v>36.741773191442654</v>
+      </c>
+      <c r="L15">
+        <v>38.962246098925824</v>
+      </c>
+      <c r="M15">
+        <v>37.266665983254953</v>
+      </c>
+      <c r="N15">
+        <v>37.742208702045104</v>
+      </c>
+      <c r="O15">
+        <v>37.926598689166809</v>
+      </c>
+      <c r="P15">
+        <v>36.501668499162456</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>61.073313472895634</v>
+      </c>
+      <c r="E16">
+        <v>61.073313472823642</v>
+      </c>
+      <c r="F16">
+        <v>62.327526793196704</v>
+      </c>
+      <c r="G16">
+        <v>63.622703452038728</v>
+      </c>
+      <c r="H16">
+        <v>63.496702180821892</v>
+      </c>
+      <c r="I16">
+        <v>64.196536165199802</v>
+      </c>
+      <c r="J16">
+        <v>63.622703380015693</v>
+      </c>
+      <c r="K16">
+        <v>63.496702180821885</v>
+      </c>
+      <c r="L16">
+        <v>61.052960199979267</v>
+      </c>
+      <c r="M16">
+        <v>62.841791142654223</v>
+      </c>
+      <c r="N16">
+        <v>62.331212543599925</v>
+      </c>
+      <c r="O16">
+        <v>62.135132465669322</v>
+      </c>
+      <c r="P16">
+        <v>63.678287301078122</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>58.945549132481268</v>
+      </c>
+      <c r="E17">
+        <v>58.945549132550752</v>
+      </c>
+      <c r="F17">
+        <v>57.759391158658246</v>
+      </c>
+      <c r="G17">
+        <v>56.583574803824867</v>
+      </c>
+      <c r="H17">
+        <v>56.695857837595206</v>
+      </c>
+      <c r="I17">
+        <v>56.077791965846245</v>
+      </c>
+      <c r="J17">
+        <v>56.583574867879364</v>
+      </c>
+      <c r="K17">
+        <v>56.695857837595227</v>
+      </c>
+      <c r="L17">
+        <v>58.606334436129941</v>
+      </c>
+      <c r="M17">
+        <v>56.286003007094564</v>
+      </c>
+      <c r="N17">
+        <v>56.942195509126336</v>
+      </c>
+      <c r="O17">
+        <v>57.195490828323436</v>
+      </c>
+      <c r="P17">
+        <v>55.221484067444962</v>
+      </c>
+      <c r="Q17">
+        <v>50.510257216772381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>40</v>
+      </c>
+      <c r="D18">
+        <v>41.078099264723591</v>
+      </c>
+      <c r="E18">
+        <v>41.078099264650952</v>
+      </c>
+      <c r="F18">
+        <v>42.349955357975226</v>
+      </c>
+      <c r="G18">
+        <v>43.676848518197758</v>
+      </c>
+      <c r="H18">
+        <v>43.547163378947886</v>
+      </c>
+      <c r="I18">
+        <v>44.2690812820871</v>
+      </c>
+      <c r="J18">
+        <v>43.676848444032274</v>
+      </c>
+      <c r="K18">
+        <v>43.547163378947864</v>
+      </c>
+      <c r="L18">
+        <v>41.414136337644095</v>
+      </c>
+      <c r="M18">
+        <v>43.862309050474138</v>
+      </c>
+      <c r="N18">
+        <v>43.15776591871434</v>
+      </c>
+      <c r="O18">
+        <v>42.888411696208443</v>
+      </c>
+      <c r="P18">
+        <v>45.026343428197329</v>
+      </c>
+      <c r="Q18">
+        <v>50.510257216882515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+      <c r="D19">
+        <v>200</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+      <c r="F19">
+        <v>200</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+      <c r="H19">
+        <v>200</v>
+      </c>
+      <c r="I19">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>200</v>
+      </c>
+      <c r="K19">
+        <v>200</v>
+      </c>
+      <c r="L19">
+        <v>200</v>
+      </c>
+      <c r="M19">
+        <v>200</v>
+      </c>
+      <c r="N19">
+        <v>200</v>
+      </c>
+      <c r="O19">
+        <v>200</v>
+      </c>
+      <c r="P19">
+        <v>200</v>
+      </c>
+      <c r="Q19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>93.806404102931722</v>
+      </c>
+      <c r="E20">
+        <v>93.806404102884244</v>
+      </c>
+      <c r="F20">
+        <v>87.102474531839732</v>
+      </c>
+      <c r="G20">
+        <v>87.417781586558661</v>
+      </c>
+      <c r="H20">
+        <v>87.306656982865633</v>
+      </c>
+      <c r="I20">
+        <v>87.484881822108363</v>
+      </c>
+      <c r="J20">
+        <v>87.417781538771095</v>
+      </c>
+      <c r="K20">
+        <v>87.306656982865675</v>
+      </c>
+      <c r="L20">
+        <v>93.038917913952417</v>
+      </c>
+      <c r="M20">
+        <v>92.92183526645816</v>
+      </c>
+      <c r="N20">
+        <v>93.024340642293922</v>
+      </c>
+      <c r="O20">
+        <v>92.944309968961193</v>
+      </c>
+      <c r="P20">
+        <v>89.310036642749864</v>
+      </c>
+      <c r="Q20">
+        <v>81.498026247360883</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>106.60252991924966</v>
+      </c>
+      <c r="E21">
+        <v>106.60252991930359</v>
+      </c>
+      <c r="F21">
+        <v>114.80730086886987</v>
+      </c>
+      <c r="G21">
+        <v>114.39320260144412</v>
+      </c>
+      <c r="H21">
+        <v>114.5388031746829</v>
+      </c>
+      <c r="I21">
+        <v>114.30546388956648</v>
+      </c>
+      <c r="J21">
+        <v>114.39320266397803</v>
+      </c>
+      <c r="K21">
+        <v>114.53880317468281</v>
+      </c>
+      <c r="L21">
+        <v>108.08696224654723</v>
+      </c>
+      <c r="M21">
+        <v>108.24541249180129</v>
+      </c>
+      <c r="N21">
+        <v>108.10664295323195</v>
+      </c>
+      <c r="O21">
+        <v>108.21493002930822</v>
+      </c>
+      <c r="P21">
+        <v>113.59698981509563</v>
+      </c>
+      <c r="Q21">
+        <v>129.37005259843761</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>199.99999999979775</v>
+      </c>
+      <c r="D22">
+        <v>199.5448354929313</v>
+      </c>
+      <c r="E22">
+        <v>199.54483549293934</v>
+      </c>
+      <c r="F22">
+        <v>197.89295130594959</v>
+      </c>
+      <c r="G22">
+        <v>196.76877991123038</v>
+      </c>
+      <c r="H22">
+        <v>196.77738273926926</v>
+      </c>
+      <c r="I22">
+        <v>196.09126736158467</v>
+      </c>
+      <c r="J22">
+        <v>196.76877988306461</v>
+      </c>
+      <c r="K22">
+        <v>196.77738273926923</v>
+      </c>
+      <c r="L22">
+        <v>198.84429879258502</v>
+      </c>
+      <c r="M22">
+        <v>196.66926198933004</v>
+      </c>
+      <c r="N22">
+        <v>197.52500814053451</v>
+      </c>
+      <c r="O22">
+        <v>197.57336970586019</v>
+      </c>
+      <c r="P22">
+        <v>193.10258927643696</v>
+      </c>
+      <c r="Q22">
+        <v>170.18833094777852</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.99999999999898881</v>
+      </c>
+      <c r="D23">
+        <v>0.99772417746465647</v>
+      </c>
+      <c r="E23">
+        <v>0.99772417746469666</v>
+      </c>
+      <c r="F23">
+        <v>0.98946475652974797</v>
+      </c>
+      <c r="G23">
+        <v>0.98384389955615192</v>
+      </c>
+      <c r="H23">
+        <v>0.98388691369634629</v>
+      </c>
+      <c r="I23">
+        <v>0.98045633680792332</v>
+      </c>
+      <c r="J23">
+        <v>0.98384389941532302</v>
+      </c>
+      <c r="K23">
+        <v>0.98388691369634618</v>
+      </c>
+      <c r="L23">
+        <v>0.99422149396292514</v>
+      </c>
+      <c r="M23">
+        <v>0.98334630994665018</v>
+      </c>
+      <c r="N23">
+        <v>0.98762504070267254</v>
+      </c>
+      <c r="O23">
+        <v>0.98786684852930096</v>
+      </c>
+      <c r="P23">
+        <v>0.96551294638218477</v>
+      </c>
+      <c r="Q23">
+        <v>0.85094165473889261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update tests for Outtax non-0 tr_elas
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EC14CB-8026-4392-8FDC-CB6AF227E69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797361AB-1A26-4CF4-BE77-8106D1BA2B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3864" yWindow="3072" windowWidth="13824" windowHeight="7260" firstSheet="7" activeTab="8" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
@@ -389,7 +389,7 @@
     <t>OUTTAX=0.2</t>
   </si>
   <si>
-    <t>S1Tr=3,1</t>
+    <t>S1Tr2,1.5</t>
   </si>
 </sst>
 </file>
@@ -5967,10 +5967,10 @@
         <v>96</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>99</v>
@@ -6023,25 +6023,25 @@
         <v>0.59043552853534853</v>
       </c>
       <c r="J2">
-        <v>0.64533631351198184</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="K2">
-        <v>0.65743472294980621</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="L2">
-        <v>0.87514262265812059</v>
+        <v>0.87514262258757747</v>
       </c>
       <c r="M2">
-        <v>0.65301554051929644</v>
+        <v>0.65301554051929678</v>
       </c>
       <c r="N2">
-        <v>0.71778700395030315</v>
+        <v>0.71778700395030381</v>
       </c>
       <c r="O2">
-        <v>0.74236189253677176</v>
+        <v>0.7423618925367752</v>
       </c>
       <c r="P2">
-        <v>0.54435839325680246</v>
+        <v>0.54435839325680269</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -6073,28 +6073,28 @@
         <v>1.4026964717016865</v>
       </c>
       <c r="J3">
-        <v>1.3495011908864791</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="K3">
-        <v>1.3377464494522311</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="L3">
-        <v>1.1244941079798842</v>
+        <v>1.1244941080643807</v>
       </c>
       <c r="M3">
-        <v>1.3442824845818007</v>
+        <v>1.3442824845817996</v>
       </c>
       <c r="N3">
-        <v>1.2804060756948956</v>
+        <v>1.2804060756948938</v>
       </c>
       <c r="O3">
-        <v>1.2561259176857724</v>
+        <v>1.2561259176857693</v>
       </c>
       <c r="P3">
-        <v>1.4510658620714896</v>
+        <v>1.4510658620714891</v>
       </c>
       <c r="Q3">
-        <v>1.9797958971136496</v>
+        <v>1.9797958971136493</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -6126,25 +6126,25 @@
         <v>0.98045633684843492</v>
       </c>
       <c r="J4">
-        <v>0.98384389959535268</v>
+        <v>0.99836641864624298</v>
       </c>
       <c r="K4">
-        <v>0.98388691369682346</v>
+        <v>0.99893794959861781</v>
       </c>
       <c r="L4">
-        <v>0.99422149404419036</v>
+        <v>0.99422149404252358</v>
       </c>
       <c r="M4">
-        <v>0.98334630994723393</v>
+        <v>0.98334630994723327</v>
       </c>
       <c r="N4">
-        <v>0.98762504070267321</v>
+        <v>0.98762504070267221</v>
       </c>
       <c r="O4">
-        <v>0.98786684869299235</v>
+        <v>0.98786684869299268</v>
       </c>
       <c r="P4">
-        <v>0.96551294640069996</v>
+        <v>0.96551294640069951</v>
       </c>
       <c r="Q4">
         <v>0.85094165473951278</v>
@@ -6179,28 +6179,28 @@
         <v>1.1430546388918983</v>
       </c>
       <c r="J5">
-        <v>1.1439320266250896</v>
+        <v>1.0831733772497101</v>
       </c>
       <c r="K5">
-        <v>1.1453880317467473</v>
+        <v>1.0557280901465067</v>
       </c>
       <c r="L5">
-        <v>1.1552359586956371</v>
+        <v>1.1552359587842187</v>
       </c>
       <c r="M5">
         <v>1.1581490156249072</v>
       </c>
       <c r="N5">
-        <v>1.155598046894343</v>
+        <v>1.1555980468943421</v>
       </c>
       <c r="O5">
-        <v>1.1575889833220461</v>
+        <v>1.1575889833220443</v>
       </c>
       <c r="P5">
-        <v>1.2537168559460676</v>
+        <v>1.2537168559460672</v>
       </c>
       <c r="Q5">
-        <v>1.5055868680147453</v>
+        <v>1.5055868680147451</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -6232,28 +6232,28 @@
         <v>0.87484881821820093</v>
       </c>
       <c r="J6">
-        <v>0.87417781537648442</v>
+        <v>0.91682662275028926</v>
       </c>
       <c r="K6">
-        <v>0.8730665698285951</v>
+        <v>0.9442719098534933</v>
       </c>
       <c r="L6">
-        <v>0.85595981739436022</v>
+        <v>0.85595981732131754</v>
       </c>
       <c r="M6">
         <v>0.85345573386848617</v>
       </c>
       <c r="N6">
-        <v>0.85564819249958657</v>
+        <v>0.85564819249958746</v>
       </c>
       <c r="O6">
-        <v>0.85393661198955706</v>
+        <v>0.85393661198955839</v>
       </c>
       <c r="P6">
-        <v>0.7749369221744975</v>
+        <v>0.77493692217449794</v>
       </c>
       <c r="Q6">
-        <v>0.59749254452861233</v>
+        <v>0.59749254452861256</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -6338,28 +6338,28 @@
         <v>1.0035788978164959</v>
       </c>
       <c r="J8">
-        <v>0.99079612939730155</v>
+        <v>1.1026615242409006</v>
       </c>
       <c r="K8">
-        <v>0.98833168062153542</v>
+        <v>1.1718933282765274</v>
       </c>
       <c r="L8">
-        <v>0.92664016312691877</v>
+        <v>0.92664016290016515</v>
       </c>
       <c r="M8">
         <v>0.95693303095438265</v>
       </c>
       <c r="N8">
-        <v>0.94793633761497709</v>
+        <v>0.94793633761497686</v>
       </c>
       <c r="O8">
-        <v>0.94504731852562995</v>
+        <v>0.94504731852562951</v>
       </c>
       <c r="P8">
         <v>0.92927845149325294</v>
       </c>
       <c r="Q8">
-        <v>0.93690421845409078</v>
+        <v>0.93690421845409066</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -6391,25 +6391,25 @@
         <v>0.84752137041884756</v>
       </c>
       <c r="J9">
-        <v>0.8557208828592785</v>
+        <v>0.72706545913678722</v>
       </c>
       <c r="K9">
-        <v>0.85783333307382881</v>
+        <v>0.661136947939996</v>
       </c>
       <c r="L9">
-        <v>0.90004342852983255</v>
+        <v>0.90004342873448051</v>
       </c>
       <c r="M9">
-        <v>0.88509599493431801</v>
+        <v>0.88509599493431845</v>
       </c>
       <c r="N9">
-        <v>0.88903972814453491</v>
+        <v>0.88903972814453536</v>
       </c>
       <c r="O9">
-        <v>0.89108439606482159</v>
+        <v>0.89108439606482148</v>
       </c>
       <c r="P9">
-        <v>0.84027401686099978</v>
+        <v>0.84027401686099956</v>
       </c>
       <c r="Q9">
         <v>0.76497909102369444</v>
@@ -6444,25 +6444,25 @@
         <v>196.09126736158467</v>
       </c>
       <c r="J10">
-        <v>196.76877988306461</v>
+        <v>199.67328372924806</v>
       </c>
       <c r="K10">
-        <v>196.77738273926923</v>
+        <v>199.787589545804</v>
       </c>
       <c r="L10">
-        <v>198.84429879258502</v>
+        <v>198.84429879031092</v>
       </c>
       <c r="M10">
-        <v>196.66926198933004</v>
+        <v>196.6692619893301</v>
       </c>
       <c r="N10">
         <v>197.52500814053451</v>
       </c>
       <c r="O10">
-        <v>197.57336970586019</v>
+        <v>197.57336970586016</v>
       </c>
       <c r="P10">
-        <v>193.10258927643696</v>
+        <v>193.10258927643693</v>
       </c>
       <c r="Q10">
         <v>170.18833094777852</v>
@@ -6497,10 +6497,10 @@
         <v>81.354566612697411</v>
       </c>
       <c r="J11">
-        <v>82.069466167985382</v>
+        <v>77.091007507421452</v>
       </c>
       <c r="K11">
-        <v>80.747628722199366</v>
+        <v>78.072005841314947</v>
       </c>
       <c r="L11">
         <v>80</v>
@@ -6509,10 +6509,10 @@
         <v>82.417927311586453</v>
       </c>
       <c r="N11">
-        <v>83.35049623579954</v>
+        <v>83.350496235799483</v>
       </c>
       <c r="O11">
-        <v>81.225339410207141</v>
+        <v>81.225339410207084</v>
       </c>
       <c r="P11">
         <v>83.433232535582817</v>
@@ -6550,10 +6550,10 @@
         <v>18.615470122805476</v>
       </c>
       <c r="J12">
-        <v>17.883410337779104</v>
+        <v>22.826613486796894</v>
       </c>
       <c r="K12">
-        <v>19.2342172685935</v>
+        <v>21.821789018740443</v>
       </c>
       <c r="L12">
         <v>20</v>
@@ -6562,13 +6562,13 @@
         <v>17.482954987675999</v>
       </c>
       <c r="N12">
-        <v>16.521274681467307</v>
+        <v>16.521274681467379</v>
       </c>
       <c r="O12">
-        <v>18.72461106202643</v>
+        <v>18.724611062026483</v>
       </c>
       <c r="P12">
-        <v>16.115952567746049</v>
+        <v>16.11595256774606</v>
       </c>
       <c r="Q12" t="s">
         <v>106</v>
@@ -6603,10 +6603,10 @@
         <v>26.905664219245825</v>
       </c>
       <c r="J13">
-        <v>24.485376237890613</v>
+        <v>22.745634357202448</v>
       </c>
       <c r="K13">
-        <v>24.528999781244671</v>
+        <v>21.821789028458028</v>
       </c>
       <c r="L13">
         <v>20</v>
@@ -6615,16 +6615,16 @@
         <v>27.936209019788301</v>
       </c>
       <c r="N13">
-        <v>25.027423604599701</v>
+        <v>25.027423604599669</v>
       </c>
       <c r="O13">
-        <v>25.091438252400668</v>
+        <v>25.091438252400611</v>
       </c>
       <c r="P13">
-        <v>28.125819289701205</v>
+        <v>28.125819289701191</v>
       </c>
       <c r="Q13">
-        <v>35.02889636959808</v>
+        <v>35.028896369598066</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -6656,10 +6656,10 @@
         <v>72.061407044880269</v>
       </c>
       <c r="J14">
-        <v>74.845610438794367</v>
+        <v>77.010028377827553</v>
       </c>
       <c r="K14">
-        <v>74.788452844852955</v>
+        <v>78.072005830450337</v>
       </c>
       <c r="L14">
         <v>80</v>
@@ -6668,16 +6668,16 @@
         <v>70.68907519906378</v>
       </c>
       <c r="N14">
-        <v>74.124977375131124</v>
+        <v>74.124977375131166</v>
       </c>
       <c r="O14">
-        <v>74.038361041448354</v>
+        <v>74.038361041448425</v>
       </c>
       <c r="P14">
-        <v>69.5395797882924</v>
+        <v>69.539579788292428</v>
       </c>
       <c r="Q14">
-        <v>55.604906946346318</v>
+        <v>55.60490694634634</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -6709,19 +6709,19 @@
         <v>36.142606841209023</v>
       </c>
       <c r="J15">
-        <v>36.63267971475203</v>
+        <v>40</v>
       </c>
       <c r="K15">
-        <v>36.741773191442654</v>
+        <v>40</v>
       </c>
       <c r="L15">
-        <v>38.962246098925824</v>
+        <v>38.962246115576093</v>
       </c>
       <c r="M15">
         <v>37.266665983254953</v>
       </c>
       <c r="N15">
-        <v>37.742208702045104</v>
+        <v>37.742208702045119</v>
       </c>
       <c r="O15">
         <v>37.926598689166809</v>
@@ -6762,25 +6762,25 @@
         <v>64.196536165199802</v>
       </c>
       <c r="J16">
-        <v>63.622703380015693</v>
+        <v>60</v>
       </c>
       <c r="K16">
-        <v>63.496702180821885</v>
+        <v>60</v>
       </c>
       <c r="L16">
-        <v>61.052960199979267</v>
+        <v>61.052960182836976</v>
       </c>
       <c r="M16">
-        <v>62.841791142654223</v>
+        <v>62.841791142654181</v>
       </c>
       <c r="N16">
-        <v>62.331212543599925</v>
+        <v>62.331212543599889</v>
       </c>
       <c r="O16">
-        <v>62.135132465669322</v>
+        <v>62.135132465669287</v>
       </c>
       <c r="P16">
-        <v>63.678287301078122</v>
+        <v>63.678287301078129</v>
       </c>
       <c r="Q16" t="s">
         <v>106</v>
@@ -6815,28 +6815,28 @@
         <v>56.077791965846245</v>
       </c>
       <c r="J17">
-        <v>56.583574867879364</v>
+        <v>60</v>
       </c>
       <c r="K17">
-        <v>56.695857837595227</v>
+        <v>60</v>
       </c>
       <c r="L17">
-        <v>58.606334436129941</v>
+        <v>58.606334458651354</v>
       </c>
       <c r="M17">
-        <v>56.286003007094564</v>
+        <v>56.286003007094578</v>
       </c>
       <c r="N17">
-        <v>56.942195509126336</v>
+        <v>56.942195509126392</v>
       </c>
       <c r="O17">
-        <v>57.195490828323436</v>
+        <v>57.195490828323443</v>
       </c>
       <c r="P17">
-        <v>55.221484067444962</v>
+        <v>55.221484067444941</v>
       </c>
       <c r="Q17">
-        <v>50.510257216772381</v>
+        <v>50.510257216772395</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -6868,22 +6868,22 @@
         <v>44.2690812820871</v>
       </c>
       <c r="J18">
-        <v>43.676848444032274</v>
+        <v>40</v>
       </c>
       <c r="K18">
-        <v>43.547163378947864</v>
+        <v>40</v>
       </c>
       <c r="L18">
-        <v>41.414136337644095</v>
+        <v>41.41413631445721</v>
       </c>
       <c r="M18">
-        <v>43.862309050474138</v>
+        <v>43.86230905047411</v>
       </c>
       <c r="N18">
-        <v>43.15776591871434</v>
+        <v>43.157765918714325</v>
       </c>
       <c r="O18">
-        <v>42.888411696208443</v>
+        <v>42.888411696208422</v>
       </c>
       <c r="P18">
         <v>45.026343428197329</v>
@@ -6974,25 +6974,25 @@
         <v>87.484881822108363</v>
       </c>
       <c r="J20">
-        <v>87.417781538771095</v>
+        <v>100</v>
       </c>
       <c r="K20">
-        <v>87.306656982865675</v>
+        <v>100</v>
       </c>
       <c r="L20">
-        <v>93.038917913952417</v>
+        <v>93.038917910466012</v>
       </c>
       <c r="M20">
         <v>92.92183526645816</v>
       </c>
       <c r="N20">
-        <v>93.024340642293922</v>
+        <v>93.02434064229395</v>
       </c>
       <c r="O20">
-        <v>92.944309968961193</v>
+        <v>92.944309968961264</v>
       </c>
       <c r="P20">
-        <v>89.310036642749864</v>
+        <v>89.310036642749893</v>
       </c>
       <c r="Q20">
         <v>81.498026247360883</v>
@@ -7027,28 +7027,28 @@
         <v>114.30546388956648</v>
       </c>
       <c r="J21">
-        <v>114.39320266397803</v>
+        <v>100</v>
       </c>
       <c r="K21">
-        <v>114.53880317468281</v>
+        <v>100</v>
       </c>
       <c r="L21">
-        <v>108.08696224654723</v>
+        <v>108.08696225125264</v>
       </c>
       <c r="M21">
         <v>108.24541249180129</v>
       </c>
       <c r="N21">
-        <v>108.10664295323195</v>
+        <v>108.10664295323191</v>
       </c>
       <c r="O21">
-        <v>108.21493002930822</v>
+        <v>108.21493002930814</v>
       </c>
       <c r="P21">
-        <v>113.59698981509563</v>
+        <v>113.59698981509561</v>
       </c>
       <c r="Q21">
-        <v>129.37005259843761</v>
+        <v>129.37005259843758</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -7080,25 +7080,25 @@
         <v>196.09126736158467</v>
       </c>
       <c r="J22">
-        <v>196.76877988306461</v>
+        <v>199.67328372924806</v>
       </c>
       <c r="K22">
-        <v>196.77738273926923</v>
+        <v>199.787589545804</v>
       </c>
       <c r="L22">
-        <v>198.84429879258502</v>
+        <v>198.84429879031092</v>
       </c>
       <c r="M22">
-        <v>196.66926198933004</v>
+        <v>196.6692619893301</v>
       </c>
       <c r="N22">
         <v>197.52500814053451</v>
       </c>
       <c r="O22">
-        <v>197.57336970586019</v>
+        <v>197.57336970586016</v>
       </c>
       <c r="P22">
-        <v>193.10258927643696</v>
+        <v>193.10258927643693</v>
       </c>
       <c r="Q22">
         <v>170.18833094777852</v>
@@ -7133,25 +7133,25 @@
         <v>0.98045633680792332</v>
       </c>
       <c r="J23">
-        <v>0.98384389941532302</v>
+        <v>0.99836641864624032</v>
       </c>
       <c r="K23">
-        <v>0.98388691369634618</v>
+        <v>0.99893794772902</v>
       </c>
       <c r="L23">
-        <v>0.99422149396292514</v>
+        <v>0.99422149395155457</v>
       </c>
       <c r="M23">
-        <v>0.98334630994665018</v>
+        <v>0.98334630994665051</v>
       </c>
       <c r="N23">
         <v>0.98762504070267254</v>
       </c>
       <c r="O23">
-        <v>0.98786684852930096</v>
+        <v>0.98786684852930084</v>
       </c>
       <c r="P23">
-        <v>0.96551294638218477</v>
+        <v>0.96551294638218466</v>
       </c>
       <c r="Q23">
         <v>0.85094165473889261</v>

</xml_diff>

<commit_message>
add more Outtax tests
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797361AB-1A26-4CF4-BE77-8106D1BA2B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71F2693-8C2D-4398-BDDC-468A70B5AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3864" yWindow="3072" windowWidth="13824" windowHeight="7260" firstSheet="7" activeTab="8" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="123">
   <si>
     <t>X.L</t>
   </si>
@@ -390,6 +390,18 @@
   </si>
   <si>
     <t>S1Tr2,1.5</t>
+  </si>
+  <si>
+    <t>S...T1</t>
+  </si>
+  <si>
+    <t>S.T1,O2=.1</t>
+  </si>
+  <si>
+    <t>S.T1,O3=.1</t>
+  </si>
+  <si>
+    <t>S.T1,O4=.1</t>
   </si>
 </sst>
 </file>
@@ -5938,13 +5950,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F07C38F-0BBA-4014-8D0C-146F422C055E}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -5985,16 +5997,25 @@
         <v>102</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -6041,10 +6062,19 @@
         <v>0.7423618925367752</v>
       </c>
       <c r="P2">
-        <v>0.54435839325680269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.69377214014432131</v>
+      </c>
+      <c r="Q2">
+        <v>0.83618649566317793</v>
+      </c>
+      <c r="R2">
+        <v>0.85040405052448198</v>
+      </c>
+      <c r="S2">
+        <v>0.63672356266481245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -6091,13 +6121,22 @@
         <v>1.2561259176857693</v>
       </c>
       <c r="P3">
-        <v>1.4510658620714891</v>
+        <v>1.3041089181496648</v>
       </c>
       <c r="Q3">
-        <v>1.9797958971136493</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1.1631923403568185</v>
+      </c>
+      <c r="R3">
+        <v>1.1490766698982966</v>
+      </c>
+      <c r="S3">
+        <v>1.3603228285174447</v>
+      </c>
+      <c r="T3">
+        <v>1.9797958971155629</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -6144,13 +6183,22 @@
         <v>0.98786684869299268</v>
       </c>
       <c r="P4">
-        <v>0.96551294640069951</v>
+        <v>0.98418612250917614</v>
       </c>
       <c r="Q4">
-        <v>0.85094165473951278</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.99442372344833319</v>
+      </c>
+      <c r="R4">
+        <v>0.99396861965710737</v>
+      </c>
+      <c r="S4">
+        <v>0.97648968838754668</v>
+      </c>
+      <c r="T4">
+        <v>0.85056947165921182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -6197,13 +6245,22 @@
         <v>1.1575889833220443</v>
       </c>
       <c r="P5">
-        <v>1.2537168559460672</v>
+        <v>1.1725176580766463</v>
       </c>
       <c r="Q5">
-        <v>1.5055868680147451</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1.1319256299272371</v>
+      </c>
+      <c r="R5">
+        <v>1.0849624848283628</v>
+      </c>
+      <c r="S5">
+        <v>1.1824559830178498</v>
+      </c>
+      <c r="T5">
+        <v>1.4648348042647581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -6250,13 +6307,22 @@
         <v>0.85393661198955839</v>
       </c>
       <c r="P6">
-        <v>0.77493692217449794</v>
+        <v>0.84120347768908854</v>
       </c>
       <c r="Q6">
-        <v>0.59749254452861256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.87624588647428336</v>
+      </c>
+      <c r="R6">
+        <v>0.91850118568567074</v>
+      </c>
+      <c r="S6">
+        <v>0.83282430569964583</v>
+      </c>
+      <c r="T6">
+        <v>0.62362040411274389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -6308,8 +6374,17 @@
       <c r="Q7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -6356,13 +6431,22 @@
         <v>0.94504731852562951</v>
       </c>
       <c r="P8">
-        <v>0.92927845149325294</v>
+        <v>0.94342777899101993</v>
       </c>
       <c r="Q8">
-        <v>0.93690421845409066</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.92056787331633572</v>
+      </c>
+      <c r="R8">
+        <v>0.8968790646206628</v>
+      </c>
+      <c r="S8">
+        <v>0.88286436730008111</v>
+      </c>
+      <c r="T8">
+        <v>0.89951712296347752</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -6409,13 +6493,22 @@
         <v>0.89108439606482148</v>
       </c>
       <c r="P9">
-        <v>0.84027401686099956</v>
+        <v>0.8802349330443886</v>
       </c>
       <c r="Q9">
-        <v>0.76497909102369444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.88627413482653572</v>
+      </c>
+      <c r="R9">
+        <v>0.8662472661043461</v>
+      </c>
+      <c r="S9">
+        <v>0.81377743568132777</v>
+      </c>
+      <c r="T9">
+        <v>0.73445265538062998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -6462,13 +6555,22 @@
         <v>197.57336970586016</v>
       </c>
       <c r="P10">
-        <v>193.10258927643693</v>
+        <v>196.83722450183529</v>
       </c>
       <c r="Q10">
-        <v>170.18833094777852</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>198.88474468966345</v>
+      </c>
+      <c r="R10">
+        <v>198.79372393141773</v>
+      </c>
+      <c r="S10">
+        <v>195.29793766496834</v>
+      </c>
+      <c r="T10">
+        <v>170.11389433125416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -6515,13 +6617,22 @@
         <v>81.225339410207084</v>
       </c>
       <c r="P11">
-        <v>83.433232535582817</v>
-      </c>
-      <c r="Q11" t="s">
+        <v>82.943374540427769</v>
+      </c>
+      <c r="Q11">
+        <v>80.514148762097307</v>
+      </c>
+      <c r="R11">
+        <v>79.058295270308733</v>
+      </c>
+      <c r="S11">
+        <v>81.862278102834352</v>
+      </c>
+      <c r="T11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
@@ -6568,13 +6679,22 @@
         <v>18.724611062026483</v>
       </c>
       <c r="P12">
-        <v>16.11595256774606</v>
-      </c>
-      <c r="Q12" t="s">
+        <v>16.736163089596715</v>
+      </c>
+      <c r="Q12">
+        <v>19.4773705175703</v>
+      </c>
+      <c r="R12">
+        <v>20.915221424555138</v>
+      </c>
+      <c r="S12">
+        <v>18.017820510637556</v>
+      </c>
+      <c r="T12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
@@ -6621,13 +6741,22 @@
         <v>25.091438252400611</v>
       </c>
       <c r="P13">
-        <v>28.125819289701191</v>
+        <v>25.570332306536635</v>
       </c>
       <c r="Q13">
-        <v>35.028896369598066</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>22.475273219007104</v>
+      </c>
+      <c r="R13">
+        <v>24.536392619677358</v>
+      </c>
+      <c r="S13">
+        <v>27.696453088650369</v>
+      </c>
+      <c r="T13">
+        <v>35.49727753675554</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>82</v>
       </c>
@@ -6674,13 +6803,22 @@
         <v>74.038361041448425</v>
       </c>
       <c r="P14">
-        <v>69.539579788292428</v>
+        <v>73.38005466700848</v>
       </c>
       <c r="Q14">
-        <v>55.60490694634634</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>77.326892960495485</v>
+      </c>
+      <c r="R14">
+        <v>74.778751987795104</v>
+      </c>
+      <c r="S14">
+        <v>70.225536275864485</v>
+      </c>
+      <c r="T14">
+        <v>54.403797201245055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
@@ -6727,13 +6865,22 @@
         <v>37.926598689166809</v>
       </c>
       <c r="P15">
-        <v>36.501668499162456</v>
-      </c>
-      <c r="Q15" t="s">
+        <v>37.564144245789578</v>
+      </c>
+      <c r="Q15">
+        <v>38.651358465980621</v>
+      </c>
+      <c r="R15">
+        <v>38.764129586006291</v>
+      </c>
+      <c r="S15">
+        <v>37.149389102107399</v>
+      </c>
+      <c r="T15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -6780,13 +6927,22 @@
         <v>62.135132465669287</v>
       </c>
       <c r="P16">
-        <v>63.678287301078129</v>
-      </c>
-      <c r="Q16" t="s">
+        <v>62.521566128006533</v>
+      </c>
+      <c r="Q16">
+        <v>61.374452484344168</v>
+      </c>
+      <c r="R16">
+        <v>61.257505860021823</v>
+      </c>
+      <c r="S16">
+        <v>62.968805282449473</v>
+      </c>
+      <c r="T16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -6833,13 +6989,22 @@
         <v>57.195490828323443</v>
       </c>
       <c r="P17">
-        <v>55.221484067444941</v>
+        <v>56.696984603722349</v>
       </c>
       <c r="Q17">
-        <v>50.510257216772395</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>58.184922358539822</v>
+      </c>
+      <c r="R17">
+        <v>58.337993400336217</v>
+      </c>
+      <c r="S17">
+        <v>56.123522311498256</v>
+      </c>
+      <c r="T17">
+        <v>50.510257216513139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>86</v>
       </c>
@@ -6886,13 +7051,22 @@
         <v>42.888411696208422</v>
       </c>
       <c r="P18">
-        <v>45.026343428197329</v>
+        <v>43.41990034278696</v>
       </c>
       <c r="Q18">
-        <v>50.510257216882515</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>41.849924526617386</v>
+      </c>
+      <c r="R18">
+        <v>41.691185755123989</v>
+      </c>
+      <c r="S18">
+        <v>44.038280264995819</v>
+      </c>
+      <c r="T18">
+        <v>50.510257217200085</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
@@ -6944,8 +7118,17 @@
       <c r="Q19">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <v>200</v>
+      </c>
+      <c r="S19">
+        <v>200</v>
+      </c>
+      <c r="T19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
@@ -6992,13 +7175,22 @@
         <v>92.944309968961264</v>
       </c>
       <c r="P20">
-        <v>89.310036642749893</v>
+        <v>92.35072390066351</v>
       </c>
       <c r="Q20">
-        <v>81.498026247360883</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>93.992035142064012</v>
+      </c>
+      <c r="R20">
+        <v>96.00473190097928</v>
+      </c>
+      <c r="S20">
+        <v>91.961809567869651</v>
+      </c>
+      <c r="T20">
+        <v>82.623897009689543</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
@@ -7045,13 +7237,22 @@
         <v>108.21493002930814</v>
       </c>
       <c r="P21">
-        <v>113.59698981509561</v>
+        <v>109.03086818218077</v>
       </c>
       <c r="Q21">
-        <v>129.37005259843758</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>106.8284688791214</v>
+      </c>
+      <c r="R21">
+        <v>104.34223604174038</v>
+      </c>
+      <c r="S21">
+        <v>109.57798354612098</v>
+      </c>
+      <c r="T21">
+        <v>126.63094323947512</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
@@ -7098,13 +7299,22 @@
         <v>197.57336970586016</v>
       </c>
       <c r="P22">
-        <v>193.10258927643693</v>
+        <v>196.83722450183529</v>
       </c>
       <c r="Q22">
-        <v>170.18833094777852</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>198.88474468966345</v>
+      </c>
+      <c r="R22">
+        <v>198.79372393141773</v>
+      </c>
+      <c r="S22">
+        <v>195.29793766496834</v>
+      </c>
+      <c r="T22">
+        <v>170.11389433125416</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -7151,10 +7361,19 @@
         <v>0.98786684852930084</v>
       </c>
       <c r="P23">
-        <v>0.96551294638218466</v>
+        <v>0.98418612250917648</v>
       </c>
       <c r="Q23">
-        <v>0.85094165473889261</v>
+        <v>0.9944237234483172</v>
+      </c>
+      <c r="R23">
+        <v>0.9939686196570886</v>
+      </c>
+      <c r="S23">
+        <v>0.97648968832484173</v>
+      </c>
+      <c r="T23">
+        <v>0.85056947165627084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tests, taxes in combination
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71F2693-8C2D-4398-BDDC-468A70B5AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A98C6B-EF7F-408B-B117-065C63E183A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3864" yWindow="3072" windowWidth="13824" windowHeight="7260" firstSheet="7" activeTab="8" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="7" activeTab="8" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="127">
   <si>
     <t>X.L</t>
   </si>
@@ -402,6 +402,18 @@
   </si>
   <si>
     <t>S.T1,O4=.1</t>
+  </si>
+  <si>
+    <t>O4,I=0.1</t>
+  </si>
+  <si>
+    <t>ITAX=0.1</t>
+  </si>
+  <si>
+    <t>O2=.3,I=.2</t>
+  </si>
+  <si>
+    <t>ITAX=100%</t>
   </si>
 </sst>
 </file>
@@ -5950,13 +5962,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F07C38F-0BBA-4014-8D0C-146F422C055E}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -6009,13 +6021,19 @@
         <v>122</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -6073,8 +6091,14 @@
       <c r="S2">
         <v>0.63672356266481245</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T2">
+        <v>0.54435839324634638</v>
+      </c>
+      <c r="U2">
+        <v>0.26298581656113768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -6133,10 +6157,16 @@
         <v>1.3603228285174447</v>
       </c>
       <c r="T3">
-        <v>1.9797958971155629</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+        <v>1.4510658620690864</v>
+      </c>
+      <c r="U3">
+        <v>1.7255770390585923</v>
+      </c>
+      <c r="V3">
+        <v>1.9797958977022081</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -6195,10 +6225,16 @@
         <v>0.97648968838754668</v>
       </c>
       <c r="T4">
-        <v>0.85056947165921182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0.96551294639121377</v>
+      </c>
+      <c r="U4">
+        <v>0.91527149061040103</v>
+      </c>
+      <c r="V4">
+        <v>0.85094165634213248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -6257,10 +6293,16 @@
         <v>1.1824559830178498</v>
       </c>
       <c r="T5">
-        <v>1.4648348042647581</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>1.253716855956764</v>
+      </c>
+      <c r="U5">
+        <v>1.3799838239044699</v>
+      </c>
+      <c r="V5">
+        <v>1.5055868687041585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -6319,10 +6361,16 @@
         <v>0.83282430569964583</v>
       </c>
       <c r="T6">
-        <v>0.62362040411274389</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0.77493692216806154</v>
+      </c>
+      <c r="U6">
+        <v>0.68107531417393674</v>
+      </c>
+      <c r="V6">
+        <v>0.59749254327701107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -6383,8 +6431,14 @@
       <c r="T7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -6443,10 +6497,16 @@
         <v>0.88286436730008111</v>
       </c>
       <c r="T8">
-        <v>0.89951712296347752</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0.9292784514896667</v>
+      </c>
+      <c r="U8">
+        <v>0.92558632011647268</v>
+      </c>
+      <c r="V8">
+        <v>0.93690421725376627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -6505,10 +6565,16 @@
         <v>0.81377743568132777</v>
       </c>
       <c r="T9">
-        <v>0.73445265538062998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0.84027401688006276</v>
+      </c>
+      <c r="U9">
+        <v>0.79214910866172539</v>
+      </c>
+      <c r="V9">
+        <v>0.76497908901895417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -6567,10 +6633,16 @@
         <v>195.29793766496834</v>
       </c>
       <c r="T10">
-        <v>170.11389433125416</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>193.10258927785549</v>
+      </c>
+      <c r="U10">
+        <v>183.05429809302706</v>
+      </c>
+      <c r="V10">
+        <v>170.18833062727202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -6628,11 +6700,17 @@
       <c r="S11">
         <v>81.862278102834352</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11">
+        <v>83.433232535765256</v>
+      </c>
+      <c r="U11">
+        <v>87.427869776331136</v>
+      </c>
+      <c r="V11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
@@ -6690,11 +6768,17 @@
       <c r="S12">
         <v>18.017820510637556</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12">
+        <v>16.115952567509943</v>
+      </c>
+      <c r="U12">
+        <v>9.4388503851486849</v>
+      </c>
+      <c r="V12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
@@ -6753,10 +6837,16 @@
         <v>27.696453088650369</v>
       </c>
       <c r="T13">
-        <v>35.49727753675554</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+        <v>28.125819289987454</v>
+      </c>
+      <c r="U13">
+        <v>31.827759090372432</v>
+      </c>
+      <c r="V13">
+        <v>35.02889640415664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>82</v>
       </c>
@@ -6815,10 +6905,16 @@
         <v>70.225536275864485</v>
       </c>
       <c r="T14">
-        <v>54.403797201245055</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+        <v>69.539579787829297</v>
+      </c>
+      <c r="U14">
+        <v>62.832913390522151</v>
+      </c>
+      <c r="V14">
+        <v>55.604906859264212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
@@ -6876,11 +6972,17 @@
       <c r="S15">
         <v>37.149389102107399</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15">
+        <v>36.501668500052006</v>
+      </c>
+      <c r="U15">
+        <v>34.695155696294023</v>
+      </c>
+      <c r="V15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -6938,11 +7040,17 @@
       <c r="S16">
         <v>62.968805282449473</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16">
+        <v>63.678287300094347</v>
+      </c>
+      <c r="U16">
+        <v>65.731733209666629</v>
+      </c>
+      <c r="V16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -7001,10 +7109,16 @@
         <v>56.123522311498256</v>
       </c>
       <c r="T17">
-        <v>50.510257216513139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+        <v>55.221484068689186</v>
+      </c>
+      <c r="U17">
+        <v>52.663928705525308</v>
+      </c>
+      <c r="V17">
+        <v>50.510257155949404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>86</v>
       </c>
@@ -7063,10 +7177,16 @@
         <v>44.038280264995819</v>
       </c>
       <c r="T18">
-        <v>50.510257217200085</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+        <v>45.026343426821327</v>
+      </c>
+      <c r="U18">
+        <v>47.933812623576941</v>
+      </c>
+      <c r="V18">
+        <v>50.510257291375197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
@@ -7127,8 +7247,14 @@
       <c r="T19">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U19">
+        <v>200</v>
+      </c>
+      <c r="V19">
+        <v>200.00000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>88</v>
       </c>
@@ -7187,10 +7313,16 @@
         <v>91.961809567869651</v>
       </c>
       <c r="T20">
-        <v>82.623897009689543</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+        <v>89.310036642418936</v>
+      </c>
+      <c r="U20">
+        <v>85.126151992605983</v>
+      </c>
+      <c r="V20">
+        <v>81.498026207158986</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
@@ -7249,10 +7381,16 @@
         <v>109.57798354612098</v>
       </c>
       <c r="T21">
-        <v>126.63094323947512</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+        <v>113.59698981563102</v>
+      </c>
+      <c r="U21">
+        <v>121.17204299879612</v>
+      </c>
+      <c r="V21">
+        <v>129.37005269973994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
@@ -7311,10 +7449,16 @@
         <v>195.29793766496834</v>
       </c>
       <c r="T22">
-        <v>170.11389433125416</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+        <v>193.10258927785549</v>
+      </c>
+      <c r="U22">
+        <v>183.05429809302706</v>
+      </c>
+      <c r="V22">
+        <v>170.18833062727202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -7373,7 +7517,13 @@
         <v>0.97648968832484173</v>
       </c>
       <c r="T23">
-        <v>0.85056947165627084</v>
+        <v>0.96551294638927743</v>
+      </c>
+      <c r="U23">
+        <v>0.91527149046513534</v>
+      </c>
+      <c r="V23">
+        <v>0.85094165313636017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add indexed input tax ex and test
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A98C6B-EF7F-408B-B117-065C63E183A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B019F-EE8C-498E-A4B2-0F1C4FF83561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="7" activeTab="8" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="9072" firstSheet="5" activeTab="5" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="128">
   <si>
     <t>X.L</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>ITAX=100%</t>
+  </si>
+  <si>
+    <t>Itax=.1</t>
   </si>
 </sst>
 </file>
@@ -3205,13 +3208,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEAD0FC-6E99-420C-BC7A-3D842CD4A7CD}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -3236,8 +3239,11 @@
       <c r="I1" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3265,8 +3271,11 @@
       <c r="I2">
         <v>0.26532998322513834</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>1.03413946975517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3294,8 +3303,11 @@
       <c r="I3">
         <v>2.5753333516762882</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>1.0671374602439139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3323,8 +3335,11 @@
       <c r="I4">
         <v>0.56598124103192959</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>1.0450238394808722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3352,8 +3367,11 @@
       <c r="I5">
         <v>11.608186765877146</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>1.137553415066088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3381,8 +3399,11 @@
       <c r="I6">
         <v>1.195961679231847</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>1.1023780243665877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3410,8 +3431,11 @@
       <c r="I7">
         <v>5.4418764732304421</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>1.1257053102015093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3439,8 +3463,11 @@
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3468,8 +3495,11 @@
       <c r="I9">
         <v>1.347499999874207</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>1.1763888813745906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3497,8 +3527,11 @@
       <c r="I10">
         <v>461.99999997773762</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>176.45833271126418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -3526,8 +3559,11 @@
       <c r="I11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -3555,8 +3591,11 @@
       <c r="I12">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
@@ -3584,8 +3623,11 @@
       <c r="I13">
         <v>58.040933828510354</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>51.706973359820239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -3613,8 +3655,11 @@
       <c r="I14">
         <v>43.073049227405299</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>48.349377995940998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -3642,8 +3687,11 @@
       <c r="I15">
         <v>23.919233584290627</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>22.047560465933849</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
@@ -3671,8 +3719,11 @@
       <c r="I16">
         <v>26.626234048078171</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>28.112592036960997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -3700,8 +3751,11 @@
       <c r="I17">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -3729,8 +3783,11 @@
       <c r="I18">
         <v>46.879642643468536</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>98.958457271621995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
@@ -3758,8 +3815,11 @@
       <c r="I19">
         <v>227.51048665392318</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>51.058043851920374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -3787,8 +3847,11 @@
       <c r="I20">
         <v>149.9999999995207</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>149.9999999172434</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
@@ -3815,6 +3878,9 @@
       </c>
       <c r="I21">
         <v>84.897186154518167</v>
+      </c>
+      <c r="J21">
+        <v>156.75357583564821</v>
       </c>
     </row>
   </sheetData>
@@ -5964,7 +6030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F07C38F-0BBA-4014-8D0C-146F422C055E}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
more test and clean-up
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B019F-EE8C-498E-A4B2-0F1C4FF83561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D5B43-8CD6-4A83-BB20-1B7CB0C102D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="9072" firstSheet="5" activeTab="5" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" firstSheet="7" activeTab="9" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="TwoxTwoCET-Scalar" sheetId="9" r:id="rId7"/>
     <sheet name="TwoxTwowOTax_IndCon" sheetId="10" r:id="rId8"/>
     <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
+    <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="160">
   <si>
     <t>X.L</t>
   </si>
@@ -417,6 +418,102 @@
   </si>
   <si>
     <t>Itax=.1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>PX</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>PFX</t>
+  </si>
+  <si>
+    <t>SCY</t>
+  </si>
+  <si>
+    <t>SFXY</t>
+  </si>
+  <si>
+    <t>SXM</t>
+  </si>
+  <si>
+    <t>DKY</t>
+  </si>
+  <si>
+    <t>DLY</t>
+  </si>
+  <si>
+    <t>DFXM</t>
+  </si>
+  <si>
+    <t>GOVT</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>CFXC</t>
+  </si>
+  <si>
+    <t>CXG</t>
+  </si>
+  <si>
+    <t>CXHH</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>endow=1.1</t>
+  </si>
+  <si>
+    <t>sigmac=0.5</t>
+  </si>
+  <si>
+    <t>sigmadm=4</t>
+  </si>
+  <si>
+    <t>sigma=0.4</t>
+  </si>
+  <si>
+    <t>esubkl=1.5</t>
+  </si>
+  <si>
+    <t>t_elasY=1</t>
+  </si>
+  <si>
+    <t>endow=2</t>
+  </si>
+  <si>
+    <t>sigmac=4</t>
+  </si>
+  <si>
+    <t>sigma=3</t>
+  </si>
+  <si>
+    <t>t_elY=0.5</t>
+  </si>
+  <si>
+    <t>sigmac=.1</t>
+  </si>
+  <si>
+    <t>esubkl=0</t>
   </si>
 </sst>
 </file>
@@ -1157,6 +1254,975 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A1C099-339A-499F-B548-AD9626FC6E95}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0409467150618095</v>
+      </c>
+      <c r="D2">
+        <v>1.0409467150618095</v>
+      </c>
+      <c r="E2">
+        <v>1.0409467150618095</v>
+      </c>
+      <c r="F2">
+        <v>1.0409467150618095</v>
+      </c>
+      <c r="G2">
+        <v>1.0413315905142031</v>
+      </c>
+      <c r="H2">
+        <v>1.0413315905141234</v>
+      </c>
+      <c r="I2">
+        <v>1.3655637484781848</v>
+      </c>
+      <c r="J2">
+        <v>1.3655637484781848</v>
+      </c>
+      <c r="K2">
+        <v>1.3655637484781848</v>
+      </c>
+      <c r="L2">
+        <v>1.3655637484548107</v>
+      </c>
+      <c r="M2">
+        <v>1.3655637484548107</v>
+      </c>
+      <c r="N2">
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0409467150618097</v>
+      </c>
+      <c r="D3">
+        <v>1.0409467150618097</v>
+      </c>
+      <c r="E3">
+        <v>1.0409467150618097</v>
+      </c>
+      <c r="F3">
+        <v>1.0409467150618097</v>
+      </c>
+      <c r="G3">
+        <v>1.0486808002757482</v>
+      </c>
+      <c r="H3">
+        <v>1.0512865797894155</v>
+      </c>
+      <c r="I3">
+        <v>1.4615181132137973</v>
+      </c>
+      <c r="J3">
+        <v>1.4615181132137973</v>
+      </c>
+      <c r="K3">
+        <v>1.4615181132137973</v>
+      </c>
+      <c r="L3">
+        <v>1.4531870931903248</v>
+      </c>
+      <c r="M3">
+        <v>1.4531870931903248</v>
+      </c>
+      <c r="N3">
+        <v>0.49256427487327714</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.96066396630169593</v>
+      </c>
+      <c r="D4">
+        <v>0.96066396630169593</v>
+      </c>
+      <c r="E4">
+        <v>0.96066396630169593</v>
+      </c>
+      <c r="F4">
+        <v>0.96066396630169593</v>
+      </c>
+      <c r="G4">
+        <v>0.98510801142359916</v>
+      </c>
+      <c r="H4">
+        <v>0.9792169213926406</v>
+      </c>
+      <c r="I4">
+        <v>0.84773893640196851</v>
+      </c>
+      <c r="J4">
+        <v>0.84773893640196851</v>
+      </c>
+      <c r="K4">
+        <v>0.84773893640196851</v>
+      </c>
+      <c r="L4">
+        <v>0.85984235927002339</v>
+      </c>
+      <c r="M4">
+        <v>0.85984235927002339</v>
+      </c>
+      <c r="N4">
+        <v>0.28503598493747223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="H5">
+        <v>0.99999999999955436</v>
+      </c>
+      <c r="I5">
+        <v>0.99999999999999967</v>
+      </c>
+      <c r="J5">
+        <v>0.99999999999999967</v>
+      </c>
+      <c r="K5">
+        <v>0.99999999999999967</v>
+      </c>
+      <c r="L5">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="M5">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="N5">
+        <v>0.99999999999999956</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.99999999999999944</v>
+      </c>
+      <c r="H6">
+        <v>0.99999999999955447</v>
+      </c>
+      <c r="I6">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="J6">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="K6">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="L6">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="M6">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="N6">
+        <v>0.99999999999999967</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.96066396630169604</v>
+      </c>
+      <c r="D7">
+        <v>0.96066396630169604</v>
+      </c>
+      <c r="E7">
+        <v>0.96066396630169604</v>
+      </c>
+      <c r="F7">
+        <v>0.96066396630169604</v>
+      </c>
+      <c r="G7">
+        <v>0.97820432308343963</v>
+      </c>
+      <c r="H7">
+        <v>0.97577968773204271</v>
+      </c>
+      <c r="I7">
+        <v>0.82649460766956562</v>
+      </c>
+      <c r="J7">
+        <v>0.82649460766956562</v>
+      </c>
+      <c r="K7">
+        <v>0.82649460766956562</v>
+      </c>
+      <c r="L7">
+        <v>0.83123284371043515</v>
+      </c>
+      <c r="M7">
+        <v>0.83123284371043515</v>
+      </c>
+      <c r="N7">
+        <v>0.40603837956264377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.90909090909090839</v>
+      </c>
+      <c r="D8">
+        <v>0.90909090909090839</v>
+      </c>
+      <c r="E8">
+        <v>0.90909090909090839</v>
+      </c>
+      <c r="F8">
+        <v>0.90909090909090839</v>
+      </c>
+      <c r="G8">
+        <v>0.93843646859576813</v>
+      </c>
+      <c r="H8">
+        <v>0.93843646666839553</v>
+      </c>
+      <c r="I8">
+        <v>0.62996052472375974</v>
+      </c>
+      <c r="J8">
+        <v>0.62996052472375974</v>
+      </c>
+      <c r="K8">
+        <v>0.62996052472375974</v>
+      </c>
+      <c r="L8">
+        <v>0.6299605249474346</v>
+      </c>
+      <c r="M8">
+        <v>0.6299605249474346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="D9">
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="E9">
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="F9">
+        <v>0.99999999999999956</v>
+      </c>
+      <c r="G9">
+        <v>0.99999999999955469</v>
+      </c>
+      <c r="H9">
+        <v>0.99999999794519723</v>
+      </c>
+      <c r="I9">
+        <v>0.99999999980729937</v>
+      </c>
+      <c r="J9">
+        <v>0.99999999980729937</v>
+      </c>
+      <c r="K9">
+        <v>0.99999999980729937</v>
+      </c>
+      <c r="L9">
+        <v>0.999999999999997</v>
+      </c>
+      <c r="M9">
+        <v>0.999999999999997</v>
+      </c>
+      <c r="N9">
+        <v>0.99999999999998435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.96066396630169637</v>
+      </c>
+      <c r="D10">
+        <v>0.96066396630169637</v>
+      </c>
+      <c r="E10">
+        <v>0.96066396630169637</v>
+      </c>
+      <c r="F10">
+        <v>0.96066396630169637</v>
+      </c>
+      <c r="G10">
+        <v>0.9679393996641118</v>
+      </c>
+      <c r="H10">
+        <v>0.97064644621227558</v>
+      </c>
+      <c r="I10">
+        <v>0.79562214965188616</v>
+      </c>
+      <c r="J10">
+        <v>0.79562214965188616</v>
+      </c>
+      <c r="K10">
+        <v>0.79562214965188616</v>
+      </c>
+      <c r="L10">
+        <v>0.79009348793890188</v>
+      </c>
+      <c r="M10">
+        <v>0.79009348793890188</v>
+      </c>
+      <c r="N10">
+        <v>0.69034816848588632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>60.360967186806775</v>
+      </c>
+      <c r="I11">
+        <v>62.606779928077714</v>
+      </c>
+      <c r="J11">
+        <v>62.606779928077714</v>
+      </c>
+      <c r="K11">
+        <v>62.606779928077714</v>
+      </c>
+      <c r="L11">
+        <v>61.725506400393442</v>
+      </c>
+      <c r="M11">
+        <v>61.725506400393442</v>
+      </c>
+      <c r="N11">
+        <v>42.099947494810046</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>130</v>
+      </c>
+      <c r="C12">
+        <v>130</v>
+      </c>
+      <c r="D12">
+        <v>130</v>
+      </c>
+      <c r="E12">
+        <v>130</v>
+      </c>
+      <c r="F12">
+        <v>130</v>
+      </c>
+      <c r="G12">
+        <v>130</v>
+      </c>
+      <c r="H12">
+        <v>129.63744143029052</v>
+      </c>
+      <c r="I12">
+        <v>127.30873522758507</v>
+      </c>
+      <c r="J12">
+        <v>127.30873522758507</v>
+      </c>
+      <c r="K12">
+        <v>127.30873522758507</v>
+      </c>
+      <c r="L12">
+        <v>128.19957530716826</v>
+      </c>
+      <c r="M12">
+        <v>128.19957530716826</v>
+      </c>
+      <c r="N12">
+        <v>141.95735496038023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14">
+        <v>110</v>
+      </c>
+      <c r="C14">
+        <v>105.67303629318663</v>
+      </c>
+      <c r="D14">
+        <v>105.67303629318663</v>
+      </c>
+      <c r="E14">
+        <v>105.67303629318663</v>
+      </c>
+      <c r="F14">
+        <v>105.67303629318663</v>
+      </c>
+      <c r="G14">
+        <v>105.63397961033002</v>
+      </c>
+      <c r="H14">
+        <v>105.63397961036699</v>
+      </c>
+      <c r="I14">
+        <v>80.552812061435645</v>
+      </c>
+      <c r="J14">
+        <v>80.552812061435645</v>
+      </c>
+      <c r="K14">
+        <v>80.552812061435645</v>
+      </c>
+      <c r="L14">
+        <v>80.552812070816401</v>
+      </c>
+      <c r="M14">
+        <v>80.552812070816401</v>
+      </c>
+      <c r="N14">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15">
+        <v>80</v>
+      </c>
+      <c r="C15">
+        <v>84.538429034549324</v>
+      </c>
+      <c r="D15">
+        <v>84.538429034549324</v>
+      </c>
+      <c r="E15">
+        <v>84.538429034549324</v>
+      </c>
+      <c r="F15">
+        <v>84.538429034549324</v>
+      </c>
+      <c r="G15">
+        <v>84.507183688333086</v>
+      </c>
+      <c r="H15">
+        <v>84.507183688293594</v>
+      </c>
+      <c r="I15">
+        <v>117.16772666335125</v>
+      </c>
+      <c r="J15">
+        <v>117.16772666335125</v>
+      </c>
+      <c r="K15">
+        <v>117.16772666335125</v>
+      </c>
+      <c r="L15">
+        <v>117.16772664846026</v>
+      </c>
+      <c r="M15">
+        <v>117.16772664846026</v>
+      </c>
+      <c r="N15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>39.999999999999993</v>
+      </c>
+      <c r="D16">
+        <v>39.999999999999993</v>
+      </c>
+      <c r="E16">
+        <v>39.999999999999993</v>
+      </c>
+      <c r="F16">
+        <v>39.999999999999993</v>
+      </c>
+      <c r="G16">
+        <v>40.424196945504349</v>
+      </c>
+      <c r="H16">
+        <v>40.211539080021154</v>
+      </c>
+      <c r="I16">
+        <v>41.552116568193583</v>
+      </c>
+      <c r="J16">
+        <v>41.552116568193583</v>
+      </c>
+      <c r="K16">
+        <v>41.552116568193583</v>
+      </c>
+      <c r="L16">
+        <v>42.082758883577291</v>
+      </c>
+      <c r="M16">
+        <v>42.082758883577291</v>
+      </c>
+      <c r="N16">
+        <v>23.526585459229359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17">
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>110</v>
+      </c>
+      <c r="D17">
+        <v>109.99999999999996</v>
+      </c>
+      <c r="E17">
+        <v>109.99999999999996</v>
+      </c>
+      <c r="F17">
+        <v>109.99999999999996</v>
+      </c>
+      <c r="G17">
+        <v>109.99999999999996</v>
+      </c>
+      <c r="H17">
+        <v>109.99999999995102</v>
+      </c>
+      <c r="I17">
+        <v>110</v>
+      </c>
+      <c r="J17">
+        <v>110</v>
+      </c>
+      <c r="K17">
+        <v>110</v>
+      </c>
+      <c r="L17">
+        <v>110</v>
+      </c>
+      <c r="M17">
+        <v>110</v>
+      </c>
+      <c r="N17">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="C18">
+        <v>79.999999999999943</v>
+      </c>
+      <c r="D18">
+        <v>79.999999999999943</v>
+      </c>
+      <c r="E18">
+        <v>79.999999999999943</v>
+      </c>
+      <c r="F18">
+        <v>79.999999999999943</v>
+      </c>
+      <c r="G18">
+        <v>82.582409236427594</v>
+      </c>
+      <c r="H18">
+        <v>82.582409066818812</v>
+      </c>
+      <c r="I18">
+        <v>100.79368395580155</v>
+      </c>
+      <c r="J18">
+        <v>100.79368395580155</v>
+      </c>
+      <c r="K18">
+        <v>100.79368395580155</v>
+      </c>
+      <c r="L18">
+        <v>100.79368399158953</v>
+      </c>
+      <c r="M18">
+        <v>100.79368399158953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>90</v>
+      </c>
+      <c r="C19">
+        <v>90</v>
+      </c>
+      <c r="D19">
+        <v>90</v>
+      </c>
+      <c r="E19">
+        <v>90</v>
+      </c>
+      <c r="F19">
+        <v>90</v>
+      </c>
+      <c r="G19">
+        <v>89.999999999999943</v>
+      </c>
+      <c r="H19">
+        <v>89.999999999959897</v>
+      </c>
+      <c r="I19">
+        <v>89.999999999999972</v>
+      </c>
+      <c r="J19">
+        <v>89.999999999999972</v>
+      </c>
+      <c r="K19">
+        <v>89.999999999999972</v>
+      </c>
+      <c r="L19">
+        <v>90.000000000000028</v>
+      </c>
+      <c r="M19">
+        <v>90.000000000000028</v>
+      </c>
+      <c r="N19">
+        <v>89.999999999999972</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <v>93.685204355562888</v>
+      </c>
+      <c r="D20">
+        <v>93.685204355562888</v>
+      </c>
+      <c r="E20">
+        <v>93.685204355562888</v>
+      </c>
+      <c r="F20">
+        <v>93.685204355562888</v>
+      </c>
+      <c r="G20">
+        <v>92.981027563534639</v>
+      </c>
+      <c r="H20">
+        <v>92.721711753197241</v>
+      </c>
+      <c r="I20">
+        <v>113.11902269108303</v>
+      </c>
+      <c r="J20">
+        <v>113.11902269108303</v>
+      </c>
+      <c r="K20">
+        <v>113.11902269108303</v>
+      </c>
+      <c r="L20">
+        <v>113.91057055131651</v>
+      </c>
+      <c r="M20">
+        <v>113.91057055131651</v>
+      </c>
+      <c r="N20">
+        <v>130.36899945341128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>20.818934301236194</v>
+      </c>
+      <c r="D21">
+        <v>20.818934301236194</v>
+      </c>
+      <c r="E21">
+        <v>20.818934301236194</v>
+      </c>
+      <c r="F21">
+        <v>20.818934301236194</v>
+      </c>
+      <c r="G21">
+        <v>20.445626264406847</v>
+      </c>
+      <c r="H21">
+        <v>20.496429891248273</v>
+      </c>
+      <c r="I21">
+        <v>24.198584980963417</v>
+      </c>
+      <c r="J21">
+        <v>24.198584980963417</v>
+      </c>
+      <c r="K21">
+        <v>24.198584980963417</v>
+      </c>
+      <c r="L21">
+        <v>24.060646967129607</v>
+      </c>
+      <c r="M21">
+        <v>24.060646967129607</v>
+      </c>
+      <c r="N21">
+        <v>49.256427487329155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22">
+        <v>80</v>
+      </c>
+      <c r="C22">
+        <v>83.275737204944761</v>
+      </c>
+      <c r="D22">
+        <v>83.275737204944761</v>
+      </c>
+      <c r="E22">
+        <v>83.275737204944761</v>
+      </c>
+      <c r="F22">
+        <v>83.275737204944761</v>
+      </c>
+      <c r="G22">
+        <v>84.422453763152532</v>
+      </c>
+      <c r="H22">
+        <v>84.632228058324415</v>
+      </c>
+      <c r="I22">
+        <v>121.95322633744162</v>
+      </c>
+      <c r="J22">
+        <v>121.95322633744162</v>
+      </c>
+      <c r="K22">
+        <v>121.95322633744162</v>
+      </c>
+      <c r="L22">
+        <v>121.25806235190294</v>
+      </c>
+      <c r="M22">
+        <v>121.25806235190294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD2B994-3CF8-4777-9095-AA4EE6BD17EC}">
   <dimension ref="A1:F18"/>
@@ -3210,7 +4276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEAD0FC-6E99-420C-BC7A-3D842CD4A7CD}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Add test of Aux Var in Demand
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D5B43-8CD6-4A83-BB20-1B7CB0C102D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ABEA84-EC44-438C-8545-FABA2064CF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" firstSheet="7" activeTab="9" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" firstSheet="8" activeTab="10" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="TwoxTwowOTax_IndCon" sheetId="10" r:id="rId8"/>
     <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
     <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
+    <sheet name="TwoxTwowAuxDem" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="174">
   <si>
     <t>X.L</t>
   </si>
@@ -514,6 +515,48 @@
   </si>
   <si>
     <t>esubkl=0</t>
+  </si>
+  <si>
+    <t>SXX.L</t>
+  </si>
+  <si>
+    <t>SYY.L</t>
+  </si>
+  <si>
+    <t>SWW.L</t>
+  </si>
+  <si>
+    <t>DKX.L</t>
+  </si>
+  <si>
+    <t>DLX.L</t>
+  </si>
+  <si>
+    <t>DLY.L</t>
+  </si>
+  <si>
+    <t>DKY.L</t>
+  </si>
+  <si>
+    <t>DXW.L</t>
+  </si>
+  <si>
+    <t>DYW.L</t>
+  </si>
+  <si>
+    <t>CWCONS.L</t>
+  </si>
+  <si>
+    <t>UnEmp=.1</t>
+  </si>
+  <si>
+    <t>TKX=0.25</t>
+  </si>
+  <si>
+    <t>TY=0.5</t>
+  </si>
+  <si>
+    <t>&amp;TY=.5</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A1C099-339A-499F-B548-AD9626FC6E95}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2216,6 +2259,456 @@
       </c>
       <c r="M22">
         <v>121.25806235190294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F8E8DA-95C7-4996-9A21-15383900C73E}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D2">
+        <v>1.0371252977019936</v>
+      </c>
+      <c r="E2">
+        <v>0.98447088030257324</v>
+      </c>
+      <c r="F2">
+        <v>1.0069367675479344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="D3">
+        <v>1.053409075564238</v>
+      </c>
+      <c r="E3">
+        <v>0.44661553192056858</v>
+      </c>
+      <c r="F3">
+        <v>0.41177381270347702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D4">
+        <v>1.0452354763862961</v>
+      </c>
+      <c r="E4">
+        <v>0.66308369432539305</v>
+      </c>
+      <c r="F4">
+        <v>0.64391784561311827</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D6">
+        <v>0.9845418287728368</v>
+      </c>
+      <c r="E6">
+        <v>2.2042916262845966</v>
+      </c>
+      <c r="F6">
+        <v>2.4453637808572513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D7">
+        <v>0.99224081188632707</v>
+      </c>
+      <c r="E7">
+        <v>1.4846856995121664</v>
+      </c>
+      <c r="F7">
+        <v>1.5637658970763419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D8">
+        <v>0.99224081188632707</v>
+      </c>
+      <c r="E8">
+        <v>1.4846856995121667</v>
+      </c>
+      <c r="F8">
+        <v>1.5637658970763419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0499999999722394</v>
+      </c>
+      <c r="D9">
+        <v>0.97310521759683544</v>
+      </c>
+      <c r="E9">
+        <v>0.704929765951823</v>
+      </c>
+      <c r="F9">
+        <v>0.84532963183954124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0.19999999999999957</v>
+      </c>
+      <c r="D10">
+        <v>0.10830961355206511</v>
+      </c>
+      <c r="E10">
+        <v>0.70637102840442134</v>
+      </c>
+      <c r="F10">
+        <v>0.72063893707626925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>200</v>
+      </c>
+      <c r="E13">
+        <v>200</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>45.67280458551334</v>
+      </c>
+      <c r="E14">
+        <v>63.048046154598161</v>
+      </c>
+      <c r="F14">
+        <v>65.720582199051307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>40.000000000000007</v>
+      </c>
+      <c r="D15">
+        <v>44.79199395149989</v>
+      </c>
+      <c r="E15">
+        <v>29.935254602427996</v>
+      </c>
+      <c r="F15">
+        <v>28.421418146269836</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>60.000000000000014</v>
+      </c>
+      <c r="D16">
+        <v>59.53444871317862</v>
+      </c>
+      <c r="E16">
+        <v>44.540570960010214</v>
+      </c>
+      <c r="F16">
+        <v>46.91297691147642</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>40.470107896625159</v>
+      </c>
+      <c r="E17">
+        <v>62.539326087466797</v>
+      </c>
+      <c r="F17">
+        <v>57.855863291935997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>99.224081188632667</v>
+      </c>
+      <c r="E18">
+        <v>148.46856994948786</v>
+      </c>
+      <c r="F18">
+        <v>156.37658970757903</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>100.78198639087648</v>
+      </c>
+      <c r="E19">
+        <v>67.354322894079274</v>
+      </c>
+      <c r="F19">
+        <v>63.948190830224604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>210</v>
+      </c>
+      <c r="D20">
+        <v>207.42505954038575</v>
+      </c>
+      <c r="E20">
+        <v>196.89417562455813</v>
+      </c>
+      <c r="F20">
+        <v>201.38735349872735</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>200.00000000000006</v>
+      </c>
+      <c r="D21">
+        <v>209.0470952772589</v>
+      </c>
+      <c r="E21">
+        <v>132.61673880825623</v>
+      </c>
+      <c r="F21">
+        <v>128.78356912325972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D22">
+        <v>1.0452354763862945</v>
+      </c>
+      <c r="E22">
+        <v>0.66308369404128109</v>
+      </c>
+      <c r="F22">
+        <v>0.64391784561629861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for Aux in Input
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ABEA84-EC44-438C-8545-FABA2064CF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FB02F2-B1E3-4C22-999B-B93660607B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" firstSheet="8" activeTab="10" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" firstSheet="9" activeTab="11" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
     <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
     <sheet name="TwoxTwowAuxDem" sheetId="13" r:id="rId11"/>
+    <sheet name="two_by_two_AuxinInput" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="203">
   <si>
     <t>X.L</t>
   </si>
@@ -557,6 +558,93 @@
   </si>
   <si>
     <t>&amp;TY=.5</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>PKS</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t>TAU</t>
+  </si>
+  <si>
+    <t>SXX</t>
+  </si>
+  <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>SWW</t>
+  </si>
+  <si>
+    <t>SLSTL</t>
+  </si>
+  <si>
+    <t>SKSTK</t>
+  </si>
+  <si>
+    <t>DLSX</t>
+  </si>
+  <si>
+    <t>DKSX</t>
+  </si>
+  <si>
+    <t>DLSY</t>
+  </si>
+  <si>
+    <t>DKSY</t>
+  </si>
+  <si>
+    <t>DXW</t>
+  </si>
+  <si>
+    <t>DYW</t>
+  </si>
+  <si>
+    <t>DLW</t>
+  </si>
+  <si>
+    <t>DLTL</t>
+  </si>
+  <si>
+    <t>DKTK</t>
+  </si>
+  <si>
+    <t>CONS</t>
+  </si>
+  <si>
+    <t>CWCONS</t>
+  </si>
+  <si>
+    <t>L.15,K.25</t>
+  </si>
+  <si>
+    <t>L.1,K.3</t>
+  </si>
+  <si>
+    <t>L.05,K.35</t>
+  </si>
+  <si>
+    <t>L.0,K.4</t>
+  </si>
+  <si>
+    <t>L-.05,K.45</t>
   </si>
 </sst>
 </file>
@@ -2270,7 +2358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F8E8DA-95C7-4996-9A21-15383900C73E}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2710,6 +2798,709 @@
       <c r="F22">
         <v>0.64391784561629861</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E9F4BC-EEDA-4A84-A728-E202F2F9DA58}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.006387575650056</v>
+      </c>
+      <c r="D2">
+        <v>1.0126852580817098</v>
+      </c>
+      <c r="E2">
+        <v>1.0193022237638398</v>
+      </c>
+      <c r="F2">
+        <v>1.026928314669364</v>
+      </c>
+      <c r="G2">
+        <v>1.0377545680283367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0095966476462173</v>
+      </c>
+      <c r="D3">
+        <v>1.0190881035617243</v>
+      </c>
+      <c r="E3">
+        <v>1.0290926053375762</v>
+      </c>
+      <c r="F3">
+        <v>1.0406631890486693</v>
+      </c>
+      <c r="G3">
+        <v>1.0571630630829592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0008350269671129</v>
+      </c>
+      <c r="D4">
+        <v>1.0014491088570601</v>
+      </c>
+      <c r="E4">
+        <v>1.001862188438271</v>
+      </c>
+      <c r="F4">
+        <v>1.0020312308441757</v>
+      </c>
+      <c r="G4">
+        <v>1.0016777194890492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0160455226090923</v>
+      </c>
+      <c r="D5">
+        <v>1.0320154991633979</v>
+      </c>
+      <c r="E5">
+        <v>1.0489563810795042</v>
+      </c>
+      <c r="F5">
+        <v>1.0686864948681873</v>
+      </c>
+      <c r="G5">
+        <v>1.0970757978651695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.99062365945204522</v>
+      </c>
+      <c r="D7">
+        <v>0.98023361021433086</v>
+      </c>
+      <c r="E7">
+        <v>0.96816873805100456</v>
+      </c>
+      <c r="F7">
+        <v>0.95318925131473309</v>
+      </c>
+      <c r="G7">
+        <v>0.93155409308673487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.98747489439651848</v>
+      </c>
+      <c r="D8">
+        <v>0.97407488427239663</v>
+      </c>
+      <c r="E8">
+        <v>0.95895796214597595</v>
+      </c>
+      <c r="F8">
+        <v>0.94060887491218026</v>
+      </c>
+      <c r="G8">
+        <v>0.91445165767240888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.99916566972116849</v>
+      </c>
+      <c r="D9">
+        <v>0.99732896542206706</v>
+      </c>
+      <c r="E9">
+        <v>0.9943694698123019</v>
+      </c>
+      <c r="F9">
+        <v>0.99001673768539966</v>
+      </c>
+      <c r="G9">
+        <v>0.98375023335117484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.0237432725840783</v>
+      </c>
+      <c r="D10">
+        <v>1.0469473301163175</v>
+      </c>
+      <c r="E10">
+        <v>1.0711351761369892</v>
+      </c>
+      <c r="F10">
+        <v>1.0991328545245336</v>
+      </c>
+      <c r="G10">
+        <v>1.1409855970537344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.95689374406213035</v>
+      </c>
+      <c r="D11">
+        <v>0.91107593331151671</v>
+      </c>
+      <c r="E11">
+        <v>0.85945629637063958</v>
+      </c>
+      <c r="F11">
+        <v>0.79586881245096153</v>
+      </c>
+      <c r="G11">
+        <v>0.69919000272678622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.99695134301753163</v>
+      </c>
+      <c r="D12">
+        <v>0.9926681265402667</v>
+      </c>
+      <c r="E12">
+        <v>0.98685654767402087</v>
+      </c>
+      <c r="F12">
+        <v>0.97885703141359282</v>
+      </c>
+      <c r="G12">
+        <v>0.96672451546625382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.98120735816782156</v>
+      </c>
+      <c r="D13">
+        <v>0.96187327355543928</v>
+      </c>
+      <c r="E13">
+        <v>0.94079845975902054</v>
+      </c>
+      <c r="F13">
+        <v>0.91594404543711139</v>
+      </c>
+      <c r="G13">
+        <v>0.88118297509381738</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.0009381670421438</v>
+      </c>
+      <c r="D14">
+        <v>1.024890126404802</v>
+      </c>
+      <c r="E14">
+        <v>1.0796578594751951</v>
+      </c>
+      <c r="F14">
+        <v>1.1897677711350092</v>
+      </c>
+      <c r="G14">
+        <v>1.464804238667671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15">
+        <v>120</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15">
+        <v>120</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16">
+        <v>120</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>120</v>
+      </c>
+      <c r="F16">
+        <v>120</v>
+      </c>
+      <c r="G16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17">
+        <v>340</v>
+      </c>
+      <c r="C17">
+        <v>340</v>
+      </c>
+      <c r="D17">
+        <v>340</v>
+      </c>
+      <c r="E17">
+        <v>340</v>
+      </c>
+      <c r="F17">
+        <v>340</v>
+      </c>
+      <c r="G17">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18">
+        <v>120</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>120</v>
+      </c>
+      <c r="E18">
+        <v>120</v>
+      </c>
+      <c r="F18">
+        <v>119.99999999999999</v>
+      </c>
+      <c r="G18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19">
+        <v>120</v>
+      </c>
+      <c r="C19">
+        <v>120</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
+      </c>
+      <c r="E19">
+        <v>120</v>
+      </c>
+      <c r="F19">
+        <v>120</v>
+      </c>
+      <c r="G19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>48.460639087018805</v>
+      </c>
+      <c r="D20">
+        <v>48.916228970963118</v>
+      </c>
+      <c r="E20">
+        <v>49.396445056204186</v>
+      </c>
+      <c r="F20">
+        <v>49.951833074336434</v>
+      </c>
+      <c r="G20">
+        <v>50.74382702798205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21">
+        <v>72</v>
+      </c>
+      <c r="C21">
+        <v>71.543013588470316</v>
+      </c>
+      <c r="D21">
+        <v>71.09810222416634</v>
+      </c>
+      <c r="E21">
+        <v>70.63655736385509</v>
+      </c>
+      <c r="F21">
+        <v>70.11200194940696</v>
+      </c>
+      <c r="G21">
+        <v>69.380566675601443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22">
+        <v>72</v>
+      </c>
+      <c r="C22">
+        <v>72.459905446804385</v>
+      </c>
+      <c r="D22">
+        <v>72.913338581883423</v>
+      </c>
+      <c r="E22">
+        <v>73.389760110996932</v>
+      </c>
+      <c r="F22">
+        <v>73.938838656194577</v>
+      </c>
+      <c r="G22">
+        <v>74.718328898040255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>47.543739484384446</v>
+      </c>
+      <c r="D23">
+        <v>47.100932522162822</v>
+      </c>
+      <c r="E23">
+        <v>46.643032659100584</v>
+      </c>
+      <c r="F23">
+        <v>46.124433443138592</v>
+      </c>
+      <c r="G23">
+        <v>45.404537555464387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24">
+        <v>120</v>
+      </c>
+      <c r="C24">
+        <v>120.66574992281421</v>
+      </c>
+      <c r="D24">
+        <v>121.34638684585452</v>
+      </c>
+      <c r="E24">
+        <v>122.08891428703427</v>
+      </c>
+      <c r="F24">
+        <v>122.98159375382461</v>
+      </c>
+      <c r="G24">
+        <v>124.32197077012238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25">
+        <v>120</v>
+      </c>
+      <c r="C25">
+        <v>121.05051727124193</v>
+      </c>
+      <c r="D25">
+        <v>122.11361650416337</v>
+      </c>
+      <c r="E25">
+        <v>123.26157635813239</v>
+      </c>
+      <c r="F25">
+        <v>124.62643762174304</v>
+      </c>
+      <c r="G25">
+        <v>126.64708928003867</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>98.313353437742862</v>
+      </c>
+      <c r="D26">
+        <v>96.658381566822541</v>
+      </c>
+      <c r="E26">
+        <v>94.927588833650503</v>
+      </c>
+      <c r="F26">
+        <v>92.9425627130626</v>
+      </c>
+      <c r="G26">
+        <v>90.141188584628551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+      <c r="G27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29">
+        <v>340</v>
+      </c>
+      <c r="C29">
+        <v>340</v>
+      </c>
+      <c r="D29">
+        <v>339.58322924414983</v>
+      </c>
+      <c r="E29">
+        <v>338.71519886840156</v>
+      </c>
+      <c r="F29">
+        <v>337.28941467454194</v>
+      </c>
+      <c r="G29">
+        <v>335.03623469860844</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30">
+        <v>340</v>
+      </c>
+      <c r="C30">
+        <v>340.28390916881636</v>
+      </c>
+      <c r="D30">
+        <v>340.49269701139843</v>
+      </c>
+      <c r="E30">
+        <v>340.63314406901054</v>
+      </c>
+      <c r="F30">
+        <v>340.69061848670492</v>
+      </c>
+      <c r="G30">
+        <v>340.57042462627646</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add test for price in Inputs
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7D5B43-8CD6-4A83-BB20-1B7CB0C102D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8579E12D-0498-48F8-A1E2-3BFC2D221ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" firstSheet="7" activeTab="9" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2928" yWindow="2316" windowWidth="17280" windowHeight="9072" firstSheet="8" activeTab="10" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="TwoxTwowOTax_IndCon" sheetId="10" r:id="rId8"/>
     <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
     <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
+    <sheet name="two_by_two_PriceinIntput" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="182">
   <si>
     <t>X.L</t>
   </si>
@@ -514,6 +515,72 @@
   </si>
   <si>
     <t>esubkl=0</t>
+  </si>
+  <si>
+    <t>Itax=0.1</t>
+  </si>
+  <si>
+    <t>Otax=0.1</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>SX</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>DXL</t>
+  </si>
+  <si>
+    <t>DXK</t>
+  </si>
+  <si>
+    <t>DYL</t>
+  </si>
+  <si>
+    <t>DYK</t>
+  </si>
+  <si>
+    <t>DUX</t>
+  </si>
+  <si>
+    <t>DUY</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>PX/PX</t>
+  </si>
+  <si>
+    <t>PY/PX</t>
+  </si>
+  <si>
+    <t>PU/PX</t>
+  </si>
+  <si>
+    <t>PL/PX</t>
+  </si>
+  <si>
+    <t>PK/PX</t>
+  </si>
+  <si>
+    <t>RA/PX</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A1C099-339A-499F-B548-AD9626FC6E95}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2216,6 +2283,637 @@
       </c>
       <c r="M22">
         <v>121.25806235190294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11282225-CC33-40D0-A467-E5A8A58B1ADF}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0533624393223964</v>
+      </c>
+      <c r="D2">
+        <v>1.0533624393076026</v>
+      </c>
+      <c r="E2">
+        <v>1.0533624392983827</v>
+      </c>
+      <c r="F2">
+        <v>1.0692230525392665</v>
+      </c>
+      <c r="G2">
+        <v>1.0306253077634344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0432700717339818</v>
+      </c>
+      <c r="D3">
+        <v>1.0432700717206651</v>
+      </c>
+      <c r="E3">
+        <v>1.043270071718168</v>
+      </c>
+      <c r="F3">
+        <v>1.0159922067315308</v>
+      </c>
+      <c r="G3">
+        <v>1.0873120422296021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0500286076528291</v>
+      </c>
+      <c r="D4">
+        <v>1.0500286076372356</v>
+      </c>
+      <c r="E4">
+        <v>1.0500286076315015</v>
+      </c>
+      <c r="F4">
+        <v>1.0513947937746249</v>
+      </c>
+      <c r="G4">
+        <v>1.0489563308826293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.99683505738742828</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.0442749417809107</v>
+      </c>
+      <c r="F5">
+        <v>0.96924826808406228</v>
+      </c>
+      <c r="G5">
+        <v>1.080588241014147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.006478222756964</v>
+      </c>
+      <c r="D6">
+        <v>1.0096737823300179</v>
+      </c>
+      <c r="E6">
+        <v>1.0543770302540776</v>
+      </c>
+      <c r="F6">
+        <v>1.0200300602347367</v>
+      </c>
+      <c r="G6">
+        <v>1.0242520502029886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.0031749912758545</v>
+      </c>
+      <c r="E7">
+        <v>1.0475905056086889</v>
+      </c>
+      <c r="F7">
+        <v>0.98568358717211357</v>
+      </c>
+      <c r="G7">
+        <v>1.0617044348776998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.95457146145108884</v>
+      </c>
+      <c r="D8">
+        <v>0.95760221755176367</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0500286076528458</v>
+      </c>
+      <c r="D9">
+        <v>1.0533624393068366</v>
+      </c>
+      <c r="E9">
+        <v>1.0999999999351249</v>
+      </c>
+      <c r="F9">
+        <v>1.0363425908479043</v>
+      </c>
+      <c r="G9">
+        <v>1.0440764845854245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>110</v>
+      </c>
+      <c r="C10">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>110</v>
+      </c>
+      <c r="E10">
+        <v>110</v>
+      </c>
+      <c r="F10">
+        <v>110</v>
+      </c>
+      <c r="G10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>54</v>
+      </c>
+      <c r="G11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12">
+        <v>164</v>
+      </c>
+      <c r="C12">
+        <v>164</v>
+      </c>
+      <c r="D12">
+        <v>164</v>
+      </c>
+      <c r="E12">
+        <v>164</v>
+      </c>
+      <c r="F12">
+        <v>164</v>
+      </c>
+      <c r="G12">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52.213747091206962</v>
+      </c>
+      <c r="D13">
+        <v>52.213747089924226</v>
+      </c>
+      <c r="E13">
+        <v>52.213747088526816</v>
+      </c>
+      <c r="F13">
+        <v>52.868087335139379</v>
+      </c>
+      <c r="G13">
+        <v>53.047059029882369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>47.467042807627351</v>
+      </c>
+      <c r="D14">
+        <v>47.46704280902668</v>
+      </c>
+      <c r="E14">
+        <v>47.467042810551135</v>
+      </c>
+      <c r="F14">
+        <v>46.762927451330512</v>
+      </c>
+      <c r="G14">
+        <v>46.573667250728739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>25.305048727435071</v>
+      </c>
+      <c r="D15">
+        <v>25.305048726675256</v>
+      </c>
+      <c r="E15">
+        <v>25.305048725847506</v>
+      </c>
+      <c r="F15">
+        <v>24.480721438762444</v>
+      </c>
+      <c r="G15">
+        <v>24.582049170514459</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.755737188715777</v>
+      </c>
+      <c r="D16">
+        <v>28.755737189406524</v>
+      </c>
+      <c r="E16">
+        <v>28.755737190159014</v>
+      </c>
+      <c r="F16">
+        <v>29.527785568878645</v>
+      </c>
+      <c r="G16">
+        <v>29.43037403561884</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17">
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>110.3492490405403</v>
+      </c>
+      <c r="D17">
+        <v>110.34924904034398</v>
+      </c>
+      <c r="E17">
+        <v>110.34924904012642</v>
+      </c>
+      <c r="F17">
+        <v>111.86524460134066</v>
+      </c>
+      <c r="G17">
+        <v>108.07769639007446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>53.652427622403614</v>
+      </c>
+      <c r="D18">
+        <v>53.652427622598076</v>
+      </c>
+      <c r="E18">
+        <v>53.652427622813583</v>
+      </c>
+      <c r="F18">
+        <v>52.181710894781091</v>
+      </c>
+      <c r="G18">
+        <v>55.974542078075267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19">
+        <v>164</v>
+      </c>
+      <c r="C19">
+        <v>172.20469165071995</v>
+      </c>
+      <c r="D19">
+        <v>172.75144004633617</v>
+      </c>
+      <c r="E19">
+        <v>180.39999999442588</v>
+      </c>
+      <c r="F19">
+        <v>169.96018504007139</v>
+      </c>
+      <c r="G19">
+        <v>182.64378039376402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20">
+        <v>164</v>
+      </c>
+      <c r="C20">
+        <v>172.20469165071995</v>
+      </c>
+      <c r="D20">
+        <v>172.20469165267772</v>
+      </c>
+      <c r="E20">
+        <v>172.20469165058611</v>
+      </c>
+      <c r="F20">
+        <v>172.42874615339829</v>
+      </c>
+      <c r="G20">
+        <v>172.02883815287367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>1.0933333333333333</v>
+      </c>
+      <c r="C21">
+        <v>1.1480312776714663</v>
+      </c>
+      <c r="D21">
+        <v>1.1480312776845181</v>
+      </c>
+      <c r="E21">
+        <v>1.1480312776705741</v>
+      </c>
+      <c r="F21">
+        <v>1.1495249743559885</v>
+      </c>
+      <c r="G21">
+        <v>1.1468589210191578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1.009673782335474</v>
+      </c>
+      <c r="D23">
+        <v>1.0096737823300179</v>
+      </c>
+      <c r="E23">
+        <v>1.0096737823239719</v>
+      </c>
+      <c r="F23">
+        <v>1.0523929666142775</v>
+      </c>
+      <c r="G23">
+        <v>0.94786525646597253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1.0031749912777612</v>
+      </c>
+      <c r="D24">
+        <v>1.0031749912758545</v>
+      </c>
+      <c r="E24">
+        <v>1.0031749912739683</v>
+      </c>
+      <c r="F24">
+        <v>1.0169567691057517</v>
+      </c>
+      <c r="G24">
+        <v>0.98252451264995777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.95760221751519581</v>
+      </c>
+      <c r="D25">
+        <v>0.95760221755176367</v>
+      </c>
+      <c r="E25">
+        <v>0.95760221756790975</v>
+      </c>
+      <c r="F25">
+        <v>1.0317274045552081</v>
+      </c>
+      <c r="G25">
+        <v>0.92542187860705039</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1.0533624393235435</v>
+      </c>
+      <c r="D26">
+        <v>1.0533624393068366</v>
+      </c>
+      <c r="E26">
+        <v>1.0533624392625762</v>
+      </c>
+      <c r="F26">
+        <v>1.0692230514855281</v>
+      </c>
+      <c r="G26">
+        <v>0.96621122177448859</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27">
+        <v>164</v>
+      </c>
+      <c r="C27">
+        <v>172.75144004470056</v>
+      </c>
+      <c r="D27">
+        <v>172.75144004633617</v>
+      </c>
+      <c r="E27">
+        <v>172.75144004391314</v>
+      </c>
+      <c r="F27">
+        <v>175.35258058911575</v>
+      </c>
+      <c r="G27">
+        <v>169.02255036789066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for Price in Output
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8579E12D-0498-48F8-A1E2-3BFC2D221ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F4175F-36E1-4122-AAD0-3252ACA3B1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2316" windowWidth="17280" windowHeight="9072" firstSheet="8" activeTab="10" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="2928" yWindow="2316" windowWidth="17280" windowHeight="9072" firstSheet="9" activeTab="11" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
     <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
     <sheet name="two_by_two_PriceinIntput" sheetId="13" r:id="rId11"/>
+    <sheet name="two_by_two_PriceinOutput" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="182">
   <si>
     <t>X.L</t>
   </si>
@@ -2294,6 +2295,637 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11282225-CC33-40D0-A467-E5A8A58B1ADF}">
   <dimension ref="A1:G27"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0533624393223964</v>
+      </c>
+      <c r="D2">
+        <v>1.0533624393076026</v>
+      </c>
+      <c r="E2">
+        <v>1.0533624392983827</v>
+      </c>
+      <c r="F2">
+        <v>1.0692230525392665</v>
+      </c>
+      <c r="G2">
+        <v>1.0306253077634344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0432700717339818</v>
+      </c>
+      <c r="D3">
+        <v>1.0432700717206651</v>
+      </c>
+      <c r="E3">
+        <v>1.043270071718168</v>
+      </c>
+      <c r="F3">
+        <v>1.0159922067315308</v>
+      </c>
+      <c r="G3">
+        <v>1.0873120422296021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0500286076528291</v>
+      </c>
+      <c r="D4">
+        <v>1.0500286076372356</v>
+      </c>
+      <c r="E4">
+        <v>1.0500286076315015</v>
+      </c>
+      <c r="F4">
+        <v>1.0513947937746249</v>
+      </c>
+      <c r="G4">
+        <v>1.0489563308826293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.99683505738742828</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.0442749417809107</v>
+      </c>
+      <c r="F5">
+        <v>0.96924826808406228</v>
+      </c>
+      <c r="G5">
+        <v>1.080588241014147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.006478222756964</v>
+      </c>
+      <c r="D6">
+        <v>1.0096737823300179</v>
+      </c>
+      <c r="E6">
+        <v>1.0543770302540776</v>
+      </c>
+      <c r="F6">
+        <v>1.0200300602347367</v>
+      </c>
+      <c r="G6">
+        <v>1.0242520502029886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.0031749912758545</v>
+      </c>
+      <c r="E7">
+        <v>1.0475905056086889</v>
+      </c>
+      <c r="F7">
+        <v>0.98568358717211357</v>
+      </c>
+      <c r="G7">
+        <v>1.0617044348776998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.95457146145108884</v>
+      </c>
+      <c r="D8">
+        <v>0.95760221755176367</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0500286076528458</v>
+      </c>
+      <c r="D9">
+        <v>1.0533624393068366</v>
+      </c>
+      <c r="E9">
+        <v>1.0999999999351249</v>
+      </c>
+      <c r="F9">
+        <v>1.0363425908479043</v>
+      </c>
+      <c r="G9">
+        <v>1.0440764845854245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>110</v>
+      </c>
+      <c r="C10">
+        <v>110</v>
+      </c>
+      <c r="D10">
+        <v>110</v>
+      </c>
+      <c r="E10">
+        <v>110</v>
+      </c>
+      <c r="F10">
+        <v>110</v>
+      </c>
+      <c r="G10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>54</v>
+      </c>
+      <c r="G11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12">
+        <v>164</v>
+      </c>
+      <c r="C12">
+        <v>164</v>
+      </c>
+      <c r="D12">
+        <v>164</v>
+      </c>
+      <c r="E12">
+        <v>164</v>
+      </c>
+      <c r="F12">
+        <v>164</v>
+      </c>
+      <c r="G12">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>52.213747091206962</v>
+      </c>
+      <c r="D13">
+        <v>52.213747089924226</v>
+      </c>
+      <c r="E13">
+        <v>52.213747088526816</v>
+      </c>
+      <c r="F13">
+        <v>52.868087335139379</v>
+      </c>
+      <c r="G13">
+        <v>53.047059029882369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>47.467042807627351</v>
+      </c>
+      <c r="D14">
+        <v>47.46704280902668</v>
+      </c>
+      <c r="E14">
+        <v>47.467042810551135</v>
+      </c>
+      <c r="F14">
+        <v>46.762927451330512</v>
+      </c>
+      <c r="G14">
+        <v>46.573667250728739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>25.305048727435071</v>
+      </c>
+      <c r="D15">
+        <v>25.305048726675256</v>
+      </c>
+      <c r="E15">
+        <v>25.305048725847506</v>
+      </c>
+      <c r="F15">
+        <v>24.480721438762444</v>
+      </c>
+      <c r="G15">
+        <v>24.582049170514459</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.755737188715777</v>
+      </c>
+      <c r="D16">
+        <v>28.755737189406524</v>
+      </c>
+      <c r="E16">
+        <v>28.755737190159014</v>
+      </c>
+      <c r="F16">
+        <v>29.527785568878645</v>
+      </c>
+      <c r="G16">
+        <v>29.43037403561884</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17">
+        <v>110</v>
+      </c>
+      <c r="C17">
+        <v>110.3492490405403</v>
+      </c>
+      <c r="D17">
+        <v>110.34924904034398</v>
+      </c>
+      <c r="E17">
+        <v>110.34924904012642</v>
+      </c>
+      <c r="F17">
+        <v>111.86524460134066</v>
+      </c>
+      <c r="G17">
+        <v>108.07769639007446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>53.652427622403614</v>
+      </c>
+      <c r="D18">
+        <v>53.652427622598076</v>
+      </c>
+      <c r="E18">
+        <v>53.652427622813583</v>
+      </c>
+      <c r="F18">
+        <v>52.181710894781091</v>
+      </c>
+      <c r="G18">
+        <v>55.974542078075267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19">
+        <v>164</v>
+      </c>
+      <c r="C19">
+        <v>172.20469165071995</v>
+      </c>
+      <c r="D19">
+        <v>172.75144004633617</v>
+      </c>
+      <c r="E19">
+        <v>180.39999999442588</v>
+      </c>
+      <c r="F19">
+        <v>169.96018504007139</v>
+      </c>
+      <c r="G19">
+        <v>182.64378039376402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20">
+        <v>164</v>
+      </c>
+      <c r="C20">
+        <v>172.20469165071995</v>
+      </c>
+      <c r="D20">
+        <v>172.20469165267772</v>
+      </c>
+      <c r="E20">
+        <v>172.20469165058611</v>
+      </c>
+      <c r="F20">
+        <v>172.42874615339829</v>
+      </c>
+      <c r="G20">
+        <v>172.02883815287367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>1.0933333333333333</v>
+      </c>
+      <c r="C21">
+        <v>1.1480312776714663</v>
+      </c>
+      <c r="D21">
+        <v>1.1480312776845181</v>
+      </c>
+      <c r="E21">
+        <v>1.1480312776705741</v>
+      </c>
+      <c r="F21">
+        <v>1.1495249743559885</v>
+      </c>
+      <c r="G21">
+        <v>1.1468589210191578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1.009673782335474</v>
+      </c>
+      <c r="D23">
+        <v>1.0096737823300179</v>
+      </c>
+      <c r="E23">
+        <v>1.0096737823239719</v>
+      </c>
+      <c r="F23">
+        <v>1.0523929666142775</v>
+      </c>
+      <c r="G23">
+        <v>0.94786525646597253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1.0031749912777612</v>
+      </c>
+      <c r="D24">
+        <v>1.0031749912758545</v>
+      </c>
+      <c r="E24">
+        <v>1.0031749912739683</v>
+      </c>
+      <c r="F24">
+        <v>1.0169567691057517</v>
+      </c>
+      <c r="G24">
+        <v>0.98252451264995777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.95760221751519581</v>
+      </c>
+      <c r="D25">
+        <v>0.95760221755176367</v>
+      </c>
+      <c r="E25">
+        <v>0.95760221756790975</v>
+      </c>
+      <c r="F25">
+        <v>1.0317274045552081</v>
+      </c>
+      <c r="G25">
+        <v>0.92542187860705039</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1.0533624393235435</v>
+      </c>
+      <c r="D26">
+        <v>1.0533624393068366</v>
+      </c>
+      <c r="E26">
+        <v>1.0533624392625762</v>
+      </c>
+      <c r="F26">
+        <v>1.0692230514855281</v>
+      </c>
+      <c r="G26">
+        <v>0.96621122177448859</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27">
+        <v>164</v>
+      </c>
+      <c r="C27">
+        <v>172.75144004470056</v>
+      </c>
+      <c r="D27">
+        <v>172.75144004633617</v>
+      </c>
+      <c r="E27">
+        <v>172.75144004391314</v>
+      </c>
+      <c r="F27">
+        <v>175.35258058911575</v>
+      </c>
+      <c r="G27">
+        <v>169.02255036789066</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA46F24-F233-430F-8251-B777E1D305D5}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2326,19 +2958,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.0533624393223964</v>
+        <v>1.0363877164159934</v>
       </c>
       <c r="D2">
-        <v>1.0533624393076026</v>
+        <v>1.0363877163707826</v>
       </c>
       <c r="E2">
-        <v>1.0533624392983827</v>
+        <v>1.0363877163440884</v>
       </c>
       <c r="F2">
-        <v>1.0692230525392665</v>
+        <v>1.019624477737967</v>
       </c>
       <c r="G2">
-        <v>1.0306253077634344</v>
+        <v>1.0682942220014657</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2349,19 +2981,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.0432700717339818</v>
+        <v>1.0432700717765628</v>
       </c>
       <c r="D3">
-        <v>1.0432700717206651</v>
+        <v>1.0432700717215022</v>
       </c>
       <c r="E3">
-        <v>1.043270071718168</v>
+        <v>1.0432700716683327</v>
       </c>
       <c r="F3">
-        <v>1.0159922067315308</v>
+        <v>1.0675789736310193</v>
       </c>
       <c r="G3">
-        <v>1.0873120422296021</v>
+        <v>0.99500526524801314</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2372,19 +3004,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1.0500286076528291</v>
+        <v>1.0387958255232288</v>
       </c>
       <c r="D4">
-        <v>1.0500286076372356</v>
+        <v>1.0387958254741989</v>
       </c>
       <c r="E4">
-        <v>1.0500286076315015</v>
+        <v>1.0387958254390572</v>
       </c>
       <c r="F4">
-        <v>1.0513947937746249</v>
+        <v>1.0361893620037979</v>
       </c>
       <c r="G4">
-        <v>1.0489563308826293</v>
+        <v>1.0420004625145436</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2395,19 +3027,19 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.99683505738742828</v>
+        <v>1.0023235600640814</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1.0442749417809107</v>
+        <v>1.0613788472823071</v>
       </c>
       <c r="F5">
-        <v>0.96924826808406228</v>
+        <v>1.1362130503366883</v>
       </c>
       <c r="G5">
-        <v>1.080588241014147</v>
+        <v>1.0168399930513876</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2418,19 +3050,19 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1.006478222756964</v>
+        <v>0.99571132501722914</v>
       </c>
       <c r="D6">
-        <v>1.0096737823300179</v>
+        <v>0.99340309327606224</v>
       </c>
       <c r="E6">
-        <v>1.0543770302540776</v>
+        <v>1.0543770300718067</v>
       </c>
       <c r="F6">
-        <v>1.0200300602347367</v>
+        <v>1.0851755857677472</v>
       </c>
       <c r="G6">
-        <v>1.0242520502029886</v>
+        <v>1.0917372271452674</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2444,16 +3076,16 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1.0031749912758545</v>
+        <v>0.9976818263563586</v>
       </c>
       <c r="E7">
-        <v>1.0475905056086889</v>
+        <v>1.0589183868286272</v>
       </c>
       <c r="F7">
-        <v>0.98568358717211357</v>
+        <v>1.1180491525357026</v>
       </c>
       <c r="G7">
-        <v>1.0617044348776998</v>
+        <v>1.0424988551880285</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2464,10 +3096,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.95457146145108884</v>
+        <v>0.94435984116129768</v>
       </c>
       <c r="D8">
-        <v>0.95760221755176367</v>
+        <v>0.94217065124599342</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2487,19 +3119,19 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1.0500286076528458</v>
+        <v>1.0387958255234089</v>
       </c>
       <c r="D9">
-        <v>1.0533624393068366</v>
+        <v>1.0363877163706223</v>
       </c>
       <c r="E9">
-        <v>1.0999999999351249</v>
+        <v>1.0999999994203249</v>
       </c>
       <c r="F9">
-        <v>1.0363425908479043</v>
+        <v>1.1585106377976897</v>
       </c>
       <c r="G9">
-        <v>1.0440764845854245</v>
+        <v>1.1711502493765573</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2507,22 +3139,22 @@
         <v>165</v>
       </c>
       <c r="B10">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C10">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D10">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E10">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F10">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G10">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2553,22 +3185,22 @@
         <v>167</v>
       </c>
       <c r="B12">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C12">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D12">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E12">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F12">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="G12">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2576,22 +3208,22 @@
         <v>168</v>
       </c>
       <c r="B13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C13">
-        <v>52.213747091206962</v>
+        <v>31.841365430736488</v>
       </c>
       <c r="D13">
-        <v>52.213747089924226</v>
+        <v>31.84136542602463</v>
       </c>
       <c r="E13">
-        <v>52.213747088526816</v>
+        <v>31.841365415536767</v>
       </c>
       <c r="F13">
-        <v>52.868087335139379</v>
+        <v>30.987628643211458</v>
       </c>
       <c r="G13">
-        <v>53.047059029882369</v>
+        <v>31.198499786803925</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2602,19 +3234,19 @@
         <v>50</v>
       </c>
       <c r="C14">
-        <v>47.467042807627351</v>
+        <v>48.244493065449426</v>
       </c>
       <c r="D14">
-        <v>47.46704280902668</v>
+        <v>48.244493069732918</v>
       </c>
       <c r="E14">
-        <v>47.467042810551135</v>
+        <v>48.244493079267343</v>
       </c>
       <c r="F14">
-        <v>46.762927451330512</v>
+        <v>49.037661510429018</v>
       </c>
       <c r="G14">
-        <v>46.573667250728739</v>
+        <v>48.838524040436795</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2625,19 +3257,19 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>25.305048727435071</v>
+        <v>25.305048730005584</v>
       </c>
       <c r="D15">
-        <v>25.305048726675256</v>
+        <v>25.305048726677036</v>
       </c>
       <c r="E15">
-        <v>25.305048725847506</v>
+        <v>25.3050487192682</v>
       </c>
       <c r="F15">
-        <v>24.480721438762444</v>
+        <v>26.044214056358804</v>
       </c>
       <c r="G15">
-        <v>24.582049170514459</v>
+        <v>26.201693451486413</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2648,19 +3280,19 @@
         <v>30</v>
       </c>
       <c r="C16">
-        <v>28.755737188715777</v>
+        <v>28.755737186378955</v>
       </c>
       <c r="D16">
-        <v>28.755737189406524</v>
+        <v>28.755737189404904</v>
       </c>
       <c r="E16">
-        <v>28.755737190159014</v>
+        <v>28.755737196140213</v>
       </c>
       <c r="F16">
-        <v>29.527785568878645</v>
+        <v>28.100965591766641</v>
       </c>
       <c r="G16">
-        <v>29.43037403561884</v>
+        <v>27.965768552577323</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -2668,22 +3300,22 @@
         <v>172</v>
       </c>
       <c r="B17">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C17">
-        <v>110.3492490405403</v>
+        <v>99.768182635147326</v>
       </c>
       <c r="D17">
-        <v>110.34924904034398</v>
+        <v>99.768182635635839</v>
       </c>
       <c r="E17">
-        <v>110.34924904012642</v>
+        <v>99.768182637088472</v>
       </c>
       <c r="F17">
-        <v>111.86524460134066</v>
+        <v>98.401365149245521</v>
       </c>
       <c r="G17">
-        <v>108.07769639007446</v>
+        <v>102.52339230478557</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -2694,19 +3326,19 @@
         <v>54</v>
       </c>
       <c r="C18">
-        <v>53.652427622403614</v>
+        <v>54.232585934539976</v>
       </c>
       <c r="D18">
-        <v>53.652427622598076</v>
+        <v>54.232585934048203</v>
       </c>
       <c r="E18">
-        <v>53.652427622813583</v>
+        <v>54.232585932585913</v>
       </c>
       <c r="F18">
-        <v>52.181710894781091</v>
+        <v>55.635839055654536</v>
       </c>
       <c r="G18">
-        <v>55.974542078075267</v>
+        <v>51.564549399269403</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2714,22 +3346,22 @@
         <v>174</v>
       </c>
       <c r="B19">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C19">
-        <v>172.20469165071995</v>
+        <v>159.97455711734904</v>
       </c>
       <c r="D19">
-        <v>172.75144004633617</v>
+        <v>159.60370832107745</v>
       </c>
       <c r="E19">
-        <v>180.39999999442588</v>
+        <v>169.39999994784262</v>
       </c>
       <c r="F19">
-        <v>169.96018504007139</v>
+        <v>178.41063825195459</v>
       </c>
       <c r="G19">
-        <v>182.64378039376402</v>
+        <v>167.28778054862835</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2737,22 +3369,22 @@
         <v>175</v>
       </c>
       <c r="B20">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C20">
-        <v>172.20469165071995</v>
+        <v>159.97455711734904</v>
       </c>
       <c r="D20">
-        <v>172.20469165267772</v>
+        <v>159.97455712305333</v>
       </c>
       <c r="E20">
-        <v>172.20469165058611</v>
+        <v>159.97455710933642</v>
       </c>
       <c r="F20">
-        <v>172.42874615339829</v>
+        <v>159.57316174098833</v>
       </c>
       <c r="G20">
-        <v>172.02883815287367</v>
+        <v>160.46807122723965</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2760,22 +3392,22 @@
         <v>58</v>
       </c>
       <c r="B21">
-        <v>1.0933333333333333</v>
+        <v>1.0266666666666666</v>
       </c>
       <c r="C21">
-        <v>1.1480312776714663</v>
+        <v>1.0664970474489937</v>
       </c>
       <c r="D21">
-        <v>1.1480312776845181</v>
+        <v>1.0664970474870221</v>
       </c>
       <c r="E21">
-        <v>1.1480312776705741</v>
+        <v>1.0664970473955762</v>
       </c>
       <c r="F21">
-        <v>1.1495249743559885</v>
+        <v>1.0638210782732556</v>
       </c>
       <c r="G21">
-        <v>1.1468589210191578</v>
+        <v>1.0697871415149309</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2809,19 +3441,19 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1.009673782335474</v>
+        <v>0.99340309326219023</v>
       </c>
       <c r="D23">
-        <v>1.0096737823300179</v>
+        <v>0.99340309327606224</v>
       </c>
       <c r="E23">
-        <v>1.0096737823239719</v>
+        <v>0.99340309331731191</v>
       </c>
       <c r="F23">
-        <v>1.0523929666142775</v>
+        <v>0.95508107871686787</v>
       </c>
       <c r="G23">
-        <v>0.94786525646597253</v>
+        <v>1.0736568531978412</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2832,19 +3464,19 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>1.0031749912777612</v>
+        <v>0.9976818263516295</v>
       </c>
       <c r="D24">
-        <v>1.0031749912758545</v>
+        <v>0.9976818263563586</v>
       </c>
       <c r="E24">
-        <v>1.0031749912739683</v>
+        <v>0.9976818263714412</v>
       </c>
       <c r="F24">
-        <v>1.0169567691057517</v>
+        <v>0.98401365149291031</v>
       </c>
       <c r="G24">
-        <v>0.98252451264995777</v>
+        <v>1.0252339230478558</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2855,19 +3487,19 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0.95760221751519581</v>
+        <v>0.94217065106293829</v>
       </c>
       <c r="D25">
-        <v>0.95760221755176367</v>
+        <v>0.94217065124599342</v>
       </c>
       <c r="E25">
-        <v>0.95760221756790975</v>
+        <v>0.94217065146957701</v>
       </c>
       <c r="F25">
-        <v>1.0317274045552081</v>
+        <v>0.88011662927447898</v>
       </c>
       <c r="G25">
-        <v>0.92542187860705039</v>
+        <v>0.98343889582779564</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2878,19 +3510,19 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>1.0533624393235435</v>
+        <v>1.0363877164146433</v>
       </c>
       <c r="D26">
-        <v>1.0533624393068366</v>
+        <v>1.0363877163706223</v>
       </c>
       <c r="E26">
-        <v>1.0533624392625762</v>
+        <v>1.0363877160703818</v>
       </c>
       <c r="F26">
-        <v>1.0692230514855281</v>
+        <v>1.0196244775171295</v>
       </c>
       <c r="G26">
-        <v>0.96621122177448859</v>
+        <v>1.151754708095329</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2898,22 +3530,22 @@
         <v>181</v>
       </c>
       <c r="B27">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C27">
-        <v>172.75144004470056</v>
+        <v>159.60370831462987</v>
       </c>
       <c r="D27">
-        <v>172.75144004633617</v>
+        <v>159.60370832107745</v>
       </c>
       <c r="E27">
-        <v>172.75144004391314</v>
+        <v>159.6037083098052</v>
       </c>
       <c r="F27">
-        <v>175.35258058911575</v>
+        <v>157.02216956501869</v>
       </c>
       <c r="G27">
-        <v>169.02255036789066</v>
+        <v>164.51731018822565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try things for prices in Demand
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F4175F-36E1-4122-AAD0-3252ACA3B1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8ED1DD-6AD1-4768-9648-D97791C9EEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2316" windowWidth="17280" windowHeight="9072" firstSheet="9" activeTab="11" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9072" firstSheet="11" activeTab="12" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
     <sheet name="two_by_two_PriceinIntput" sheetId="13" r:id="rId11"/>
     <sheet name="two_by_two_PriceinOutput" sheetId="14" r:id="rId12"/>
+    <sheet name="two_by_two_PriceinDem" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="187">
   <si>
     <t>X.L</t>
   </si>
@@ -582,6 +583,21 @@
   </si>
   <si>
     <t>RA/PX</t>
+  </si>
+  <si>
+    <t>DY</t>
+  </si>
+  <si>
+    <t>eRA=.5</t>
+  </si>
+  <si>
+    <t>pr_Ud=2</t>
+  </si>
+  <si>
+    <t>prU2,eRA.6</t>
+  </si>
+  <si>
+    <t>prU.5,eRA.6</t>
   </si>
 </sst>
 </file>
@@ -2926,7 +2942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA46F24-F233-430F-8251-B777E1D305D5}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3546,6 +3562,828 @@
       </c>
       <c r="G27">
         <v>164.51731018822565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A14072-42EB-4D8D-A8E8-16263FAFBB19}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0363877164248041</v>
+      </c>
+      <c r="D2">
+        <v>1.0365519507521972</v>
+      </c>
+      <c r="E2">
+        <v>1.0595609099982088</v>
+      </c>
+      <c r="F2">
+        <v>1.0633532225145439</v>
+      </c>
+      <c r="G2">
+        <v>0.99833470833445848</v>
+      </c>
+      <c r="H2">
+        <v>0.98248710709607423</v>
+      </c>
+      <c r="I2">
+        <v>0.94048657015713999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0432700717660239</v>
+      </c>
+      <c r="D3">
+        <v>1.0430251457731119</v>
+      </c>
+      <c r="E3">
+        <v>1.0087067867541124</v>
+      </c>
+      <c r="F3">
+        <v>1.0030495908339756</v>
+      </c>
+      <c r="G3">
+        <v>1.1000067470042523</v>
+      </c>
+      <c r="H3">
+        <v>1.122931737696433</v>
+      </c>
+      <c r="I3">
+        <v>1.1855074833626025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0388246300487494</v>
+      </c>
+      <c r="D4">
+        <v>1.0389899529717939</v>
+      </c>
+      <c r="E4">
+        <v>1.0621536850625561</v>
+      </c>
+      <c r="F4">
+        <v>1.0659719353994179</v>
+      </c>
+      <c r="G4">
+        <v>1.0005254867593421</v>
+      </c>
+      <c r="H4">
+        <v>0.99843756359281499</v>
+      </c>
+      <c r="I4">
+        <v>0.99193526198210002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0023513532505028</v>
+      </c>
+      <c r="D5">
+        <v>1.0023520310092886</v>
+      </c>
+      <c r="E5">
+        <v>1.0024470278582813</v>
+      </c>
+      <c r="F5">
+        <v>1.0024626933265708</v>
+      </c>
+      <c r="G5">
+        <v>1.0021944327932055</v>
+      </c>
+      <c r="H5">
+        <v>1.0162347743614695</v>
+      </c>
+      <c r="I5">
+        <v>1.054704334391892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.99573893485424703</v>
+      </c>
+      <c r="D6">
+        <v>0.99573771069529127</v>
+      </c>
+      <c r="E6">
+        <v>0.99556615181885155</v>
+      </c>
+      <c r="F6">
+        <v>0.99553786527941868</v>
+      </c>
+      <c r="G6">
+        <v>0.99602242514969408</v>
+      </c>
+      <c r="H6">
+        <v>0.97114380037066672</v>
+      </c>
+      <c r="I6">
+        <v>0.90770374205596749</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.94438602708152408</v>
+      </c>
+      <c r="D8">
+        <v>0.94437046939986447</v>
+      </c>
+      <c r="E8">
+        <v>0.94219250114219932</v>
+      </c>
+      <c r="F8">
+        <v>0.94183384552627059</v>
+      </c>
+      <c r="G8">
+        <v>0.9479952509302686</v>
+      </c>
+      <c r="H8">
+        <v>0.89903690333116493</v>
+      </c>
+      <c r="I8">
+        <v>0.84467427236056358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0388246300416317</v>
+      </c>
+      <c r="D9">
+        <v>1.0388360220635884</v>
+      </c>
+      <c r="E9">
+        <v>1.0404339284158413</v>
+      </c>
+      <c r="F9">
+        <v>1.0406976527852307</v>
+      </c>
+      <c r="G9">
+        <v>1.0361901997164102</v>
+      </c>
+      <c r="H9">
+        <v>1.0329715504842176</v>
+      </c>
+      <c r="I9">
+        <v>0.96149717694622527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>80</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>54</v>
+      </c>
+      <c r="G11">
+        <v>54</v>
+      </c>
+      <c r="H11">
+        <v>54</v>
+      </c>
+      <c r="I11">
+        <v>54.000000000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12">
+        <v>124</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>123.99999999999999</v>
+      </c>
+      <c r="E12">
+        <v>124</v>
+      </c>
+      <c r="F12">
+        <v>124</v>
+      </c>
+      <c r="G12">
+        <v>124</v>
+      </c>
+      <c r="H12">
+        <v>124</v>
+      </c>
+      <c r="I12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>31.841365430850797</v>
+      </c>
+      <c r="D13">
+        <v>31.841911518828791</v>
+      </c>
+      <c r="E13">
+        <v>31.918541910798012</v>
+      </c>
+      <c r="F13">
+        <v>31.931195659031214</v>
+      </c>
+      <c r="G13">
+        <v>31.715172575173078</v>
+      </c>
+      <c r="H13">
+        <v>30.827982414866039</v>
+      </c>
+      <c r="I13">
+        <v>30.648734246825121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>48.244493065345502</v>
+      </c>
+      <c r="D14">
+        <v>48.243996628540472</v>
+      </c>
+      <c r="E14">
+        <v>48.174468386692752</v>
+      </c>
+      <c r="F14">
+        <v>48.16301308279445</v>
+      </c>
+      <c r="G14">
+        <v>48.359578823666638</v>
+      </c>
+      <c r="H14">
+        <v>49.189872358276297</v>
+      </c>
+      <c r="I14">
+        <v>49.36228226730212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>25.305048730086334</v>
+      </c>
+      <c r="D15">
+        <v>25.305434497175867</v>
+      </c>
+      <c r="E15">
+        <v>25.359560402662385</v>
+      </c>
+      <c r="F15">
+        <v>25.368496662333634</v>
+      </c>
+      <c r="G15">
+        <v>25.215883919305377</v>
+      </c>
+      <c r="H15">
+        <v>25.924910448641455</v>
+      </c>
+      <c r="I15">
+        <v>25.790876462309562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.755737186305545</v>
+      </c>
+      <c r="D16">
+        <v>28.755386493763073</v>
+      </c>
+      <c r="E16">
+        <v>28.706277005056187</v>
+      </c>
+      <c r="F16">
+        <v>28.698187104056096</v>
+      </c>
+      <c r="G16">
+        <v>28.837054010514596</v>
+      </c>
+      <c r="H16">
+        <v>28.204372131496182</v>
+      </c>
+      <c r="I16">
+        <v>28.321572766511753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>79.812333011330708</v>
+      </c>
+      <c r="D17">
+        <v>79.812279044731554</v>
+      </c>
+      <c r="E17">
+        <v>79.804715637612503</v>
+      </c>
+      <c r="F17">
+        <v>79.803468530612463</v>
+      </c>
+      <c r="G17">
+        <v>79.824829775826657</v>
+      </c>
+      <c r="H17">
+        <v>78.721966634399251</v>
+      </c>
+      <c r="I17">
+        <v>75.850641162032716</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>44.188289178863421</v>
+      </c>
+      <c r="D18">
+        <v>44.18834350389114</v>
+      </c>
+      <c r="E18">
+        <v>44.195958168740567</v>
+      </c>
+      <c r="F18">
+        <v>44.197213922797879</v>
+      </c>
+      <c r="G18">
+        <v>44.175712201847752</v>
+      </c>
+      <c r="H18">
+        <v>45.307399360636374</v>
+      </c>
+      <c r="I18">
+        <v>48.473965635901294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19">
+        <v>134</v>
+      </c>
+      <c r="C19">
+        <v>139.20250041197306</v>
+      </c>
+      <c r="D19">
+        <v>139.202487647439</v>
+      </c>
+      <c r="E19">
+        <v>139.20094884111393</v>
+      </c>
+      <c r="F19">
+        <v>139.20074264707893</v>
+      </c>
+      <c r="G19">
+        <v>139.20613388257078</v>
+      </c>
+      <c r="H19">
+        <v>138.76352763367868</v>
+      </c>
+      <c r="I19">
+        <v>137.46365821827374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20">
+        <v>124</v>
+      </c>
+      <c r="C20">
+        <v>128.81425411257209</v>
+      </c>
+      <c r="D20">
+        <v>128.83475414329422</v>
+      </c>
+      <c r="E20">
+        <v>131.70705694774205</v>
+      </c>
+      <c r="F20">
+        <v>132.18051998952777</v>
+      </c>
+      <c r="G20">
+        <v>124.06516035720092</v>
+      </c>
+      <c r="H20">
+        <v>123.80625788538022</v>
+      </c>
+      <c r="I20">
+        <v>122.99997248577242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>10.432700716801408</v>
+      </c>
+      <c r="D21">
+        <v>10.412112941775911</v>
+      </c>
+      <c r="E21">
+        <v>7.5272666509210593</v>
+      </c>
+      <c r="F21">
+        <v>7.0516882404877128</v>
+      </c>
+      <c r="G21">
+        <v>15.201438384376063</v>
+      </c>
+      <c r="H21">
+        <v>15.401704405248296</v>
+      </c>
+      <c r="I21">
+        <v>15.934368299221509</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.0391557242667655</v>
+      </c>
+      <c r="D22">
+        <v>1.0391553971951093</v>
+      </c>
+      <c r="E22">
+        <v>1.0454956618531788</v>
+      </c>
+      <c r="F22">
+        <v>1.046614299839608</v>
+      </c>
+      <c r="G22">
+        <v>1.0534806670456223</v>
+      </c>
+      <c r="H22">
+        <v>1.0530112713727526</v>
+      </c>
+      <c r="I22">
+        <v>1.0506793942727906</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.99340309326184617</v>
+      </c>
+      <c r="D24">
+        <v>0.99340120026759737</v>
+      </c>
+      <c r="E24">
+        <v>0.99313592055419553</v>
+      </c>
+      <c r="F24">
+        <v>0.99309218378573993</v>
+      </c>
+      <c r="G24">
+        <v>0.9938415067560199</v>
+      </c>
+      <c r="H24">
+        <v>0.95562937312479324</v>
+      </c>
+      <c r="I24">
+        <v>0.86062388525151912</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.99765416264179452</v>
+      </c>
+      <c r="D25">
+        <v>0.997653488059559</v>
+      </c>
+      <c r="E25">
+        <v>0.99755894547015678</v>
+      </c>
+      <c r="F25">
+        <v>0.9975433566326557</v>
+      </c>
+      <c r="G25">
+        <v>0.99781037219784841</v>
+      </c>
+      <c r="H25">
+        <v>0.98402458292999251</v>
+      </c>
+      <c r="I25">
+        <v>0.94813301452540932</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.94217065105862896</v>
+      </c>
+      <c r="D26">
+        <v>0.94215449281721775</v>
+      </c>
+      <c r="E26">
+        <v>0.93989255786930181</v>
+      </c>
+      <c r="F26">
+        <v>0.93952009565651817</v>
+      </c>
+      <c r="G26">
+        <v>0.94591949417252408</v>
+      </c>
+      <c r="H26">
+        <v>0.88467441383912149</v>
+      </c>
+      <c r="I26">
+        <v>0.80086356414527782</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1.0363877164158561</v>
+      </c>
+      <c r="D27">
+        <v>1.0363983809336559</v>
+      </c>
+      <c r="E27">
+        <v>1.0378941724618791</v>
+      </c>
+      <c r="F27">
+        <v>1.0381410297991052</v>
+      </c>
+      <c r="G27">
+        <v>1.0339213288467941</v>
+      </c>
+      <c r="H27">
+        <v>1.0164693991437799</v>
+      </c>
+      <c r="I27">
+        <v>0.91162721683569548</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28">
+        <v>134</v>
+      </c>
+      <c r="C28">
+        <v>138.87595398615105</v>
+      </c>
+      <c r="D28">
+        <v>138.87584734803519</v>
+      </c>
+      <c r="E28">
+        <v>138.86115173438685</v>
+      </c>
+      <c r="F28">
+        <v>138.85877606592558</v>
+      </c>
+      <c r="G28">
+        <v>138.90132426159147</v>
+      </c>
+      <c r="H28">
+        <v>136.54672240562513</v>
+      </c>
+      <c r="I28">
+        <v>130.33383265418243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 123 example and test
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A974A849-D1F9-453D-AF47-780ADA818E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46DA6A1-3EB7-408B-AA10-986167F4266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9435" yWindow="-16200" windowWidth="19200" windowHeight="15750" firstSheet="12" activeTab="13" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="13" activeTab="16" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -28,6 +28,8 @@
     <sheet name="two_by_two_AuxinOutput" sheetId="15" r:id="rId13"/>
     <sheet name="two_by_two_PriceinIntput" sheetId="17" r:id="rId14"/>
     <sheet name="two_by_two_PriceinOutput" sheetId="16" r:id="rId15"/>
+    <sheet name="123" sheetId="18" r:id="rId16"/>
+    <sheet name="The123" sheetId="19" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="253">
   <si>
     <t>X.L</t>
   </si>
@@ -729,6 +731,75 @@
   </si>
   <si>
     <t>RA/PX</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>YD</t>
+  </si>
+  <si>
+    <t>YX</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>CAHH</t>
+  </si>
+  <si>
+    <t>CAG</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>PAA</t>
+  </si>
+  <si>
+    <t>PMM</t>
+  </si>
+  <si>
+    <t>PFXX</t>
+  </si>
+  <si>
+    <t>PFXM</t>
+  </si>
+  <si>
+    <t>PXX</t>
+  </si>
+  <si>
+    <t>TAU_LS</t>
+  </si>
+  <si>
+    <t>TAU_TL</t>
+  </si>
+  <si>
+    <t>UR</t>
+  </si>
+  <si>
+    <t>Lump Sum F</t>
+  </si>
+  <si>
+    <t>Wage Tax F</t>
+  </si>
+  <si>
+    <t>Lump Sum R</t>
+  </si>
+  <si>
+    <t>Wage Tax R</t>
   </si>
 </sst>
 </file>
@@ -3924,7 +3995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC547432-C581-4E9F-9FCD-4D8C390A851F}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5175,6 +5246,1246 @@
       </c>
       <c r="G27">
         <v>164.51731018822565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00B6D55-9979-44CC-A647-170B2883E40E}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D2">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E2">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F2">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0070022344597493</v>
+      </c>
+      <c r="D3">
+        <v>1.0647664462896207</v>
+      </c>
+      <c r="E3">
+        <v>1.0393745275783166</v>
+      </c>
+      <c r="F3">
+        <v>1.1815614680983193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0347436346818013</v>
+      </c>
+      <c r="D4">
+        <v>1.0851741633351151</v>
+      </c>
+      <c r="E4">
+        <v>1.068007736401561</v>
+      </c>
+      <c r="F4">
+        <v>1.1324982091819222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.028143742844291</v>
+      </c>
+      <c r="D5">
+        <v>1.0058066298219333</v>
+      </c>
+      <c r="E5">
+        <v>1.0611956758123793</v>
+      </c>
+      <c r="F5">
+        <v>1.1514791966109479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.98238636886087427</v>
+      </c>
+      <c r="D6">
+        <v>1.0386148317802442</v>
+      </c>
+      <c r="E6">
+        <v>1.0139673311008839</v>
+      </c>
+      <c r="F6">
+        <v>1.1514791966109481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7">
+        <v>35.583000148600661</v>
+      </c>
+      <c r="C7">
+        <v>34.956254142742267</v>
+      </c>
+      <c r="D7">
+        <v>36.957031549322892</v>
+      </c>
+      <c r="E7">
+        <v>36.07999954124368</v>
+      </c>
+      <c r="F7">
+        <v>40.973084253007229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8">
+        <v>414.18399999999997</v>
+      </c>
+      <c r="C8">
+        <v>414.18399999999997</v>
+      </c>
+      <c r="D8">
+        <v>427.49885183400283</v>
+      </c>
+      <c r="E8">
+        <v>427.49885184051067</v>
+      </c>
+      <c r="F8">
+        <v>441.241739054047</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D9">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E9">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F9">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.0033052715012549</v>
+      </c>
+      <c r="D10">
+        <v>0.99522228336449259</v>
+      </c>
+      <c r="E10">
+        <v>1.0033052714923001</v>
+      </c>
+      <c r="F10">
+        <v>0.93669213122219863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1.0068124561470682</v>
+      </c>
+      <c r="D11">
+        <v>0.99958436023046626</v>
+      </c>
+      <c r="E11">
+        <v>1.0068124561223903</v>
+      </c>
+      <c r="F11">
+        <v>0.9472408940241287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1.1372188172900564</v>
+      </c>
+      <c r="D12">
+        <v>1.1296637752263212</v>
+      </c>
+      <c r="E12">
+        <v>1.1372188172832904</v>
+      </c>
+      <c r="F12">
+        <v>1.0749730402403119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1.1866382802313127</v>
+      </c>
+      <c r="D13">
+        <v>1.1763622839379608</v>
+      </c>
+      <c r="E13">
+        <v>1.1866382802221103</v>
+      </c>
+      <c r="F13">
+        <v>1.1019746385409115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D14">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E14">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F14">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15">
+        <v>218.30799991386419</v>
+      </c>
+      <c r="C15">
+        <v>198.42331840632735</v>
+      </c>
+      <c r="D15">
+        <v>198.50418277240834</v>
+      </c>
+      <c r="E15">
+        <v>198.42331836459431</v>
+      </c>
+      <c r="F15">
+        <v>199.12799494751147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16">
+        <v>106.38600008706536</v>
+      </c>
+      <c r="C16">
+        <v>125.82581157214146</v>
+      </c>
+      <c r="D16">
+        <v>125.74927232940006</v>
+      </c>
+      <c r="E16">
+        <v>125.82581161163735</v>
+      </c>
+      <c r="F16">
+        <v>125.15817095937935</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17">
+        <v>143.8619999197816</v>
+      </c>
+      <c r="C17">
+        <v>143.38806357451722</v>
+      </c>
+      <c r="D17">
+        <v>144.55263150907996</v>
+      </c>
+      <c r="E17">
+        <v>143.38806352119306</v>
+      </c>
+      <c r="F17">
+        <v>153.58514842255414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18">
+        <v>163.32000008552319</v>
+      </c>
+      <c r="C18">
+        <v>163.82689661913358</v>
+      </c>
+      <c r="D18">
+        <v>162.58710861084509</v>
+      </c>
+      <c r="E18">
+        <v>163.82689667634895</v>
+      </c>
+      <c r="F18">
+        <v>153.5909766849224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19">
+        <v>218.30799867558773</v>
+      </c>
+      <c r="C19">
+        <v>197.73211986280506</v>
+      </c>
+      <c r="D19">
+        <v>197.63793222090473</v>
+      </c>
+      <c r="E19">
+        <v>197.73211991140732</v>
+      </c>
+      <c r="F19">
+        <v>196.91044500939407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20">
+        <v>144.70100117343947</v>
+      </c>
+      <c r="C20">
+        <v>163.44325015529287</v>
+      </c>
+      <c r="D20">
+        <v>163.53144811235779</v>
+      </c>
+      <c r="E20">
+        <v>163.4432501097871</v>
+      </c>
+      <c r="F20">
+        <v>164.21342752105784</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21">
+        <v>291.69399999999996</v>
+      </c>
+      <c r="C21">
+        <v>294.51199292542111</v>
+      </c>
+      <c r="D21">
+        <v>291.52206936434942</v>
+      </c>
+      <c r="E21">
+        <v>294.51199291362445</v>
+      </c>
+      <c r="F21">
+        <v>269.87003753576283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22">
+        <v>35.583000148600661</v>
+      </c>
+      <c r="C22">
+        <v>35.582999979199407</v>
+      </c>
+      <c r="D22">
+        <v>35.582999990455043</v>
+      </c>
+      <c r="E22">
+        <v>35.582999998699101</v>
+      </c>
+      <c r="F22">
+        <v>35.582999999999878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23">
+        <v>122.48999999999998</v>
+      </c>
+      <c r="C23">
+        <v>121.4416109430898</v>
+      </c>
+      <c r="D23">
+        <v>123.99968652971447</v>
+      </c>
+      <c r="E23">
+        <v>121.44161095256374</v>
+      </c>
+      <c r="F23">
+        <v>113.32554285571725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="C24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="D24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="E24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="F24">
+        <v>413.65300000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="C25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="D25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="E25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="F25">
+        <v>144.70099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26">
+        <v>106.386</v>
+      </c>
+      <c r="C26">
+        <v>106.386</v>
+      </c>
+      <c r="D26">
+        <v>106.386</v>
+      </c>
+      <c r="E26">
+        <v>106.386</v>
+      </c>
+      <c r="F26">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="C27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="D27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="E27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="F27">
+        <v>144.70099999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28">
+        <v>106.386</v>
+      </c>
+      <c r="C28">
+        <v>106.386</v>
+      </c>
+      <c r="D28">
+        <v>106.386</v>
+      </c>
+      <c r="E28">
+        <v>106.386</v>
+      </c>
+      <c r="F28">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29">
+        <v>0.38090042610962555</v>
+      </c>
+      <c r="E29">
+        <v>0.38090042654947287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30">
+        <v>9.09035579940565E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.11902313383111375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31">
+        <v>0.10012595030539158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C32">
+        <v>1.0041857009029531</v>
+      </c>
+      <c r="D32">
+        <v>1.0031868420707351</v>
+      </c>
+      <c r="E32">
+        <v>1.0041857008984718</v>
+      </c>
+      <c r="F32">
+        <v>0.92518199735257778</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3694F3D5-F7B8-4C96-9882-2E0CBB4FB167}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D2">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E2">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F2">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0070022344597493</v>
+      </c>
+      <c r="D3">
+        <v>1.0647664462896207</v>
+      </c>
+      <c r="E3">
+        <v>1.0393745275783166</v>
+      </c>
+      <c r="F3">
+        <v>1.1815614680983193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0347436346818013</v>
+      </c>
+      <c r="D4">
+        <v>1.0851741633351151</v>
+      </c>
+      <c r="E4">
+        <v>1.068007736401561</v>
+      </c>
+      <c r="F4">
+        <v>1.1324982091819222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.028143742844291</v>
+      </c>
+      <c r="D5">
+        <v>1.0058066298219333</v>
+      </c>
+      <c r="E5">
+        <v>1.0611956758123793</v>
+      </c>
+      <c r="F5">
+        <v>1.1514791966109479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.98238636886087427</v>
+      </c>
+      <c r="D6">
+        <v>1.0386148317802442</v>
+      </c>
+      <c r="E6">
+        <v>1.0139673311008839</v>
+      </c>
+      <c r="F6">
+        <v>1.1514791966109481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7">
+        <v>35.583000148600661</v>
+      </c>
+      <c r="C7">
+        <v>34.956254142742267</v>
+      </c>
+      <c r="D7">
+        <v>36.957031549322892</v>
+      </c>
+      <c r="E7">
+        <v>36.07999954124368</v>
+      </c>
+      <c r="F7">
+        <v>40.973084253007229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8">
+        <v>414.18399999999997</v>
+      </c>
+      <c r="C8">
+        <v>414.18399999999997</v>
+      </c>
+      <c r="D8">
+        <v>427.49885183400283</v>
+      </c>
+      <c r="E8">
+        <v>427.49885184051067</v>
+      </c>
+      <c r="F8">
+        <v>441.241739054047</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D9">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E9">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F9">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.0033052715012549</v>
+      </c>
+      <c r="D10">
+        <v>0.99522228336449259</v>
+      </c>
+      <c r="E10">
+        <v>1.0033052714923001</v>
+      </c>
+      <c r="F10">
+        <v>0.93669213122219863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1.0068124561470682</v>
+      </c>
+      <c r="D11">
+        <v>0.99958436023046626</v>
+      </c>
+      <c r="E11">
+        <v>1.0068124561223903</v>
+      </c>
+      <c r="F11">
+        <v>0.9472408940241287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1.1372188172900564</v>
+      </c>
+      <c r="D12">
+        <v>1.1296637752263212</v>
+      </c>
+      <c r="E12">
+        <v>1.1372188172832904</v>
+      </c>
+      <c r="F12">
+        <v>1.0749730402403119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1.1866382802313127</v>
+      </c>
+      <c r="D13">
+        <v>1.1763622839379608</v>
+      </c>
+      <c r="E13">
+        <v>1.1866382802221103</v>
+      </c>
+      <c r="F13">
+        <v>1.1019746385409115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D14">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E14">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F14">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15">
+        <v>218.30799991386419</v>
+      </c>
+      <c r="C15">
+        <v>198.42331840632735</v>
+      </c>
+      <c r="D15">
+        <v>198.50418277240834</v>
+      </c>
+      <c r="E15">
+        <v>198.42331836459431</v>
+      </c>
+      <c r="F15">
+        <v>199.12799494751147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16">
+        <v>106.38600008706536</v>
+      </c>
+      <c r="C16">
+        <v>125.82581157214146</v>
+      </c>
+      <c r="D16">
+        <v>125.74927232940006</v>
+      </c>
+      <c r="E16">
+        <v>125.82581161163735</v>
+      </c>
+      <c r="F16">
+        <v>125.15817095937935</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17">
+        <v>143.8619999197816</v>
+      </c>
+      <c r="C17">
+        <v>143.38806357451722</v>
+      </c>
+      <c r="D17">
+        <v>144.55263150907996</v>
+      </c>
+      <c r="E17">
+        <v>143.38806352119306</v>
+      </c>
+      <c r="F17">
+        <v>153.58514842255414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18">
+        <v>163.32000008552319</v>
+      </c>
+      <c r="C18">
+        <v>163.82689661913358</v>
+      </c>
+      <c r="D18">
+        <v>162.58710861084509</v>
+      </c>
+      <c r="E18">
+        <v>163.82689667634895</v>
+      </c>
+      <c r="F18">
+        <v>153.5909766849224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19">
+        <v>218.30799867558773</v>
+      </c>
+      <c r="C19">
+        <v>197.73211986280506</v>
+      </c>
+      <c r="D19">
+        <v>197.63793222090473</v>
+      </c>
+      <c r="E19">
+        <v>197.73211991140732</v>
+      </c>
+      <c r="F19">
+        <v>196.91044500939407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20">
+        <v>144.70100117343947</v>
+      </c>
+      <c r="C20">
+        <v>163.44325015529287</v>
+      </c>
+      <c r="D20">
+        <v>163.53144811235779</v>
+      </c>
+      <c r="E20">
+        <v>163.4432501097871</v>
+      </c>
+      <c r="F20">
+        <v>164.21342752105784</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21">
+        <v>291.69399999999996</v>
+      </c>
+      <c r="C21">
+        <v>294.51199292542111</v>
+      </c>
+      <c r="D21">
+        <v>291.52206936434942</v>
+      </c>
+      <c r="E21">
+        <v>294.51199291362445</v>
+      </c>
+      <c r="F21">
+        <v>269.87003753576283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22">
+        <v>35.583000148600661</v>
+      </c>
+      <c r="C22">
+        <v>35.582999979199407</v>
+      </c>
+      <c r="D22">
+        <v>35.582999990455043</v>
+      </c>
+      <c r="E22">
+        <v>35.582999998699101</v>
+      </c>
+      <c r="F22">
+        <v>35.582999999999878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23">
+        <v>122.48999999999998</v>
+      </c>
+      <c r="C23">
+        <v>121.4416109430898</v>
+      </c>
+      <c r="D23">
+        <v>123.99968652971447</v>
+      </c>
+      <c r="E23">
+        <v>121.44161095256374</v>
+      </c>
+      <c r="F23">
+        <v>113.32554285571725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="C24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="D24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="E24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="F24">
+        <v>413.65300000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="C25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="D25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="E25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="F25">
+        <v>144.70099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26">
+        <v>106.386</v>
+      </c>
+      <c r="C26">
+        <v>106.386</v>
+      </c>
+      <c r="D26">
+        <v>106.386</v>
+      </c>
+      <c r="E26">
+        <v>106.386</v>
+      </c>
+      <c r="F26">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="C27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="D27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="E27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="F27">
+        <v>144.70099999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28">
+        <v>106.386</v>
+      </c>
+      <c r="C28">
+        <v>106.386</v>
+      </c>
+      <c r="D28">
+        <v>106.386</v>
+      </c>
+      <c r="E28">
+        <v>106.386</v>
+      </c>
+      <c r="F28">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29">
+        <v>0.38090042610962555</v>
+      </c>
+      <c r="E29">
+        <v>0.38090042654947287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30">
+        <v>9.09035579940565E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.11902313383111375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31">
+        <v>0.10012595030539158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C32">
+        <v>1.0041857009029531</v>
+      </c>
+      <c r="D32">
+        <v>1.0031868420707351</v>
+      </c>
+      <c r="E32">
+        <v>1.0041857008984718</v>
+      </c>
+      <c r="F32">
+        <v>0.92518199735257778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for nested 123
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46DA6A1-3EB7-408B-AA10-986167F4266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBA0310-A59A-4C5C-8242-EE447E93296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="13" activeTab="16" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="14" activeTab="17" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="two_by_two_PriceinOutput" sheetId="16" r:id="rId15"/>
     <sheet name="123" sheetId="18" r:id="rId16"/>
     <sheet name="The123" sheetId="19" r:id="rId17"/>
+    <sheet name="The123Nested" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="255">
   <si>
     <t>X.L</t>
   </si>
@@ -800,6 +801,12 @@
   </si>
   <si>
     <t>Wage Tax R</t>
+  </si>
+  <si>
+    <t>PDHHC</t>
+  </si>
+  <si>
+    <t>PMHHC</t>
   </si>
 </sst>
 </file>
@@ -5877,6 +5884,626 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3694F3D5-F7B8-4C96-9882-2E0CBB4FB167}">
   <dimension ref="A1:F32"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D2">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E2">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F2">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0070022344597493</v>
+      </c>
+      <c r="D3">
+        <v>1.0647664462896207</v>
+      </c>
+      <c r="E3">
+        <v>1.0393745275783166</v>
+      </c>
+      <c r="F3">
+        <v>1.1815614680983193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0347436346818013</v>
+      </c>
+      <c r="D4">
+        <v>1.0851741633351151</v>
+      </c>
+      <c r="E4">
+        <v>1.068007736401561</v>
+      </c>
+      <c r="F4">
+        <v>1.1324982091819222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.028143742844291</v>
+      </c>
+      <c r="D5">
+        <v>1.0058066298219333</v>
+      </c>
+      <c r="E5">
+        <v>1.0611956758123793</v>
+      </c>
+      <c r="F5">
+        <v>1.1514791966109479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.98238636886087427</v>
+      </c>
+      <c r="D6">
+        <v>1.0386148317802442</v>
+      </c>
+      <c r="E6">
+        <v>1.0139673311008839</v>
+      </c>
+      <c r="F6">
+        <v>1.1514791966109481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7">
+        <v>35.583000148600661</v>
+      </c>
+      <c r="C7">
+        <v>34.956254142742267</v>
+      </c>
+      <c r="D7">
+        <v>36.957031549322892</v>
+      </c>
+      <c r="E7">
+        <v>36.07999954124368</v>
+      </c>
+      <c r="F7">
+        <v>40.973084253007229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8">
+        <v>414.18399999999997</v>
+      </c>
+      <c r="C8">
+        <v>414.18399999999997</v>
+      </c>
+      <c r="D8">
+        <v>427.49885183400283</v>
+      </c>
+      <c r="E8">
+        <v>427.49885184051067</v>
+      </c>
+      <c r="F8">
+        <v>441.241739054047</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D9">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E9">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F9">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.0033052715012549</v>
+      </c>
+      <c r="D10">
+        <v>0.99522228336449259</v>
+      </c>
+      <c r="E10">
+        <v>1.0033052714923001</v>
+      </c>
+      <c r="F10">
+        <v>0.93669213122219863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1.0068124561470682</v>
+      </c>
+      <c r="D11">
+        <v>0.99958436023046626</v>
+      </c>
+      <c r="E11">
+        <v>1.0068124561223903</v>
+      </c>
+      <c r="F11">
+        <v>0.9472408940241287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1.1372188172900564</v>
+      </c>
+      <c r="D12">
+        <v>1.1296637752263212</v>
+      </c>
+      <c r="E12">
+        <v>1.1372188172832904</v>
+      </c>
+      <c r="F12">
+        <v>1.0749730402403119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1.1866382802313127</v>
+      </c>
+      <c r="D13">
+        <v>1.1763622839379608</v>
+      </c>
+      <c r="E13">
+        <v>1.1866382802221103</v>
+      </c>
+      <c r="F13">
+        <v>1.1019746385409115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.0755261761982433</v>
+      </c>
+      <c r="D14">
+        <v>1.1369322976554099</v>
+      </c>
+      <c r="E14">
+        <v>1.1101013217020295</v>
+      </c>
+      <c r="F14">
+        <v>1.2591699016841988</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15">
+        <v>218.30799991386419</v>
+      </c>
+      <c r="C15">
+        <v>198.42331840632735</v>
+      </c>
+      <c r="D15">
+        <v>198.50418277240834</v>
+      </c>
+      <c r="E15">
+        <v>198.42331836459431</v>
+      </c>
+      <c r="F15">
+        <v>199.12799494751147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16">
+        <v>106.38600008706536</v>
+      </c>
+      <c r="C16">
+        <v>125.82581157214146</v>
+      </c>
+      <c r="D16">
+        <v>125.74927232940006</v>
+      </c>
+      <c r="E16">
+        <v>125.82581161163735</v>
+      </c>
+      <c r="F16">
+        <v>125.15817095937935</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17">
+        <v>143.8619999197816</v>
+      </c>
+      <c r="C17">
+        <v>143.38806357451722</v>
+      </c>
+      <c r="D17">
+        <v>144.55263150907996</v>
+      </c>
+      <c r="E17">
+        <v>143.38806352119306</v>
+      </c>
+      <c r="F17">
+        <v>153.58514842255414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18">
+        <v>163.32000008552319</v>
+      </c>
+      <c r="C18">
+        <v>163.82689661913358</v>
+      </c>
+      <c r="D18">
+        <v>162.58710861084509</v>
+      </c>
+      <c r="E18">
+        <v>163.82689667634895</v>
+      </c>
+      <c r="F18">
+        <v>153.5909766849224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19">
+        <v>218.30799867558773</v>
+      </c>
+      <c r="C19">
+        <v>197.73211986280506</v>
+      </c>
+      <c r="D19">
+        <v>197.63793222090473</v>
+      </c>
+      <c r="E19">
+        <v>197.73211991140732</v>
+      </c>
+      <c r="F19">
+        <v>196.91044500939407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20">
+        <v>144.70100117343947</v>
+      </c>
+      <c r="C20">
+        <v>163.44325015529287</v>
+      </c>
+      <c r="D20">
+        <v>163.53144811235779</v>
+      </c>
+      <c r="E20">
+        <v>163.4432501097871</v>
+      </c>
+      <c r="F20">
+        <v>164.21342752105784</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21">
+        <v>291.69399999999996</v>
+      </c>
+      <c r="C21">
+        <v>294.51199292542111</v>
+      </c>
+      <c r="D21">
+        <v>291.52206936434942</v>
+      </c>
+      <c r="E21">
+        <v>294.51199291362445</v>
+      </c>
+      <c r="F21">
+        <v>269.87003753576283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22">
+        <v>35.583000148600661</v>
+      </c>
+      <c r="C22">
+        <v>35.582999979199407</v>
+      </c>
+      <c r="D22">
+        <v>35.582999990455043</v>
+      </c>
+      <c r="E22">
+        <v>35.582999998699101</v>
+      </c>
+      <c r="F22">
+        <v>35.582999999999878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23">
+        <v>122.48999999999998</v>
+      </c>
+      <c r="C23">
+        <v>121.4416109430898</v>
+      </c>
+      <c r="D23">
+        <v>123.99968652971447</v>
+      </c>
+      <c r="E23">
+        <v>121.44161095256374</v>
+      </c>
+      <c r="F23">
+        <v>113.32554285571725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="C24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="D24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="E24">
+        <v>413.65300000000002</v>
+      </c>
+      <c r="F24">
+        <v>413.65300000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="C25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="D25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="E25">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="F25">
+        <v>144.70099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26">
+        <v>106.386</v>
+      </c>
+      <c r="C26">
+        <v>106.386</v>
+      </c>
+      <c r="D26">
+        <v>106.386</v>
+      </c>
+      <c r="E26">
+        <v>106.386</v>
+      </c>
+      <c r="F26">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="C27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="D27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="E27">
+        <v>144.70099999999999</v>
+      </c>
+      <c r="F27">
+        <v>144.70099999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28">
+        <v>106.386</v>
+      </c>
+      <c r="C28">
+        <v>106.386</v>
+      </c>
+      <c r="D28">
+        <v>106.386</v>
+      </c>
+      <c r="E28">
+        <v>106.386</v>
+      </c>
+      <c r="F28">
+        <v>106.386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29">
+        <v>0.38090042610962555</v>
+      </c>
+      <c r="E29">
+        <v>0.38090042654947287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30">
+        <v>9.09035579940565E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.11902313383111375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31">
+        <v>0.10012595030539158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32">
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="C32">
+        <v>1.0041857009029531</v>
+      </c>
+      <c r="D32">
+        <v>1.0031868420707351</v>
+      </c>
+      <c r="E32">
+        <v>1.0041857008984718</v>
+      </c>
+      <c r="F32">
+        <v>0.92518199735257778</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC21389E-4BBB-4228-B023-E87E0DD3496F}">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5906,16 +6533,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.0755261761982433</v>
+        <v>1.0574822307388072</v>
       </c>
       <c r="D2">
-        <v>1.1369322976554099</v>
+        <v>1.1208854073780947</v>
       </c>
       <c r="E2">
-        <v>1.1101013217020295</v>
+        <v>1.093845224084691</v>
       </c>
       <c r="F2">
-        <v>1.2591699016841988</v>
+        <v>1.2159780481743121</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5926,16 +6553,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.0070022344597493</v>
+        <v>1.021386644660353</v>
       </c>
       <c r="D3">
-        <v>1.0647664462896207</v>
+        <v>1.0829933415282671</v>
       </c>
       <c r="E3">
-        <v>1.0393745275783166</v>
+        <v>1.0565084411957109</v>
       </c>
       <c r="F3">
-        <v>1.1815614680983193</v>
+        <v>1.1770495671905572</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5946,16 +6573,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1.0347436346818013</v>
+        <v>1.0378734693729745</v>
       </c>
       <c r="D4">
-        <v>1.0851741633351151</v>
+        <v>1.0908152401097198</v>
       </c>
       <c r="E4">
-        <v>1.068007736401561</v>
+        <v>1.0735621882843041</v>
       </c>
       <c r="F4">
-        <v>1.1324982091819222</v>
+        <v>1.1308395339573694</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5966,16 +6593,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1.028143742844291</v>
+        <v>1.0297727391968678</v>
       </c>
       <c r="D5">
-        <v>1.0058066298219333</v>
+        <v>1.0063236931541308</v>
       </c>
       <c r="E5">
-        <v>1.0611956758123793</v>
+        <v>1.0651829032082272</v>
       </c>
       <c r="F5">
-        <v>1.1514791966109479</v>
+        <v>1.1300212683742732</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5986,16 +6613,16 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.98238636886087427</v>
+        <v>0.98163793480205663</v>
       </c>
       <c r="D6">
-        <v>1.0386148317802442</v>
+        <v>1.0406731332718653</v>
       </c>
       <c r="E6">
-        <v>1.0139673311008839</v>
+        <v>1.0153929168191886</v>
       </c>
       <c r="F6">
-        <v>1.1514791966109481</v>
+        <v>1.1300212683742734</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -6003,19 +6630,19 @@
         <v>142</v>
       </c>
       <c r="B7">
-        <v>35.583000148600661</v>
+        <v>35.583000010682497</v>
       </c>
       <c r="C7">
-        <v>34.956254142742267</v>
+        <v>34.929622632672398</v>
       </c>
       <c r="D7">
-        <v>36.957031549322892</v>
+        <v>37.030272059403188</v>
       </c>
       <c r="E7">
-        <v>36.07999954124368</v>
+        <v>36.130726157936543</v>
       </c>
       <c r="F7">
-        <v>40.973084253007229</v>
+        <v>40.20954679256181</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -6029,13 +6656,13 @@
         <v>414.18399999999997</v>
       </c>
       <c r="D8">
-        <v>427.49885183400283</v>
+        <v>428.42629130657741</v>
       </c>
       <c r="E8">
-        <v>427.49885184051067</v>
+        <v>428.42629132493204</v>
       </c>
       <c r="F8">
-        <v>441.241739054047</v>
+        <v>443.1583236012043</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -6046,16 +6673,16 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1.0755261761982433</v>
+        <v>1.0574822307388074</v>
       </c>
       <c r="D9">
-        <v>1.1369322976554099</v>
+        <v>1.1208854073780949</v>
       </c>
       <c r="E9">
-        <v>1.1101013217020295</v>
+        <v>1.093845224084691</v>
       </c>
       <c r="F9">
-        <v>1.2591699016841988</v>
+        <v>1.2159780481743123</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -6066,16 +6693,16 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1.0033052715012549</v>
+        <v>1.0040490717945083</v>
       </c>
       <c r="D10">
-        <v>0.99522228336449259</v>
+        <v>0.99535920768400654</v>
       </c>
       <c r="E10">
-        <v>1.0033052714923001</v>
+        <v>1.0040490717929504</v>
       </c>
       <c r="F10">
-        <v>0.93669213122219863</v>
+        <v>0.95006363418230078</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -6086,16 +6713,16 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1.0068124561470682</v>
+        <v>0.99999999999534794</v>
       </c>
       <c r="D11">
-        <v>0.99958436023046626</v>
+        <v>1.0000000000678941</v>
       </c>
       <c r="E11">
-        <v>1.0068124561223903</v>
+        <v>0.99999999998997346</v>
       </c>
       <c r="F11">
-        <v>0.9472408940241287</v>
+        <v>0.99999999999999978</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -6106,16 +6733,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1.1372188172900564</v>
+        <v>1.0733288863492836</v>
       </c>
       <c r="D12">
-        <v>1.1296637752263212</v>
+        <v>1.0656392915983663</v>
       </c>
       <c r="E12">
-        <v>1.1372188172832904</v>
+        <v>1.0733288863487671</v>
       </c>
       <c r="F12">
-        <v>1.0749730402403119</v>
+        <v>1.0255960162277276</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -6126,16 +6753,16 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1.1866382802313127</v>
+        <v>1.0997383413572057</v>
       </c>
       <c r="D13">
-        <v>1.1763622839379608</v>
+        <v>1.0892793331225463</v>
       </c>
       <c r="E13">
-        <v>1.1866382802221103</v>
+        <v>1.0997383413565034</v>
       </c>
       <c r="F13">
-        <v>1.1019746385409115</v>
+        <v>1.0348144412250524</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -6146,16 +6773,16 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1.0755261761982433</v>
+        <v>0.93693736312063669</v>
       </c>
       <c r="D14">
-        <v>1.1369322976554099</v>
+        <v>0.99311306367343266</v>
       </c>
       <c r="E14">
-        <v>1.1101013217020295</v>
+        <v>0.96915525398473434</v>
       </c>
       <c r="F14">
-        <v>1.2591699016841988</v>
+        <v>1.077365872401518</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -6166,16 +6793,16 @@
         <v>218.30799991386419</v>
       </c>
       <c r="C15">
-        <v>198.42331840632735</v>
+        <v>208.10018361533406</v>
       </c>
       <c r="D15">
-        <v>198.50418277240834</v>
+        <v>208.20318131403775</v>
       </c>
       <c r="E15">
-        <v>198.42331836459431</v>
+        <v>208.10018361109925</v>
       </c>
       <c r="F15">
-        <v>199.12799494751147</v>
+        <v>208.76394986753999</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -6186,16 +6813,16 @@
         <v>106.38600008706536</v>
       </c>
       <c r="C16">
-        <v>125.82581157214146</v>
+        <v>116.52494531022273</v>
       </c>
       <c r="D16">
-        <v>125.74927232940006</v>
+        <v>116.42437246751885</v>
       </c>
       <c r="E16">
-        <v>125.82581161163735</v>
+        <v>116.52494531435714</v>
       </c>
       <c r="F16">
-        <v>125.15817095937935</v>
+        <v>115.87620574375572</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -6206,16 +6833,16 @@
         <v>143.8619999197816</v>
       </c>
       <c r="C17">
-        <v>143.38806357451722</v>
+        <v>143.28184154070982</v>
       </c>
       <c r="D17">
-        <v>144.55263150907996</v>
+        <v>144.53274644770912</v>
       </c>
       <c r="E17">
-        <v>143.38806352119306</v>
+        <v>143.28184153681914</v>
       </c>
       <c r="F17">
-        <v>153.58514842255414</v>
+        <v>151.42354135448923</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -6226,16 +6853,16 @@
         <v>163.32000008552319</v>
       </c>
       <c r="C18">
-        <v>163.82689661913358</v>
+        <v>163.94095191372836</v>
       </c>
       <c r="D18">
-        <v>162.58710861084509</v>
+        <v>162.60811549096849</v>
       </c>
       <c r="E18">
-        <v>163.82689667634895</v>
+        <v>163.94095191790899</v>
       </c>
       <c r="F18">
-        <v>153.5909766849224</v>
+        <v>155.64913036779717</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -6243,19 +6870,19 @@
         <v>236</v>
       </c>
       <c r="B19">
-        <v>218.30799867558773</v>
+        <v>51.445328799999999</v>
       </c>
       <c r="C19">
-        <v>197.73211986280506</v>
+        <v>43.892526476037276</v>
       </c>
       <c r="D19">
-        <v>197.63793222090473</v>
+        <v>43.863185803202192</v>
       </c>
       <c r="E19">
-        <v>197.73211991140732</v>
+        <v>43.892526477243379</v>
       </c>
       <c r="F19">
-        <v>196.91044500939407</v>
+        <v>43.70321723812647</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -6263,229 +6890,249 @@
         <v>237</v>
       </c>
       <c r="B20">
-        <v>144.70100117343947</v>
+        <v>38.486671200000004</v>
       </c>
       <c r="C20">
-        <v>163.44325015529287</v>
+        <v>46.373881647352938</v>
       </c>
       <c r="D20">
-        <v>163.53144811235779</v>
+        <v>46.40587232379157</v>
       </c>
       <c r="E20">
-        <v>163.4432501097871</v>
+        <v>46.373881646038136</v>
       </c>
       <c r="F20">
-        <v>164.21342752105784</v>
+        <v>46.580480256246055</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="B21">
-        <v>291.69399999999996</v>
+        <v>166.86267100000001</v>
       </c>
       <c r="C21">
-        <v>294.51199292542111</v>
+        <v>165.05026971742276</v>
       </c>
       <c r="D21">
-        <v>291.52206936434942</v>
+        <v>163.37376779290139</v>
       </c>
       <c r="E21">
-        <v>294.51199291362445</v>
+        <v>165.05026971788689</v>
       </c>
       <c r="F21">
-        <v>269.87003753576283</v>
+        <v>154.63581965928029</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="B22">
-        <v>35.583000148600661</v>
+        <v>124.831329</v>
       </c>
       <c r="C22">
-        <v>35.582999979199407</v>
+        <v>128.92004541555693</v>
       </c>
       <c r="D22">
-        <v>35.582999990455043</v>
+        <v>127.63220550400438</v>
       </c>
       <c r="E22">
-        <v>35.582999998699101</v>
+        <v>128.92004541501973</v>
       </c>
       <c r="F22">
-        <v>35.582999999999878</v>
+        <v>120.91780992203401</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B23">
-        <v>122.48999999999998</v>
+        <v>35.583000010682497</v>
       </c>
       <c r="C23">
-        <v>121.4416109430898</v>
+        <v>35.582999998584832</v>
       </c>
       <c r="D23">
-        <v>123.99968652971447</v>
+        <v>35.58299995982447</v>
       </c>
       <c r="E23">
-        <v>121.44161095256374</v>
+        <v>35.582999998778163</v>
       </c>
       <c r="F23">
-        <v>113.32554285571725</v>
+        <v>35.583000000000034</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24">
-        <v>413.65300000000002</v>
+        <v>122.49</v>
       </c>
       <c r="C24">
-        <v>413.65300000000002</v>
+        <v>121.20523939719774</v>
       </c>
       <c r="D24">
-        <v>413.65300000000002</v>
+        <v>123.95651502786397</v>
       </c>
       <c r="E24">
-        <v>413.65300000000002</v>
+        <v>121.20523939823869</v>
       </c>
       <c r="F24">
-        <v>413.65300000000002</v>
+        <v>115.81337527552746</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B25">
-        <v>144.70099999999999</v>
+        <v>121.959</v>
       </c>
       <c r="C25">
-        <v>144.70099999999999</v>
+        <v>121.959</v>
       </c>
       <c r="D25">
-        <v>144.70099999999999</v>
+        <v>121.959</v>
       </c>
       <c r="E25">
-        <v>144.70099999999999</v>
+        <v>121.959</v>
       </c>
       <c r="F25">
-        <v>144.70099999999999</v>
+        <v>121.959</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B26">
-        <v>106.386</v>
+        <v>163.31800000000001</v>
       </c>
       <c r="C26">
-        <v>106.386</v>
+        <v>163.31800000000001</v>
       </c>
       <c r="D26">
-        <v>106.386</v>
+        <v>163.31800000000001</v>
       </c>
       <c r="E26">
-        <v>106.386</v>
+        <v>163.31800000000001</v>
       </c>
       <c r="F26">
-        <v>106.386</v>
+        <v>163.31800000000001</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B27">
-        <v>144.70099999999999</v>
+        <v>106.386</v>
       </c>
       <c r="C27">
-        <v>144.70099999999999</v>
+        <v>106.386</v>
       </c>
       <c r="D27">
-        <v>144.70099999999999</v>
+        <v>106.386</v>
       </c>
       <c r="E27">
-        <v>144.70099999999999</v>
+        <v>106.386</v>
       </c>
       <c r="F27">
-        <v>144.70099999999999</v>
+        <v>106.386</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B28">
-        <v>106.386</v>
+        <v>144.70099999999999</v>
       </c>
       <c r="C28">
-        <v>106.386</v>
+        <v>144.70099999999999</v>
       </c>
       <c r="D28">
-        <v>106.386</v>
+        <v>144.70099999999999</v>
       </c>
       <c r="E28">
-        <v>106.386</v>
+        <v>144.70099999999999</v>
       </c>
       <c r="F28">
-        <v>106.386</v>
+        <v>144.70099999999999</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="B29">
+        <v>106.386</v>
       </c>
       <c r="C29">
-        <v>0.38090042610962555</v>
+        <v>106.386</v>
+      </c>
+      <c r="D29">
+        <v>106.386</v>
       </c>
       <c r="E29">
-        <v>0.38090042654947287</v>
+        <v>106.386</v>
+      </c>
+      <c r="F29">
+        <v>106.386</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D30">
-        <v>9.09035579940565E-2</v>
-      </c>
-      <c r="F30">
-        <v>0.11902313383111375</v>
+        <v>246</v>
+      </c>
+      <c r="C30">
+        <v>0.40774249079963698</v>
+      </c>
+      <c r="E30">
+        <v>0.40774249079698927</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="D31">
+        <v>9.5814285352822548E-2</v>
       </c>
       <c r="F31">
-        <v>0.10012595030539158</v>
+        <v>0.10751460657981388</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32">
+        <v>7.7394234876065712E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B32">
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="C32">
-        <v>1.0041857009029531</v>
-      </c>
-      <c r="D32">
-        <v>1.0031868420707351</v>
-      </c>
-      <c r="E32">
-        <v>1.0041857008984718</v>
-      </c>
-      <c r="F32">
-        <v>0.92518199735257778</v>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1.001987242980396</v>
+      </c>
+      <c r="D33">
+        <v>1.0015004288360945</v>
+      </c>
+      <c r="E33">
+        <v>1.0019872429829184</v>
+      </c>
+      <c r="F33">
+        <v>0.94459176904078701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert commit to b4 demand prices
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F4175F-36E1-4122-AAD0-3252ACA3B1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8ED1DD-6AD1-4768-9648-D97791C9EEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2316" windowWidth="17280" windowHeight="9072" firstSheet="9" activeTab="11" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9072" firstSheet="11" activeTab="12" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="SimpleDemNest" sheetId="12" r:id="rId10"/>
     <sheet name="two_by_two_PriceinIntput" sheetId="13" r:id="rId11"/>
     <sheet name="two_by_two_PriceinOutput" sheetId="14" r:id="rId12"/>
+    <sheet name="two_by_two_PriceinDem" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="187">
   <si>
     <t>X.L</t>
   </si>
@@ -582,6 +583,21 @@
   </si>
   <si>
     <t>RA/PX</t>
+  </si>
+  <si>
+    <t>DY</t>
+  </si>
+  <si>
+    <t>eRA=.5</t>
+  </si>
+  <si>
+    <t>pr_Ud=2</t>
+  </si>
+  <si>
+    <t>prU2,eRA.6</t>
+  </si>
+  <si>
+    <t>prU.5,eRA.6</t>
   </si>
 </sst>
 </file>
@@ -2926,7 +2942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA46F24-F233-430F-8251-B777E1D305D5}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3546,6 +3562,828 @@
       </c>
       <c r="G27">
         <v>164.51731018822565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A14072-42EB-4D8D-A8E8-16263FAFBB19}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0363877164248041</v>
+      </c>
+      <c r="D2">
+        <v>1.0365519507521972</v>
+      </c>
+      <c r="E2">
+        <v>1.0595609099982088</v>
+      </c>
+      <c r="F2">
+        <v>1.0633532225145439</v>
+      </c>
+      <c r="G2">
+        <v>0.99833470833445848</v>
+      </c>
+      <c r="H2">
+        <v>0.98248710709607423</v>
+      </c>
+      <c r="I2">
+        <v>0.94048657015713999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0432700717660239</v>
+      </c>
+      <c r="D3">
+        <v>1.0430251457731119</v>
+      </c>
+      <c r="E3">
+        <v>1.0087067867541124</v>
+      </c>
+      <c r="F3">
+        <v>1.0030495908339756</v>
+      </c>
+      <c r="G3">
+        <v>1.1000067470042523</v>
+      </c>
+      <c r="H3">
+        <v>1.122931737696433</v>
+      </c>
+      <c r="I3">
+        <v>1.1855074833626025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0388246300487494</v>
+      </c>
+      <c r="D4">
+        <v>1.0389899529717939</v>
+      </c>
+      <c r="E4">
+        <v>1.0621536850625561</v>
+      </c>
+      <c r="F4">
+        <v>1.0659719353994179</v>
+      </c>
+      <c r="G4">
+        <v>1.0005254867593421</v>
+      </c>
+      <c r="H4">
+        <v>0.99843756359281499</v>
+      </c>
+      <c r="I4">
+        <v>0.99193526198210002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0023513532505028</v>
+      </c>
+      <c r="D5">
+        <v>1.0023520310092886</v>
+      </c>
+      <c r="E5">
+        <v>1.0024470278582813</v>
+      </c>
+      <c r="F5">
+        <v>1.0024626933265708</v>
+      </c>
+      <c r="G5">
+        <v>1.0021944327932055</v>
+      </c>
+      <c r="H5">
+        <v>1.0162347743614695</v>
+      </c>
+      <c r="I5">
+        <v>1.054704334391892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.99573893485424703</v>
+      </c>
+      <c r="D6">
+        <v>0.99573771069529127</v>
+      </c>
+      <c r="E6">
+        <v>0.99556615181885155</v>
+      </c>
+      <c r="F6">
+        <v>0.99553786527941868</v>
+      </c>
+      <c r="G6">
+        <v>0.99602242514969408</v>
+      </c>
+      <c r="H6">
+        <v>0.97114380037066672</v>
+      </c>
+      <c r="I6">
+        <v>0.90770374205596749</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.94438602708152408</v>
+      </c>
+      <c r="D8">
+        <v>0.94437046939986447</v>
+      </c>
+      <c r="E8">
+        <v>0.94219250114219932</v>
+      </c>
+      <c r="F8">
+        <v>0.94183384552627059</v>
+      </c>
+      <c r="G8">
+        <v>0.9479952509302686</v>
+      </c>
+      <c r="H8">
+        <v>0.89903690333116493</v>
+      </c>
+      <c r="I8">
+        <v>0.84467427236056358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0388246300416317</v>
+      </c>
+      <c r="D9">
+        <v>1.0388360220635884</v>
+      </c>
+      <c r="E9">
+        <v>1.0404339284158413</v>
+      </c>
+      <c r="F9">
+        <v>1.0406976527852307</v>
+      </c>
+      <c r="G9">
+        <v>1.0361901997164102</v>
+      </c>
+      <c r="H9">
+        <v>1.0329715504842176</v>
+      </c>
+      <c r="I9">
+        <v>0.96149717694622527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>80</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>54</v>
+      </c>
+      <c r="G11">
+        <v>54</v>
+      </c>
+      <c r="H11">
+        <v>54</v>
+      </c>
+      <c r="I11">
+        <v>54.000000000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12">
+        <v>124</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>123.99999999999999</v>
+      </c>
+      <c r="E12">
+        <v>124</v>
+      </c>
+      <c r="F12">
+        <v>124</v>
+      </c>
+      <c r="G12">
+        <v>124</v>
+      </c>
+      <c r="H12">
+        <v>124</v>
+      </c>
+      <c r="I12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>31.841365430850797</v>
+      </c>
+      <c r="D13">
+        <v>31.841911518828791</v>
+      </c>
+      <c r="E13">
+        <v>31.918541910798012</v>
+      </c>
+      <c r="F13">
+        <v>31.931195659031214</v>
+      </c>
+      <c r="G13">
+        <v>31.715172575173078</v>
+      </c>
+      <c r="H13">
+        <v>30.827982414866039</v>
+      </c>
+      <c r="I13">
+        <v>30.648734246825121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>48.244493065345502</v>
+      </c>
+      <c r="D14">
+        <v>48.243996628540472</v>
+      </c>
+      <c r="E14">
+        <v>48.174468386692752</v>
+      </c>
+      <c r="F14">
+        <v>48.16301308279445</v>
+      </c>
+      <c r="G14">
+        <v>48.359578823666638</v>
+      </c>
+      <c r="H14">
+        <v>49.189872358276297</v>
+      </c>
+      <c r="I14">
+        <v>49.36228226730212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>25.305048730086334</v>
+      </c>
+      <c r="D15">
+        <v>25.305434497175867</v>
+      </c>
+      <c r="E15">
+        <v>25.359560402662385</v>
+      </c>
+      <c r="F15">
+        <v>25.368496662333634</v>
+      </c>
+      <c r="G15">
+        <v>25.215883919305377</v>
+      </c>
+      <c r="H15">
+        <v>25.924910448641455</v>
+      </c>
+      <c r="I15">
+        <v>25.790876462309562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.755737186305545</v>
+      </c>
+      <c r="D16">
+        <v>28.755386493763073</v>
+      </c>
+      <c r="E16">
+        <v>28.706277005056187</v>
+      </c>
+      <c r="F16">
+        <v>28.698187104056096</v>
+      </c>
+      <c r="G16">
+        <v>28.837054010514596</v>
+      </c>
+      <c r="H16">
+        <v>28.204372131496182</v>
+      </c>
+      <c r="I16">
+        <v>28.321572766511753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>79.812333011330708</v>
+      </c>
+      <c r="D17">
+        <v>79.812279044731554</v>
+      </c>
+      <c r="E17">
+        <v>79.804715637612503</v>
+      </c>
+      <c r="F17">
+        <v>79.803468530612463</v>
+      </c>
+      <c r="G17">
+        <v>79.824829775826657</v>
+      </c>
+      <c r="H17">
+        <v>78.721966634399251</v>
+      </c>
+      <c r="I17">
+        <v>75.850641162032716</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>44.188289178863421</v>
+      </c>
+      <c r="D18">
+        <v>44.18834350389114</v>
+      </c>
+      <c r="E18">
+        <v>44.195958168740567</v>
+      </c>
+      <c r="F18">
+        <v>44.197213922797879</v>
+      </c>
+      <c r="G18">
+        <v>44.175712201847752</v>
+      </c>
+      <c r="H18">
+        <v>45.307399360636374</v>
+      </c>
+      <c r="I18">
+        <v>48.473965635901294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19">
+        <v>134</v>
+      </c>
+      <c r="C19">
+        <v>139.20250041197306</v>
+      </c>
+      <c r="D19">
+        <v>139.202487647439</v>
+      </c>
+      <c r="E19">
+        <v>139.20094884111393</v>
+      </c>
+      <c r="F19">
+        <v>139.20074264707893</v>
+      </c>
+      <c r="G19">
+        <v>139.20613388257078</v>
+      </c>
+      <c r="H19">
+        <v>138.76352763367868</v>
+      </c>
+      <c r="I19">
+        <v>137.46365821827374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20">
+        <v>124</v>
+      </c>
+      <c r="C20">
+        <v>128.81425411257209</v>
+      </c>
+      <c r="D20">
+        <v>128.83475414329422</v>
+      </c>
+      <c r="E20">
+        <v>131.70705694774205</v>
+      </c>
+      <c r="F20">
+        <v>132.18051998952777</v>
+      </c>
+      <c r="G20">
+        <v>124.06516035720092</v>
+      </c>
+      <c r="H20">
+        <v>123.80625788538022</v>
+      </c>
+      <c r="I20">
+        <v>122.99997248577242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>10.432700716801408</v>
+      </c>
+      <c r="D21">
+        <v>10.412112941775911</v>
+      </c>
+      <c r="E21">
+        <v>7.5272666509210593</v>
+      </c>
+      <c r="F21">
+        <v>7.0516882404877128</v>
+      </c>
+      <c r="G21">
+        <v>15.201438384376063</v>
+      </c>
+      <c r="H21">
+        <v>15.401704405248296</v>
+      </c>
+      <c r="I21">
+        <v>15.934368299221509</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.0391557242667655</v>
+      </c>
+      <c r="D22">
+        <v>1.0391553971951093</v>
+      </c>
+      <c r="E22">
+        <v>1.0454956618531788</v>
+      </c>
+      <c r="F22">
+        <v>1.046614299839608</v>
+      </c>
+      <c r="G22">
+        <v>1.0534806670456223</v>
+      </c>
+      <c r="H22">
+        <v>1.0530112713727526</v>
+      </c>
+      <c r="I22">
+        <v>1.0506793942727906</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.99340309326184617</v>
+      </c>
+      <c r="D24">
+        <v>0.99340120026759737</v>
+      </c>
+      <c r="E24">
+        <v>0.99313592055419553</v>
+      </c>
+      <c r="F24">
+        <v>0.99309218378573993</v>
+      </c>
+      <c r="G24">
+        <v>0.9938415067560199</v>
+      </c>
+      <c r="H24">
+        <v>0.95562937312479324</v>
+      </c>
+      <c r="I24">
+        <v>0.86062388525151912</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.99765416264179452</v>
+      </c>
+      <c r="D25">
+        <v>0.997653488059559</v>
+      </c>
+      <c r="E25">
+        <v>0.99755894547015678</v>
+      </c>
+      <c r="F25">
+        <v>0.9975433566326557</v>
+      </c>
+      <c r="G25">
+        <v>0.99781037219784841</v>
+      </c>
+      <c r="H25">
+        <v>0.98402458292999251</v>
+      </c>
+      <c r="I25">
+        <v>0.94813301452540932</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.94217065105862896</v>
+      </c>
+      <c r="D26">
+        <v>0.94215449281721775</v>
+      </c>
+      <c r="E26">
+        <v>0.93989255786930181</v>
+      </c>
+      <c r="F26">
+        <v>0.93952009565651817</v>
+      </c>
+      <c r="G26">
+        <v>0.94591949417252408</v>
+      </c>
+      <c r="H26">
+        <v>0.88467441383912149</v>
+      </c>
+      <c r="I26">
+        <v>0.80086356414527782</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1.0363877164158561</v>
+      </c>
+      <c r="D27">
+        <v>1.0363983809336559</v>
+      </c>
+      <c r="E27">
+        <v>1.0378941724618791</v>
+      </c>
+      <c r="F27">
+        <v>1.0381410297991052</v>
+      </c>
+      <c r="G27">
+        <v>1.0339213288467941</v>
+      </c>
+      <c r="H27">
+        <v>1.0164693991437799</v>
+      </c>
+      <c r="I27">
+        <v>0.91162721683569548</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28">
+        <v>134</v>
+      </c>
+      <c r="C28">
+        <v>138.87595398615105</v>
+      </c>
+      <c r="D28">
+        <v>138.87584734803519</v>
+      </c>
+      <c r="E28">
+        <v>138.86115173438685</v>
+      </c>
+      <c r="F28">
+        <v>138.85877606592558</v>
+      </c>
+      <c r="G28">
+        <v>138.90132426159147</v>
+      </c>
+      <c r="H28">
+        <v>136.54672240562513</v>
+      </c>
+      <c r="I28">
+        <v>130.33383265418243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-add xlsx rest values (after merge conflict)
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8ED1DD-6AD1-4768-9648-D97791C9EEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE8EB6-CB6F-4316-B0D7-9D83F1478608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9072" firstSheet="11" activeTab="12" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="13" activeTab="15" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="two_by_two_PriceinIntput" sheetId="13" r:id="rId11"/>
     <sheet name="two_by_two_PriceinOutput" sheetId="14" r:id="rId12"/>
     <sheet name="two_by_two_PriceinDem" sheetId="15" r:id="rId13"/>
+    <sheet name="TwoxTwowAuxDem" sheetId="16" r:id="rId14"/>
+    <sheet name="two_by_two_AuxinInput" sheetId="17" r:id="rId15"/>
+    <sheet name="two_by_two_AuxinOutput" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="235">
   <si>
     <t>X.L</t>
   </si>
@@ -598,6 +601,150 @@
   </si>
   <si>
     <t>prU.5,eRA.6</t>
+  </si>
+  <si>
+    <t>SXX.L</t>
+  </si>
+  <si>
+    <t>SYY.L</t>
+  </si>
+  <si>
+    <t>SWW.L</t>
+  </si>
+  <si>
+    <t>DKX.L</t>
+  </si>
+  <si>
+    <t>DLX.L</t>
+  </si>
+  <si>
+    <t>DLY.L</t>
+  </si>
+  <si>
+    <t>DKY.L</t>
+  </si>
+  <si>
+    <t>DXW.L</t>
+  </si>
+  <si>
+    <t>DYW.L</t>
+  </si>
+  <si>
+    <t>CWCONS.L</t>
+  </si>
+  <si>
+    <t>UnEmp=.1</t>
+  </si>
+  <si>
+    <t>TKX=0.25</t>
+  </si>
+  <si>
+    <t>&amp;TY=.5</t>
+  </si>
+  <si>
+    <t>TY=0.5</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>PKS</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t>TAU</t>
+  </si>
+  <si>
+    <t>SXX</t>
+  </si>
+  <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>SWW</t>
+  </si>
+  <si>
+    <t>SLSTL</t>
+  </si>
+  <si>
+    <t>SKSTK</t>
+  </si>
+  <si>
+    <t>DLSX</t>
+  </si>
+  <si>
+    <t>DKSX</t>
+  </si>
+  <si>
+    <t>DLSY</t>
+  </si>
+  <si>
+    <t>DKSY</t>
+  </si>
+  <si>
+    <t>DXW</t>
+  </si>
+  <si>
+    <t>DYW</t>
+  </si>
+  <si>
+    <t>DLW</t>
+  </si>
+  <si>
+    <t>DLTL</t>
+  </si>
+  <si>
+    <t>DKTK</t>
+  </si>
+  <si>
+    <t>CONS</t>
+  </si>
+  <si>
+    <t>CWCONS</t>
+  </si>
+  <si>
+    <t>L.15,K.25</t>
+  </si>
+  <si>
+    <t>L.1,K.3</t>
+  </si>
+  <si>
+    <t>L.05,K.35</t>
+  </si>
+  <si>
+    <t>L.0,K.4</t>
+  </si>
+  <si>
+    <t>L-.05,K.45</t>
+  </si>
+  <si>
+    <t>SHAREX</t>
+  </si>
+  <si>
+    <t>MARKUP</t>
+  </si>
+  <si>
+    <t>DLX</t>
+  </si>
+  <si>
+    <t>DKX</t>
+  </si>
+  <si>
+    <t>S.5,M.FX=0</t>
+  </si>
+  <si>
+    <t>S.FX.2,M.5</t>
   </si>
 </sst>
 </file>
@@ -3573,7 +3720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A14072-42EB-4D8D-A8E8-16263FAFBB19}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4384,6 +4531,1485 @@
       </c>
       <c r="I28">
         <v>130.33383265418243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19CE32B-082C-4B1E-A36F-A00937C7D439}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D2">
+        <v>1.0371252977019936</v>
+      </c>
+      <c r="E2">
+        <v>0.98447088030257324</v>
+      </c>
+      <c r="F2">
+        <v>1.0069367675479344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="D3">
+        <v>1.053409075564238</v>
+      </c>
+      <c r="E3">
+        <v>0.44661553192056858</v>
+      </c>
+      <c r="F3">
+        <v>0.41177381270347702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D4">
+        <v>1.0452354763862961</v>
+      </c>
+      <c r="E4">
+        <v>0.66308369432539305</v>
+      </c>
+      <c r="F4">
+        <v>0.64391784561311827</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D6">
+        <v>0.9845418287728368</v>
+      </c>
+      <c r="E6">
+        <v>2.2042916262845966</v>
+      </c>
+      <c r="F6">
+        <v>2.4453637808572513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D7">
+        <v>0.99224081188632707</v>
+      </c>
+      <c r="E7">
+        <v>1.4846856995121664</v>
+      </c>
+      <c r="F7">
+        <v>1.5637658970763419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.0499999999722391</v>
+      </c>
+      <c r="D8">
+        <v>0.99224081188632707</v>
+      </c>
+      <c r="E8">
+        <v>1.4846856995121667</v>
+      </c>
+      <c r="F8">
+        <v>1.5637658970763419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0499999999722394</v>
+      </c>
+      <c r="D9">
+        <v>0.97310521759683544</v>
+      </c>
+      <c r="E9">
+        <v>0.704929765951823</v>
+      </c>
+      <c r="F9">
+        <v>0.84532963183954124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0.19999999999999957</v>
+      </c>
+      <c r="D10">
+        <v>0.10830961355206511</v>
+      </c>
+      <c r="E10">
+        <v>0.70637102840442134</v>
+      </c>
+      <c r="F10">
+        <v>0.72063893707626925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>200</v>
+      </c>
+      <c r="E13">
+        <v>200</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>45.67280458551334</v>
+      </c>
+      <c r="E14">
+        <v>63.048046154598161</v>
+      </c>
+      <c r="F14">
+        <v>65.720582199051307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>40.000000000000007</v>
+      </c>
+      <c r="D15">
+        <v>44.79199395149989</v>
+      </c>
+      <c r="E15">
+        <v>29.935254602427996</v>
+      </c>
+      <c r="F15">
+        <v>28.421418146269836</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>60.000000000000014</v>
+      </c>
+      <c r="D16">
+        <v>59.53444871317862</v>
+      </c>
+      <c r="E16">
+        <v>44.540570960010214</v>
+      </c>
+      <c r="F16">
+        <v>46.91297691147642</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>40.470107896625159</v>
+      </c>
+      <c r="E17">
+        <v>62.539326087466797</v>
+      </c>
+      <c r="F17">
+        <v>57.855863291935997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>99.224081188632667</v>
+      </c>
+      <c r="E18">
+        <v>148.46856994948786</v>
+      </c>
+      <c r="F18">
+        <v>156.37658970757903</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>100.78198639087648</v>
+      </c>
+      <c r="E19">
+        <v>67.354322894079274</v>
+      </c>
+      <c r="F19">
+        <v>63.948190830224604</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>210</v>
+      </c>
+      <c r="D20">
+        <v>207.42505954038575</v>
+      </c>
+      <c r="E20">
+        <v>196.89417562455813</v>
+      </c>
+      <c r="F20">
+        <v>201.38735349872735</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>200.00000000000006</v>
+      </c>
+      <c r="D21">
+        <v>209.0470952772589</v>
+      </c>
+      <c r="E21">
+        <v>132.61673880825623</v>
+      </c>
+      <c r="F21">
+        <v>128.78356912325972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D22">
+        <v>1.0452354763862945</v>
+      </c>
+      <c r="E22">
+        <v>0.66308369404128109</v>
+      </c>
+      <c r="F22">
+        <v>0.64391784561629861</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C81B5D1-B345-4C07-AAF1-065CD1BD27E8}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.006387575650056</v>
+      </c>
+      <c r="D2">
+        <v>1.0126852580817098</v>
+      </c>
+      <c r="E2">
+        <v>1.0193022237638398</v>
+      </c>
+      <c r="F2">
+        <v>1.026928314669364</v>
+      </c>
+      <c r="G2">
+        <v>1.0377545680283367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0095966476462173</v>
+      </c>
+      <c r="D3">
+        <v>1.0190881035617243</v>
+      </c>
+      <c r="E3">
+        <v>1.0290926053375762</v>
+      </c>
+      <c r="F3">
+        <v>1.0406631890486693</v>
+      </c>
+      <c r="G3">
+        <v>1.0571630630829592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0008350269671129</v>
+      </c>
+      <c r="D4">
+        <v>1.0014491088570601</v>
+      </c>
+      <c r="E4">
+        <v>1.001862188438271</v>
+      </c>
+      <c r="F4">
+        <v>1.0020312308441757</v>
+      </c>
+      <c r="G4">
+        <v>1.0016777194890492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0160455226090923</v>
+      </c>
+      <c r="D5">
+        <v>1.0320154991633979</v>
+      </c>
+      <c r="E5">
+        <v>1.0489563810795042</v>
+      </c>
+      <c r="F5">
+        <v>1.0686864948681873</v>
+      </c>
+      <c r="G5">
+        <v>1.0970757978651695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.99062365945204522</v>
+      </c>
+      <c r="D7">
+        <v>0.98023361021433086</v>
+      </c>
+      <c r="E7">
+        <v>0.96816873805100456</v>
+      </c>
+      <c r="F7">
+        <v>0.95318925131473309</v>
+      </c>
+      <c r="G7">
+        <v>0.93155409308673487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.98747489439651848</v>
+      </c>
+      <c r="D8">
+        <v>0.97407488427239663</v>
+      </c>
+      <c r="E8">
+        <v>0.95895796214597595</v>
+      </c>
+      <c r="F8">
+        <v>0.94060887491218026</v>
+      </c>
+      <c r="G8">
+        <v>0.91445165767240888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.99916566972116849</v>
+      </c>
+      <c r="D9">
+        <v>0.99732896542206706</v>
+      </c>
+      <c r="E9">
+        <v>0.9943694698123019</v>
+      </c>
+      <c r="F9">
+        <v>0.99001673768539966</v>
+      </c>
+      <c r="G9">
+        <v>0.98375023335117484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.0237432725840783</v>
+      </c>
+      <c r="D10">
+        <v>1.0469473301163175</v>
+      </c>
+      <c r="E10">
+        <v>1.0711351761369892</v>
+      </c>
+      <c r="F10">
+        <v>1.0991328545245336</v>
+      </c>
+      <c r="G10">
+        <v>1.1409855970537344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.95689374406213035</v>
+      </c>
+      <c r="D11">
+        <v>0.91107593331151671</v>
+      </c>
+      <c r="E11">
+        <v>0.85945629637063958</v>
+      </c>
+      <c r="F11">
+        <v>0.79586881245096153</v>
+      </c>
+      <c r="G11">
+        <v>0.69919000272678622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.99695134301753163</v>
+      </c>
+      <c r="D12">
+        <v>0.9926681265402667</v>
+      </c>
+      <c r="E12">
+        <v>0.98685654767402087</v>
+      </c>
+      <c r="F12">
+        <v>0.97885703141359282</v>
+      </c>
+      <c r="G12">
+        <v>0.96672451546625382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.98120735816782156</v>
+      </c>
+      <c r="D13">
+        <v>0.96187327355543928</v>
+      </c>
+      <c r="E13">
+        <v>0.94079845975902054</v>
+      </c>
+      <c r="F13">
+        <v>0.91594404543711139</v>
+      </c>
+      <c r="G13">
+        <v>0.88118297509381738</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.0009381670421438</v>
+      </c>
+      <c r="D14">
+        <v>1.024890126404802</v>
+      </c>
+      <c r="E14">
+        <v>1.0796578594751951</v>
+      </c>
+      <c r="F14">
+        <v>1.1897677711350092</v>
+      </c>
+      <c r="G14">
+        <v>1.464804238667671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15">
+        <v>120</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15">
+        <v>120</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16">
+        <v>120</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>120</v>
+      </c>
+      <c r="F16">
+        <v>120</v>
+      </c>
+      <c r="G16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17">
+        <v>340</v>
+      </c>
+      <c r="C17">
+        <v>340</v>
+      </c>
+      <c r="D17">
+        <v>340</v>
+      </c>
+      <c r="E17">
+        <v>340</v>
+      </c>
+      <c r="F17">
+        <v>340</v>
+      </c>
+      <c r="G17">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18">
+        <v>120</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>120</v>
+      </c>
+      <c r="E18">
+        <v>120</v>
+      </c>
+      <c r="F18">
+        <v>119.99999999999999</v>
+      </c>
+      <c r="G18">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19">
+        <v>120</v>
+      </c>
+      <c r="C19">
+        <v>120</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
+      </c>
+      <c r="E19">
+        <v>120</v>
+      </c>
+      <c r="F19">
+        <v>120</v>
+      </c>
+      <c r="G19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>48.460639087018805</v>
+      </c>
+      <c r="D20">
+        <v>48.916228970963118</v>
+      </c>
+      <c r="E20">
+        <v>49.396445056204186</v>
+      </c>
+      <c r="F20">
+        <v>49.951833074336434</v>
+      </c>
+      <c r="G20">
+        <v>50.74382702798205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21">
+        <v>72</v>
+      </c>
+      <c r="C21">
+        <v>71.543013588470316</v>
+      </c>
+      <c r="D21">
+        <v>71.09810222416634</v>
+      </c>
+      <c r="E21">
+        <v>70.63655736385509</v>
+      </c>
+      <c r="F21">
+        <v>70.11200194940696</v>
+      </c>
+      <c r="G21">
+        <v>69.380566675601443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22">
+        <v>72</v>
+      </c>
+      <c r="C22">
+        <v>72.459905446804385</v>
+      </c>
+      <c r="D22">
+        <v>72.913338581883423</v>
+      </c>
+      <c r="E22">
+        <v>73.389760110996932</v>
+      </c>
+      <c r="F22">
+        <v>73.938838656194577</v>
+      </c>
+      <c r="G22">
+        <v>74.718328898040255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>47.543739484384446</v>
+      </c>
+      <c r="D23">
+        <v>47.100932522162822</v>
+      </c>
+      <c r="E23">
+        <v>46.643032659100584</v>
+      </c>
+      <c r="F23">
+        <v>46.124433443138592</v>
+      </c>
+      <c r="G23">
+        <v>45.404537555464387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24">
+        <v>120</v>
+      </c>
+      <c r="C24">
+        <v>120.66574992281421</v>
+      </c>
+      <c r="D24">
+        <v>121.34638684585452</v>
+      </c>
+      <c r="E24">
+        <v>122.08891428703427</v>
+      </c>
+      <c r="F24">
+        <v>122.98159375382461</v>
+      </c>
+      <c r="G24">
+        <v>124.32197077012238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25">
+        <v>120</v>
+      </c>
+      <c r="C25">
+        <v>121.05051727124193</v>
+      </c>
+      <c r="D25">
+        <v>122.11361650416337</v>
+      </c>
+      <c r="E25">
+        <v>123.26157635813239</v>
+      </c>
+      <c r="F25">
+        <v>124.62643762174304</v>
+      </c>
+      <c r="G25">
+        <v>126.64708928003867</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>98.313353437742862</v>
+      </c>
+      <c r="D26">
+        <v>96.658381566822541</v>
+      </c>
+      <c r="E26">
+        <v>94.927588833650503</v>
+      </c>
+      <c r="F26">
+        <v>92.9425627130626</v>
+      </c>
+      <c r="G26">
+        <v>90.141188584628551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>100</v>
+      </c>
+      <c r="G27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B29">
+        <v>340</v>
+      </c>
+      <c r="C29">
+        <v>340</v>
+      </c>
+      <c r="D29">
+        <v>339.58322924414983</v>
+      </c>
+      <c r="E29">
+        <v>338.71519886840156</v>
+      </c>
+      <c r="F29">
+        <v>337.28941467454194</v>
+      </c>
+      <c r="G29">
+        <v>335.03623469860844</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30">
+        <v>340</v>
+      </c>
+      <c r="C30">
+        <v>340.28390916881636</v>
+      </c>
+      <c r="D30">
+        <v>340.49269701139843</v>
+      </c>
+      <c r="E30">
+        <v>340.63314406901054</v>
+      </c>
+      <c r="F30">
+        <v>340.69061848670492</v>
+      </c>
+      <c r="G30">
+        <v>340.57042462627646</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E4A9CC-FD66-466A-9BFD-5A01D2004702}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.4753291369925161</v>
+      </c>
+      <c r="D2">
+        <v>1.172020118830339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.67462966970460647</v>
+      </c>
+      <c r="D3">
+        <v>0.88730009696688272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0219884210945194</v>
+      </c>
+      <c r="D4">
+        <v>1.0127539873734788</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.85587331307868264</v>
+      </c>
+      <c r="D5">
+        <v>1.1577604455328296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.93361463212308304</v>
+      </c>
+      <c r="D6">
+        <v>1.1941203540878473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.89150825224546415</v>
+      </c>
+      <c r="D7">
+        <v>1.1767023168054411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.8092946958164402</v>
+      </c>
+      <c r="D8">
+        <v>1.1366179966603065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.1568021389813885</v>
+      </c>
+      <c r="D9">
+        <v>1.2858741341480677</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.66719621535058538</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="D11">
+        <v>0.13513513513513509</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12">
+        <v>80</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14">
+        <v>180</v>
+      </c>
+      <c r="C14">
+        <v>180</v>
+      </c>
+      <c r="D14">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>18.507205170502843</v>
+      </c>
+      <c r="D15">
+        <v>15.416666680220644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>46.241340904254422</v>
+      </c>
+      <c r="D16">
+        <v>48.668562530759708</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>69.21690975728059</v>
+      </c>
+      <c r="D17">
+        <v>63.035445027072385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>32.282603935879955</v>
+      </c>
+      <c r="D18">
+        <v>37.145792807438056</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>115.48695515904296</v>
+      </c>
+      <c r="D19">
+        <v>92.580834712218973</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>66.011478777535345</v>
+      </c>
+      <c r="D20">
+        <v>87.612599703686627</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21">
+        <v>180</v>
+      </c>
+      <c r="C21">
+        <v>164</v>
+      </c>
+      <c r="D21">
+        <v>214.50779345311349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22">
+        <v>180</v>
+      </c>
+      <c r="C22">
+        <v>183.95791579682032</v>
+      </c>
+      <c r="D22">
+        <v>182.29571772712671</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>0.9</v>
+      </c>
+      <c r="C23">
+        <v>0.91978957898410163</v>
+      </c>
+      <c r="D23">
+        <v>0.91147858863563358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update xslx post-merge and add gams
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBA0310-A59A-4C5C-8242-EE447E93296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6550B1E6-5E9B-4C0F-BFE1-A8CE03D1C0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="14" activeTab="17" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="15" activeTab="18" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="123" sheetId="18" r:id="rId16"/>
     <sheet name="The123" sheetId="19" r:id="rId17"/>
     <sheet name="The123Nested" sheetId="20" r:id="rId18"/>
+    <sheet name="two_by_two_PriceinDem" sheetId="21" r:id="rId19"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="260">
   <si>
     <t>X.L</t>
   </si>
@@ -807,6 +808,21 @@
   </si>
   <si>
     <t>PMHHC</t>
+  </si>
+  <si>
+    <t>DY</t>
+  </si>
+  <si>
+    <t>eRA=.6</t>
+  </si>
+  <si>
+    <t>pr_Ud=3</t>
+  </si>
+  <si>
+    <t>prU2,eRA.5</t>
+  </si>
+  <si>
+    <t>prU.5,eRA.6</t>
   </si>
 </sst>
 </file>
@@ -6504,7 +6520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC21389E-4BBB-4228-B023-E87E0DD3496F}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -7133,6 +7149,828 @@
       </c>
       <c r="F33">
         <v>0.94459176904078701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6126CD16-64E6-45FB-8C64-23F2A918E49C}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0363877164248041</v>
+      </c>
+      <c r="D2">
+        <v>1.0365191201635342</v>
+      </c>
+      <c r="E2">
+        <v>1.0750070482317526</v>
+      </c>
+      <c r="F2">
+        <v>1.0595609099982375</v>
+      </c>
+      <c r="G2">
+        <v>0.99833470833488758</v>
+      </c>
+      <c r="H2">
+        <v>0.98248710709607356</v>
+      </c>
+      <c r="I2">
+        <v>0.94048657015713999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0432700717660239</v>
+      </c>
+      <c r="D3">
+        <v>1.0430741066727305</v>
+      </c>
+      <c r="E3">
+        <v>0.9856633946311647</v>
+      </c>
+      <c r="F3">
+        <v>1.0087067867539614</v>
+      </c>
+      <c r="G3">
+        <v>1.1000067470017649</v>
+      </c>
+      <c r="H3">
+        <v>1.1229317376964334</v>
+      </c>
+      <c r="I3">
+        <v>1.1855074833626029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0388246300487494</v>
+      </c>
+      <c r="D4">
+        <v>1.0389569047712837</v>
+      </c>
+      <c r="E4">
+        <v>1.077706227526201</v>
+      </c>
+      <c r="F4">
+        <v>1.062153685062508</v>
+      </c>
+      <c r="G4">
+        <v>1.0005254867585018</v>
+      </c>
+      <c r="H4">
+        <v>0.99843756359281455</v>
+      </c>
+      <c r="I4">
+        <v>0.99193526198210025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0023513532505028</v>
+      </c>
+      <c r="D5">
+        <v>1.0023518955237618</v>
+      </c>
+      <c r="E5">
+        <v>1.0025108479973333</v>
+      </c>
+      <c r="F5">
+        <v>1.0024470278582356</v>
+      </c>
+      <c r="G5">
+        <v>1.0021944327924277</v>
+      </c>
+      <c r="H5">
+        <v>1.0162347743614697</v>
+      </c>
+      <c r="I5">
+        <v>1.0547043343918923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.99573893485424703</v>
+      </c>
+      <c r="D6">
+        <v>0.9957379554075485</v>
+      </c>
+      <c r="E6">
+        <v>0.99545092202416496</v>
+      </c>
+      <c r="F6">
+        <v>0.99556615181893504</v>
+      </c>
+      <c r="G6">
+        <v>0.99602242515110884</v>
+      </c>
+      <c r="H6">
+        <v>0.97114380037066661</v>
+      </c>
+      <c r="I6">
+        <v>0.90770374205596738</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.94438602708152408</v>
+      </c>
+      <c r="D8">
+        <v>0.94437357942991329</v>
+      </c>
+      <c r="E8">
+        <v>0.94073225025073981</v>
+      </c>
+      <c r="F8">
+        <v>0.94219250114330766</v>
+      </c>
+      <c r="G8">
+        <v>0.94799525094925208</v>
+      </c>
+      <c r="H8">
+        <v>0.89903690333116504</v>
+      </c>
+      <c r="I8">
+        <v>0.84467427236056347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.0388246300416317</v>
+      </c>
+      <c r="D9">
+        <v>1.0388337447788984</v>
+      </c>
+      <c r="E9">
+        <v>1.0415087178322844</v>
+      </c>
+      <c r="F9">
+        <v>1.0404339284150994</v>
+      </c>
+      <c r="G9">
+        <v>1.0361901997038321</v>
+      </c>
+      <c r="H9">
+        <v>1.0329715504842174</v>
+      </c>
+      <c r="I9">
+        <v>0.96149717694622538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>80</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>54</v>
+      </c>
+      <c r="G11">
+        <v>54</v>
+      </c>
+      <c r="H11">
+        <v>54</v>
+      </c>
+      <c r="I11">
+        <v>53.999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12">
+        <v>124</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>124</v>
+      </c>
+      <c r="E12">
+        <v>124</v>
+      </c>
+      <c r="F12">
+        <v>124.00000000000001</v>
+      </c>
+      <c r="G12">
+        <v>124</v>
+      </c>
+      <c r="H12">
+        <v>124</v>
+      </c>
+      <c r="I12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>31.841365430850797</v>
+      </c>
+      <c r="D13">
+        <v>31.841802353436101</v>
+      </c>
+      <c r="E13">
+        <v>31.970122669751873</v>
+      </c>
+      <c r="F13">
+        <v>31.918541910760322</v>
+      </c>
+      <c r="G13">
+        <v>31.715172574535519</v>
+      </c>
+      <c r="H13">
+        <v>30.827982414866039</v>
+      </c>
+      <c r="I13">
+        <v>30.648734246825121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>48.244493065345502</v>
+      </c>
+      <c r="D14">
+        <v>48.244095867355547</v>
+      </c>
+      <c r="E14">
+        <v>48.127818367352575</v>
+      </c>
+      <c r="F14">
+        <v>48.174468386726872</v>
+      </c>
+      <c r="G14">
+        <v>48.359578824249922</v>
+      </c>
+      <c r="H14">
+        <v>49.189872358276311</v>
+      </c>
+      <c r="I14">
+        <v>49.362282267302113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>25.305048730086334</v>
+      </c>
+      <c r="D15">
+        <v>25.305357380693888</v>
+      </c>
+      <c r="E15">
+        <v>25.395985012953503</v>
+      </c>
+      <c r="F15">
+        <v>25.359560402635765</v>
+      </c>
+      <c r="G15">
+        <v>25.215883918854793</v>
+      </c>
+      <c r="H15">
+        <v>25.924910448641455</v>
+      </c>
+      <c r="I15">
+        <v>25.790876462309562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>28.755737186305545</v>
+      </c>
+      <c r="D16">
+        <v>28.755456597924343</v>
+      </c>
+      <c r="E16">
+        <v>28.673334317227702</v>
+      </c>
+      <c r="F16">
+        <v>28.706277005080288</v>
+      </c>
+      <c r="G16">
+        <v>28.837054010926813</v>
+      </c>
+      <c r="H16">
+        <v>28.204372131496193</v>
+      </c>
+      <c r="I16">
+        <v>28.321572766511746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>79.812333011330708</v>
+      </c>
+      <c r="D17">
+        <v>79.812289832779825</v>
+      </c>
+      <c r="E17">
+        <v>79.799635245655324</v>
+      </c>
+      <c r="F17">
+        <v>79.804715637616169</v>
+      </c>
+      <c r="G17">
+        <v>79.824829775888887</v>
+      </c>
+      <c r="H17">
+        <v>78.721966634399237</v>
+      </c>
+      <c r="I17">
+        <v>75.850641162032716</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>44.188289178863421</v>
+      </c>
+      <c r="D18">
+        <v>44.188332644183888</v>
+      </c>
+      <c r="E18">
+        <v>44.201074132845875</v>
+      </c>
+      <c r="F18">
+        <v>44.195958168736873</v>
+      </c>
+      <c r="G18">
+        <v>44.175712201785153</v>
+      </c>
+      <c r="H18">
+        <v>45.307399360636381</v>
+      </c>
+      <c r="I18">
+        <v>48.473965635901315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19">
+        <v>134</v>
+      </c>
+      <c r="C19">
+        <v>139.20250041197306</v>
+      </c>
+      <c r="D19">
+        <v>139.20249020044872</v>
+      </c>
+      <c r="E19">
+        <v>139.20019309147671</v>
+      </c>
+      <c r="F19">
+        <v>139.20094884112044</v>
+      </c>
+      <c r="G19">
+        <v>139.20613388269214</v>
+      </c>
+      <c r="H19">
+        <v>138.76352763367868</v>
+      </c>
+      <c r="I19">
+        <v>137.46365821827374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20">
+        <v>124</v>
+      </c>
+      <c r="C20">
+        <v>128.81425411257209</v>
+      </c>
+      <c r="D20">
+        <v>128.83065617550108</v>
+      </c>
+      <c r="E20">
+        <v>133.63557221313272</v>
+      </c>
+      <c r="F20">
+        <v>131.70705694774796</v>
+      </c>
+      <c r="G20">
+        <v>124.06516035730138</v>
+      </c>
+      <c r="H20">
+        <v>123.80625788538022</v>
+      </c>
+      <c r="I20">
+        <v>122.99997248577242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>10.432700716801408</v>
+      </c>
+      <c r="D21">
+        <v>10.416228455108469</v>
+      </c>
+      <c r="E21">
+        <v>5.5900504537469322</v>
+      </c>
+      <c r="F21">
+        <v>7.5272666509210788</v>
+      </c>
+      <c r="G21">
+        <v>15.201438384375418</v>
+      </c>
+      <c r="H21">
+        <v>15.401704405248296</v>
+      </c>
+      <c r="I21">
+        <v>15.934368299221513</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.0391557242667655</v>
+      </c>
+      <c r="D22">
+        <v>1.0391554626179134</v>
+      </c>
+      <c r="E22">
+        <v>1.0548832266630734</v>
+      </c>
+      <c r="F22">
+        <v>1.0454956618532232</v>
+      </c>
+      <c r="G22">
+        <v>1.0534806670463777</v>
+      </c>
+      <c r="H22">
+        <v>1.0530112713727526</v>
+      </c>
+      <c r="I22">
+        <v>1.0506793942727906</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.99340309326184617</v>
+      </c>
+      <c r="D24">
+        <v>0.99340157868134993</v>
+      </c>
+      <c r="E24">
+        <v>0.99295775603099801</v>
+      </c>
+      <c r="F24">
+        <v>0.9931359205543242</v>
+      </c>
+      <c r="G24">
+        <v>0.99384150675820293</v>
+      </c>
+      <c r="H24">
+        <v>0.9556293731247929</v>
+      </c>
+      <c r="I24">
+        <v>0.86062388525151878</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.99765416264179452</v>
+      </c>
+      <c r="D25">
+        <v>0.99765362291001314</v>
+      </c>
+      <c r="E25">
+        <v>0.99749544057069406</v>
+      </c>
+      <c r="F25">
+        <v>0.9975589454702023</v>
+      </c>
+      <c r="G25">
+        <v>0.9978103721986229</v>
+      </c>
+      <c r="H25">
+        <v>0.98402458292999229</v>
+      </c>
+      <c r="I25">
+        <v>0.94813301452540921</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.94217065105862896</v>
+      </c>
+      <c r="D26">
+        <v>0.94215772289875011</v>
+      </c>
+      <c r="E26">
+        <v>0.93837613042292212</v>
+      </c>
+      <c r="F26">
+        <v>0.93989255787045034</v>
+      </c>
+      <c r="G26">
+        <v>0.94591949419220012</v>
+      </c>
+      <c r="H26">
+        <v>0.88467441383912149</v>
+      </c>
+      <c r="I26">
+        <v>0.8008635641452776</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1.0363877164158561</v>
+      </c>
+      <c r="D27">
+        <v>1.036396249079844</v>
+      </c>
+      <c r="E27">
+        <v>1.0389001973523331</v>
+      </c>
+      <c r="F27">
+        <v>1.0378941724611865</v>
+      </c>
+      <c r="G27">
+        <v>1.0339213288350459</v>
+      </c>
+      <c r="H27">
+        <v>1.0164693991437794</v>
+      </c>
+      <c r="I27">
+        <v>0.91162721683569548</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B28">
+        <v>134</v>
+      </c>
+      <c r="C28">
+        <v>138.87595398615105</v>
+      </c>
+      <c r="D28">
+        <v>138.87586866657327</v>
+      </c>
+      <c r="E28">
+        <v>138.85155793530822</v>
+      </c>
+      <c r="F28">
+        <v>138.86115173439967</v>
+      </c>
+      <c r="G28">
+        <v>138.90132426182038</v>
+      </c>
+      <c r="H28">
+        <v>136.5467224056251</v>
+      </c>
+      <c r="I28">
+        <v>130.3338326541824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tests for Non1 prices in Demand
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6550B1E6-5E9B-4C0F-BFE1-A8CE03D1C0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B907D860-3BA5-42AE-B0D8-7E6166417A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="15" activeTab="18" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
@@ -822,7 +822,7 @@
     <t>prU2,eRA.5</t>
   </si>
   <si>
-    <t>prU.5,eRA.6</t>
+    <t>prUd.5,e.6</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update non-1 Demand price test w 0 elas & add gams
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B907D860-3BA5-42AE-B0D8-7E6166417A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51A386C-75FF-44C1-B6EF-CBAFE049B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="15" activeTab="18" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="261">
   <si>
     <t>X.L</t>
   </si>
@@ -823,6 +823,9 @@
   </si>
   <si>
     <t>prUd.5,e.6</t>
+  </si>
+  <si>
+    <t>prUd.5,e.0</t>
   </si>
 </sst>
 </file>
@@ -7158,13 +7161,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6126CD16-64E6-45FB-8C64-23F2A918E49C}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -7184,13 +7187,16 @@
         <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -7213,13 +7219,16 @@
         <v>0.99833470833488758</v>
       </c>
       <c r="H2">
-        <v>0.98248710709607356</v>
+        <v>1.0367159805528305</v>
       </c>
       <c r="I2">
-        <v>0.94048657015713999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0218924908754679</v>
+      </c>
+      <c r="J2">
+        <v>0.98256190948137989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -7242,13 +7251,16 @@
         <v>1.1000067470017649</v>
       </c>
       <c r="H3">
-        <v>1.1229317376964334</v>
+        <v>1.0427805239888699</v>
       </c>
       <c r="I3">
-        <v>1.1855074833626029</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0641978434498767</v>
+      </c>
+      <c r="J3">
+        <v>1.1228202670038634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>211</v>
       </c>
@@ -7271,13 +7283,16 @@
         <v>1.0005254867585018</v>
       </c>
       <c r="H4">
-        <v>0.99843756359281455</v>
+        <v>1.03915507046988</v>
       </c>
       <c r="I4">
-        <v>0.99193526198210025</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0387071207235727</v>
+      </c>
+      <c r="J4">
+        <v>1.0365510187680878</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>132</v>
       </c>
@@ -7300,13 +7315,16 @@
         <v>1.0021944327924277</v>
       </c>
       <c r="H5">
-        <v>1.0162347743614697</v>
+        <v>1.0023527079378749</v>
       </c>
       <c r="I5">
-        <v>1.0547043343918923</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0164544020024273</v>
+      </c>
+      <c r="J5">
+        <v>1.0549472850165791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -7329,13 +7347,16 @@
         <v>0.99602242515110884</v>
       </c>
       <c r="H6">
-        <v>0.97114380037066661</v>
+        <v>0.99573648804003345</v>
       </c>
       <c r="I6">
-        <v>0.90770374205596738</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.9707623117768589</v>
+      </c>
+      <c r="J6">
+        <v>0.9073237033949143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>212</v>
       </c>
@@ -7363,8 +7384,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>133</v>
       </c>
@@ -7387,13 +7411,16 @@
         <v>0.94799525094925208</v>
       </c>
       <c r="H8">
-        <v>0.89903690333116504</v>
+        <v>0.94435493123749292</v>
       </c>
       <c r="I8">
-        <v>0.84467427236056347</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.89431602404483068</v>
+      </c>
+      <c r="J8">
+        <v>0.83994765227154744</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>178</v>
       </c>
@@ -7416,13 +7443,16 @@
         <v>1.0361901997038321</v>
       </c>
       <c r="H9">
-        <v>1.0329715504842174</v>
+        <v>1.0388474003327777</v>
       </c>
       <c r="I9">
-        <v>0.96149717694622538</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0365981349629205</v>
+      </c>
+      <c r="J9">
+        <v>0.96509548914632604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>213</v>
       </c>
@@ -7450,8 +7480,11 @@
       <c r="I10">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>214</v>
       </c>
@@ -7477,10 +7510,13 @@
         <v>54</v>
       </c>
       <c r="I11">
-        <v>53.999999999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="J11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>215</v>
       </c>
@@ -7508,8 +7544,11 @@
       <c r="I12">
         <v>124</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>216</v>
       </c>
@@ -7532,13 +7571,16 @@
         <v>31.715172574535519</v>
       </c>
       <c r="H13">
-        <v>30.827982414866039</v>
+        <v>31.842456944360443</v>
       </c>
       <c r="I13">
-        <v>30.648734246825121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30.997413605068637</v>
+      </c>
+      <c r="J13">
+        <v>30.828302885539017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>217</v>
       </c>
@@ -7561,13 +7603,16 @@
         <v>48.359578824249922</v>
       </c>
       <c r="H14">
-        <v>49.189872358276311</v>
+        <v>48.243500807548365</v>
       </c>
       <c r="I14">
-        <v>49.362282267302113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>49.028373084915735</v>
+      </c>
+      <c r="J14">
+        <v>49.189565550386192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>218</v>
       </c>
@@ -7590,13 +7635,16 @@
         <v>25.215883918854793</v>
       </c>
       <c r="H15">
-        <v>25.924910448641455</v>
+        <v>25.305819795566755</v>
       </c>
       <c r="I15">
-        <v>25.790876462309562</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26.051524132661086</v>
+      </c>
+      <c r="J15">
+        <v>25.925150004988197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>219</v>
       </c>
@@ -7619,13 +7667,16 @@
         <v>28.837054010926813</v>
       </c>
       <c r="H16">
-        <v>28.204372131496193</v>
+        <v>28.755036236909774</v>
       </c>
       <c r="I16">
-        <v>28.321572766511746</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28.094657293907357</v>
+      </c>
+      <c r="J16">
+        <v>28.204163637656286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>220</v>
       </c>
@@ -7648,13 +7699,16 @@
         <v>79.824829775888887</v>
       </c>
       <c r="H17">
-        <v>78.721966634399237</v>
+        <v>79.812225144363239</v>
       </c>
       <c r="I17">
-        <v>75.850641162032716</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>78.704956997971451</v>
+      </c>
+      <c r="J17">
+        <v>75.833173027923138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>221</v>
       </c>
@@ -7677,13 +7731,16 @@
         <v>44.175712201785153</v>
       </c>
       <c r="H18">
-        <v>45.307399360636381</v>
+        <v>44.188397762351457</v>
       </c>
       <c r="I18">
-        <v>48.473965635901315</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45.325204188719908</v>
+      </c>
+      <c r="J18">
+        <v>48.494269283791553</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>222</v>
       </c>
@@ -7706,13 +7763,16 @@
         <v>139.20613388269214</v>
       </c>
       <c r="H19">
-        <v>138.76352763367868</v>
+        <v>139.2024749421293</v>
       </c>
       <c r="I19">
-        <v>137.46365821827374</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>138.88306022726826</v>
+      </c>
+      <c r="J19">
+        <v>137.93719941830233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>223</v>
       </c>
@@ -7735,13 +7795,16 @@
         <v>124.06516035730138</v>
       </c>
       <c r="H20">
-        <v>123.80625788538022</v>
+        <v>128.85522873815168</v>
       </c>
       <c r="I20">
-        <v>122.99997248577242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128.79968296955442</v>
+      </c>
+      <c r="J20">
+        <v>128.53232632723834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>255</v>
       </c>
@@ -7764,13 +7827,16 @@
         <v>15.201438384375418</v>
       </c>
       <c r="H21">
-        <v>15.401704405248296</v>
+        <v>10.391550704689651</v>
       </c>
       <c r="I21">
-        <v>15.934368299221513</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.387071207222132</v>
+      </c>
+      <c r="J21">
+        <v>10.365510187680512</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -7793,13 +7859,16 @@
         <v>1.0534806670463777</v>
       </c>
       <c r="H22">
-        <v>1.0530112713727526</v>
+        <v>1.0391550704689652</v>
       </c>
       <c r="I22">
-        <v>1.0506793942727906</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0387071207222132</v>
+      </c>
+      <c r="J22">
+        <v>1.0365510187680511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>224</v>
       </c>
@@ -7827,8 +7896,11 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>225</v>
       </c>
@@ -7851,13 +7923,16 @@
         <v>0.99384150675820293</v>
       </c>
       <c r="H24">
-        <v>0.9556293731247929</v>
+        <v>0.9933993095988608</v>
       </c>
       <c r="I24">
-        <v>0.86062388525151878</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.95504757504561499</v>
+      </c>
+      <c r="J24">
+        <v>0.860065442398532</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>226</v>
       </c>
@@ -7880,13 +7955,16 @@
         <v>0.9978103721986229</v>
       </c>
       <c r="H25">
-        <v>0.98402458292999229</v>
+        <v>0.99765281430454245</v>
       </c>
       <c r="I25">
-        <v>0.94813301452540921</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.9838119624746452</v>
+      </c>
+      <c r="J25">
+        <v>0.94791466284903936</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>227</v>
       </c>
@@ -7909,13 +7987,16 @@
         <v>0.94591949419220012</v>
       </c>
       <c r="H26">
-        <v>0.88467441383912149</v>
+        <v>0.94213835485145747</v>
       </c>
       <c r="I26">
-        <v>0.8008635641452776</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.87983880268806691</v>
+      </c>
+      <c r="J26">
+        <v>0.79619869561382606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>228</v>
       </c>
@@ -7938,13 +8019,16 @@
         <v>1.0339213288350459</v>
       </c>
       <c r="H27">
-        <v>1.0164693991437794</v>
+        <v>1.0364090325749533</v>
       </c>
       <c r="I27">
-        <v>0.91162721683569548</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.019817645455428</v>
+      </c>
+      <c r="J27">
+        <v>0.91482816521126842</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>229</v>
       </c>
@@ -7967,10 +8051,13 @@
         <v>138.90132426182038</v>
       </c>
       <c r="H28">
-        <v>136.5467224056251</v>
+        <v>138.87574088417284</v>
       </c>
       <c r="I28">
-        <v>130.3338326541824</v>
+        <v>136.63481603667313</v>
+      </c>
+      <c r="J28">
+        <v>130.75269388094077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test indexed_non-1 price
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9022499-15D9-4809-BDDB-B8F8A8280CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B717B9F-4B47-412F-B41E-711EE24BA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9072" firstSheet="15" activeTab="18" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="-16200" yWindow="-13815" windowWidth="16200" windowHeight="11430" firstSheet="18" activeTab="19" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="The123" sheetId="19" r:id="rId17"/>
     <sheet name="The123Nested" sheetId="20" r:id="rId18"/>
     <sheet name="two_by_two_PriceinDem" sheetId="21" r:id="rId19"/>
+    <sheet name="TwoxTwowOTax_IndPrice_Nest" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="271">
   <si>
     <t>X.L</t>
   </si>
@@ -826,6 +827,36 @@
   </si>
   <si>
     <t>prUd.5,e.0</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>PC.L</t>
+  </si>
+  <si>
+    <t>PF.L</t>
+  </si>
+  <si>
+    <t>SY.L(i)</t>
+  </si>
+  <si>
+    <t>Pr.x=2</t>
+  </si>
+  <si>
+    <t>PC.x=1</t>
+  </si>
+  <si>
+    <t>PF.l=1</t>
   </si>
 </sst>
 </file>
@@ -7163,7 +7194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6126CD16-64E6-45FB-8C64-23F2A918E49C}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -8421,6 +8452,450 @@
       </c>
       <c r="F18">
         <v>6.552950283452402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FD2B6C-BADC-4482-8705-A7286C663A49}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>52.440442414743885</v>
+      </c>
+      <c r="E2">
+        <v>52.440442408506513</v>
+      </c>
+      <c r="F2">
+        <v>52.440442406059617</v>
+      </c>
+      <c r="G2">
+        <v>51.056545362143005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>47.673129456610248</v>
+      </c>
+      <c r="E3">
+        <v>47.673129462280592</v>
+      </c>
+      <c r="F3">
+        <v>47.673129464505024</v>
+      </c>
+      <c r="G3">
+        <v>48.965318398797884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>21.177057061457788</v>
+      </c>
+      <c r="E4">
+        <v>21.177057058435174</v>
+      </c>
+      <c r="F4">
+        <v>21.177057057249421</v>
+      </c>
+      <c r="G4">
+        <v>20.508207428582388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>28.87780507693768</v>
+      </c>
+      <c r="E5">
+        <v>28.877805079685501</v>
+      </c>
+      <c r="F5">
+        <v>28.877805080763462</v>
+      </c>
+      <c r="G5">
+        <v>29.502316482825769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1.0488088482223459</v>
+      </c>
+      <c r="E6">
+        <v>1.0488088481702902</v>
+      </c>
+      <c r="F6">
+        <v>1.0488088481593993</v>
+      </c>
+      <c r="G6">
+        <v>1.256776502947158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.0388601182966062</v>
+      </c>
+      <c r="E7">
+        <v>1.0388601182538628</v>
+      </c>
+      <c r="F7">
+        <v>1.0388601182505186</v>
+      </c>
+      <c r="G7">
+        <v>0.6257657257513739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1.0454820636283344</v>
+      </c>
+      <c r="E8">
+        <v>1.0454820635787618</v>
+      </c>
+      <c r="F8">
+        <v>1.0454820635708382</v>
+      </c>
+      <c r="G8">
+        <v>1.0931727477635904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.99795751000197275</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1.0488088481386344</v>
+      </c>
+      <c r="G9">
+        <v>1.0211309078784696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1.0075145327263733</v>
+      </c>
+      <c r="E10">
+        <v>1.0095765827768823</v>
+      </c>
+      <c r="F10">
+        <v>1.0588528528793757</v>
+      </c>
+      <c r="G10">
+        <v>1.0254103720418588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.95151515128525777</v>
+      </c>
+      <c r="E11">
+        <v>0.95346258924559502</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1.0466666666627262</v>
+      </c>
+      <c r="E12">
+        <v>1.0488088481701119</v>
+      </c>
+      <c r="F12">
+        <v>1.0999999998973025</v>
+      </c>
+      <c r="G12">
+        <v>1.0427083297266266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1.0011330687136686</v>
+      </c>
+      <c r="E13">
+        <v>1.0031820580257127</v>
+      </c>
+      <c r="F13">
+        <v>1.0521462187479673</v>
+      </c>
+      <c r="G13">
+        <v>0.97829409400508083</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>100.31820580330329</v>
+      </c>
+      <c r="E14">
+        <v>100.31820580257127</v>
+      </c>
+      <c r="F14">
+        <v>100.318205802237</v>
+      </c>
+      <c r="G14">
+        <v>114.96595624939472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>49.683306602247974</v>
+      </c>
+      <c r="E15">
+        <v>49.68330660297304</v>
+      </c>
+      <c r="F15">
+        <v>49.683306603304153</v>
+      </c>
+      <c r="G15">
+        <v>28.6215388689448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16">
+        <v>150</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+      <c r="G16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>50</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+      <c r="D19">
+        <v>157</v>
+      </c>
+      <c r="E19">
+        <v>157.32132722551978</v>
+      </c>
+      <c r="F19">
+        <v>164.99999999178419</v>
+      </c>
+      <c r="G19">
+        <v>160.41666637813012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for Indexed Demand non-1 prices, plus
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B717B9F-4B47-412F-B41E-711EE24BA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0694E654-8E77-43B2-87AA-7A353EEC9676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-13815" windowWidth="16200" windowHeight="11430" firstSheet="18" activeTab="19" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="-16200" yWindow="-13815" windowWidth="16200" windowHeight="11430" firstSheet="19" activeTab="20" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="The123Nested" sheetId="20" r:id="rId18"/>
     <sheet name="two_by_two_PriceinDem" sheetId="21" r:id="rId19"/>
     <sheet name="TwoxTwowOTax_IndPrice_Nest" sheetId="22" r:id="rId20"/>
+    <sheet name="TwoxTwo_DemandIndPrice_Nest" sheetId="23" r:id="rId21"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="274">
   <si>
     <t>X.L</t>
   </si>
@@ -857,6 +858,15 @@
   </si>
   <si>
     <t>PF.l=1</t>
+  </si>
+  <si>
+    <t>FDRA</t>
+  </si>
+  <si>
+    <t>FDRA.L</t>
+  </si>
+  <si>
+    <t>Pr.l=1.5</t>
   </si>
 </sst>
 </file>
@@ -8461,7 +8471,474 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FD2B6C-BADC-4482-8705-A7286C663A49}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>52.440442414743885</v>
+      </c>
+      <c r="E2">
+        <v>52.440442408506513</v>
+      </c>
+      <c r="F2">
+        <v>52.440442406059617</v>
+      </c>
+      <c r="G2">
+        <v>51.056545362143005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>47.673129456610248</v>
+      </c>
+      <c r="E3">
+        <v>47.673129462280592</v>
+      </c>
+      <c r="F3">
+        <v>47.673129464505024</v>
+      </c>
+      <c r="G3">
+        <v>48.965318398797884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>21.177057061457788</v>
+      </c>
+      <c r="E4">
+        <v>21.177057058435174</v>
+      </c>
+      <c r="F4">
+        <v>21.177057057249421</v>
+      </c>
+      <c r="G4">
+        <v>20.508207428582388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>28.87780507693768</v>
+      </c>
+      <c r="E5">
+        <v>28.877805079685501</v>
+      </c>
+      <c r="F5">
+        <v>28.877805080763462</v>
+      </c>
+      <c r="G5">
+        <v>29.502316482825769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1.0488088482223459</v>
+      </c>
+      <c r="E6">
+        <v>1.0488088481702902</v>
+      </c>
+      <c r="F6">
+        <v>1.0488088481593993</v>
+      </c>
+      <c r="G6">
+        <v>1.256776502947158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.0388601182966062</v>
+      </c>
+      <c r="E7">
+        <v>1.0388601182538628</v>
+      </c>
+      <c r="F7">
+        <v>1.0388601182505186</v>
+      </c>
+      <c r="G7">
+        <v>0.6257657257513739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1.0454820636283344</v>
+      </c>
+      <c r="E8">
+        <v>1.0454820635787618</v>
+      </c>
+      <c r="F8">
+        <v>1.0454820635708382</v>
+      </c>
+      <c r="G8">
+        <v>1.0931727477635904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.99795751000197275</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1.0488088481386344</v>
+      </c>
+      <c r="G9">
+        <v>1.0211309078784696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1.0075145327263733</v>
+      </c>
+      <c r="E10">
+        <v>1.0095765827768823</v>
+      </c>
+      <c r="F10">
+        <v>1.0588528528793757</v>
+      </c>
+      <c r="G10">
+        <v>1.0254103720418588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.95151515128525777</v>
+      </c>
+      <c r="E11">
+        <v>0.95346258924559502</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1.0466666666627262</v>
+      </c>
+      <c r="E12">
+        <v>1.0488088481701119</v>
+      </c>
+      <c r="F12">
+        <v>1.0999999998973025</v>
+      </c>
+      <c r="G12">
+        <v>1.0427083297266266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1.0011330687136686</v>
+      </c>
+      <c r="E13">
+        <v>1.0031820580257127</v>
+      </c>
+      <c r="F13">
+        <v>1.0521462187479673</v>
+      </c>
+      <c r="G13">
+        <v>0.97829409400508083</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>100.31820580330329</v>
+      </c>
+      <c r="E14">
+        <v>100.31820580257127</v>
+      </c>
+      <c r="F14">
+        <v>100.318205802237</v>
+      </c>
+      <c r="G14">
+        <v>114.96595624939472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>49.683306602247974</v>
+      </c>
+      <c r="E15">
+        <v>49.68330660297304</v>
+      </c>
+      <c r="F15">
+        <v>49.683306603304153</v>
+      </c>
+      <c r="G15">
+        <v>28.6215388689448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16">
+        <v>150</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+      <c r="G16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>50</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+      <c r="D19">
+        <v>157</v>
+      </c>
+      <c r="E19">
+        <v>157.32132722551978</v>
+      </c>
+      <c r="F19">
+        <v>164.99999999178419</v>
+      </c>
+      <c r="G19">
+        <v>160.41666637813012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20">
+        <v>156.82230954744654</v>
+      </c>
+      <c r="E20">
+        <v>156.82230953684729</v>
+      </c>
+      <c r="F20">
+        <v>156.82230953424977</v>
+      </c>
+      <c r="G20">
+        <v>163.97591211186131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391905BC-1CB1-477C-AE0B-70AD8093AF6F}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8478,10 +8955,10 @@
         <v>269</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -8498,13 +8975,13 @@
         <v>52.440442414743885</v>
       </c>
       <c r="E2">
-        <v>52.440442408506513</v>
+        <v>52.44044240850053</v>
       </c>
       <c r="F2">
-        <v>52.440442406059617</v>
+        <v>52.440442408507572</v>
       </c>
       <c r="G2">
-        <v>51.056545362143005</v>
+        <v>56.505734300898233</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -8518,16 +8995,16 @@
         <v>50</v>
       </c>
       <c r="D3">
-        <v>47.673129456610248</v>
+        <v>47.673129456610255</v>
       </c>
       <c r="E3">
-        <v>47.673129462280592</v>
+        <v>47.673129462286035</v>
       </c>
       <c r="F3">
-        <v>47.673129464505024</v>
+        <v>47.673129462279618</v>
       </c>
       <c r="G3">
-        <v>48.965318398797884</v>
+        <v>44.243297267623674</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -8535,22 +9012,22 @@
         <v>264</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>21.177057061457788</v>
+        <v>1.0488088482223461</v>
       </c>
       <c r="E4">
-        <v>21.177057058435174</v>
+        <v>1.0488088481701505</v>
       </c>
       <c r="F4">
-        <v>21.177057057249421</v>
+        <v>1.0488088481701512</v>
       </c>
       <c r="G4">
-        <v>20.508207428582388</v>
+        <v>1.1301146860180615</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -8558,73 +9035,73 @@
         <v>264</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>28.87780507693768</v>
+        <v>1.038860118296606</v>
       </c>
       <c r="E5">
-        <v>28.877805079685501</v>
+        <v>1.0388601182540864</v>
       </c>
       <c r="F5">
-        <v>28.877805080763462</v>
+        <v>1.0388601182540844</v>
       </c>
       <c r="G5">
-        <v>29.502316482825769</v>
+        <v>1.1028031931984548</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>264</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>1.0488088482223459</v>
+        <v>21.177057061457777</v>
       </c>
       <c r="E6">
-        <v>1.0488088481702902</v>
+        <v>21.177057058432275</v>
       </c>
       <c r="F6">
-        <v>1.0488088481593993</v>
+        <v>21.17705705843569</v>
       </c>
       <c r="G6">
-        <v>1.256776502947158</v>
+        <v>23.162051242333568</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>264</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>1.0388601182966062</v>
+        <v>28.87780507693768</v>
       </c>
       <c r="E7">
-        <v>1.0388601182538628</v>
+        <v>28.877805079688141</v>
       </c>
       <c r="F7">
-        <v>1.0388601182505186</v>
+        <v>28.877805079685036</v>
       </c>
       <c r="G7">
-        <v>0.6257657257513739</v>
+        <v>27.203403277237111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>211</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>36</v>
@@ -8636,266 +9113,358 @@
         <v>1.0454820636283344</v>
       </c>
       <c r="E8">
-        <v>1.0454820635787618</v>
+        <v>1.0454820635789994</v>
       </c>
       <c r="F8">
-        <v>1.0454820635708382</v>
+        <v>1.0454820635789992</v>
       </c>
       <c r="G8">
-        <v>1.0931727477635904</v>
+        <v>1.120936516833051</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>265</v>
+        <v>222</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>261</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D9">
-        <v>0.99795751000197275</v>
+        <v>157</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>156.82230953684154</v>
       </c>
       <c r="F9">
-        <v>1.0488088481386344</v>
+        <v>196.02788418875843</v>
       </c>
       <c r="G9">
-        <v>1.0211309078784696</v>
+        <v>179.17273628427864</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>265</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1.0075145327263733</v>
+        <v>0.99795751000197275</v>
       </c>
       <c r="E10">
-        <v>1.0095765827768823</v>
+        <v>0.99682803534981368</v>
       </c>
       <c r="F10">
-        <v>1.0588528528793757</v>
+        <v>1.2460350268196583</v>
       </c>
       <c r="G10">
-        <v>1.0254103720418588</v>
+        <v>1.1301146860180069</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>266</v>
+        <v>129</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.95151515128525777</v>
+        <v>1.0075145327263735</v>
       </c>
       <c r="E11">
-        <v>0.95346258924559502</v>
+        <v>1.0063742415446353</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>1.2579677843968975</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>1.15810256211672</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>266</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1.0466666666627262</v>
+        <v>0.95151515128525788</v>
       </c>
       <c r="E12">
-        <v>1.0488088481701119</v>
+        <v>0.95043823961735774</v>
       </c>
       <c r="F12">
-        <v>1.0999999998973025</v>
+        <v>1.1880477829621725</v>
       </c>
       <c r="G12">
-        <v>1.0427083297266266</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>263</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1.0011330687136686</v>
+        <v>1.046666666662726</v>
       </c>
       <c r="E13">
-        <v>1.0031820580257127</v>
+        <v>1.0454820635788122</v>
       </c>
       <c r="F13">
-        <v>1.0521462187479673</v>
+        <v>1.3068525612583894</v>
       </c>
       <c r="G13">
-        <v>0.97829409400508083</v>
+        <v>1.2771592035534829</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>212</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>100.31820580330329</v>
+        <v>1.0011330687136686</v>
       </c>
       <c r="E14">
-        <v>100.31820580257127</v>
+        <v>0.99999999999989331</v>
       </c>
       <c r="F14">
-        <v>100.318205802237</v>
+        <v>1.4999999651541418</v>
       </c>
       <c r="G14">
-        <v>114.96595624939472</v>
+        <v>1.2787360111381831</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>212</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>49.683306602247974</v>
+        <v>1.0011330687136686</v>
       </c>
       <c r="E15">
-        <v>49.68330660297304</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>49.683306603304153</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>28.6215388689448</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>223</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>261</v>
       </c>
       <c r="C16">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D16">
-        <v>150</v>
+        <v>100.31820580330329</v>
       </c>
       <c r="E16">
-        <v>150</v>
+        <v>100.31820580257052</v>
       </c>
       <c r="F16">
-        <v>150</v>
+        <v>100.31820580257143</v>
       </c>
       <c r="G16">
-        <v>150</v>
+        <v>100.81879473522184</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>267</v>
+        <v>223</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>100</v>
+        <v>49.68330660224796</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>49.683306602973794</v>
       </c>
       <c r="F17">
-        <v>100</v>
+        <v>49.683306602972884</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>49.191152961729621</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="E18">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F18">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="G18">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>215</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>263</v>
       </c>
       <c r="C19">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="D19">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="E19">
-        <v>157.32132722551978</v>
+        <v>75</v>
       </c>
       <c r="F19">
-        <v>164.99999999178419</v>
+        <v>75</v>
       </c>
       <c r="G19">
-        <v>160.41666637813012</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22">
+        <v>75</v>
+      </c>
+      <c r="D22">
+        <v>78.411154773723268</v>
+      </c>
+      <c r="E22">
+        <v>78.411154768429128</v>
+      </c>
+      <c r="F22">
+        <v>78.411155497039374</v>
+      </c>
+      <c r="G22">
+        <v>84.070238762479107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>78.411154773723268</v>
+      </c>
+      <c r="E23">
+        <v>78.411154768420772</v>
+      </c>
+      <c r="F23">
+        <v>78.411153675503371</v>
+      </c>
+      <c r="G23">
+        <v>71.669094513711457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>